<commit_message>
updated how mortality is calculated, fixed formatting of cause of death dist in spreadsheet to be %
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Jan/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Jan/InputForCode_Bangladesh.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-33520" yWindow="1580" windowWidth="25380" windowHeight="14140" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="-35060" yWindow="500" windowWidth="26160" windowHeight="14760" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="demographics" sheetId="1" r:id="rId1"/>
@@ -755,7 +755,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2135,7 +2135,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B14" sqref="B13:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -4897,8 +4897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -4947,8 +4947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -5390,7 +5390,7 @@
         <v>0</v>
       </c>
       <c r="G19" s="25">
-        <v>2.5897000000000001</v>
+        <v>2.5897E-2</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="15.75" customHeight="1">
@@ -5413,7 +5413,7 @@
         <v>0</v>
       </c>
       <c r="G20" s="25">
-        <v>0.71409999999999996</v>
+        <v>7.1409999999999998E-3</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1">
@@ -5436,7 +5436,7 @@
         <v>0</v>
       </c>
       <c r="G21" s="25">
-        <v>25.594200000000001</v>
+        <v>0.255942</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1">
@@ -5459,7 +5459,7 @@
         <v>0</v>
       </c>
       <c r="G22" s="25">
-        <v>14.636699999999999</v>
+        <v>0.146367</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15.75" customHeight="1">
@@ -5482,7 +5482,7 @@
         <v>0</v>
       </c>
       <c r="G23" s="25">
-        <v>1.7554000000000001</v>
+        <v>1.7554E-2</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1">
@@ -5505,7 +5505,7 @@
         <v>0</v>
       </c>
       <c r="G24" s="25">
-        <v>1.8078000000000001</v>
+        <v>1.8078E-2</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1">
@@ -5528,7 +5528,7 @@
         <v>0</v>
       </c>
       <c r="G25" s="25">
-        <v>1.1439999999999999</v>
+        <v>1.1440000000000001E-2</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1">
@@ -5551,7 +5551,7 @@
         <v>0</v>
       </c>
       <c r="G26" s="25">
-        <v>15.1288</v>
+        <v>0.15128800000000001</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1">
@@ -5574,7 +5574,7 @@
         <v>0</v>
       </c>
       <c r="G27" s="25">
-        <v>36.629300000000001</v>
+        <v>0.36629299999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added delivery type to spreadsheet, data.py and keylist in helper. Now reads delivery type distribution into data
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Jan/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Jan/InputForCode_Bangladesh.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-35060" yWindow="500" windowWidth="26160" windowHeight="14760" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="-35900" yWindow="80" windowWidth="25600" windowHeight="14600" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="demographics" sheetId="1" r:id="rId1"/>
@@ -178,6 +178,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
+    <author>Ruth</author>
   </authors>
   <commentList>
     <comment ref="E12" authorId="0">
@@ -190,6 +191,50 @@
           </rPr>
           <t>Nick:
 Any breastfeeding. Other categories don't matter for this age upwards as relative risks are the same.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B17" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Basic Emergency Obstetric Care Centre</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B18" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Comprehensive Emergency Obstetric Care Services</t>
         </r>
       </text>
     </comment>
@@ -306,7 +351,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="95">
   <si>
     <t>indicators</t>
   </si>
@@ -573,6 +618,24 @@
   </si>
   <si>
     <t>maternal: Indirect causes</t>
+  </si>
+  <si>
+    <t>BEmOC</t>
+  </si>
+  <si>
+    <t>CEmOC</t>
+  </si>
+  <si>
+    <t>Delivery</t>
+  </si>
+  <si>
+    <t>unassisted</t>
+  </si>
+  <si>
+    <t>assisted at home</t>
+  </si>
+  <si>
+    <t>essential care</t>
   </si>
 </sst>
 </file>
@@ -659,7 +722,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -678,6 +741,30 @@
         <bgColor rgb="FFDAEEF3"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -688,7 +775,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -700,8 +787,12 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -717,9 +808,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -756,18 +844,33 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="4" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2179,7 +2282,7 @@
       <c r="A5" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="B5" s="13">
+      <c r="B5" s="12">
         <v>0.56799999999999995</v>
       </c>
     </row>
@@ -2187,7 +2290,7 @@
       <c r="A6" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="B6" s="23">
+      <c r="B6" s="22">
         <v>0.4</v>
       </c>
     </row>
@@ -2195,7 +2298,7 @@
       <c r="A7" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="B7" s="23">
+      <c r="B7" s="22">
         <v>0.20599999999999999</v>
       </c>
     </row>
@@ -2855,7 +2958,7 @@
       <c r="A1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>53</v>
       </c>
       <c r="C1" t="s">
@@ -2869,152 +2972,152 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="14">
+      <c r="B2" s="13">
         <v>1</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2" s="14">
-        <v>1</v>
-      </c>
-      <c r="E2" s="14">
+      <c r="D2" s="13">
+        <v>1</v>
+      </c>
+      <c r="E2" s="13">
         <v>1</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B3" s="13">
         <v>1</v>
       </c>
       <c r="C3">
         <v>2.0099999999999998</v>
       </c>
-      <c r="D3" s="14">
+      <c r="D3" s="13">
         <v>3.39</v>
       </c>
-      <c r="E3" s="14">
+      <c r="E3" s="13">
         <v>11.89</v>
       </c>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4" s="13">
         <v>1</v>
       </c>
       <c r="C4">
         <v>2.0099999999999998</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4" s="13">
         <v>3.39</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E4" s="13">
         <v>11.89</v>
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="13">
         <v>1</v>
       </c>
       <c r="C5">
         <v>2.0099999999999998</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="13">
         <v>3.39</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E5" s="13">
         <v>11.89</v>
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="13">
         <v>1</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="13">
         <v>999.99</v>
       </c>
-      <c r="E6" s="14">
+      <c r="E6" s="13">
         <v>999.99</v>
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="14">
+      <c r="B7" s="13">
         <v>1</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
-      <c r="D7" s="14">
-        <v>1</v>
-      </c>
-      <c r="E7" s="14">
+      <c r="D7" s="13">
+        <v>1</v>
+      </c>
+      <c r="E7" s="13">
         <v>1</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="B8" s="14">
+      <c r="B8" s="13">
         <v>1</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
-      <c r="D8" s="14">
-        <v>1</v>
-      </c>
-      <c r="E8" s="14">
+      <c r="D8" s="13">
+        <v>1</v>
+      </c>
+      <c r="E8" s="13">
         <v>1</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="14">
+      <c r="B9" s="13">
         <v>1</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
-      <c r="D9" s="14">
-        <v>1</v>
-      </c>
-      <c r="E9" s="14">
+      <c r="D9" s="13">
+        <v>1</v>
+      </c>
+      <c r="E9" s="13">
         <v>1</v>
       </c>
       <c r="F9" s="6"/>
@@ -3375,30 +3478,30 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="14" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A2" s="16">
-        <v>1</v>
-      </c>
-      <c r="B2" s="16">
+      <c r="A2" s="15">
+        <v>1</v>
+      </c>
+      <c r="B2" s="15">
         <v>5</v>
       </c>
-      <c r="C2" s="16">
+      <c r="C2" s="15">
         <v>6.4</v>
       </c>
-      <c r="D2" s="16">
+      <c r="D2" s="15">
         <v>46.5</v>
       </c>
     </row>
@@ -3661,19 +3764,19 @@
       <c r="A2" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="B2" s="17">
+      <c r="B2" s="16">
         <v>5.16</v>
       </c>
-      <c r="C2" s="17">
+      <c r="C2" s="16">
         <v>5.16</v>
       </c>
-      <c r="D2" s="17">
-        <v>1</v>
-      </c>
-      <c r="E2" s="18">
-        <v>1</v>
-      </c>
-      <c r="F2" s="19">
+      <c r="D2" s="16">
+        <v>1</v>
+      </c>
+      <c r="E2" s="17">
+        <v>1</v>
+      </c>
+      <c r="F2" s="18">
         <v>1</v>
       </c>
     </row>
@@ -3681,19 +3784,19 @@
       <c r="A3" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="B3" s="17">
-        <v>1</v>
-      </c>
-      <c r="C3" s="17">
-        <v>1</v>
-      </c>
-      <c r="D3" s="17">
+      <c r="B3" s="16">
+        <v>1</v>
+      </c>
+      <c r="C3" s="16">
+        <v>1</v>
+      </c>
+      <c r="D3" s="16">
         <v>1.82</v>
       </c>
-      <c r="E3" s="19">
+      <c r="E3" s="18">
         <v>1.82</v>
       </c>
-      <c r="F3" s="19">
+      <c r="F3" s="18">
         <v>1</v>
       </c>
     </row>
@@ -3744,19 +3847,19 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="14">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="17" t="s">
         <v>48</v>
       </c>
     </row>
@@ -3788,7 +3891,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
@@ -3970,7 +4075,7 @@
         <v>0.35</v>
       </c>
       <c r="E2" s="6"/>
-      <c r="F2" s="20"/>
+      <c r="F2" s="19"/>
       <c r="G2" s="6"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1">
@@ -3987,7 +4092,7 @@
         <v>3.56</v>
       </c>
       <c r="E3" s="6"/>
-      <c r="F3" s="20"/>
+      <c r="F3" s="19"/>
       <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1">
@@ -4004,7 +4109,7 @@
         <v>48</v>
       </c>
       <c r="E4" s="6"/>
-      <c r="F4" s="20"/>
+      <c r="F4" s="19"/>
       <c r="G4" s="6"/>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1">
@@ -4021,7 +4126,7 @@
         <v>3.56</v>
       </c>
       <c r="E5" s="6"/>
-      <c r="F5" s="20"/>
+      <c r="F5" s="19"/>
       <c r="G5" s="6"/>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1">
@@ -4038,7 +4143,7 @@
         <v>25</v>
       </c>
       <c r="E6" s="6"/>
-      <c r="F6" s="20"/>
+      <c r="F6" s="19"/>
       <c r="G6" s="6"/>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1">
@@ -4055,7 +4160,7 @@
         <v>1.8</v>
       </c>
       <c r="E7" s="6"/>
-      <c r="F7" s="20"/>
+      <c r="F7" s="19"/>
       <c r="G7" s="6"/>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1">
@@ -4484,16 +4589,16 @@
       <c r="B2" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="21">
+      <c r="C2" s="20">
         <v>0.21</v>
       </c>
-      <c r="D2" s="21">
+      <c r="D2" s="20">
         <v>0.21</v>
       </c>
-      <c r="E2" s="21">
-        <v>0</v>
-      </c>
-      <c r="F2" s="21">
+      <c r="E2" s="20">
+        <v>0</v>
+      </c>
+      <c r="F2" s="20">
         <v>0</v>
       </c>
     </row>
@@ -4501,18 +4606,18 @@
       <c r="B3" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="21">
+      <c r="C3" s="20">
         <f>demographics!$B$5 * 'Interventions target population'!$G$6</f>
         <v>0.22719999999999999</v>
       </c>
-      <c r="D3" s="21">
+      <c r="D3" s="20">
         <f>demographics!$B$5 * 'Interventions target population'!$G$6</f>
         <v>0.22719999999999999</v>
       </c>
-      <c r="E3" s="21">
-        <v>0</v>
-      </c>
-      <c r="F3" s="21">
+      <c r="E3" s="20">
+        <v>0</v>
+      </c>
+      <c r="F3" s="20">
         <v>0</v>
       </c>
     </row>
@@ -4523,16 +4628,16 @@
       <c r="B4" t="s">
         <v>66</v>
       </c>
-      <c r="C4" s="21">
+      <c r="C4" s="20">
         <v>0.1</v>
       </c>
-      <c r="D4" s="21">
+      <c r="D4" s="20">
         <v>0.1</v>
       </c>
-      <c r="E4" s="21">
-        <v>0</v>
-      </c>
-      <c r="F4" s="21">
+      <c r="E4" s="20">
+        <v>0</v>
+      </c>
+      <c r="F4" s="20">
         <v>0</v>
       </c>
     </row>
@@ -4540,16 +4645,16 @@
       <c r="B5" t="s">
         <v>69</v>
       </c>
-      <c r="C5" s="21">
-        <v>1</v>
-      </c>
-      <c r="D5" s="21">
-        <v>1</v>
-      </c>
-      <c r="E5" s="21">
-        <v>0</v>
-      </c>
-      <c r="F5" s="21">
+      <c r="C5" s="20">
+        <v>1</v>
+      </c>
+      <c r="D5" s="20">
+        <v>1</v>
+      </c>
+      <c r="E5" s="20">
+        <v>0</v>
+      </c>
+      <c r="F5" s="20">
         <v>0</v>
       </c>
     </row>
@@ -4615,10 +4720,10 @@
       <c r="E2" s="6">
         <v>0.33500000000000002</v>
       </c>
-      <c r="F2" s="22">
+      <c r="F2" s="21">
         <v>0.33500000000000002</v>
       </c>
-      <c r="G2" s="22">
+      <c r="G2" s="21">
         <v>0.33500000000000002</v>
       </c>
     </row>
@@ -4947,7 +5052,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
@@ -4983,7 +5088,7 @@
       <c r="A2" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="10">
+      <c r="B2" s="9">
         <v>7.0000000000000001E-3</v>
       </c>
       <c r="C2" s="6">
@@ -5006,7 +5111,7 @@
       <c r="A3" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="9">
         <v>0.19900000000000001</v>
       </c>
       <c r="C3" s="6">
@@ -5029,7 +5134,7 @@
       <c r="A4" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="9">
         <v>5.8999999999999997E-2</v>
       </c>
       <c r="C4" s="6">
@@ -5052,7 +5157,7 @@
       <c r="A5" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="9">
         <v>0.22900000000000001</v>
       </c>
       <c r="C5" s="6">
@@ -5075,7 +5180,7 @@
       <c r="A6" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="9">
         <v>0.29699999999999999</v>
       </c>
       <c r="C6" s="6">
@@ -5098,7 +5203,7 @@
       <c r="A7" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7" s="9">
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="C7" s="6">
@@ -5121,7 +5226,7 @@
       <c r="A8" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="9">
         <v>0.127</v>
       </c>
       <c r="C8" s="6">
@@ -5144,7 +5249,7 @@
       <c r="A9" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B9" s="9">
         <v>7.5999999999999998E-2</v>
       </c>
       <c r="C9" s="6">
@@ -5167,19 +5272,19 @@
       <c r="A10" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="10">
-        <v>0</v>
-      </c>
-      <c r="C10" s="10">
+      <c r="B10" s="9">
+        <v>0</v>
+      </c>
+      <c r="C10" s="9">
         <v>0.14810000000000001</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="9">
         <v>0.14810000000000001</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="9">
         <v>0.14810000000000001</v>
       </c>
-      <c r="F10" s="10">
+      <c r="F10" s="9">
         <v>0.14810000000000001</v>
       </c>
       <c r="G10" s="6">
@@ -5190,19 +5295,19 @@
       <c r="A11" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="10">
-        <v>0</v>
-      </c>
-      <c r="C11" s="10">
+      <c r="B11" s="9">
+        <v>0</v>
+      </c>
+      <c r="C11" s="9">
         <v>0.2883</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="9">
         <v>0.2883</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="9">
         <v>0.2883</v>
       </c>
-      <c r="F11" s="10">
+      <c r="F11" s="9">
         <v>0.2883</v>
       </c>
       <c r="G11" s="6">
@@ -5213,19 +5318,19 @@
       <c r="A12" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="10">
-        <v>0</v>
-      </c>
-      <c r="C12" s="10">
+      <c r="B12" s="9">
+        <v>0</v>
+      </c>
+      <c r="C12" s="9">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="9">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="9">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="F12" s="10">
+      <c r="F12" s="9">
         <v>4.1000000000000002E-2</v>
       </c>
       <c r="G12" s="6">
@@ -5239,16 +5344,16 @@
       <c r="B13" s="6">
         <v>0</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="9">
         <v>5.0099999999999999E-2</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="9">
         <v>5.0099999999999999E-2</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13" s="9">
         <v>5.0099999999999999E-2</v>
       </c>
-      <c r="F13" s="10">
+      <c r="F13" s="9">
         <v>5.0099999999999999E-2</v>
       </c>
       <c r="G13" s="6">
@@ -5262,16 +5367,16 @@
       <c r="B14" s="6">
         <v>0</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C14" s="9">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="D14" s="10">
+      <c r="D14" s="9">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="E14" s="10">
+      <c r="E14" s="9">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="F14" s="10">
+      <c r="F14" s="9">
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="G14" s="6">
@@ -5285,16 +5390,16 @@
       <c r="B15" s="6">
         <v>0</v>
       </c>
-      <c r="C15" s="10">
+      <c r="C15" s="9">
         <v>0.01</v>
       </c>
-      <c r="D15" s="10">
+      <c r="D15" s="9">
         <v>0.01</v>
       </c>
-      <c r="E15" s="10">
+      <c r="E15" s="9">
         <v>0.01</v>
       </c>
-      <c r="F15" s="10">
+      <c r="F15" s="9">
         <v>0.01</v>
       </c>
       <c r="G15" s="6">
@@ -5308,16 +5413,16 @@
       <c r="B16" s="6">
         <v>0</v>
       </c>
-      <c r="C16" s="10">
-        <v>0</v>
-      </c>
-      <c r="D16" s="10">
-        <v>0</v>
-      </c>
-      <c r="E16" s="10">
-        <v>0</v>
-      </c>
-      <c r="F16" s="10">
+      <c r="C16" s="9">
+        <v>0</v>
+      </c>
+      <c r="D16" s="9">
+        <v>0</v>
+      </c>
+      <c r="E16" s="9">
+        <v>0</v>
+      </c>
+      <c r="F16" s="9">
         <v>0</v>
       </c>
       <c r="G16" s="6">
@@ -5331,16 +5436,16 @@
       <c r="B17" s="6">
         <v>0</v>
       </c>
-      <c r="C17" s="10">
+      <c r="C17" s="9">
         <v>0.14510000000000001</v>
       </c>
-      <c r="D17" s="10">
+      <c r="D17" s="9">
         <v>0.14510000000000001</v>
       </c>
-      <c r="E17" s="10">
+      <c r="E17" s="9">
         <v>0.14510000000000001</v>
       </c>
-      <c r="F17" s="10">
+      <c r="F17" s="9">
         <v>0.14510000000000001</v>
       </c>
       <c r="G17" s="6">
@@ -5354,16 +5459,16 @@
       <c r="B18" s="6">
         <v>0</v>
       </c>
-      <c r="C18" s="10">
+      <c r="C18" s="9">
         <v>0.31130000000000002</v>
       </c>
-      <c r="D18" s="10">
+      <c r="D18" s="9">
         <v>0.31130000000000002</v>
       </c>
-      <c r="E18" s="10">
+      <c r="E18" s="9">
         <v>0.31130000000000002</v>
       </c>
-      <c r="F18" s="10">
+      <c r="F18" s="9">
         <v>0.31130000000000002</v>
       </c>
       <c r="G18" s="6">
@@ -5371,7 +5476,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A19" s="24" t="s">
+      <c r="A19" s="23" t="s">
         <v>80</v>
       </c>
       <c r="B19" s="6">
@@ -5389,12 +5494,12 @@
       <c r="F19" s="6">
         <v>0</v>
       </c>
-      <c r="G19" s="25">
+      <c r="G19" s="24">
         <v>2.5897E-2</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A20" s="24" t="s">
+      <c r="A20" s="23" t="s">
         <v>81</v>
       </c>
       <c r="B20" s="6">
@@ -5412,12 +5517,12 @@
       <c r="F20" s="6">
         <v>0</v>
       </c>
-      <c r="G20" s="25">
+      <c r="G20" s="24">
         <v>7.1409999999999998E-3</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A21" s="24" t="s">
+      <c r="A21" s="23" t="s">
         <v>82</v>
       </c>
       <c r="B21" s="6">
@@ -5435,12 +5540,12 @@
       <c r="F21" s="6">
         <v>0</v>
       </c>
-      <c r="G21" s="25">
+      <c r="G21" s="24">
         <v>0.255942</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A22" s="24" t="s">
+      <c r="A22" s="23" t="s">
         <v>83</v>
       </c>
       <c r="B22" s="6">
@@ -5458,12 +5563,12 @@
       <c r="F22" s="6">
         <v>0</v>
       </c>
-      <c r="G22" s="25">
+      <c r="G22" s="24">
         <v>0.146367</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A23" s="24" t="s">
+      <c r="A23" s="23" t="s">
         <v>84</v>
       </c>
       <c r="B23" s="6">
@@ -5481,12 +5586,12 @@
       <c r="F23" s="6">
         <v>0</v>
       </c>
-      <c r="G23" s="25">
+      <c r="G23" s="24">
         <v>1.7554E-2</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A24" s="24" t="s">
+      <c r="A24" s="23" t="s">
         <v>85</v>
       </c>
       <c r="B24" s="6">
@@ -5504,12 +5609,12 @@
       <c r="F24" s="6">
         <v>0</v>
       </c>
-      <c r="G24" s="25">
+      <c r="G24" s="24">
         <v>1.8078E-2</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A25" s="24" t="s">
+      <c r="A25" s="23" t="s">
         <v>86</v>
       </c>
       <c r="B25" s="6">
@@ -5527,12 +5632,12 @@
       <c r="F25" s="6">
         <v>0</v>
       </c>
-      <c r="G25" s="25">
+      <c r="G25" s="24">
         <v>1.1440000000000001E-2</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A26" s="24" t="s">
+      <c r="A26" s="23" t="s">
         <v>87</v>
       </c>
       <c r="B26" s="6">
@@ -5550,12 +5655,12 @@
       <c r="F26" s="6">
         <v>0</v>
       </c>
-      <c r="G26" s="25">
+      <c r="G26" s="24">
         <v>0.15128800000000001</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="23" t="s">
         <v>88</v>
       </c>
       <c r="B27" s="6">
@@ -5573,7 +5678,7 @@
       <c r="F27" s="6">
         <v>0</v>
       </c>
-      <c r="G27" s="25">
+      <c r="G27" s="24">
         <v>0.36629299999999998</v>
       </c>
     </row>
@@ -5594,13 +5699,18 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="20.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>17</v>
       </c>
@@ -5622,258 +5732,342 @@
       <c r="G1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1">
+      <c r="H1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" customHeight="1">
       <c r="A2" s="6" t="s">
         <v>19</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="11">
+      <c r="C2" s="10">
         <v>63.4</v>
       </c>
-      <c r="D2" s="11">
+      <c r="D2" s="10">
         <v>63.4</v>
       </c>
-      <c r="E2" s="11">
+      <c r="E2" s="10">
         <v>49</v>
       </c>
-      <c r="F2" s="11">
+      <c r="F2" s="10">
         <v>28</v>
       </c>
-      <c r="G2" s="11">
+      <c r="G2" s="10">
         <v>25.3</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1">
+      <c r="H2" s="25"/>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" customHeight="1">
       <c r="B3" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="11">
+      <c r="C3" s="10">
         <v>22.6</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="10">
         <v>22.6</v>
       </c>
-      <c r="E3" s="11">
+      <c r="E3" s="10">
         <v>31.4</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F3" s="10">
         <v>33.9</v>
       </c>
-      <c r="G3" s="11">
+      <c r="G3" s="10">
         <v>33.200000000000003</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1">
+      <c r="H3" s="25"/>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" customHeight="1">
       <c r="B4" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="10">
         <v>10.199999999999999</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="10">
         <v>10.199999999999999</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4" s="10">
         <v>14.7</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="10">
         <v>24.7</v>
       </c>
-      <c r="G4" s="11">
+      <c r="G4" s="10">
         <v>28.1</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1">
+      <c r="H4" s="25"/>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" customHeight="1">
       <c r="B5" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="10">
         <v>3.8</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="10">
         <v>3.8</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5" s="10">
         <v>4.9000000000000004</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="10">
         <v>13.4</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="10">
         <v>13.3</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1">
+      <c r="H5" s="25"/>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" customHeight="1">
       <c r="A6" s="6" t="s">
         <v>35</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="11">
         <v>56.8</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="11">
         <v>56.8</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="11">
         <v>58.6</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="11">
         <v>54.9</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G6" s="11">
         <v>49</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1">
+      <c r="H6" s="26"/>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" customHeight="1">
       <c r="B7" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="11">
         <v>23.3</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="11">
         <v>23.3</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="11">
         <v>23.1</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="11">
         <v>30</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="11">
         <v>38.4</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1">
+      <c r="H7" s="26"/>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" customHeight="1">
       <c r="B8" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="11">
         <v>15</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="11">
         <v>15</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="11">
         <v>12.9</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F8" s="11">
         <v>11</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8" s="11">
         <v>10.5</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1">
+      <c r="H8" s="26"/>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" customHeight="1">
       <c r="B9" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="11">
         <v>4.9000000000000004</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D9" s="11">
         <v>4.9000000000000004</v>
       </c>
-      <c r="E9" s="12">
+      <c r="E9" s="11">
         <v>5.3</v>
       </c>
-      <c r="F9" s="12">
+      <c r="F9" s="11">
         <v>4.0999999999999996</v>
       </c>
-      <c r="G9" s="12">
+      <c r="G9" s="11">
         <v>2.1</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1">
+      <c r="H9" s="26"/>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" customHeight="1">
       <c r="A10" s="6" t="s">
         <v>44</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="13">
+      <c r="C10" s="28">
         <v>80.3</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D10" s="28">
         <v>46.2</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10" s="28">
         <v>3.3</v>
       </c>
-      <c r="F10" s="13">
+      <c r="F10" s="28">
         <v>0.7</v>
       </c>
-      <c r="G10" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1">
+      <c r="G10" s="29">
+        <v>0</v>
+      </c>
+      <c r="H10" s="27"/>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" customHeight="1">
       <c r="B11" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="13">
+      <c r="C11" s="28">
         <v>6.8</v>
       </c>
-      <c r="D11" s="13">
+      <c r="D11" s="28">
         <v>16.3</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="29">
         <v>9.4</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="29">
         <v>4.4000000000000004</v>
       </c>
-      <c r="G11" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1">
+      <c r="G11" s="29">
+        <v>0</v>
+      </c>
+      <c r="H11" s="27"/>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" customHeight="1">
       <c r="B12" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="13">
+      <c r="C12" s="28">
         <v>10.7</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D12" s="28">
         <v>37.1</v>
       </c>
-      <c r="E12" s="13">
+      <c r="E12" s="28">
         <v>83.7</v>
       </c>
-      <c r="F12" s="13">
+      <c r="F12" s="28">
         <v>87.9</v>
       </c>
-      <c r="G12" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1">
+      <c r="G12" s="29">
+        <v>0</v>
+      </c>
+      <c r="H12" s="27"/>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" customHeight="1">
       <c r="B13" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="29">
         <v>2.2000000000000002</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="29">
         <v>0.5</v>
       </c>
-      <c r="E13" s="13">
+      <c r="E13" s="28">
         <v>3.6</v>
       </c>
-      <c r="F13" s="13">
+      <c r="F13" s="28">
         <v>6.9</v>
       </c>
-      <c r="G13" s="9">
+      <c r="G13" s="29">
         <v>100</v>
+      </c>
+      <c r="H13" s="27"/>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A14" t="s">
+        <v>91</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="31">
+        <v>57.9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" customHeight="1">
+      <c r="B15" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="31">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" customHeight="1">
+      <c r="B16" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="31">
+        <v>18.7</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="15.75" customHeight="1">
+      <c r="B17" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="31">
+        <v>11.22</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" ht="15.75" customHeight="1">
+      <c r="B18" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="C18" s="30"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="31">
+        <v>7.48</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
   <extLst>
@@ -5960,19 +6154,19 @@
       <c r="A2" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="23">
+      <c r="B2" s="22">
         <v>2.4300000000000002</v>
       </c>
-      <c r="C2" s="23">
+      <c r="C2" s="22">
         <v>2.4300000000000002</v>
       </c>
-      <c r="D2" s="23">
+      <c r="D2" s="22">
         <v>3.71</v>
       </c>
-      <c r="E2" s="23">
+      <c r="E2" s="22">
         <v>3</v>
       </c>
-      <c r="F2" s="23">
+      <c r="F2" s="22">
         <v>1.92</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed some key errors and merged the new .xls spreadsheet into the original .xlsx spreadsheet
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Jan/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Jan/InputForCode_Bangladesh.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-35900" yWindow="80" windowWidth="25600" windowHeight="14600" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="-35260" yWindow="0" windowWidth="29420" windowHeight="15960" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="demographics" sheetId="1" r:id="rId1"/>
@@ -351,7 +351,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="104">
   <si>
     <t>indicators</t>
   </si>
@@ -636,6 +636,33 @@
   </si>
   <si>
     <t>essential care</t>
+  </si>
+  <si>
+    <t>Tetanus toxoid vaccination</t>
+  </si>
+  <si>
+    <t>Malaria case management</t>
+  </si>
+  <si>
+    <t>Calcium supplementation</t>
+  </si>
+  <si>
+    <t>Hypertensive disorder case management</t>
+  </si>
+  <si>
+    <t>MgSO4 management of pre-eclampsia</t>
+  </si>
+  <si>
+    <t>Maternal sepsis case management</t>
+  </si>
+  <si>
+    <t>Safe abortion services</t>
+  </si>
+  <si>
+    <t>Post abortion case management</t>
+  </si>
+  <si>
+    <t>Ectopic pregnancy case management</t>
   </si>
 </sst>
 </file>
@@ -645,7 +672,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -721,6 +748,12 @@
       <sz val="8"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -775,7 +808,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -791,8 +824,13 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -855,8 +893,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="15"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="15" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="15" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="15" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="15" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="20">
+    <cellStyle name="Excel Built-in Normal" xfId="15"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -864,6 +915,8 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -871,6 +924,8 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4036,7 +4091,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A8" sqref="A8:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -4164,58 +4219,148 @@
       <c r="G7" s="6"/>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B8" s="6"/>
-      <c r="D8" s="6"/>
+      <c r="A8" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8" s="32">
+        <v>96</v>
+      </c>
+      <c r="C8" s="33">
+        <v>0.85</v>
+      </c>
+      <c r="D8" s="33">
+        <v>1</v>
+      </c>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B9" s="6"/>
-      <c r="D9" s="6"/>
+      <c r="A9" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="B9" s="32">
+        <v>1.6</v>
+      </c>
+      <c r="C9" s="33">
+        <v>0.85</v>
+      </c>
+      <c r="D9" s="33">
+        <v>1</v>
+      </c>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B10" s="6"/>
-      <c r="D10" s="6"/>
+      <c r="A10" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="B10" s="32">
+        <v>0</v>
+      </c>
+      <c r="C10" s="33">
+        <v>0.85</v>
+      </c>
+      <c r="D10" s="33">
+        <v>1</v>
+      </c>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B11" s="6"/>
-      <c r="D11" s="6"/>
+      <c r="A11" s="32" t="s">
+        <v>98</v>
+      </c>
+      <c r="B11" s="32">
+        <v>1.6</v>
+      </c>
+      <c r="C11" s="33">
+        <v>0.85</v>
+      </c>
+      <c r="D11" s="33">
+        <v>1</v>
+      </c>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B12" s="6"/>
-      <c r="D12" s="6"/>
+      <c r="A12" s="32" t="s">
+        <v>99</v>
+      </c>
+      <c r="B12" s="34">
+        <v>1.6</v>
+      </c>
+      <c r="C12" s="33">
+        <v>0.85</v>
+      </c>
+      <c r="D12" s="33">
+        <v>1</v>
+      </c>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B13" s="6"/>
-      <c r="D13" s="6"/>
+      <c r="A13" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="B13" s="32">
+        <v>0</v>
+      </c>
+      <c r="C13" s="33">
+        <v>0.85</v>
+      </c>
+      <c r="D13" s="33">
+        <v>1</v>
+      </c>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
+      <c r="A14" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="B14" s="32">
+        <v>35.1</v>
+      </c>
+      <c r="C14" s="33">
+        <v>0.85</v>
+      </c>
+      <c r="D14" s="32">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
+      <c r="A15" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="B15" s="32">
+        <v>0</v>
+      </c>
+      <c r="C15" s="33">
+        <v>0.85</v>
+      </c>
+      <c r="D15" s="32">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
+      <c r="A16" s="32" t="s">
+        <v>103</v>
+      </c>
+      <c r="B16" s="32">
+        <v>0</v>
+      </c>
+      <c r="C16" s="33">
+        <v>0.85</v>
+      </c>
+      <c r="D16" s="32">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="2:3" ht="15.75" customHeight="1">
       <c r="B17" s="6"/>
@@ -4268,7 +4413,7 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+      <selection activeCell="A8" sqref="A8:G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -4448,58 +4593,211 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="15.75" customHeight="1">
-      <c r="B8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
+      <c r="A8" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8" s="33">
+        <v>0</v>
+      </c>
+      <c r="C8" s="33">
+        <v>0</v>
+      </c>
+      <c r="D8" s="33">
+        <v>0</v>
+      </c>
+      <c r="E8" s="33">
+        <v>0</v>
+      </c>
+      <c r="F8" s="33">
+        <v>0</v>
+      </c>
+      <c r="G8" s="33">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:10" ht="15.75" customHeight="1">
-      <c r="B9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
+      <c r="A9" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="B9" s="33">
+        <v>0</v>
+      </c>
+      <c r="C9" s="33">
+        <v>0</v>
+      </c>
+      <c r="D9" s="33">
+        <v>0</v>
+      </c>
+      <c r="E9" s="33">
+        <v>0</v>
+      </c>
+      <c r="F9" s="33">
+        <v>0</v>
+      </c>
+      <c r="G9" s="33">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:10" ht="15.75" customHeight="1">
-      <c r="B10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
+      <c r="A10" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="B10" s="33">
+        <v>0</v>
+      </c>
+      <c r="C10" s="33">
+        <v>0</v>
+      </c>
+      <c r="D10" s="33">
+        <v>0</v>
+      </c>
+      <c r="E10" s="33">
+        <v>0</v>
+      </c>
+      <c r="F10" s="33">
+        <v>0</v>
+      </c>
+      <c r="G10" s="33">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:10" ht="15.75" customHeight="1">
-      <c r="B11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
+      <c r="A11" s="32" t="s">
+        <v>98</v>
+      </c>
+      <c r="B11" s="33">
+        <v>0</v>
+      </c>
+      <c r="C11" s="33">
+        <v>0</v>
+      </c>
+      <c r="D11" s="33">
+        <v>0</v>
+      </c>
+      <c r="E11" s="33">
+        <v>0</v>
+      </c>
+      <c r="F11" s="33">
+        <v>0</v>
+      </c>
+      <c r="G11" s="33">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:10" ht="15.75" customHeight="1">
-      <c r="B12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
+      <c r="A12" s="32" t="s">
+        <v>99</v>
+      </c>
+      <c r="B12" s="33">
+        <v>0</v>
+      </c>
+      <c r="C12" s="33">
+        <v>0</v>
+      </c>
+      <c r="D12" s="33">
+        <v>0</v>
+      </c>
+      <c r="E12" s="33">
+        <v>0</v>
+      </c>
+      <c r="F12" s="33">
+        <v>0</v>
+      </c>
+      <c r="G12" s="33">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:10" ht="15.75" customHeight="1">
-      <c r="B13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
+      <c r="A13" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="B13" s="33">
+        <v>0</v>
+      </c>
+      <c r="C13" s="33">
+        <v>0</v>
+      </c>
+      <c r="D13" s="33">
+        <v>0</v>
+      </c>
+      <c r="E13" s="33">
+        <v>0</v>
+      </c>
+      <c r="F13" s="33">
+        <v>0</v>
+      </c>
+      <c r="G13" s="33">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:10" ht="15.75" customHeight="1">
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
+      <c r="A14" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="B14" s="33">
+        <v>0</v>
+      </c>
+      <c r="C14" s="33">
+        <v>0</v>
+      </c>
+      <c r="D14" s="33">
+        <v>0</v>
+      </c>
+      <c r="E14" s="33">
+        <v>0</v>
+      </c>
+      <c r="F14" s="33">
+        <v>0</v>
+      </c>
+      <c r="G14" s="32">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:10" ht="15.75" customHeight="1">
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
+      <c r="A15" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="B15" s="33">
+        <v>0</v>
+      </c>
+      <c r="C15" s="33">
+        <v>0</v>
+      </c>
+      <c r="D15" s="33">
+        <v>0</v>
+      </c>
+      <c r="E15" s="33">
+        <v>0</v>
+      </c>
+      <c r="F15" s="33">
+        <v>0</v>
+      </c>
+      <c r="G15" s="32">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:10" ht="15.75" customHeight="1">
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
+      <c r="A16" s="32" t="s">
+        <v>103</v>
+      </c>
+      <c r="B16" s="33">
+        <v>0</v>
+      </c>
+      <c r="C16" s="33">
+        <v>0</v>
+      </c>
+      <c r="D16" s="33">
+        <v>0</v>
+      </c>
+      <c r="E16" s="33">
+        <v>0</v>
+      </c>
+      <c r="F16" s="33">
+        <v>0</v>
+      </c>
+      <c r="G16" s="32">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="2:3" ht="15.75" customHeight="1">
       <c r="B17" s="6"/>
@@ -4670,18 +4968,19 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
+    <col min="2" max="2" width="28.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>68</v>
       </c>
@@ -4703,12 +5002,15 @@
       <c r="G1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1">
+      <c r="H1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" customHeight="1">
       <c r="A2" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="35" t="s">
         <v>34</v>
       </c>
       <c r="C2" s="6">
@@ -4726,9 +5028,12 @@
       <c r="G2" s="21">
         <v>0.33500000000000002</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B3" s="6" t="s">
+      <c r="H2" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" customHeight="1">
+      <c r="B3" s="35" t="s">
         <v>36</v>
       </c>
       <c r="C3" s="6">
@@ -4746,30 +5051,247 @@
       <c r="G3" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
+      <c r="H3" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A4" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" s="6">
+        <v>0</v>
+      </c>
+      <c r="D4" s="6">
+        <v>0</v>
+      </c>
+      <c r="E4" s="6">
+        <v>0</v>
+      </c>
+      <c r="F4" s="6">
+        <v>0</v>
+      </c>
+      <c r="G4" s="6">
+        <v>0</v>
+      </c>
+      <c r="H4" s="32">
+        <v>4.895E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A5" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5" s="37" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5" s="6">
+        <v>0</v>
+      </c>
+      <c r="D5" s="6">
+        <v>0</v>
+      </c>
+      <c r="E5" s="6">
+        <v>0</v>
+      </c>
+      <c r="F5" s="6">
+        <v>0</v>
+      </c>
+      <c r="G5" s="6">
+        <v>0</v>
+      </c>
+      <c r="H5" s="32">
+        <v>2.0998000000000003E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A6" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6" s="37" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" s="6">
+        <v>0</v>
+      </c>
+      <c r="D6" s="6">
+        <v>0</v>
+      </c>
+      <c r="E6" s="6">
+        <v>0</v>
+      </c>
+      <c r="F6" s="6">
+        <v>0</v>
+      </c>
+      <c r="G6" s="6">
+        <v>0</v>
+      </c>
+      <c r="H6" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A7" s="32" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" s="37" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" s="6">
+        <v>0</v>
+      </c>
+      <c r="D7" s="6">
+        <v>0</v>
+      </c>
+      <c r="E7" s="6">
+        <v>0</v>
+      </c>
+      <c r="F7" s="6">
+        <v>0</v>
+      </c>
+      <c r="G7" s="6">
+        <v>0</v>
+      </c>
+      <c r="H7" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A8" s="32" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8" s="37" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" s="6">
+        <v>0</v>
+      </c>
+      <c r="D8" s="6">
+        <v>0</v>
+      </c>
+      <c r="E8" s="6">
+        <v>0</v>
+      </c>
+      <c r="F8" s="6">
+        <v>0</v>
+      </c>
+      <c r="G8" s="6">
+        <v>0</v>
+      </c>
+      <c r="H8" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A9" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="B9" s="37" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9" s="6">
+        <v>0</v>
+      </c>
+      <c r="D9" s="6">
+        <v>0</v>
+      </c>
+      <c r="E9" s="6">
+        <v>0</v>
+      </c>
+      <c r="F9" s="6">
+        <v>0</v>
+      </c>
+      <c r="G9" s="6">
+        <v>0</v>
+      </c>
+      <c r="H9" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A10" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10" s="37" t="s">
+        <v>85</v>
+      </c>
+      <c r="C10" s="6">
+        <v>0</v>
+      </c>
+      <c r="D10" s="6">
+        <v>0</v>
+      </c>
+      <c r="E10" s="6">
+        <v>0</v>
+      </c>
+      <c r="F10" s="6">
+        <v>0</v>
+      </c>
+      <c r="G10" s="6">
+        <v>0</v>
+      </c>
+      <c r="H10" s="32">
+        <v>0.90526300000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A11" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="B11" s="37" t="s">
+        <v>85</v>
+      </c>
+      <c r="C11" s="6">
+        <v>0</v>
+      </c>
+      <c r="D11" s="6">
+        <v>0</v>
+      </c>
+      <c r="E11" s="6">
+        <v>0</v>
+      </c>
+      <c r="F11" s="6">
+        <v>0</v>
+      </c>
+      <c r="G11" s="6">
+        <v>0</v>
+      </c>
+      <c r="H11" s="32">
+        <v>0.90526300000000004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A12" s="32" t="s">
+        <v>103</v>
+      </c>
+      <c r="B12" s="37" t="s">
+        <v>85</v>
+      </c>
+      <c r="C12" s="6">
+        <v>0</v>
+      </c>
+      <c r="D12" s="6">
+        <v>0</v>
+      </c>
+      <c r="E12" s="6">
+        <v>0</v>
+      </c>
+      <c r="F12" s="6">
+        <v>0</v>
+      </c>
+      <c r="G12" s="6">
+        <v>0</v>
+      </c>
+      <c r="H12" s="32">
+        <v>9.4737000000000016E-2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -4780,18 +5302,19 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="28.83203125" customWidth="1"/>
+    <col min="2" max="2" width="27.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>68</v>
       </c>
@@ -4813,8 +5336,11 @@
       <c r="G1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1">
+      <c r="H1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" customHeight="1">
       <c r="A2" s="6" t="s">
         <v>64</v>
       </c>
@@ -4836,8 +5362,11 @@
       <c r="G2" s="6">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1">
+      <c r="H2" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" customHeight="1">
       <c r="B3" s="6" t="s">
         <v>36</v>
       </c>
@@ -4856,30 +5385,247 @@
       <c r="G3" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
+      <c r="H3" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A4" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" s="6">
+        <v>0</v>
+      </c>
+      <c r="D4" s="6">
+        <v>0</v>
+      </c>
+      <c r="E4" s="6">
+        <v>0</v>
+      </c>
+      <c r="F4" s="6">
+        <v>0</v>
+      </c>
+      <c r="G4" s="6">
+        <v>0</v>
+      </c>
+      <c r="H4" s="32">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A5" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5" s="6">
+        <v>0</v>
+      </c>
+      <c r="D5" s="6">
+        <v>0</v>
+      </c>
+      <c r="E5" s="6">
+        <v>0</v>
+      </c>
+      <c r="F5" s="6">
+        <v>0</v>
+      </c>
+      <c r="G5" s="6">
+        <v>0</v>
+      </c>
+      <c r="H5" s="32">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A6" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" s="6">
+        <v>0</v>
+      </c>
+      <c r="D6" s="6">
+        <v>0</v>
+      </c>
+      <c r="E6" s="6">
+        <v>0</v>
+      </c>
+      <c r="F6" s="6">
+        <v>0</v>
+      </c>
+      <c r="G6" s="6">
+        <v>0</v>
+      </c>
+      <c r="H6" s="32">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A7" s="32" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" s="6">
+        <v>0</v>
+      </c>
+      <c r="D7" s="6">
+        <v>0</v>
+      </c>
+      <c r="E7" s="6">
+        <v>0</v>
+      </c>
+      <c r="F7" s="6">
+        <v>0</v>
+      </c>
+      <c r="G7" s="6">
+        <v>0</v>
+      </c>
+      <c r="H7" s="32">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A8" s="32" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" s="6">
+        <v>0</v>
+      </c>
+      <c r="D8" s="6">
+        <v>0</v>
+      </c>
+      <c r="E8" s="6">
+        <v>0</v>
+      </c>
+      <c r="F8" s="6">
+        <v>0</v>
+      </c>
+      <c r="G8" s="6">
+        <v>0</v>
+      </c>
+      <c r="H8" s="32">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A9" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="B9" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9" s="6">
+        <v>0</v>
+      </c>
+      <c r="D9" s="6">
+        <v>0</v>
+      </c>
+      <c r="E9" s="6">
+        <v>0</v>
+      </c>
+      <c r="F9" s="6">
+        <v>0</v>
+      </c>
+      <c r="G9" s="6">
+        <v>0</v>
+      </c>
+      <c r="H9" s="32">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A10" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="C10" s="6">
+        <v>0</v>
+      </c>
+      <c r="D10" s="6">
+        <v>0</v>
+      </c>
+      <c r="E10" s="6">
+        <v>0</v>
+      </c>
+      <c r="F10" s="6">
+        <v>0</v>
+      </c>
+      <c r="G10" s="6">
+        <v>0</v>
+      </c>
+      <c r="H10" s="32">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A11" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="B11" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="C11" s="6">
+        <v>0</v>
+      </c>
+      <c r="D11" s="6">
+        <v>0</v>
+      </c>
+      <c r="E11" s="6">
+        <v>0</v>
+      </c>
+      <c r="F11" s="6">
+        <v>0</v>
+      </c>
+      <c r="G11" s="6">
+        <v>0</v>
+      </c>
+      <c r="H11" s="32">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A12" s="32" t="s">
+        <v>103</v>
+      </c>
+      <c r="B12" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="C12" s="6">
+        <v>0</v>
+      </c>
+      <c r="D12" s="6">
+        <v>0</v>
+      </c>
+      <c r="E12" s="6">
+        <v>0</v>
+      </c>
+      <c r="F12" s="6">
+        <v>0</v>
+      </c>
+      <c r="G12" s="6">
+        <v>0</v>
+      </c>
+      <c r="H12" s="32">
+        <v>0.9</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -5052,7 +5798,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
@@ -5701,7 +6447,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added 'obese' to wasting stratification
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Jan/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Jan/InputForCode_Bangladesh.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-35260" yWindow="0" windowWidth="29420" windowHeight="15960" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="-37720" yWindow="1120" windowWidth="31360" windowHeight="14560" tabRatio="500" firstSheet="5" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="demographics" sheetId="1" r:id="rId1"/>
@@ -181,7 +181,7 @@
     <author>Ruth</author>
   </authors>
   <commentList>
-    <comment ref="E12" authorId="0">
+    <comment ref="E13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -194,7 +194,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B17" authorId="1">
+    <comment ref="B18" authorId="1">
       <text>
         <r>
           <rPr>
@@ -216,7 +216,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B18" authorId="1">
+    <comment ref="B19" authorId="1">
       <text>
         <r>
           <rPr>
@@ -351,7 +351,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="105">
   <si>
     <t>indicators</t>
   </si>
@@ -663,6 +663,9 @@
   </si>
   <si>
     <t>Ectopic pregnancy case management</t>
+  </si>
+  <si>
+    <t>obese</t>
   </si>
 </sst>
 </file>
@@ -755,7 +758,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -798,6 +801,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor rgb="FFFDE9D9"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -808,7 +817,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -829,8 +838,24 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -905,8 +930,11 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="15" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="20">
+  <cellStyles count="36">
     <cellStyle name="Excel Built-in Normal" xfId="15"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -917,6 +945,14 @@
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -926,6 +962,14 @@
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="34" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1057,7 +1101,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>546100</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:row>67</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1108,7 +1152,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>546100</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:row>67</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1159,7 +1203,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>546100</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:row>67</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1210,7 +1254,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>546100</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:row>67</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1261,7 +1305,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>546100</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:row>67</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1312,7 +1356,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>546100</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:row>67</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1363,7 +1407,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>546100</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:row>67</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1414,7 +1458,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>546100</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:row>67</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1465,7 +1509,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>546100</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:row>67</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1516,7 +1560,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>546100</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:row>67</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1567,7 +1611,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>546100</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:row>67</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1618,7 +1662,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>546100</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:row>67</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1669,7 +1713,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>546100</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:row>67</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1720,7 +1764,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>546100</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:row>67</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1771,7 +1815,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>546100</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:row>67</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1822,7 +1866,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>546100</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:row>67</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1873,7 +1917,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>546100</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:row>67</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1924,7 +1968,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>546100</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:row>67</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3527,7 +3571,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D2"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -4091,7 +4135,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:D16"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -5798,7 +5842,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
@@ -6445,10 +6489,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -6574,127 +6618,128 @@
         <v>35</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C6" s="38">
+        <v>28.4</v>
+      </c>
+      <c r="D6" s="26">
+        <v>28.4</v>
+      </c>
+      <c r="E6" s="26">
+        <v>29.3</v>
+      </c>
+      <c r="F6" s="26">
+        <v>27.45</v>
+      </c>
+      <c r="G6" s="26">
+        <v>24.5</v>
+      </c>
+      <c r="H6" s="26"/>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="11">
-        <v>56.8</v>
-      </c>
-      <c r="D6" s="11">
-        <v>56.8</v>
-      </c>
-      <c r="E6" s="11">
-        <v>58.6</v>
-      </c>
-      <c r="F6" s="11">
-        <v>54.9</v>
-      </c>
-      <c r="G6" s="11">
-        <v>49</v>
-      </c>
-      <c r="H6" s="26"/>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" customHeight="1">
-      <c r="B7" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="11">
-        <v>23.3</v>
-      </c>
-      <c r="D7" s="11">
-        <v>23.3</v>
-      </c>
-      <c r="E7" s="11">
-        <v>23.1</v>
-      </c>
-      <c r="F7" s="11">
-        <v>30</v>
-      </c>
-      <c r="G7" s="11">
-        <v>38.4</v>
+      <c r="C7" s="38">
+        <v>28.4</v>
+      </c>
+      <c r="D7" s="26">
+        <v>28.4</v>
+      </c>
+      <c r="E7" s="26">
+        <v>29.3</v>
+      </c>
+      <c r="F7" s="26">
+        <v>27.45</v>
+      </c>
+      <c r="G7" s="26">
+        <v>24.5</v>
       </c>
       <c r="H7" s="26"/>
     </row>
     <row r="8" spans="1:8" ht="15.75" customHeight="1">
       <c r="B8" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C8" s="11">
-        <v>15</v>
+        <v>23.3</v>
       </c>
       <c r="D8" s="11">
-        <v>15</v>
+        <v>23.3</v>
       </c>
       <c r="E8" s="11">
-        <v>12.9</v>
+        <v>23.1</v>
       </c>
       <c r="F8" s="11">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="G8" s="11">
-        <v>10.5</v>
+        <v>38.4</v>
       </c>
       <c r="H8" s="26"/>
     </row>
     <row r="9" spans="1:8" ht="15.75" customHeight="1">
       <c r="B9" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="11">
+        <v>15</v>
+      </c>
+      <c r="D9" s="11">
+        <v>15</v>
+      </c>
+      <c r="E9" s="11">
+        <v>12.9</v>
+      </c>
+      <c r="F9" s="11">
+        <v>11</v>
+      </c>
+      <c r="G9" s="11">
+        <v>10.5</v>
+      </c>
+      <c r="H9" s="26"/>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" customHeight="1">
+      <c r="B10" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C10" s="11">
         <v>4.9000000000000004</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D10" s="11">
         <v>4.9000000000000004</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E10" s="11">
         <v>5.3</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F10" s="11">
         <v>4.0999999999999996</v>
       </c>
-      <c r="G9" s="11">
+      <c r="G10" s="11">
         <v>2.1</v>
       </c>
-      <c r="H9" s="26"/>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A10" s="6" t="s">
+      <c r="H10" s="26"/>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A11" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B11" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="28">
+      <c r="C11" s="28">
         <v>80.3</v>
       </c>
-      <c r="D10" s="28">
+      <c r="D11" s="28">
         <v>46.2</v>
       </c>
-      <c r="E10" s="28">
+      <c r="E11" s="28">
         <v>3.3</v>
       </c>
-      <c r="F10" s="28">
+      <c r="F11" s="28">
         <v>0.7</v>
-      </c>
-      <c r="G10" s="29">
-        <v>0</v>
-      </c>
-      <c r="H10" s="27"/>
-    </row>
-    <row r="11" spans="1:8" ht="15.75" customHeight="1">
-      <c r="B11" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C11" s="28">
-        <v>6.8</v>
-      </c>
-      <c r="D11" s="28">
-        <v>16.3</v>
-      </c>
-      <c r="E11" s="29">
-        <v>9.4</v>
-      </c>
-      <c r="F11" s="29">
-        <v>4.4000000000000004</v>
       </c>
       <c r="G11" s="29">
         <v>0</v>
@@ -6703,19 +6748,19 @@
     </row>
     <row r="12" spans="1:8" ht="15.75" customHeight="1">
       <c r="B12" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C12" s="28">
-        <v>10.7</v>
+        <v>6.8</v>
       </c>
       <c r="D12" s="28">
-        <v>37.1</v>
-      </c>
-      <c r="E12" s="28">
-        <v>83.7</v>
-      </c>
-      <c r="F12" s="28">
-        <v>87.9</v>
+        <v>16.3</v>
+      </c>
+      <c r="E12" s="29">
+        <v>9.4</v>
+      </c>
+      <c r="F12" s="29">
+        <v>4.4000000000000004</v>
       </c>
       <c r="G12" s="29">
         <v>0</v>
@@ -6724,44 +6769,52 @@
     </row>
     <row r="13" spans="1:8" ht="15.75" customHeight="1">
       <c r="B13" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="28">
+        <v>10.7</v>
+      </c>
+      <c r="D13" s="28">
+        <v>37.1</v>
+      </c>
+      <c r="E13" s="28">
+        <v>83.7</v>
+      </c>
+      <c r="F13" s="28">
+        <v>87.9</v>
+      </c>
+      <c r="G13" s="29">
+        <v>0</v>
+      </c>
+      <c r="H13" s="27"/>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" customHeight="1">
+      <c r="B14" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="29">
+      <c r="C14" s="29">
         <v>2.2000000000000002</v>
       </c>
-      <c r="D13" s="29">
+      <c r="D14" s="29">
         <v>0.5</v>
       </c>
-      <c r="E13" s="28">
+      <c r="E14" s="28">
         <v>3.6</v>
       </c>
-      <c r="F13" s="28">
+      <c r="F14" s="28">
         <v>6.9</v>
       </c>
-      <c r="G13" s="29">
+      <c r="G14" s="29">
         <v>100</v>
       </c>
-      <c r="H13" s="27"/>
-    </row>
-    <row r="14" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A14" t="s">
+      <c r="H14" s="27"/>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A15" t="s">
         <v>91</v>
       </c>
-      <c r="B14" s="23" t="s">
+      <c r="B15" s="23" t="s">
         <v>92</v>
-      </c>
-      <c r="C14" s="30"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="31">
-        <v>57.9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="15.75" customHeight="1">
-      <c r="B15" s="23" t="s">
-        <v>93</v>
       </c>
       <c r="C15" s="30"/>
       <c r="D15" s="30"/>
@@ -6769,12 +6822,12 @@
       <c r="F15" s="30"/>
       <c r="G15" s="30"/>
       <c r="H15" s="31">
-        <v>4.7</v>
+        <v>57.9</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15.75" customHeight="1">
       <c r="B16" s="23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C16" s="30"/>
       <c r="D16" s="30"/>
@@ -6782,12 +6835,12 @@
       <c r="F16" s="30"/>
       <c r="G16" s="30"/>
       <c r="H16" s="31">
-        <v>18.7</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="17" spans="2:8" ht="15.75" customHeight="1">
       <c r="B17" s="23" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="C17" s="30"/>
       <c r="D17" s="30"/>
@@ -6795,12 +6848,12 @@
       <c r="F17" s="30"/>
       <c r="G17" s="30"/>
       <c r="H17" s="31">
-        <v>11.22</v>
+        <v>18.7</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="15.75" customHeight="1">
       <c r="B18" s="23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C18" s="30"/>
       <c r="D18" s="30"/>
@@ -6808,6 +6861,19 @@
       <c r="F18" s="30"/>
       <c r="G18" s="30"/>
       <c r="H18" s="31">
+        <v>11.22</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" ht="15.75" customHeight="1">
+      <c r="B19" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="30"/>
+      <c r="H19" s="31">
         <v>7.48</v>
       </c>
     </row>
@@ -7405,9 +7471,11 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData>
@@ -7439,9 +7507,9 @@
         <v>34</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="6">
+        <v>104</v>
+      </c>
+      <c r="C2">
         <v>1</v>
       </c>
       <c r="D2">
@@ -7459,236 +7527,233 @@
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="B3" s="6" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="C3" s="6">
         <v>1</v>
       </c>
       <c r="D3">
-        <v>1.6</v>
+        <v>1</v>
       </c>
       <c r="E3">
-        <v>1.6</v>
+        <v>1</v>
       </c>
       <c r="F3">
-        <v>1.6</v>
+        <v>1</v>
       </c>
       <c r="G3">
-        <v>1.6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="B4" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C4" s="6">
         <v>1</v>
       </c>
       <c r="D4">
-        <v>3.41</v>
+        <v>1.6</v>
       </c>
       <c r="E4">
-        <v>3.41</v>
+        <v>1.6</v>
       </c>
       <c r="F4">
-        <v>3.41</v>
+        <v>1.6</v>
       </c>
       <c r="G4">
-        <v>3.41</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="B5" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="6">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>3.41</v>
+      </c>
+      <c r="E5">
+        <v>3.41</v>
+      </c>
+      <c r="F5">
+        <v>3.41</v>
+      </c>
+      <c r="G5">
+        <v>3.41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
+      <c r="B6" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="6">
-        <v>1</v>
-      </c>
-      <c r="D5">
+      <c r="C6" s="6">
+        <v>1</v>
+      </c>
+      <c r="D6">
         <v>12.33</v>
       </c>
-      <c r="E5">
+      <c r="E6">
         <v>12.33</v>
       </c>
-      <c r="F5">
+      <c r="F6">
         <v>12.33</v>
       </c>
-      <c r="G5">
+      <c r="G6">
         <v>12.33</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A6" t="s">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A7" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="6">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="B7" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="6">
+        <v>104</v>
+      </c>
+      <c r="C7">
         <v>1</v>
       </c>
       <c r="D7">
-        <v>1.92</v>
+        <v>1</v>
       </c>
       <c r="E7">
-        <v>1.92</v>
+        <v>1</v>
       </c>
       <c r="F7">
-        <v>1.92</v>
+        <v>1</v>
       </c>
       <c r="G7">
-        <v>1.92</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="B8" s="6" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="C8" s="6">
         <v>1</v>
       </c>
       <c r="D8">
-        <v>4.66</v>
+        <v>1</v>
       </c>
       <c r="E8">
-        <v>4.66</v>
+        <v>1</v>
       </c>
       <c r="F8">
-        <v>4.66</v>
+        <v>1</v>
       </c>
       <c r="G8">
-        <v>4.66</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="B9" s="6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C9" s="6">
         <v>1</v>
       </c>
       <c r="D9">
-        <v>9.68</v>
+        <v>1.92</v>
       </c>
       <c r="E9">
-        <v>9.68</v>
+        <v>1.92</v>
       </c>
       <c r="F9">
-        <v>9.68</v>
+        <v>1.92</v>
       </c>
       <c r="G9">
-        <v>9.68</v>
+        <v>1.92</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A10" t="s">
-        <v>38</v>
-      </c>
       <c r="B10" s="6" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="C10" s="6">
         <v>1</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>4.66</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>4.66</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>4.66</v>
       </c>
       <c r="G10">
-        <v>1</v>
+        <v>4.66</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="B11" s="6" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C11" s="6">
         <v>1</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>9.68</v>
       </c>
       <c r="E11">
-        <v>1</v>
+        <v>9.68</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>9.68</v>
       </c>
       <c r="G11">
-        <v>1</v>
+        <v>9.68</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A12" t="s">
+        <v>38</v>
+      </c>
       <c r="B12" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" s="6">
+        <v>104</v>
+      </c>
+      <c r="C12">
         <v>1</v>
       </c>
       <c r="D12">
-        <v>2.58</v>
+        <v>1</v>
       </c>
       <c r="E12">
-        <v>2.58</v>
+        <v>1</v>
       </c>
       <c r="F12">
-        <v>2.58</v>
+        <v>1</v>
       </c>
       <c r="G12">
-        <v>2.58</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="B13" s="6" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="C13" s="6">
         <v>1</v>
       </c>
       <c r="D13">
-        <v>9.6300000000000008</v>
+        <v>1</v>
       </c>
       <c r="E13">
-        <v>9.6300000000000008</v>
+        <v>1</v>
       </c>
       <c r="F13">
-        <v>9.6300000000000008</v>
+        <v>1</v>
       </c>
       <c r="G13">
-        <v>9.6300000000000008</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A14" t="s">
-        <v>39</v>
-      </c>
       <c r="B14" s="6" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="C14" s="6">
         <v>1</v>
@@ -7708,49 +7773,52 @@
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="B15" s="6" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C15" s="6">
         <v>1</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>2.58</v>
       </c>
       <c r="E15">
-        <v>1</v>
+        <v>2.58</v>
       </c>
       <c r="F15">
-        <v>1</v>
+        <v>2.58</v>
       </c>
       <c r="G15">
-        <v>1</v>
+        <v>2.58</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="B16" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C16" s="6">
         <v>1</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>9.6300000000000008</v>
       </c>
       <c r="E16">
-        <v>1</v>
+        <v>9.6300000000000008</v>
       </c>
       <c r="F16">
-        <v>1</v>
+        <v>9.6300000000000008</v>
       </c>
       <c r="G16">
-        <v>1</v>
+        <v>9.6300000000000008</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A17" t="s">
+        <v>39</v>
+      </c>
       <c r="B17" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" s="6">
+        <v>104</v>
+      </c>
+      <c r="C17">
         <v>1</v>
       </c>
       <c r="D17">
@@ -7767,9 +7835,6 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A18" t="s">
-        <v>43</v>
-      </c>
       <c r="B18" s="6" t="s">
         <v>20</v>
       </c>
@@ -7797,16 +7862,16 @@
         <v>1</v>
       </c>
       <c r="D19">
-        <v>1.65</v>
+        <v>1</v>
       </c>
       <c r="E19">
-        <v>1.65</v>
+        <v>1</v>
       </c>
       <c r="F19">
-        <v>1.65</v>
+        <v>1</v>
       </c>
       <c r="G19">
-        <v>1.65</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="15.75" customHeight="1">
@@ -7817,16 +7882,16 @@
         <v>1</v>
       </c>
       <c r="D20">
-        <v>2.73</v>
+        <v>1</v>
       </c>
       <c r="E20">
-        <v>2.73</v>
+        <v>1</v>
       </c>
       <c r="F20">
-        <v>2.73</v>
+        <v>1</v>
       </c>
       <c r="G20">
-        <v>2.73</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1">
@@ -7837,20 +7902,124 @@
         <v>1</v>
       </c>
       <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="15.75" customHeight="1">
+      <c r="B23" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="6">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="15.75" customHeight="1">
+      <c r="B24" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="6">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>1.65</v>
+      </c>
+      <c r="E24">
+        <v>1.65</v>
+      </c>
+      <c r="F24">
+        <v>1.65</v>
+      </c>
+      <c r="G24">
+        <v>1.65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="15.75" customHeight="1">
+      <c r="B25" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="6">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>2.73</v>
+      </c>
+      <c r="E25">
+        <v>2.73</v>
+      </c>
+      <c r="F25">
+        <v>2.73</v>
+      </c>
+      <c r="G25">
+        <v>2.73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15.75" customHeight="1">
+      <c r="B26" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="6">
+        <v>1</v>
+      </c>
+      <c r="D26">
         <v>11.21</v>
       </c>
-      <c r="E21">
+      <c r="E26">
         <v>11.21</v>
       </c>
-      <c r="F21">
+      <c r="F26">
         <v>11.21</v>
       </c>
-      <c r="G21">
+      <c r="G26">
         <v>11.21</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
added comment to spreadsheet wasting dist: in the absence of obesity data I just split those in the 'normal' category between 'normal' and 'obese'
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Jan/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Jan/InputForCode_Bangladesh.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-37720" yWindow="1120" windowWidth="31360" windowHeight="14560" tabRatio="500" firstSheet="5" activeTab="8"/>
+    <workbookView xWindow="-37720" yWindow="1120" windowWidth="31360" windowHeight="14560" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="demographics" sheetId="1" r:id="rId1"/>
@@ -177,11 +177,33 @@
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
+    <author>Ruth</author>
     <author/>
-    <author>Ruth</author>
   </authors>
   <commentList>
-    <comment ref="E13" authorId="0">
+    <comment ref="B6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+I just split 'normal'  evenly between 'normal' and 'obese'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E13" authorId="1">
       <text>
         <r>
           <rPr>
@@ -194,7 +216,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B18" authorId="1">
+    <comment ref="B18" authorId="0">
       <text>
         <r>
           <rPr>
@@ -216,7 +238,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B19" authorId="1">
+    <comment ref="B19" authorId="0">
       <text>
         <r>
           <rPr>
@@ -6491,8 +6513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -7473,7 +7495,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
renamed former 'maternal intervetions' to 'birth outcome' interventions. added new interventions affected fraction and delivery types stratified by delivery type to spreadsheet and data object.
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Jan/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Jan/InputForCode_Bangladesh.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-37720" yWindow="1120" windowWidth="31360" windowHeight="14560" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="-35840" yWindow="-3600" windowWidth="26300" windowHeight="14840" tabRatio="500" firstSheet="24" activeTab="25"/>
   </bookViews>
   <sheets>
     <sheet name="demographics" sheetId="1" r:id="rId1"/>
@@ -28,10 +28,12 @@
     <sheet name="Appropriate breastfeeding" sheetId="19" r:id="rId19"/>
     <sheet name="Interventions cost and coverage" sheetId="20" r:id="rId20"/>
     <sheet name="Interventions target population" sheetId="21" r:id="rId21"/>
-    <sheet name="Interventions maternal" sheetId="22" r:id="rId22"/>
+    <sheet name="Interventions birth outcome" sheetId="22" r:id="rId22"/>
     <sheet name="Interventions affected fraction" sheetId="23" r:id="rId23"/>
     <sheet name="Interventions mortality eff" sheetId="24" r:id="rId24"/>
     <sheet name="Interventions incidence eff" sheetId="25" r:id="rId25"/>
+    <sheet name="Interventions maternal aff frac" sheetId="26" r:id="rId26"/>
+    <sheet name="Interventions maternal eff" sheetId="27" r:id="rId27"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -299,7 +301,40 @@
 <file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
+    <author>Ruth</author>
+  </authors>
+  <commentList>
+    <comment ref="A18" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Active management of the third stage of labor</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
     <author>Janka Petravic</author>
+    <author>Ruth</author>
   </authors>
   <commentList>
     <comment ref="D4" authorId="0">
@@ -368,12 +403,186 @@
         </r>
       </text>
     </comment>
+    <comment ref="A18" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Active management of the third stage of labor</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Ruth</author>
+  </authors>
+  <commentList>
+    <comment ref="F1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Basic Emergency Obstetric Care Centre</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Comprehensive Emergency Obstetric Care Services</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A7" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Active management of the third stage of labor</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Ruth</author>
+  </authors>
+  <commentList>
+    <comment ref="F1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Basic Emergency Obstetric Care Centre</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Comprehensive Emergency Obstetric Care Services</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A7" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Active management of the third stage of labor</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="110">
   <si>
     <t>indicators</t>
   </si>
@@ -688,6 +897,21 @@
   </si>
   <si>
     <t>obese</t>
+  </si>
+  <si>
+    <t>Labor and delivery management</t>
+  </si>
+  <si>
+    <t>Clean birth practices</t>
+  </si>
+  <si>
+    <t>Antibiotics for pPRoM</t>
+  </si>
+  <si>
+    <t>MgSO4 management of eclampsia</t>
+  </si>
+  <si>
+    <t>AMTSL</t>
   </si>
 </sst>
 </file>
@@ -839,7 +1063,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="36">
+  <cellStyleXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -876,8 +1100,54 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -955,8 +1225,18 @@
     <xf numFmtId="2" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="15" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="15" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="15" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="36">
+  <cellStyles count="82">
     <cellStyle name="Excel Built-in Normal" xfId="15"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -975,6 +1255,29 @@
     <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -992,6 +1295,29 @@
     <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="34" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="36" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="64" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="66" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="68" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="70" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="72" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="74" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="76" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="78" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="80" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3593,7 +3919,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -4153,16 +4479,16 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="37.83203125" customWidth="1"/>
+    <col min="1" max="1" width="43.6640625" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
     <col min="3" max="3" width="20.5" customWidth="1"/>
     <col min="4" max="4" width="20.1640625" customWidth="1"/>
@@ -4289,7 +4615,7 @@
         <v>95</v>
       </c>
       <c r="B8" s="32">
-        <v>96</v>
+        <v>0.96</v>
       </c>
       <c r="C8" s="33">
         <v>0.85</v>
@@ -4306,7 +4632,7 @@
         <v>96</v>
       </c>
       <c r="B9" s="32">
-        <v>1.6</v>
+        <v>1.6E-2</v>
       </c>
       <c r="C9" s="33">
         <v>0.85</v>
@@ -4340,7 +4666,7 @@
         <v>98</v>
       </c>
       <c r="B11" s="32">
-        <v>1.6</v>
+        <v>1.6E-2</v>
       </c>
       <c r="C11" s="33">
         <v>0.85</v>
@@ -4357,7 +4683,7 @@
         <v>99</v>
       </c>
       <c r="B12" s="34">
-        <v>1.6</v>
+        <v>1.6E-2</v>
       </c>
       <c r="C12" s="33">
         <v>0.85</v>
@@ -4391,7 +4717,7 @@
         <v>101</v>
       </c>
       <c r="B14" s="32">
-        <v>35.1</v>
+        <v>0.35099999999999998</v>
       </c>
       <c r="C14" s="33">
         <v>0.85</v>
@@ -4428,44 +4754,96 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-    </row>
-    <row r="18" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-    </row>
-    <row r="19" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-    </row>
-    <row r="20" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-    </row>
-    <row r="21" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-    </row>
-    <row r="22" spans="2:3" ht="15.75" customHeight="1">
+    <row r="17" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A17" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="B17" s="6">
+        <v>0</v>
+      </c>
+      <c r="C17" s="33">
+        <v>0.85</v>
+      </c>
+      <c r="D17" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A18" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="B18" s="6">
+        <v>0</v>
+      </c>
+      <c r="C18" s="33">
+        <v>0.85</v>
+      </c>
+      <c r="D18" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A19" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="B19" s="6">
+        <v>0</v>
+      </c>
+      <c r="C19" s="33">
+        <v>0.85</v>
+      </c>
+      <c r="D19" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A20" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="B20" s="6">
+        <v>0</v>
+      </c>
+      <c r="C20" s="33">
+        <v>0.85</v>
+      </c>
+      <c r="D20" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A21" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="B21" s="6">
+        <v>0</v>
+      </c>
+      <c r="C21" s="6">
+        <v>0.85</v>
+      </c>
+      <c r="D21" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15.75" customHeight="1">
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
     </row>
-    <row r="23" spans="2:3" ht="15.75" customHeight="1">
+    <row r="23" spans="1:4" ht="15.75" customHeight="1">
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
     </row>
-    <row r="24" spans="2:3" ht="15.75" customHeight="1">
+    <row r="24" spans="1:4" ht="15.75" customHeight="1">
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
     </row>
-    <row r="25" spans="2:3" ht="15.75" customHeight="1">
+    <row r="25" spans="1:4" ht="15.75" customHeight="1">
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -4479,12 +4857,12 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:G16"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="37.6640625" customWidth="1"/>
+    <col min="1" max="1" width="48" customWidth="1"/>
     <col min="2" max="6" width="13.5" customWidth="1"/>
     <col min="7" max="7" width="17.33203125" customWidth="1"/>
     <col min="8" max="8" width="9.33203125" customWidth="1"/>
@@ -4865,39 +5243,134 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-    </row>
-    <row r="18" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-    </row>
-    <row r="19" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-    </row>
-    <row r="20" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-    </row>
-    <row r="21" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-    </row>
-    <row r="22" spans="2:3" ht="15.75" customHeight="1">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A17" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="B17" s="33">
+        <v>0</v>
+      </c>
+      <c r="C17" s="33">
+        <v>0</v>
+      </c>
+      <c r="D17" s="33">
+        <v>0</v>
+      </c>
+      <c r="E17" s="33">
+        <v>0</v>
+      </c>
+      <c r="F17" s="33">
+        <v>0</v>
+      </c>
+      <c r="G17" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A18" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="B18" s="33">
+        <v>0</v>
+      </c>
+      <c r="C18" s="33">
+        <v>0</v>
+      </c>
+      <c r="D18" s="33">
+        <v>0</v>
+      </c>
+      <c r="E18" s="33">
+        <v>0</v>
+      </c>
+      <c r="F18" s="33">
+        <v>0</v>
+      </c>
+      <c r="G18" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A19" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="B19" s="33">
+        <v>0</v>
+      </c>
+      <c r="C19" s="33">
+        <v>0</v>
+      </c>
+      <c r="D19" s="33">
+        <v>0</v>
+      </c>
+      <c r="E19" s="33">
+        <v>0</v>
+      </c>
+      <c r="F19" s="33">
+        <v>0</v>
+      </c>
+      <c r="G19" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A20" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="B20" s="33">
+        <v>0</v>
+      </c>
+      <c r="C20" s="33">
+        <v>0</v>
+      </c>
+      <c r="D20" s="33">
+        <v>0</v>
+      </c>
+      <c r="E20" s="33">
+        <v>0</v>
+      </c>
+      <c r="F20" s="33">
+        <v>0</v>
+      </c>
+      <c r="G20" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A21" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="B21" s="6">
+        <v>0</v>
+      </c>
+      <c r="C21" s="6">
+        <v>0</v>
+      </c>
+      <c r="D21" s="44">
+        <v>0</v>
+      </c>
+      <c r="E21" s="44">
+        <v>0</v>
+      </c>
+      <c r="F21" s="44">
+        <v>0</v>
+      </c>
+      <c r="G21" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="15.75" customHeight="1">
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
     </row>
-    <row r="23" spans="2:3" ht="15.75" customHeight="1">
+    <row r="23" spans="1:7" ht="15.75" customHeight="1">
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
     </row>
-    <row r="24" spans="2:3" ht="15.75" customHeight="1">
+    <row r="24" spans="1:7" ht="15.75" customHeight="1">
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
     </row>
-    <row r="25" spans="2:3" ht="15.75" customHeight="1">
+    <row r="25" spans="1:7" ht="15.75" customHeight="1">
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
     </row>
@@ -5037,7 +5510,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -5371,7 +5844,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -5810,6 +6283,581 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="42.5" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" customWidth="1"/>
+    <col min="5" max="5" width="15.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="40" t="s">
+        <v>92</v>
+      </c>
+      <c r="D1" s="40" t="s">
+        <v>93</v>
+      </c>
+      <c r="E1" s="40" t="s">
+        <v>94</v>
+      </c>
+      <c r="F1" s="40" t="s">
+        <v>89</v>
+      </c>
+      <c r="G1" s="40" t="s">
+        <v>90</v>
+      </c>
+      <c r="H1" s="41"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="35">
+        <v>1</v>
+      </c>
+      <c r="D2" s="35">
+        <v>1</v>
+      </c>
+      <c r="E2" s="35">
+        <v>1</v>
+      </c>
+      <c r="F2" s="35">
+        <v>1</v>
+      </c>
+      <c r="G2" s="41">
+        <v>1</v>
+      </c>
+      <c r="H2" s="41"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="41"/>
+      <c r="B3" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" s="35">
+        <v>1</v>
+      </c>
+      <c r="D3" s="35">
+        <v>1</v>
+      </c>
+      <c r="E3" s="35">
+        <v>1</v>
+      </c>
+      <c r="F3" s="35">
+        <v>1</v>
+      </c>
+      <c r="G3" s="41">
+        <v>1</v>
+      </c>
+      <c r="H3" s="41"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="37"/>
+      <c r="B4" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" s="35">
+        <v>1</v>
+      </c>
+      <c r="D4" s="35">
+        <v>1</v>
+      </c>
+      <c r="E4" s="35">
+        <v>1</v>
+      </c>
+      <c r="F4" s="35">
+        <v>1</v>
+      </c>
+      <c r="G4" s="41">
+        <v>1</v>
+      </c>
+      <c r="H4" s="41"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="37"/>
+      <c r="B5" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="C5" s="35">
+        <v>1</v>
+      </c>
+      <c r="D5" s="35">
+        <v>1</v>
+      </c>
+      <c r="E5" s="35">
+        <v>1</v>
+      </c>
+      <c r="F5" s="35">
+        <v>1</v>
+      </c>
+      <c r="G5" s="41">
+        <v>1</v>
+      </c>
+      <c r="H5" s="41"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="37"/>
+      <c r="B6" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" s="35">
+        <v>7.8159999999999993E-2</v>
+      </c>
+      <c r="D6" s="35">
+        <v>7.8159999999999993E-2</v>
+      </c>
+      <c r="E6" s="35">
+        <v>7.8159999999999993E-2</v>
+      </c>
+      <c r="F6" s="35">
+        <v>7.8159999999999993E-2</v>
+      </c>
+      <c r="G6" s="35">
+        <v>7.8159999999999993E-2</v>
+      </c>
+      <c r="H6" s="41"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" s="35">
+        <v>1</v>
+      </c>
+      <c r="D7" s="35">
+        <v>1</v>
+      </c>
+      <c r="E7" s="35">
+        <v>1</v>
+      </c>
+      <c r="F7" s="35">
+        <v>1</v>
+      </c>
+      <c r="G7" s="41">
+        <v>1</v>
+      </c>
+      <c r="H7" s="41"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" s="35">
+        <v>1</v>
+      </c>
+      <c r="D8" s="35">
+        <v>1</v>
+      </c>
+      <c r="E8" s="35">
+        <v>1</v>
+      </c>
+      <c r="F8" s="35">
+        <v>1</v>
+      </c>
+      <c r="G8" s="41">
+        <v>1</v>
+      </c>
+      <c r="H8" s="41"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="B9" s="37" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9" s="35">
+        <v>1</v>
+      </c>
+      <c r="D9" s="35">
+        <v>1</v>
+      </c>
+      <c r="E9" s="35">
+        <v>1</v>
+      </c>
+      <c r="F9" s="35">
+        <v>1</v>
+      </c>
+      <c r="G9" s="41">
+        <v>1</v>
+      </c>
+      <c r="H9" s="41"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="B10" s="37" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" s="35">
+        <v>0.33</v>
+      </c>
+      <c r="D10" s="35">
+        <v>0.33</v>
+      </c>
+      <c r="E10" s="35">
+        <v>0.33</v>
+      </c>
+      <c r="F10" s="35">
+        <v>0.33</v>
+      </c>
+      <c r="G10" s="35">
+        <v>0.33</v>
+      </c>
+      <c r="H10" s="41"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="37"/>
+      <c r="B11" s="37"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="41"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="37"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="41"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="41"/>
+      <c r="B13" s="41"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="41"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="41"/>
+      <c r="B14" s="41"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="41"/>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" s="36"/>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" s="37"/>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" s="37"/>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" s="37"/>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" s="37"/>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" s="37"/>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="37"/>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="37"/>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" s="37"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="14" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="31.6640625" customWidth="1"/>
+    <col min="2" max="2" width="28" customWidth="1"/>
+    <col min="4" max="4" width="16.83203125" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="42" t="s">
+        <v>92</v>
+      </c>
+      <c r="D1" s="42" t="s">
+        <v>93</v>
+      </c>
+      <c r="E1" s="42" t="s">
+        <v>94</v>
+      </c>
+      <c r="F1" s="42" t="s">
+        <v>89</v>
+      </c>
+      <c r="G1" s="42" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="42" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" s="42" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="23">
+        <v>0</v>
+      </c>
+      <c r="D2" s="23">
+        <v>0</v>
+      </c>
+      <c r="E2" s="23">
+        <v>0</v>
+      </c>
+      <c r="F2" s="23">
+        <v>0.2</v>
+      </c>
+      <c r="G2" s="23">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="B3" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" s="23">
+        <v>0</v>
+      </c>
+      <c r="D3" s="23">
+        <v>0</v>
+      </c>
+      <c r="E3" s="23">
+        <v>0</v>
+      </c>
+      <c r="F3" s="23">
+        <v>0.2</v>
+      </c>
+      <c r="G3" s="23">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="43"/>
+      <c r="B4" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" s="23">
+        <v>0</v>
+      </c>
+      <c r="D4" s="23">
+        <v>0</v>
+      </c>
+      <c r="E4" s="23">
+        <v>0</v>
+      </c>
+      <c r="F4" s="23">
+        <v>0.35</v>
+      </c>
+      <c r="G4" s="23">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="43"/>
+      <c r="B5" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="C5" s="23">
+        <v>0</v>
+      </c>
+      <c r="D5" s="23">
+        <v>0</v>
+      </c>
+      <c r="E5" s="23">
+        <v>0</v>
+      </c>
+      <c r="F5" s="23">
+        <v>0</v>
+      </c>
+      <c r="G5" s="23">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="43"/>
+      <c r="B6" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" s="23">
+        <v>0</v>
+      </c>
+      <c r="D6" s="23">
+        <v>0</v>
+      </c>
+      <c r="E6" s="23">
+        <v>0</v>
+      </c>
+      <c r="F6" s="23">
+        <v>0.38</v>
+      </c>
+      <c r="G6" s="23">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="42" t="s">
+        <v>109</v>
+      </c>
+      <c r="B7" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" s="23">
+        <v>0</v>
+      </c>
+      <c r="D7" s="23">
+        <v>0.7</v>
+      </c>
+      <c r="E7" s="23">
+        <v>0.7</v>
+      </c>
+      <c r="F7" s="23">
+        <v>0.7</v>
+      </c>
+      <c r="G7" s="23">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="42" t="s">
+        <v>108</v>
+      </c>
+      <c r="B8" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" s="23">
+        <v>0</v>
+      </c>
+      <c r="D8" s="23">
+        <v>0.6</v>
+      </c>
+      <c r="E8" s="23">
+        <v>0.6</v>
+      </c>
+      <c r="F8" s="23">
+        <v>0.6</v>
+      </c>
+      <c r="G8" s="23">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="42" t="s">
+        <v>106</v>
+      </c>
+      <c r="B9" s="43" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9" s="23">
+        <v>0</v>
+      </c>
+      <c r="D9" s="23">
+        <v>0.6</v>
+      </c>
+      <c r="E9" s="23">
+        <v>0.6</v>
+      </c>
+      <c r="F9" s="23">
+        <v>0.6</v>
+      </c>
+      <c r="G9" s="23">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="B10" s="43" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" s="23">
+        <v>0</v>
+      </c>
+      <c r="D10" s="23">
+        <v>0.8</v>
+      </c>
+      <c r="E10" s="23">
+        <v>0.8</v>
+      </c>
+      <c r="F10" s="23">
+        <v>0.8</v>
+      </c>
+      <c r="G10" s="23">
+        <v>0.8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
@@ -5865,7 +6913,7 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="A19" sqref="A19:A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -6513,8 +7561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15:B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
added reproductive age to spreadsheet and new anemia prevalance tab.  Modified data.py to read them in to data object
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Jan/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Jan/InputForCode_Bangladesh.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-35840" yWindow="-3600" windowWidth="26300" windowHeight="14840" tabRatio="500" firstSheet="24" activeTab="25"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14600" tabRatio="500" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="demographics" sheetId="1" r:id="rId1"/>
@@ -12,28 +12,29 @@
     <sheet name="mortality rates" sheetId="3" r:id="rId3"/>
     <sheet name="causes of death" sheetId="4" r:id="rId4"/>
     <sheet name="distributions" sheetId="5" r:id="rId5"/>
-    <sheet name="birth outcome distribution" sheetId="6" r:id="rId6"/>
-    <sheet name="Incidence of conditions" sheetId="7" r:id="rId7"/>
-    <sheet name="RR death by stunting" sheetId="8" r:id="rId8"/>
-    <sheet name="RR death by wasting" sheetId="9" r:id="rId9"/>
-    <sheet name="RR death by breastfeeding" sheetId="10" r:id="rId10"/>
-    <sheet name="RR death by birth outcome" sheetId="11" r:id="rId11"/>
-    <sheet name="OR stunting progression" sheetId="12" r:id="rId12"/>
-    <sheet name="RR diarrhoea" sheetId="13" r:id="rId13"/>
-    <sheet name="OR stunting by condition" sheetId="14" r:id="rId14"/>
-    <sheet name="OR stunting by birth outcome" sheetId="15" r:id="rId15"/>
-    <sheet name="OR stunting by intervention" sheetId="16" r:id="rId16"/>
-    <sheet name="OR stunting by compfeeding" sheetId="17" r:id="rId17"/>
-    <sheet name="OR correctBF by interventn" sheetId="18" r:id="rId18"/>
-    <sheet name="Appropriate breastfeeding" sheetId="19" r:id="rId19"/>
-    <sheet name="Interventions cost and coverage" sheetId="20" r:id="rId20"/>
-    <sheet name="Interventions target population" sheetId="21" r:id="rId21"/>
-    <sheet name="Interventions birth outcome" sheetId="22" r:id="rId22"/>
-    <sheet name="Interventions affected fraction" sheetId="23" r:id="rId23"/>
-    <sheet name="Interventions mortality eff" sheetId="24" r:id="rId24"/>
-    <sheet name="Interventions incidence eff" sheetId="25" r:id="rId25"/>
-    <sheet name="Interventions maternal aff frac" sheetId="26" r:id="rId26"/>
-    <sheet name="Interventions maternal eff" sheetId="27" r:id="rId27"/>
+    <sheet name="anemia prevalence" sheetId="28" r:id="rId6"/>
+    <sheet name="birth outcome distribution" sheetId="6" r:id="rId7"/>
+    <sheet name="Incidence of conditions" sheetId="7" r:id="rId8"/>
+    <sheet name="RR death by stunting" sheetId="8" r:id="rId9"/>
+    <sheet name="RR death by wasting" sheetId="9" r:id="rId10"/>
+    <sheet name="RR death by breastfeeding" sheetId="10" r:id="rId11"/>
+    <sheet name="RR death by birth outcome" sheetId="11" r:id="rId12"/>
+    <sheet name="OR stunting progression" sheetId="12" r:id="rId13"/>
+    <sheet name="RR diarrhoea" sheetId="13" r:id="rId14"/>
+    <sheet name="OR stunting by condition" sheetId="14" r:id="rId15"/>
+    <sheet name="OR stunting by birth outcome" sheetId="15" r:id="rId16"/>
+    <sheet name="OR stunting by intervention" sheetId="16" r:id="rId17"/>
+    <sheet name="OR stunting by compfeeding" sheetId="17" r:id="rId18"/>
+    <sheet name="OR correctBF by interventn" sheetId="18" r:id="rId19"/>
+    <sheet name="Appropriate breastfeeding" sheetId="19" r:id="rId20"/>
+    <sheet name="Interventions cost and coverage" sheetId="20" r:id="rId21"/>
+    <sheet name="Interventions target population" sheetId="21" r:id="rId22"/>
+    <sheet name="Interventions birth outcome" sheetId="22" r:id="rId23"/>
+    <sheet name="Interventions affected fraction" sheetId="23" r:id="rId24"/>
+    <sheet name="Interventions mortality eff" sheetId="24" r:id="rId25"/>
+    <sheet name="Interventions incidence eff" sheetId="25" r:id="rId26"/>
+    <sheet name="Interventions maternal aff frac" sheetId="26" r:id="rId27"/>
+    <sheet name="Interventions maternal eff" sheetId="27" r:id="rId28"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -50,11 +51,34 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
+    <author>Ruth</author>
     <author>Janka Petravic</author>
     <author>Microsoft Office User</author>
   </authors>
   <commentList>
-    <comment ref="A5" authorId="0">
+    <comment ref="B5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+place holder value, assuming 10% of reproductive age are pregnant</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A6" authorId="1">
       <text>
         <r>
           <rPr>
@@ -76,7 +100,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A6" authorId="1">
+    <comment ref="A7" authorId="2">
       <text>
         <r>
           <rPr>
@@ -269,6 +293,39 @@
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
+    <author>Ruth</author>
+  </authors>
+  <commentList>
+    <comment ref="L2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+place holder values
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
     <author>Janka Petravic</author>
   </authors>
   <commentList>
@@ -298,7 +355,7 @@
 </comments>
 </file>
 
-<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Ruth</author>
@@ -330,7 +387,7 @@
 </comments>
 </file>
 
-<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Janka Petravic</author>
@@ -404,82 +461,6 @@
       </text>
     </comment>
     <comment ref="A18" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>Ruth:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Active management of the third stage of labor</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Ruth</author>
-  </authors>
-  <commentList>
-    <comment ref="F1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>Ruth:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Basic Emergency Obstetric Care Centre</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>Ruth:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Comprehensive Emergency Obstetric Care Services</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A7" authorId="0">
       <text>
         <r>
           <rPr>
@@ -581,8 +562,84 @@
 </comments>
 </file>
 
+<file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Ruth</author>
+  </authors>
+  <commentList>
+    <comment ref="F1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Basic Emergency Obstetric Care Centre</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Comprehensive Emergency Obstetric Care Services</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A7" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Active management of the third stage of labor</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="117">
   <si>
     <t>indicators</t>
   </si>
@@ -912,6 +969,27 @@
   </si>
   <si>
     <t>AMTSL</t>
+  </si>
+  <si>
+    <t>population reproductive age</t>
+  </si>
+  <si>
+    <t>15-19 years</t>
+  </si>
+  <si>
+    <t>20-24 years</t>
+  </si>
+  <si>
+    <t>25-29 years</t>
+  </si>
+  <si>
+    <t>30-34 years</t>
+  </si>
+  <si>
+    <t>35-39 years</t>
+  </si>
+  <si>
+    <t>40-44 years</t>
   </si>
 </sst>
 </file>
@@ -921,7 +999,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1003,6 +1081,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -1063,7 +1147,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="82">
+  <cellStyleXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1146,8 +1230,12 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1235,8 +1323,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="15" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="15" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="82">
+  <cellStyles count="86">
     <cellStyle name="Excel Built-in Normal" xfId="15"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -1278,6 +1367,8 @@
     <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1318,6 +1409,8 @@
     <cellStyle name="Hyperlink" xfId="76" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="78" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="80" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="82" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="84" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2682,10 +2775,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B13:B14"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -2727,25 +2820,34 @@
     </row>
     <row r="5" spans="1:2" ht="15.75" customHeight="1">
       <c r="A5" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="B5" s="12">
-        <v>0.56799999999999995</v>
+        <v>110</v>
+      </c>
+      <c r="B5" s="8">
+        <f>B4*10</f>
+        <v>36899440</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.75" customHeight="1">
       <c r="A6" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B6" s="22">
-        <v>0.4</v>
+        <v>71</v>
+      </c>
+      <c r="B6" s="12">
+        <v>0.56799999999999995</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.75" customHeight="1">
       <c r="A7" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" s="22">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A8" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="B7" s="22">
+      <c r="B8" s="22">
         <v>0.20599999999999999</v>
       </c>
     </row>
@@ -2761,6 +2863,565 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
+      <c r="B3" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="6">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
+      <c r="B4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="6">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1.6</v>
+      </c>
+      <c r="E4">
+        <v>1.6</v>
+      </c>
+      <c r="F4">
+        <v>1.6</v>
+      </c>
+      <c r="G4">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
+      <c r="B5" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="6">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>3.41</v>
+      </c>
+      <c r="E5">
+        <v>3.41</v>
+      </c>
+      <c r="F5">
+        <v>3.41</v>
+      </c>
+      <c r="G5">
+        <v>3.41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
+      <c r="B6" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>12.33</v>
+      </c>
+      <c r="E6">
+        <v>12.33</v>
+      </c>
+      <c r="F6">
+        <v>12.33</v>
+      </c>
+      <c r="G6">
+        <v>12.33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
+      <c r="B8" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="6">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
+      <c r="B9" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="6">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1.92</v>
+      </c>
+      <c r="E9">
+        <v>1.92</v>
+      </c>
+      <c r="F9">
+        <v>1.92</v>
+      </c>
+      <c r="G9">
+        <v>1.92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" customHeight="1">
+      <c r="B10" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="6">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>4.66</v>
+      </c>
+      <c r="E10">
+        <v>4.66</v>
+      </c>
+      <c r="F10">
+        <v>4.66</v>
+      </c>
+      <c r="G10">
+        <v>4.66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" customHeight="1">
+      <c r="B11" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="6">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>9.68</v>
+      </c>
+      <c r="E11">
+        <v>9.68</v>
+      </c>
+      <c r="F11">
+        <v>9.68</v>
+      </c>
+      <c r="G11">
+        <v>9.68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" customHeight="1">
+      <c r="B13" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="6">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" customHeight="1">
+      <c r="B14" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="6">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" customHeight="1">
+      <c r="B15" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="6">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>2.58</v>
+      </c>
+      <c r="E15">
+        <v>2.58</v>
+      </c>
+      <c r="F15">
+        <v>2.58</v>
+      </c>
+      <c r="G15">
+        <v>2.58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" customHeight="1">
+      <c r="B16" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="6">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>9.6300000000000008</v>
+      </c>
+      <c r="E16">
+        <v>9.6300000000000008</v>
+      </c>
+      <c r="F16">
+        <v>9.6300000000000008</v>
+      </c>
+      <c r="G16">
+        <v>9.6300000000000008</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" customHeight="1">
+      <c r="B18" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="6">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" customHeight="1">
+      <c r="B19" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="6">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15.75" customHeight="1">
+      <c r="B20" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="6">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" customHeight="1">
+      <c r="B21" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="6">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="15.75" customHeight="1">
+      <c r="B23" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="6">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="15.75" customHeight="1">
+      <c r="B24" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="6">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>1.65</v>
+      </c>
+      <c r="E24">
+        <v>1.65</v>
+      </c>
+      <c r="F24">
+        <v>1.65</v>
+      </c>
+      <c r="G24">
+        <v>1.65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="15.75" customHeight="1">
+      <c r="B25" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="6">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>2.73</v>
+      </c>
+      <c r="E25">
+        <v>2.73</v>
+      </c>
+      <c r="F25">
+        <v>2.73</v>
+      </c>
+      <c r="G25">
+        <v>2.73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15.75" customHeight="1">
+      <c r="B26" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="6">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>11.21</v>
+      </c>
+      <c r="E26">
+        <v>11.21</v>
+      </c>
+      <c r="F26">
+        <v>11.21</v>
+      </c>
+      <c r="G26">
+        <v>11.21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G29"/>
   <sheetViews>
@@ -3387,7 +4048,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G29"/>
   <sheetViews>
@@ -3685,7 +4346,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -3733,7 +4394,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
@@ -3854,7 +4515,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -3914,7 +4575,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -3962,7 +4623,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
@@ -4050,7 +4711,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
@@ -4173,7 +4834,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
@@ -4254,75 +4915,6 @@
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="5" width="13.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="14">
-      <c r="A2" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4479,6 +5071,75 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="5" width="13.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="14">
+      <c r="A2" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G25"/>
   <sheetViews>
@@ -4852,7 +5513,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J25"/>
   <sheetViews>
@@ -4952,11 +5613,11 @@
         <v>0</v>
       </c>
       <c r="D4" s="4">
-        <f>demographics!$B$6</f>
+        <f>demographics!$B$7</f>
         <v>0.4</v>
       </c>
       <c r="E4" s="4">
-        <f>demographics!$B$6</f>
+        <f>demographics!$B$7</f>
         <v>0.4</v>
       </c>
       <c r="F4" s="4">
@@ -5009,7 +5670,7 @@
         <v>0</v>
       </c>
       <c r="G6" s="4">
-        <f>demographics!$B$6</f>
+        <f>demographics!$B$7</f>
         <v>0.4</v>
       </c>
     </row>
@@ -5386,7 +6047,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
@@ -5444,11 +6105,11 @@
         <v>69</v>
       </c>
       <c r="C3" s="20">
-        <f>demographics!$B$5 * 'Interventions target population'!$G$6</f>
+        <f>demographics!$B$6 * 'Interventions target population'!$G$6</f>
         <v>0.22719999999999999</v>
       </c>
       <c r="D3" s="20">
-        <f>demographics!$B$5 * 'Interventions target population'!$G$6</f>
+        <f>demographics!$B$6 * 'Interventions target population'!$G$6</f>
         <v>0.22719999999999999</v>
       </c>
       <c r="E3" s="20">
@@ -5497,340 +6158,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="27" customWidth="1"/>
-    <col min="2" max="2" width="28.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A1" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A2" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="B2" s="35" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="6">
-        <v>0</v>
-      </c>
-      <c r="D2" s="6">
-        <v>0</v>
-      </c>
-      <c r="E2" s="6">
-        <v>0.33500000000000002</v>
-      </c>
-      <c r="F2" s="21">
-        <v>0.33500000000000002</v>
-      </c>
-      <c r="G2" s="21">
-        <v>0.33500000000000002</v>
-      </c>
-      <c r="H2" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="15.75" customHeight="1">
-      <c r="B3" s="35" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" s="6">
-        <v>0</v>
-      </c>
-      <c r="D3" s="6">
-        <v>0</v>
-      </c>
-      <c r="E3" s="6">
-        <v>0</v>
-      </c>
-      <c r="F3" s="6">
-        <v>0</v>
-      </c>
-      <c r="G3" s="6">
-        <v>0</v>
-      </c>
-      <c r="H3" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A4" s="32" t="s">
-        <v>95</v>
-      </c>
-      <c r="B4" s="36" t="s">
-        <v>88</v>
-      </c>
-      <c r="C4" s="6">
-        <v>0</v>
-      </c>
-      <c r="D4" s="6">
-        <v>0</v>
-      </c>
-      <c r="E4" s="6">
-        <v>0</v>
-      </c>
-      <c r="F4" s="6">
-        <v>0</v>
-      </c>
-      <c r="G4" s="6">
-        <v>0</v>
-      </c>
-      <c r="H4" s="32">
-        <v>4.895E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A5" s="32" t="s">
-        <v>96</v>
-      </c>
-      <c r="B5" s="37" t="s">
-        <v>88</v>
-      </c>
-      <c r="C5" s="6">
-        <v>0</v>
-      </c>
-      <c r="D5" s="6">
-        <v>0</v>
-      </c>
-      <c r="E5" s="6">
-        <v>0</v>
-      </c>
-      <c r="F5" s="6">
-        <v>0</v>
-      </c>
-      <c r="G5" s="6">
-        <v>0</v>
-      </c>
-      <c r="H5" s="32">
-        <v>2.0998000000000003E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A6" s="32" t="s">
-        <v>97</v>
-      </c>
-      <c r="B6" s="37" t="s">
-        <v>83</v>
-      </c>
-      <c r="C6" s="6">
-        <v>0</v>
-      </c>
-      <c r="D6" s="6">
-        <v>0</v>
-      </c>
-      <c r="E6" s="6">
-        <v>0</v>
-      </c>
-      <c r="F6" s="6">
-        <v>0</v>
-      </c>
-      <c r="G6" s="6">
-        <v>0</v>
-      </c>
-      <c r="H6" s="32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A7" s="32" t="s">
-        <v>98</v>
-      </c>
-      <c r="B7" s="37" t="s">
-        <v>83</v>
-      </c>
-      <c r="C7" s="6">
-        <v>0</v>
-      </c>
-      <c r="D7" s="6">
-        <v>0</v>
-      </c>
-      <c r="E7" s="6">
-        <v>0</v>
-      </c>
-      <c r="F7" s="6">
-        <v>0</v>
-      </c>
-      <c r="G7" s="6">
-        <v>0</v>
-      </c>
-      <c r="H7" s="32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A8" s="32" t="s">
-        <v>99</v>
-      </c>
-      <c r="B8" s="37" t="s">
-        <v>83</v>
-      </c>
-      <c r="C8" s="6">
-        <v>0</v>
-      </c>
-      <c r="D8" s="6">
-        <v>0</v>
-      </c>
-      <c r="E8" s="6">
-        <v>0</v>
-      </c>
-      <c r="F8" s="6">
-        <v>0</v>
-      </c>
-      <c r="G8" s="6">
-        <v>0</v>
-      </c>
-      <c r="H8" s="32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A9" s="32" t="s">
-        <v>100</v>
-      </c>
-      <c r="B9" s="37" t="s">
-        <v>84</v>
-      </c>
-      <c r="C9" s="6">
-        <v>0</v>
-      </c>
-      <c r="D9" s="6">
-        <v>0</v>
-      </c>
-      <c r="E9" s="6">
-        <v>0</v>
-      </c>
-      <c r="F9" s="6">
-        <v>0</v>
-      </c>
-      <c r="G9" s="6">
-        <v>0</v>
-      </c>
-      <c r="H9" s="32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A10" s="32" t="s">
-        <v>101</v>
-      </c>
-      <c r="B10" s="37" t="s">
-        <v>85</v>
-      </c>
-      <c r="C10" s="6">
-        <v>0</v>
-      </c>
-      <c r="D10" s="6">
-        <v>0</v>
-      </c>
-      <c r="E10" s="6">
-        <v>0</v>
-      </c>
-      <c r="F10" s="6">
-        <v>0</v>
-      </c>
-      <c r="G10" s="6">
-        <v>0</v>
-      </c>
-      <c r="H10" s="32">
-        <v>0.90526300000000004</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A11" s="32" t="s">
-        <v>102</v>
-      </c>
-      <c r="B11" s="37" t="s">
-        <v>85</v>
-      </c>
-      <c r="C11" s="6">
-        <v>0</v>
-      </c>
-      <c r="D11" s="6">
-        <v>0</v>
-      </c>
-      <c r="E11" s="6">
-        <v>0</v>
-      </c>
-      <c r="F11" s="6">
-        <v>0</v>
-      </c>
-      <c r="G11" s="6">
-        <v>0</v>
-      </c>
-      <c r="H11" s="32">
-        <v>0.90526300000000004</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A12" s="32" t="s">
-        <v>103</v>
-      </c>
-      <c r="B12" s="37" t="s">
-        <v>85</v>
-      </c>
-      <c r="C12" s="6">
-        <v>0</v>
-      </c>
-      <c r="D12" s="6">
-        <v>0</v>
-      </c>
-      <c r="E12" s="6">
-        <v>0</v>
-      </c>
-      <c r="F12" s="6">
-        <v>0</v>
-      </c>
-      <c r="G12" s="6">
-        <v>0</v>
-      </c>
-      <c r="H12" s="32">
-        <v>9.4737000000000016E-2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -5849,8 +6176,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="28.83203125" customWidth="1"/>
-    <col min="2" max="2" width="27.83203125" customWidth="1"/>
+    <col min="1" max="1" width="27" customWidth="1"/>
+    <col min="2" max="2" width="28.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1">
@@ -5883,7 +6210,7 @@
       <c r="A2" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="35" t="s">
         <v>34</v>
       </c>
       <c r="C2" s="6">
@@ -5893,20 +6220,20 @@
         <v>0</v>
       </c>
       <c r="E2" s="6">
-        <v>0.3</v>
-      </c>
-      <c r="F2" s="6">
-        <v>0.3</v>
-      </c>
-      <c r="G2" s="6">
-        <v>0.3</v>
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="F2" s="21">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="G2" s="21">
+        <v>0.33500000000000002</v>
       </c>
       <c r="H2" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1">
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="35" t="s">
         <v>36</v>
       </c>
       <c r="C3" s="6">
@@ -5932,7 +6259,7 @@
       <c r="A4" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="36" t="s">
         <v>88</v>
       </c>
       <c r="C4" s="6">
@@ -5951,14 +6278,14 @@
         <v>0</v>
       </c>
       <c r="H4" s="32">
-        <v>0.98</v>
+        <v>4.895E-3</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.75" customHeight="1">
       <c r="A5" s="32" t="s">
         <v>96</v>
       </c>
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="37" t="s">
         <v>88</v>
       </c>
       <c r="C5" s="6">
@@ -5977,14 +6304,14 @@
         <v>0</v>
       </c>
       <c r="H5" s="32">
-        <v>0.8</v>
+        <v>2.0998000000000003E-2</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.75" customHeight="1">
       <c r="A6" s="32" t="s">
         <v>97</v>
       </c>
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="37" t="s">
         <v>83</v>
       </c>
       <c r="C6" s="6">
@@ -6003,14 +6330,14 @@
         <v>0</v>
       </c>
       <c r="H6" s="32">
-        <v>0.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" customHeight="1">
       <c r="A7" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="37" t="s">
         <v>83</v>
       </c>
       <c r="C7" s="6">
@@ -6029,14 +6356,14 @@
         <v>0</v>
       </c>
       <c r="H7" s="32">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" customHeight="1">
       <c r="A8" s="32" t="s">
         <v>99</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="37" t="s">
         <v>83</v>
       </c>
       <c r="C8" s="6">
@@ -6055,14 +6382,14 @@
         <v>0</v>
       </c>
       <c r="H8" s="32">
-        <v>0.59</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" customHeight="1">
       <c r="A9" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="37" t="s">
         <v>84</v>
       </c>
       <c r="C9" s="6">
@@ -6081,14 +6408,14 @@
         <v>0</v>
       </c>
       <c r="H9" s="32">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" customHeight="1">
       <c r="A10" s="32" t="s">
         <v>101</v>
       </c>
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="37" t="s">
         <v>85</v>
       </c>
       <c r="C10" s="6">
@@ -6107,14 +6434,14 @@
         <v>0</v>
       </c>
       <c r="H10" s="32">
-        <v>0.95</v>
+        <v>0.90526300000000004</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1">
       <c r="A11" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="B11" s="32" t="s">
+      <c r="B11" s="37" t="s">
         <v>85</v>
       </c>
       <c r="C11" s="6">
@@ -6133,14 +6460,14 @@
         <v>0</v>
       </c>
       <c r="H11" s="32">
-        <v>0.8</v>
+        <v>0.90526300000000004</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15.75" customHeight="1">
       <c r="A12" s="32" t="s">
         <v>103</v>
       </c>
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="37" t="s">
         <v>85</v>
       </c>
       <c r="C12" s="6">
@@ -6159,7 +6486,7 @@
         <v>0</v>
       </c>
       <c r="H12" s="32">
-        <v>0.9</v>
+        <v>9.4737000000000016E-2</v>
       </c>
     </row>
   </sheetData>
@@ -6174,6 +6501,340 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="28.83203125" customWidth="1"/>
+    <col min="2" max="2" width="27.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A1" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A2" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="6">
+        <v>0</v>
+      </c>
+      <c r="D2" s="6">
+        <v>0</v>
+      </c>
+      <c r="E2" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="F2" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="G2" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="H2" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" customHeight="1">
+      <c r="B3" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0</v>
+      </c>
+      <c r="D3" s="6">
+        <v>0</v>
+      </c>
+      <c r="E3" s="6">
+        <v>0</v>
+      </c>
+      <c r="F3" s="6">
+        <v>0</v>
+      </c>
+      <c r="G3" s="6">
+        <v>0</v>
+      </c>
+      <c r="H3" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A4" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" s="6">
+        <v>0</v>
+      </c>
+      <c r="D4" s="6">
+        <v>0</v>
+      </c>
+      <c r="E4" s="6">
+        <v>0</v>
+      </c>
+      <c r="F4" s="6">
+        <v>0</v>
+      </c>
+      <c r="G4" s="6">
+        <v>0</v>
+      </c>
+      <c r="H4" s="32">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A5" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5" s="6">
+        <v>0</v>
+      </c>
+      <c r="D5" s="6">
+        <v>0</v>
+      </c>
+      <c r="E5" s="6">
+        <v>0</v>
+      </c>
+      <c r="F5" s="6">
+        <v>0</v>
+      </c>
+      <c r="G5" s="6">
+        <v>0</v>
+      </c>
+      <c r="H5" s="32">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A6" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" s="6">
+        <v>0</v>
+      </c>
+      <c r="D6" s="6">
+        <v>0</v>
+      </c>
+      <c r="E6" s="6">
+        <v>0</v>
+      </c>
+      <c r="F6" s="6">
+        <v>0</v>
+      </c>
+      <c r="G6" s="6">
+        <v>0</v>
+      </c>
+      <c r="H6" s="32">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A7" s="32" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" s="6">
+        <v>0</v>
+      </c>
+      <c r="D7" s="6">
+        <v>0</v>
+      </c>
+      <c r="E7" s="6">
+        <v>0</v>
+      </c>
+      <c r="F7" s="6">
+        <v>0</v>
+      </c>
+      <c r="G7" s="6">
+        <v>0</v>
+      </c>
+      <c r="H7" s="32">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A8" s="32" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" s="6">
+        <v>0</v>
+      </c>
+      <c r="D8" s="6">
+        <v>0</v>
+      </c>
+      <c r="E8" s="6">
+        <v>0</v>
+      </c>
+      <c r="F8" s="6">
+        <v>0</v>
+      </c>
+      <c r="G8" s="6">
+        <v>0</v>
+      </c>
+      <c r="H8" s="32">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A9" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="B9" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9" s="6">
+        <v>0</v>
+      </c>
+      <c r="D9" s="6">
+        <v>0</v>
+      </c>
+      <c r="E9" s="6">
+        <v>0</v>
+      </c>
+      <c r="F9" s="6">
+        <v>0</v>
+      </c>
+      <c r="G9" s="6">
+        <v>0</v>
+      </c>
+      <c r="H9" s="32">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A10" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="C10" s="6">
+        <v>0</v>
+      </c>
+      <c r="D10" s="6">
+        <v>0</v>
+      </c>
+      <c r="E10" s="6">
+        <v>0</v>
+      </c>
+      <c r="F10" s="6">
+        <v>0</v>
+      </c>
+      <c r="G10" s="6">
+        <v>0</v>
+      </c>
+      <c r="H10" s="32">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A11" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="B11" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="C11" s="6">
+        <v>0</v>
+      </c>
+      <c r="D11" s="6">
+        <v>0</v>
+      </c>
+      <c r="E11" s="6">
+        <v>0</v>
+      </c>
+      <c r="F11" s="6">
+        <v>0</v>
+      </c>
+      <c r="G11" s="6">
+        <v>0</v>
+      </c>
+      <c r="H11" s="32">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A12" s="32" t="s">
+        <v>103</v>
+      </c>
+      <c r="B12" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="C12" s="6">
+        <v>0</v>
+      </c>
+      <c r="D12" s="6">
+        <v>0</v>
+      </c>
+      <c r="E12" s="6">
+        <v>0</v>
+      </c>
+      <c r="F12" s="6">
+        <v>0</v>
+      </c>
+      <c r="G12" s="6">
+        <v>0</v>
+      </c>
+      <c r="H12" s="32">
+        <v>0.9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
@@ -6283,11 +6944,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
@@ -6610,7 +7271,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
@@ -6913,7 +7574,7 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:A22"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -7562,7 +8223,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:B19"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -7961,6 +8622,107 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:L1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="6" max="6" width="15.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" s="45" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="45" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="45" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="45" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1" s="45" t="s">
+        <v>111</v>
+      </c>
+      <c r="H1" s="45" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1" s="45" t="s">
+        <v>113</v>
+      </c>
+      <c r="J1" s="45" t="s">
+        <v>114</v>
+      </c>
+      <c r="K1" s="45" t="s">
+        <v>115</v>
+      </c>
+      <c r="L1" s="45" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2">
+        <v>0.5</v>
+      </c>
+      <c r="B2">
+        <v>0.5</v>
+      </c>
+      <c r="C2">
+        <v>0.5</v>
+      </c>
+      <c r="D2">
+        <v>0.5</v>
+      </c>
+      <c r="E2">
+        <v>0.5</v>
+      </c>
+      <c r="F2">
+        <v>0.5</v>
+      </c>
+      <c r="G2">
+        <v>0.5</v>
+      </c>
+      <c r="H2">
+        <v>0.5</v>
+      </c>
+      <c r="I2">
+        <v>0.5</v>
+      </c>
+      <c r="J2">
+        <v>0.5</v>
+      </c>
+      <c r="K2">
+        <v>0.5</v>
+      </c>
+      <c r="L2">
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -8002,7 +8764,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -8083,7 +8845,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G21"/>
   <sheetViews>
@@ -8537,563 +9299,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G26"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
-  <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A1" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B3" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="6">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B4" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="6">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>1.6</v>
-      </c>
-      <c r="E4">
-        <v>1.6</v>
-      </c>
-      <c r="F4">
-        <v>1.6</v>
-      </c>
-      <c r="G4">
-        <v>1.6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B5" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="6">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>3.41</v>
-      </c>
-      <c r="E5">
-        <v>3.41</v>
-      </c>
-      <c r="F5">
-        <v>3.41</v>
-      </c>
-      <c r="G5">
-        <v>3.41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B6" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" s="6">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <v>12.33</v>
-      </c>
-      <c r="E6">
-        <v>12.33</v>
-      </c>
-      <c r="F6">
-        <v>12.33</v>
-      </c>
-      <c r="G6">
-        <v>12.33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B8" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="6">
-        <v>1</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B9" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="6">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <v>1.92</v>
-      </c>
-      <c r="E9">
-        <v>1.92</v>
-      </c>
-      <c r="F9">
-        <v>1.92</v>
-      </c>
-      <c r="G9">
-        <v>1.92</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B10" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="6">
-        <v>1</v>
-      </c>
-      <c r="D10">
-        <v>4.66</v>
-      </c>
-      <c r="E10">
-        <v>4.66</v>
-      </c>
-      <c r="F10">
-        <v>4.66</v>
-      </c>
-      <c r="G10">
-        <v>4.66</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B11" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="6">
-        <v>1</v>
-      </c>
-      <c r="D11">
-        <v>9.68</v>
-      </c>
-      <c r="E11">
-        <v>9.68</v>
-      </c>
-      <c r="F11">
-        <v>9.68</v>
-      </c>
-      <c r="G11">
-        <v>9.68</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A12" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B13" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="6">
-        <v>1</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13">
-        <v>1</v>
-      </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B14" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" s="6">
-        <v>1</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-      <c r="F14">
-        <v>1</v>
-      </c>
-      <c r="G14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B15" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" s="6">
-        <v>1</v>
-      </c>
-      <c r="D15">
-        <v>2.58</v>
-      </c>
-      <c r="E15">
-        <v>2.58</v>
-      </c>
-      <c r="F15">
-        <v>2.58</v>
-      </c>
-      <c r="G15">
-        <v>2.58</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B16" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" s="6">
-        <v>1</v>
-      </c>
-      <c r="D16">
-        <v>9.6300000000000008</v>
-      </c>
-      <c r="E16">
-        <v>9.6300000000000008</v>
-      </c>
-      <c r="F16">
-        <v>9.6300000000000008</v>
-      </c>
-      <c r="G16">
-        <v>9.6300000000000008</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A17" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-      <c r="F17">
-        <v>1</v>
-      </c>
-      <c r="G17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B18" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" s="6">
-        <v>1</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-      <c r="F18">
-        <v>1</v>
-      </c>
-      <c r="G18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B19" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C19" s="6">
-        <v>1</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19">
-        <v>1</v>
-      </c>
-      <c r="F19">
-        <v>1</v>
-      </c>
-      <c r="G19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B20" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C20" s="6">
-        <v>1</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
-      <c r="F20">
-        <v>1</v>
-      </c>
-      <c r="G20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B21" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C21" s="6">
-        <v>1</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-      <c r="E21">
-        <v>1</v>
-      </c>
-      <c r="F21">
-        <v>1</v>
-      </c>
-      <c r="G21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A22" t="s">
-        <v>43</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-      <c r="E22">
-        <v>1</v>
-      </c>
-      <c r="F22">
-        <v>1</v>
-      </c>
-      <c r="G22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B23" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" s="6">
-        <v>1</v>
-      </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-      <c r="E23">
-        <v>1</v>
-      </c>
-      <c r="F23">
-        <v>1</v>
-      </c>
-      <c r="G23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B24" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C24" s="6">
-        <v>1</v>
-      </c>
-      <c r="D24">
-        <v>1.65</v>
-      </c>
-      <c r="E24">
-        <v>1.65</v>
-      </c>
-      <c r="F24">
-        <v>1.65</v>
-      </c>
-      <c r="G24">
-        <v>1.65</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B25" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C25" s="6">
-        <v>1</v>
-      </c>
-      <c r="D25">
-        <v>2.73</v>
-      </c>
-      <c r="E25">
-        <v>2.73</v>
-      </c>
-      <c r="F25">
-        <v>2.73</v>
-      </c>
-      <c r="G25">
-        <v>2.73</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B26" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C26" s="6">
-        <v>1</v>
-      </c>
-      <c r="D26">
-        <v>11.21</v>
-      </c>
-      <c r="E26">
-        <v>11.21</v>
-      </c>
-      <c r="F26">
-        <v>11.21</v>
-      </c>
-      <c r="G26">
-        <v>11.21</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
changed anemia data and read in to be as a distribution rather than a prevalence
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Jan/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Jan/InputForCode_Bangladesh.xlsx
@@ -293,39 +293,6 @@
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Ruth</author>
-  </authors>
-  <commentList>
-    <comment ref="L2" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>Ruth:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-place holder values
-</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
     <author>Janka Petravic</author>
   </authors>
   <commentList>
@@ -355,7 +322,7 @@
 </comments>
 </file>
 
-<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Ruth</author>
@@ -387,7 +354,7 @@
 </comments>
 </file>
 
-<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Janka Petravic</author>
@@ -461,6 +428,82 @@
       </text>
     </comment>
     <comment ref="A18" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Active management of the third stage of labor</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Ruth</author>
+  </authors>
+  <commentList>
+    <comment ref="F1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Basic Emergency Obstetric Care Centre</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Comprehensive Emergency Obstetric Care Services</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A7" authorId="0">
       <text>
         <r>
           <rPr>
@@ -562,84 +605,8 @@
 </comments>
 </file>
 
-<file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Ruth</author>
-  </authors>
-  <commentList>
-    <comment ref="F1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>Ruth:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Basic Emergency Obstetric Care Centre</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>Ruth:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Comprehensive Emergency Obstetric Care Services</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A7" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>Ruth:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Active management of the third stage of labor</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="120">
   <si>
     <t>indicators</t>
   </si>
@@ -990,6 +957,15 @@
   </si>
   <si>
     <t>40-44 years</t>
+  </si>
+  <si>
+    <t>Anemia</t>
+  </si>
+  <si>
+    <t>anemic</t>
+  </si>
+  <si>
+    <t>not anemic</t>
   </si>
 </sst>
 </file>
@@ -1147,7 +1123,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="86">
+  <cellStyleXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1164,6 +1140,8 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1325,7 +1303,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="15" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="86">
+  <cellStyles count="88">
     <cellStyle name="Excel Built-in Normal" xfId="15"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -1369,6 +1347,7 @@
     <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1411,6 +1390,7 @@
     <cellStyle name="Hyperlink" xfId="80" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="82" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="84" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="86" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -8223,7 +8203,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -8622,98 +8602,162 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:L1"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="6" max="6" width="15.1640625" customWidth="1"/>
+    <col min="8" max="8" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
-      <c r="A1" s="45" t="s">
+    <row r="1" spans="1:14">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="D1" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="E1" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="45" t="s">
+      <c r="F1" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="45" t="s">
+      <c r="G1" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="45" t="s">
+      <c r="H1" s="45" t="s">
         <v>67</v>
       </c>
-      <c r="G1" s="45" t="s">
+      <c r="I1" s="45" t="s">
         <v>111</v>
       </c>
-      <c r="H1" s="45" t="s">
+      <c r="J1" s="45" t="s">
         <v>112</v>
       </c>
-      <c r="I1" s="45" t="s">
+      <c r="K1" s="45" t="s">
         <v>113</v>
       </c>
-      <c r="J1" s="45" t="s">
+      <c r="L1" s="45" t="s">
         <v>114</v>
       </c>
-      <c r="K1" s="45" t="s">
+      <c r="M1" s="45" t="s">
         <v>115</v>
       </c>
-      <c r="L1" s="45" t="s">
+      <c r="N1" s="45" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
-      <c r="A2">
-        <v>0.5</v>
-      </c>
-      <c r="B2">
-        <v>0.5</v>
+    <row r="2" spans="1:14">
+      <c r="A2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" t="s">
+        <v>118</v>
       </c>
       <c r="C2">
-        <v>0.5</v>
+        <v>50</v>
       </c>
       <c r="D2">
-        <v>0.5</v>
+        <v>50</v>
       </c>
       <c r="E2">
-        <v>0.5</v>
+        <v>50</v>
       </c>
       <c r="F2">
-        <v>0.5</v>
+        <v>50</v>
       </c>
       <c r="G2">
-        <v>0.5</v>
+        <v>50</v>
       </c>
       <c r="H2">
-        <v>0.5</v>
+        <v>50</v>
       </c>
       <c r="I2">
-        <v>0.5</v>
+        <v>50</v>
       </c>
       <c r="J2">
-        <v>0.5</v>
+        <v>50</v>
       </c>
       <c r="K2">
-        <v>0.5</v>
+        <v>50</v>
       </c>
       <c r="L2">
-        <v>0.5</v>
+        <v>50</v>
+      </c>
+      <c r="M2">
+        <v>50</v>
+      </c>
+      <c r="N2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="B3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C3">
+        <f>100-C2</f>
+        <v>50</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:N3" si="0">100-D2</f>
+        <v>50</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="F3">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="G3">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="H3">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="I3">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="J3">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="K3">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="L3">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="M3">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="N3">
+        <f t="shared" si="0"/>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
added projected reproductive age data (place holder for now) to spreadsheet and updated data.py to read it in
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Jan/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Jan/InputForCode_Bangladesh.xlsx
@@ -4,37 +4,38 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14600" tabRatio="500" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="-70980" yWindow="-3340" windowWidth="25600" windowHeight="14600" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="demographics" sheetId="1" r:id="rId1"/>
     <sheet name="projected births" sheetId="2" r:id="rId2"/>
-    <sheet name="mortality rates" sheetId="3" r:id="rId3"/>
-    <sheet name="causes of death" sheetId="4" r:id="rId4"/>
-    <sheet name="distributions" sheetId="5" r:id="rId5"/>
-    <sheet name="anemia prevalence" sheetId="28" r:id="rId6"/>
-    <sheet name="birth outcome distribution" sheetId="6" r:id="rId7"/>
-    <sheet name="Incidence of conditions" sheetId="7" r:id="rId8"/>
-    <sheet name="RR death by stunting" sheetId="8" r:id="rId9"/>
-    <sheet name="RR death by wasting" sheetId="9" r:id="rId10"/>
-    <sheet name="RR death by breastfeeding" sheetId="10" r:id="rId11"/>
-    <sheet name="RR death by birth outcome" sheetId="11" r:id="rId12"/>
-    <sheet name="OR stunting progression" sheetId="12" r:id="rId13"/>
-    <sheet name="RR diarrhoea" sheetId="13" r:id="rId14"/>
-    <sheet name="OR stunting by condition" sheetId="14" r:id="rId15"/>
-    <sheet name="OR stunting by birth outcome" sheetId="15" r:id="rId16"/>
-    <sheet name="OR stunting by intervention" sheetId="16" r:id="rId17"/>
-    <sheet name="OR stunting by compfeeding" sheetId="17" r:id="rId18"/>
-    <sheet name="OR correctBF by interventn" sheetId="18" r:id="rId19"/>
-    <sheet name="Appropriate breastfeeding" sheetId="19" r:id="rId20"/>
-    <sheet name="Interventions cost and coverage" sheetId="20" r:id="rId21"/>
-    <sheet name="Interventions target population" sheetId="21" r:id="rId22"/>
-    <sheet name="Interventions birth outcome" sheetId="22" r:id="rId23"/>
-    <sheet name="Interventions affected fraction" sheetId="23" r:id="rId24"/>
-    <sheet name="Interventions mortality eff" sheetId="24" r:id="rId25"/>
-    <sheet name="Interventions incidence eff" sheetId="25" r:id="rId26"/>
-    <sheet name="Interventions maternal aff frac" sheetId="26" r:id="rId27"/>
-    <sheet name="Interventions maternal eff" sheetId="27" r:id="rId28"/>
+    <sheet name="projected reproductive age" sheetId="29" r:id="rId3"/>
+    <sheet name="mortality rates" sheetId="3" r:id="rId4"/>
+    <sheet name="causes of death" sheetId="4" r:id="rId5"/>
+    <sheet name="distributions" sheetId="5" r:id="rId6"/>
+    <sheet name="anemia prevalence" sheetId="28" r:id="rId7"/>
+    <sheet name="birth outcome distribution" sheetId="6" r:id="rId8"/>
+    <sheet name="Incidence of conditions" sheetId="7" r:id="rId9"/>
+    <sheet name="RR death by stunting" sheetId="8" r:id="rId10"/>
+    <sheet name="RR death by wasting" sheetId="9" r:id="rId11"/>
+    <sheet name="RR death by breastfeeding" sheetId="10" r:id="rId12"/>
+    <sheet name="RR death by birth outcome" sheetId="11" r:id="rId13"/>
+    <sheet name="OR stunting progression" sheetId="12" r:id="rId14"/>
+    <sheet name="RR diarrhoea" sheetId="13" r:id="rId15"/>
+    <sheet name="OR stunting by condition" sheetId="14" r:id="rId16"/>
+    <sheet name="OR stunting by birth outcome" sheetId="15" r:id="rId17"/>
+    <sheet name="OR stunting by intervention" sheetId="16" r:id="rId18"/>
+    <sheet name="OR stunting by compfeeding" sheetId="17" r:id="rId19"/>
+    <sheet name="OR correctBF by interventn" sheetId="18" r:id="rId20"/>
+    <sheet name="Appropriate breastfeeding" sheetId="19" r:id="rId21"/>
+    <sheet name="Interventions cost and coverage" sheetId="20" r:id="rId22"/>
+    <sheet name="Interventions target population" sheetId="21" r:id="rId23"/>
+    <sheet name="Interventions birth outcome" sheetId="22" r:id="rId24"/>
+    <sheet name="Interventions affected fraction" sheetId="23" r:id="rId25"/>
+    <sheet name="Interventions mortality eff" sheetId="24" r:id="rId26"/>
+    <sheet name="Interventions incidence eff" sheetId="25" r:id="rId27"/>
+    <sheet name="Interventions maternal aff frac" sheetId="26" r:id="rId28"/>
+    <sheet name="Interventions maternal eff" sheetId="27" r:id="rId29"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -151,6 +152,38 @@
     <author>Ruth</author>
   </authors>
   <commentList>
+    <comment ref="B2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+placeholder</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Ruth</author>
+  </authors>
+  <commentList>
     <comment ref="A2" authorId="0">
       <text>
         <r>
@@ -200,7 +233,7 @@
 </comments>
 </file>
 
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Ruth</author>
@@ -290,7 +323,7 @@
 </comments>
 </file>
 
-<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Janka Petravic</author>
@@ -322,7 +355,7 @@
 </comments>
 </file>
 
-<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Ruth</author>
@@ -354,7 +387,7 @@
 </comments>
 </file>
 
-<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Janka Petravic</author>
@@ -428,82 +461,6 @@
       </text>
     </comment>
     <comment ref="A18" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>Ruth:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Active management of the third stage of labor</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Ruth</author>
-  </authors>
-  <commentList>
-    <comment ref="F1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>Ruth:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Basic Emergency Obstetric Care Centre</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>Ruth:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Comprehensive Emergency Obstetric Care Services</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A7" authorId="0">
       <text>
         <r>
           <rPr>
@@ -605,8 +562,84 @@
 </comments>
 </file>
 
+<file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Ruth</author>
+  </authors>
+  <commentList>
+    <comment ref="F1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Basic Emergency Obstetric Care Centre</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Comprehensive Emergency Obstetric Care Services</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A7" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Active management of the third stage of labor</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="121">
   <si>
     <t>indicators</t>
   </si>
@@ -966,6 +999,9 @@
   </si>
   <si>
     <t>not anemic</t>
+  </si>
+  <si>
+    <t>women turning 15 years old</t>
   </si>
 </sst>
 </file>
@@ -1123,7 +1159,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="88">
+  <cellStyleXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1140,6 +1176,8 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1303,7 +1341,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="15" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="88">
+  <cellStyles count="90">
     <cellStyle name="Excel Built-in Normal" xfId="15"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -1348,6 +1386,7 @@
     <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1391,6 +1430,7 @@
     <cellStyle name="Hyperlink" xfId="82" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="84" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="86" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="88" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2844,6 +2884,462 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="6">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
+      <c r="B3" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="6">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1.67</v>
+      </c>
+      <c r="E3">
+        <v>1.67</v>
+      </c>
+      <c r="F3">
+        <v>1.67</v>
+      </c>
+      <c r="G3">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
+      <c r="B4" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="6">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>2.38</v>
+      </c>
+      <c r="E4">
+        <v>2.38</v>
+      </c>
+      <c r="F4">
+        <v>2.38</v>
+      </c>
+      <c r="G4">
+        <v>2.38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
+      <c r="B5" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="6">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>6.33</v>
+      </c>
+      <c r="E5">
+        <v>6.33</v>
+      </c>
+      <c r="F5">
+        <v>6.33</v>
+      </c>
+      <c r="G5">
+        <v>6.33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
+      <c r="B7" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="6">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1.55</v>
+      </c>
+      <c r="E7">
+        <v>1.55</v>
+      </c>
+      <c r="F7">
+        <v>1.55</v>
+      </c>
+      <c r="G7">
+        <v>1.55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
+      <c r="B8" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="6">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="E8">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="F8">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="G8">
+        <v>2.1800000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
+      <c r="B9" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="6">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>6.39</v>
+      </c>
+      <c r="E9">
+        <v>6.39</v>
+      </c>
+      <c r="F9">
+        <v>6.39</v>
+      </c>
+      <c r="G9">
+        <v>6.39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="6">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" customHeight="1">
+      <c r="B11" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="6">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" customHeight="1">
+      <c r="B12" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="6">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>2.79</v>
+      </c>
+      <c r="E12">
+        <v>2.79</v>
+      </c>
+      <c r="F12">
+        <v>2.79</v>
+      </c>
+      <c r="G12">
+        <v>2.79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" customHeight="1">
+      <c r="B13" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="6">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>6.01</v>
+      </c>
+      <c r="E13">
+        <v>6.01</v>
+      </c>
+      <c r="F13">
+        <v>6.01</v>
+      </c>
+      <c r="G13">
+        <v>6.01</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="6">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" customHeight="1">
+      <c r="B15" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="6">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" customHeight="1">
+      <c r="B16" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="6">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" customHeight="1">
+      <c r="B17" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="6">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="6">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" customHeight="1">
+      <c r="B19" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="6">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15.75" customHeight="1">
+      <c r="B20" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="6">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>1.86</v>
+      </c>
+      <c r="E20">
+        <v>1.86</v>
+      </c>
+      <c r="F20">
+        <v>1.86</v>
+      </c>
+      <c r="G20">
+        <v>1.86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" customHeight="1">
+      <c r="B21" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="6">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>3.01</v>
+      </c>
+      <c r="E21">
+        <v>3.01</v>
+      </c>
+      <c r="F21">
+        <v>3.01</v>
+      </c>
+      <c r="G21">
+        <v>3.01</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3401,7 +3897,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G29"/>
   <sheetViews>
@@ -4028,7 +4524,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G29"/>
   <sheetViews>
@@ -4326,7 +4822,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -4374,7 +4870,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
@@ -4495,7 +4991,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -4555,7 +5051,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -4603,7 +5099,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
@@ -4691,7 +5187,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
@@ -4814,7 +5310,149 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="12.5" customWidth="1"/>
+    <col min="2" max="2" width="16.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A2" s="4">
+        <v>2017</v>
+      </c>
+      <c r="B2" s="5">
+        <v>3095470</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A3" s="4">
+        <v>2018</v>
+      </c>
+      <c r="B3" s="5">
+        <v>3071259</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A4" s="4">
+        <v>2019</v>
+      </c>
+      <c r="B4" s="5">
+        <v>3045241</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A5" s="4">
+        <v>2020</v>
+      </c>
+      <c r="B5" s="5">
+        <v>3017266</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A6" s="4">
+        <v>2021</v>
+      </c>
+      <c r="B6" s="5">
+        <v>2990677</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A7" s="4">
+        <v>2022</v>
+      </c>
+      <c r="B7" s="5">
+        <v>2962144</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A8" s="4">
+        <v>2023</v>
+      </c>
+      <c r="B8" s="5">
+        <v>2931643</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A9" s="4">
+        <v>2024</v>
+      </c>
+      <c r="B9" s="5">
+        <v>2899255</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A10" s="4">
+        <v>2025</v>
+      </c>
+      <c r="B10" s="5">
+        <v>2865008</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A11" s="4">
+        <v>2026</v>
+      </c>
+      <c r="B11" s="5">
+        <v>2836142</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A12" s="4">
+        <v>2027</v>
+      </c>
+      <c r="B12" s="5">
+        <v>2805541</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A13" s="4">
+        <v>2028</v>
+      </c>
+      <c r="B13" s="5">
+        <v>2773236</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A14" s="4">
+        <v>2029</v>
+      </c>
+      <c r="B14" s="5">
+        <v>2739273</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A15" s="4">
+        <v>2030</v>
+      </c>
+      <c r="B15" s="5">
+        <v>2703670</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
@@ -4906,139 +5544,66 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="12.5" customWidth="1"/>
-    <col min="2" max="2" width="16.5" customWidth="1"/>
+    <col min="1" max="5" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A2" s="4">
-        <v>2017</v>
-      </c>
-      <c r="B2" s="5">
-        <v>3095470</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A3" s="4">
-        <v>2018</v>
-      </c>
-      <c r="B3" s="5">
-        <v>3071259</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A4" s="4">
-        <v>2019</v>
-      </c>
-      <c r="B4" s="5">
-        <v>3045241</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A5" s="4">
-        <v>2020</v>
-      </c>
-      <c r="B5" s="5">
-        <v>3017266</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A6" s="4">
-        <v>2021</v>
-      </c>
-      <c r="B6" s="5">
-        <v>2990677</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A7" s="4">
-        <v>2022</v>
-      </c>
-      <c r="B7" s="5">
-        <v>2962144</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A8" s="4">
-        <v>2023</v>
-      </c>
-      <c r="B8" s="5">
-        <v>2931643</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A9" s="4">
-        <v>2024</v>
-      </c>
-      <c r="B9" s="5">
-        <v>2899255</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A10" s="4">
-        <v>2025</v>
-      </c>
-      <c r="B10" s="5">
-        <v>2865008</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A11" s="4">
-        <v>2026</v>
-      </c>
-      <c r="B11" s="5">
-        <v>2836142</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A12" s="4">
-        <v>2027</v>
-      </c>
-      <c r="B12" s="5">
-        <v>2805541</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A13" s="4">
-        <v>2028</v>
-      </c>
-      <c r="B13" s="5">
-        <v>2773236</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A14" s="4">
-        <v>2029</v>
-      </c>
-      <c r="B14" s="5">
-        <v>2739273</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A15" s="4">
-        <v>2030</v>
-      </c>
-      <c r="B15" s="5">
-        <v>2703670</v>
-      </c>
+    <row r="1" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="14">
+      <c r="A2" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5050,81 +5615,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="5" width="13.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="14">
-      <c r="A2" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -5493,7 +5989,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J25"/>
   <sheetViews>
@@ -6027,7 +6523,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
@@ -6146,12 +6642,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -6480,7 +6976,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
@@ -6814,12 +7310,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD3"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -6924,7 +7420,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H35"/>
   <sheetViews>
@@ -7251,7 +7747,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
@@ -7501,6 +7997,152 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="12.5" customWidth="1"/>
+    <col min="2" max="2" width="32.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A2" s="4">
+        <v>2017</v>
+      </c>
+      <c r="B2" s="5">
+        <v>5000000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A3" s="4">
+        <v>2018</v>
+      </c>
+      <c r="B3" s="5">
+        <v>5000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A4" s="4">
+        <v>2019</v>
+      </c>
+      <c r="B4" s="5">
+        <v>5000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A5" s="4">
+        <v>2020</v>
+      </c>
+      <c r="B5" s="5">
+        <v>5000000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A6" s="4">
+        <v>2021</v>
+      </c>
+      <c r="B6" s="5">
+        <v>5000000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A7" s="4">
+        <v>2022</v>
+      </c>
+      <c r="B7" s="5">
+        <v>5000000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A8" s="4">
+        <v>2023</v>
+      </c>
+      <c r="B8" s="5">
+        <v>5000000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A9" s="4">
+        <v>2024</v>
+      </c>
+      <c r="B9" s="5">
+        <v>5000000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A10" s="4">
+        <v>2025</v>
+      </c>
+      <c r="B10" s="5">
+        <v>5000000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A11" s="4">
+        <v>2026</v>
+      </c>
+      <c r="B11" s="5">
+        <v>5000000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A12" s="4">
+        <v>2027</v>
+      </c>
+      <c r="B12" s="5">
+        <v>5000000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A13" s="4">
+        <v>2028</v>
+      </c>
+      <c r="B13" s="5">
+        <v>5000000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A14" s="4">
+        <v>2029</v>
+      </c>
+      <c r="B14" s="5">
+        <v>5000000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A15" s="4">
+        <v>2030</v>
+      </c>
+      <c r="B15" s="5">
+        <v>5000000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7549,7 +8191,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G27"/>
   <sheetViews>
@@ -8198,7 +8840,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H19"/>
   <sheetViews>
@@ -8601,12 +9243,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -8766,7 +9408,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -8808,7 +9450,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -8887,460 +9529,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
-  <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A1" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="6">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B3" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="6">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>1.67</v>
-      </c>
-      <c r="E3">
-        <v>1.67</v>
-      </c>
-      <c r="F3">
-        <v>1.67</v>
-      </c>
-      <c r="G3">
-        <v>1.67</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B4" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="6">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>2.38</v>
-      </c>
-      <c r="E4">
-        <v>2.38</v>
-      </c>
-      <c r="F4">
-        <v>2.38</v>
-      </c>
-      <c r="G4">
-        <v>2.38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B5" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" s="6">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>6.33</v>
-      </c>
-      <c r="E5">
-        <v>6.33</v>
-      </c>
-      <c r="F5">
-        <v>6.33</v>
-      </c>
-      <c r="G5">
-        <v>6.33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="6">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B7" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="6">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>1.55</v>
-      </c>
-      <c r="E7">
-        <v>1.55</v>
-      </c>
-      <c r="F7">
-        <v>1.55</v>
-      </c>
-      <c r="G7">
-        <v>1.55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B8" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="6">
-        <v>1</v>
-      </c>
-      <c r="D8">
-        <v>2.1800000000000002</v>
-      </c>
-      <c r="E8">
-        <v>2.1800000000000002</v>
-      </c>
-      <c r="F8">
-        <v>2.1800000000000002</v>
-      </c>
-      <c r="G8">
-        <v>2.1800000000000002</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B9" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="6">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <v>6.39</v>
-      </c>
-      <c r="E9">
-        <v>6.39</v>
-      </c>
-      <c r="F9">
-        <v>6.39</v>
-      </c>
-      <c r="G9">
-        <v>6.39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="6">
-        <v>1</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B11" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="6">
-        <v>1</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B12" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" s="6">
-        <v>1</v>
-      </c>
-      <c r="D12">
-        <v>2.79</v>
-      </c>
-      <c r="E12">
-        <v>2.79</v>
-      </c>
-      <c r="F12">
-        <v>2.79</v>
-      </c>
-      <c r="G12">
-        <v>2.79</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B13" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="6">
-        <v>1</v>
-      </c>
-      <c r="D13">
-        <v>6.01</v>
-      </c>
-      <c r="E13">
-        <v>6.01</v>
-      </c>
-      <c r="F13">
-        <v>6.01</v>
-      </c>
-      <c r="G13">
-        <v>6.01</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A14" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="6">
-        <v>1</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-      <c r="F14">
-        <v>1</v>
-      </c>
-      <c r="G14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B15" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="6">
-        <v>1</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
-      <c r="F15">
-        <v>1</v>
-      </c>
-      <c r="G15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B16" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C16" s="6">
-        <v>1</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-      <c r="F16">
-        <v>1</v>
-      </c>
-      <c r="G16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B17" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" s="6">
-        <v>1</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-      <c r="F17">
-        <v>1</v>
-      </c>
-      <c r="G17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A18" t="s">
-        <v>43</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" s="6">
-        <v>1</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-      <c r="F18">
-        <v>1</v>
-      </c>
-      <c r="G18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B19" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C19" s="6">
-        <v>1</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19">
-        <v>1</v>
-      </c>
-      <c r="F19">
-        <v>1</v>
-      </c>
-      <c r="G19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B20" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C20" s="6">
-        <v>1</v>
-      </c>
-      <c r="D20">
-        <v>1.86</v>
-      </c>
-      <c r="E20">
-        <v>1.86</v>
-      </c>
-      <c r="F20">
-        <v>1.86</v>
-      </c>
-      <c r="G20">
-        <v>1.86</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B21" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C21" s="6">
-        <v>1</v>
-      </c>
-      <c r="D21">
-        <v>3.01</v>
-      </c>
-      <c r="E21">
-        <v>3.01</v>
-      </c>
-      <c r="F21">
-        <v>3.01</v>
-      </c>
-      <c r="G21">
-        <v>3.01</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
changed reproductive age data projection to be pop size 15-19 years
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Jan/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Jan/InputForCode_Bangladesh.xlsx
@@ -1001,7 +1001,7 @@
     <t>not anemic</t>
   </si>
   <si>
-    <t>women turning 15 years old</t>
+    <t>population 15-19 years old</t>
   </si>
 </sst>
 </file>
@@ -5314,7 +5314,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
@@ -8000,7 +8002,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B15"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -8030,7 +8032,8 @@
         <v>2018</v>
       </c>
       <c r="B3" s="5">
-        <v>5000000</v>
+        <f>B2+(B2/100)</f>
+        <v>5050000</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" customHeight="1">
@@ -8038,7 +8041,8 @@
         <v>2019</v>
       </c>
       <c r="B4" s="5">
-        <v>5000000</v>
+        <f t="shared" ref="B4:B15" si="0">B3+(B3/100)</f>
+        <v>5100500</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" customHeight="1">
@@ -8046,7 +8050,8 @@
         <v>2020</v>
       </c>
       <c r="B5" s="5">
-        <v>5000000</v>
+        <f t="shared" si="0"/>
+        <v>5151505</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.75" customHeight="1">
@@ -8054,7 +8059,8 @@
         <v>2021</v>
       </c>
       <c r="B6" s="5">
-        <v>5000000</v>
+        <f t="shared" si="0"/>
+        <v>5203020.05</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.75" customHeight="1">
@@ -8062,7 +8068,8 @@
         <v>2022</v>
       </c>
       <c r="B7" s="5">
-        <v>5000000</v>
+        <f t="shared" si="0"/>
+        <v>5255050.2505000001</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" customHeight="1">
@@ -8070,7 +8077,8 @@
         <v>2023</v>
       </c>
       <c r="B8" s="5">
-        <v>5000000</v>
+        <f t="shared" si="0"/>
+        <v>5307600.7530049998</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15.75" customHeight="1">
@@ -8078,7 +8086,8 @@
         <v>2024</v>
       </c>
       <c r="B9" s="5">
-        <v>5000000</v>
+        <f t="shared" si="0"/>
+        <v>5360676.7605350502</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15.75" customHeight="1">
@@ -8086,7 +8095,8 @@
         <v>2025</v>
       </c>
       <c r="B10" s="5">
-        <v>5000000</v>
+        <f t="shared" si="0"/>
+        <v>5414283.5281404005</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.75" customHeight="1">
@@ -8094,7 +8104,8 @@
         <v>2026</v>
       </c>
       <c r="B11" s="5">
-        <v>5000000</v>
+        <f t="shared" si="0"/>
+        <v>5468426.3634218043</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15.75" customHeight="1">
@@ -8102,7 +8113,8 @@
         <v>2027</v>
       </c>
       <c r="B12" s="5">
-        <v>5000000</v>
+        <f t="shared" si="0"/>
+        <v>5523110.6270560222</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15.75" customHeight="1">
@@ -8110,7 +8122,8 @@
         <v>2028</v>
       </c>
       <c r="B13" s="5">
-        <v>5000000</v>
+        <f t="shared" si="0"/>
+        <v>5578341.7333265822</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15.75" customHeight="1">
@@ -8118,7 +8131,8 @@
         <v>2029</v>
       </c>
       <c r="B14" s="5">
-        <v>5000000</v>
+        <f t="shared" si="0"/>
+        <v>5634125.150659848</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15.75" customHeight="1">
@@ -8126,7 +8140,8 @@
         <v>2030</v>
       </c>
       <c r="B15" s="5">
-        <v>5000000</v>
+        <f t="shared" si="0"/>
+        <v>5690466.4021664467</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added all population groups to RR death by anaemia
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Jan/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Jan/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-4180" yWindow="-19700" windowWidth="25600" windowHeight="14600" tabRatio="500" firstSheet="3" activeTab="4"/>
+    <workbookView xWindow="-4180" yWindow="-19720" windowWidth="25600" windowHeight="14600" tabRatio="500" firstSheet="3" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="demographics" sheetId="1" r:id="rId1"/>
@@ -732,7 +732,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="130">
   <si>
     <t>indicators</t>
   </si>
@@ -3007,9 +3007,9 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
@@ -3018,7 +3018,7 @@
     <col min="2" max="2" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -3026,25 +3026,43 @@
         <v>121</v>
       </c>
       <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I1" t="s">
         <v>111</v>
       </c>
-      <c r="D1" t="s">
+      <c r="J1" t="s">
         <v>112</v>
       </c>
-      <c r="E1" t="s">
+      <c r="K1" t="s">
         <v>113</v>
       </c>
-      <c r="F1" t="s">
+      <c r="L1" t="s">
         <v>114</v>
       </c>
-      <c r="G1" t="s">
+      <c r="M1" t="s">
         <v>115</v>
       </c>
-      <c r="H1" t="s">
+      <c r="N1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>122</v>
       </c>
@@ -3069,8 +3087,26 @@
       <c r="H2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.15">
       <c r="B3" t="s">
         <v>126</v>
       </c>
@@ -3092,8 +3128,26 @@
       <c r="H3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>123</v>
       </c>
@@ -3118,8 +3172,26 @@
       <c r="H4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.15">
       <c r="B5" t="s">
         <v>126</v>
       </c>
@@ -3141,8 +3213,26 @@
       <c r="H5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>124</v>
       </c>
@@ -3167,8 +3257,26 @@
       <c r="H6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.15">
       <c r="B7" t="s">
         <v>126</v>
       </c>
@@ -3188,6 +3296,24 @@
         <v>1</v>
       </c>
       <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7">
         <v>1</v>
       </c>
     </row>
@@ -8446,7 +8572,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
@@ -10099,7 +10225,7 @@
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Added WRA groups to spreadsheets with placeholder values so allPops will function
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Jan/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Jan/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14400" tabRatio="500" firstSheet="3" activeTab="9"/>
+    <workbookView xWindow="-43980" yWindow="-19580" windowWidth="32620" windowHeight="18080" tabRatio="500" firstSheet="19" activeTab="26"/>
   </bookViews>
   <sheets>
     <sheet name="demographics" sheetId="1" r:id="rId1"/>
@@ -155,6 +155,70 @@
 <file path=xl/comments10.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
+    <author>Sam</author>
+  </authors>
+  <commentList>
+    <comment ref="I2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Sam:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+WRA all fictional</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments11.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Sam</author>
+  </authors>
+  <commentList>
+    <comment ref="I2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Sam:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+WRA all fictional</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments12.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
     <author>Ruth</author>
   </authors>
   <commentList>
@@ -228,7 +292,7 @@
 </comments>
 </file>
 
-<file path=xl/comments11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments13.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Ruth</author>
@@ -635,11 +699,34 @@
 <file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
+    <author>Sam</author>
     <author>Janka Petravic</author>
     <author>Ruth</author>
   </authors>
   <commentList>
-    <comment ref="D4" authorId="0">
+    <comment ref="H2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Sam:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+WRA values fictional</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D4" authorId="1">
       <text>
         <r>
           <rPr>
@@ -661,7 +748,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E4" authorId="0">
+    <comment ref="E4" authorId="1">
       <text>
         <r>
           <rPr>
@@ -683,7 +770,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G6" authorId="0">
+    <comment ref="G6" authorId="1">
       <text>
         <r>
           <rPr>
@@ -705,7 +792,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A18" authorId="1">
+    <comment ref="A18" authorId="2">
       <text>
         <r>
           <rPr>
@@ -732,7 +819,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="130">
   <si>
     <t>indicators</t>
   </si>
@@ -1279,7 +1366,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="94">
+  <cellStyleXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1296,6 +1383,8 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1465,7 +1554,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="15" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="94">
+  <cellStyles count="96">
     <cellStyle name="Excel Built-in Normal" xfId="15"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -1513,6 +1602,7 @@
     <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1559,6 +1649,7 @@
     <cellStyle name="Hyperlink" xfId="88" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="90" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="92" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="94" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3009,8 +3100,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6366,10 +6457,10 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6377,12 +6468,12 @@
     <col min="1" max="1" width="48" customWidth="1"/>
     <col min="2" max="6" width="13.5" customWidth="1"/>
     <col min="7" max="7" width="17.33203125" customWidth="1"/>
-    <col min="8" max="8" width="9.33203125" customWidth="1"/>
-    <col min="9" max="9" width="19.5" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" customWidth="1"/>
+    <col min="9" max="9" width="13.5" customWidth="1"/>
     <col min="10" max="10" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="6" t="s">
         <v>56</v>
       </c>
@@ -6404,10 +6495,26 @@
       <c r="G1" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-    </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I1" t="s">
+        <v>112</v>
+      </c>
+      <c r="J1" t="s">
+        <v>113</v>
+      </c>
+      <c r="K1" t="s">
+        <v>114</v>
+      </c>
+      <c r="L1" t="s">
+        <v>115</v>
+      </c>
+      <c r="M1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
         <v>64</v>
       </c>
@@ -6429,8 +6536,26 @@
       <c r="G2" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H2" s="4">
+        <v>0</v>
+      </c>
+      <c r="I2" s="4">
+        <v>0</v>
+      </c>
+      <c r="J2" s="4">
+        <v>0</v>
+      </c>
+      <c r="K2" s="4">
+        <v>0</v>
+      </c>
+      <c r="L2" s="4">
+        <v>0</v>
+      </c>
+      <c r="M2" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
         <v>75</v>
       </c>
@@ -6452,8 +6577,26 @@
       <c r="G3" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H3" s="4">
+        <v>0</v>
+      </c>
+      <c r="I3" s="4">
+        <v>0</v>
+      </c>
+      <c r="J3" s="4">
+        <v>0</v>
+      </c>
+      <c r="K3" s="4">
+        <v>0</v>
+      </c>
+      <c r="L3" s="4">
+        <v>0</v>
+      </c>
+      <c r="M3" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
         <v>76</v>
       </c>
@@ -6477,8 +6620,26 @@
       <c r="G4" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H4" s="4">
+        <v>0</v>
+      </c>
+      <c r="I4" s="4">
+        <v>0</v>
+      </c>
+      <c r="J4" s="4">
+        <v>0</v>
+      </c>
+      <c r="K4" s="4">
+        <v>0</v>
+      </c>
+      <c r="L4" s="4">
+        <v>0</v>
+      </c>
+      <c r="M4" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
         <v>74</v>
       </c>
@@ -6500,8 +6661,26 @@
       <c r="G5" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H5" s="4">
+        <v>0</v>
+      </c>
+      <c r="I5" s="4">
+        <v>0</v>
+      </c>
+      <c r="J5" s="4">
+        <v>0</v>
+      </c>
+      <c r="K5" s="4">
+        <v>0</v>
+      </c>
+      <c r="L5" s="4">
+        <v>0</v>
+      </c>
+      <c r="M5" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>77</v>
       </c>
@@ -6524,8 +6703,26 @@
         <f>demographics!$B$7</f>
         <v>0.4</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H6" s="4">
+        <v>0</v>
+      </c>
+      <c r="I6" s="4">
+        <v>0</v>
+      </c>
+      <c r="J6" s="4">
+        <v>0</v>
+      </c>
+      <c r="K6" s="4">
+        <v>0</v>
+      </c>
+      <c r="L6" s="4">
+        <v>0</v>
+      </c>
+      <c r="M6" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>79</v>
       </c>
@@ -6547,8 +6744,26 @@
       <c r="G7" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H7" s="4">
+        <v>0</v>
+      </c>
+      <c r="I7" s="4">
+        <v>0</v>
+      </c>
+      <c r="J7" s="4">
+        <v>0</v>
+      </c>
+      <c r="K7" s="4">
+        <v>0</v>
+      </c>
+      <c r="L7" s="4">
+        <v>0</v>
+      </c>
+      <c r="M7" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="32" t="s">
         <v>95</v>
       </c>
@@ -6570,8 +6785,26 @@
       <c r="G8" s="33">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H8" s="4">
+        <v>0</v>
+      </c>
+      <c r="I8" s="4">
+        <v>0</v>
+      </c>
+      <c r="J8" s="4">
+        <v>0</v>
+      </c>
+      <c r="K8" s="4">
+        <v>0</v>
+      </c>
+      <c r="L8" s="4">
+        <v>0</v>
+      </c>
+      <c r="M8" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="32" t="s">
         <v>96</v>
       </c>
@@ -6593,8 +6826,26 @@
       <c r="G9" s="33">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H9" s="4">
+        <v>0</v>
+      </c>
+      <c r="I9" s="4">
+        <v>0</v>
+      </c>
+      <c r="J9" s="4">
+        <v>0</v>
+      </c>
+      <c r="K9" s="4">
+        <v>0</v>
+      </c>
+      <c r="L9" s="4">
+        <v>0</v>
+      </c>
+      <c r="M9" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="32" t="s">
         <v>97</v>
       </c>
@@ -6616,8 +6867,26 @@
       <c r="G10" s="33">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H10" s="4">
+        <v>0</v>
+      </c>
+      <c r="I10" s="4">
+        <v>0</v>
+      </c>
+      <c r="J10" s="4">
+        <v>0</v>
+      </c>
+      <c r="K10" s="4">
+        <v>0</v>
+      </c>
+      <c r="L10" s="4">
+        <v>0</v>
+      </c>
+      <c r="M10" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="32" t="s">
         <v>98</v>
       </c>
@@ -6639,8 +6908,26 @@
       <c r="G11" s="33">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H11" s="4">
+        <v>0</v>
+      </c>
+      <c r="I11" s="4">
+        <v>0</v>
+      </c>
+      <c r="J11" s="4">
+        <v>0</v>
+      </c>
+      <c r="K11" s="4">
+        <v>0</v>
+      </c>
+      <c r="L11" s="4">
+        <v>0</v>
+      </c>
+      <c r="M11" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="32" t="s">
         <v>99</v>
       </c>
@@ -6662,8 +6949,26 @@
       <c r="G12" s="33">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H12" s="4">
+        <v>0</v>
+      </c>
+      <c r="I12" s="4">
+        <v>0</v>
+      </c>
+      <c r="J12" s="4">
+        <v>0</v>
+      </c>
+      <c r="K12" s="4">
+        <v>0</v>
+      </c>
+      <c r="L12" s="4">
+        <v>0</v>
+      </c>
+      <c r="M12" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="32" t="s">
         <v>100</v>
       </c>
@@ -6685,8 +6990,26 @@
       <c r="G13" s="33">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H13" s="4">
+        <v>0</v>
+      </c>
+      <c r="I13" s="4">
+        <v>0</v>
+      </c>
+      <c r="J13" s="4">
+        <v>0</v>
+      </c>
+      <c r="K13" s="4">
+        <v>0</v>
+      </c>
+      <c r="L13" s="4">
+        <v>0</v>
+      </c>
+      <c r="M13" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="32" t="s">
         <v>101</v>
       </c>
@@ -6708,8 +7031,26 @@
       <c r="G14" s="32">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H14" s="4">
+        <v>0</v>
+      </c>
+      <c r="I14" s="4">
+        <v>0</v>
+      </c>
+      <c r="J14" s="4">
+        <v>0</v>
+      </c>
+      <c r="K14" s="4">
+        <v>0</v>
+      </c>
+      <c r="L14" s="4">
+        <v>0</v>
+      </c>
+      <c r="M14" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="32" t="s">
         <v>102</v>
       </c>
@@ -6731,8 +7072,26 @@
       <c r="G15" s="32">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H15" s="4">
+        <v>0</v>
+      </c>
+      <c r="I15" s="4">
+        <v>0</v>
+      </c>
+      <c r="J15" s="4">
+        <v>0</v>
+      </c>
+      <c r="K15" s="4">
+        <v>0</v>
+      </c>
+      <c r="L15" s="4">
+        <v>0</v>
+      </c>
+      <c r="M15" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="32" t="s">
         <v>103</v>
       </c>
@@ -6754,8 +7113,26 @@
       <c r="G16" s="32">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H16" s="4">
+        <v>0</v>
+      </c>
+      <c r="I16" s="4">
+        <v>0</v>
+      </c>
+      <c r="J16" s="4">
+        <v>0</v>
+      </c>
+      <c r="K16" s="4">
+        <v>0</v>
+      </c>
+      <c r="L16" s="4">
+        <v>0</v>
+      </c>
+      <c r="M16" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="23" t="s">
         <v>105</v>
       </c>
@@ -6777,8 +7154,26 @@
       <c r="G17" s="33">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H17" s="4">
+        <v>0</v>
+      </c>
+      <c r="I17" s="4">
+        <v>0</v>
+      </c>
+      <c r="J17" s="4">
+        <v>0</v>
+      </c>
+      <c r="K17" s="4">
+        <v>0</v>
+      </c>
+      <c r="L17" s="4">
+        <v>0</v>
+      </c>
+      <c r="M17" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="23" t="s">
         <v>109</v>
       </c>
@@ -6800,8 +7195,26 @@
       <c r="G18" s="32">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H18" s="4">
+        <v>0</v>
+      </c>
+      <c r="I18" s="4">
+        <v>0</v>
+      </c>
+      <c r="J18" s="4">
+        <v>0</v>
+      </c>
+      <c r="K18" s="4">
+        <v>0</v>
+      </c>
+      <c r="L18" s="4">
+        <v>0</v>
+      </c>
+      <c r="M18" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="23" t="s">
         <v>106</v>
       </c>
@@ -6823,8 +7236,26 @@
       <c r="G19" s="32">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H19" s="4">
+        <v>0</v>
+      </c>
+      <c r="I19" s="4">
+        <v>0</v>
+      </c>
+      <c r="J19" s="4">
+        <v>0</v>
+      </c>
+      <c r="K19" s="4">
+        <v>0</v>
+      </c>
+      <c r="L19" s="4">
+        <v>0</v>
+      </c>
+      <c r="M19" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="23" t="s">
         <v>107</v>
       </c>
@@ -6846,8 +7277,26 @@
       <c r="G20" s="32">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H20" s="4">
+        <v>0</v>
+      </c>
+      <c r="I20" s="4">
+        <v>0</v>
+      </c>
+      <c r="J20" s="4">
+        <v>0</v>
+      </c>
+      <c r="K20" s="4">
+        <v>0</v>
+      </c>
+      <c r="L20" s="4">
+        <v>0</v>
+      </c>
+      <c r="M20" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="14" t="s">
         <v>108</v>
       </c>
@@ -6869,20 +7318,38 @@
       <c r="G21" s="39">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H21" s="4">
+        <v>0</v>
+      </c>
+      <c r="I21" s="4">
+        <v>0</v>
+      </c>
+      <c r="J21" s="4">
+        <v>0</v>
+      </c>
+      <c r="K21" s="4">
+        <v>0</v>
+      </c>
+      <c r="L21" s="4">
+        <v>0</v>
+      </c>
+      <c r="M21" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
     </row>
-    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
     </row>
-    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
     </row>
-    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
     </row>
@@ -7008,11 +7475,11 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7021,7 +7488,7 @@
     <col min="2" max="2" width="28.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="6" t="s">
         <v>68</v>
       </c>
@@ -7046,8 +7513,26 @@
       <c r="H1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I1" t="s">
+        <v>111</v>
+      </c>
+      <c r="J1" t="s">
+        <v>112</v>
+      </c>
+      <c r="K1" t="s">
+        <v>113</v>
+      </c>
+      <c r="L1" t="s">
+        <v>114</v>
+      </c>
+      <c r="M1" t="s">
+        <v>115</v>
+      </c>
+      <c r="N1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
         <v>64</v>
       </c>
@@ -7072,8 +7557,26 @@
       <c r="H2" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I2" s="6">
+        <v>0</v>
+      </c>
+      <c r="J2" s="6">
+        <v>0</v>
+      </c>
+      <c r="K2" s="6">
+        <v>0</v>
+      </c>
+      <c r="L2" s="6">
+        <v>0</v>
+      </c>
+      <c r="M2" s="6">
+        <v>0</v>
+      </c>
+      <c r="N2" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="35" t="s">
         <v>36</v>
       </c>
@@ -7095,8 +7598,26 @@
       <c r="H3" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I3" s="6">
+        <v>0</v>
+      </c>
+      <c r="J3" s="6">
+        <v>0</v>
+      </c>
+      <c r="K3" s="6">
+        <v>0</v>
+      </c>
+      <c r="L3" s="6">
+        <v>0</v>
+      </c>
+      <c r="M3" s="6">
+        <v>0</v>
+      </c>
+      <c r="N3" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="32" t="s">
         <v>95</v>
       </c>
@@ -7121,8 +7642,26 @@
       <c r="H4" s="32">
         <v>4.895E-3</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I4" s="6">
+        <v>0</v>
+      </c>
+      <c r="J4" s="6">
+        <v>0</v>
+      </c>
+      <c r="K4" s="6">
+        <v>0</v>
+      </c>
+      <c r="L4" s="6">
+        <v>0</v>
+      </c>
+      <c r="M4" s="6">
+        <v>0</v>
+      </c>
+      <c r="N4" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="32" t="s">
         <v>96</v>
       </c>
@@ -7147,8 +7686,26 @@
       <c r="H5" s="32">
         <v>2.0998000000000003E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I5" s="6">
+        <v>0</v>
+      </c>
+      <c r="J5" s="6">
+        <v>0</v>
+      </c>
+      <c r="K5" s="6">
+        <v>0</v>
+      </c>
+      <c r="L5" s="6">
+        <v>0</v>
+      </c>
+      <c r="M5" s="6">
+        <v>0</v>
+      </c>
+      <c r="N5" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="32" t="s">
         <v>97</v>
       </c>
@@ -7173,8 +7730,26 @@
       <c r="H6" s="32">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I6" s="6">
+        <v>0</v>
+      </c>
+      <c r="J6" s="6">
+        <v>0</v>
+      </c>
+      <c r="K6" s="6">
+        <v>0</v>
+      </c>
+      <c r="L6" s="6">
+        <v>0</v>
+      </c>
+      <c r="M6" s="6">
+        <v>0</v>
+      </c>
+      <c r="N6" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="32" t="s">
         <v>98</v>
       </c>
@@ -7199,8 +7774,26 @@
       <c r="H7" s="32">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I7" s="6">
+        <v>0</v>
+      </c>
+      <c r="J7" s="6">
+        <v>0</v>
+      </c>
+      <c r="K7" s="6">
+        <v>0</v>
+      </c>
+      <c r="L7" s="6">
+        <v>0</v>
+      </c>
+      <c r="M7" s="6">
+        <v>0</v>
+      </c>
+      <c r="N7" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="32" t="s">
         <v>99</v>
       </c>
@@ -7225,8 +7818,26 @@
       <c r="H8" s="32">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I8" s="6">
+        <v>0</v>
+      </c>
+      <c r="J8" s="6">
+        <v>0</v>
+      </c>
+      <c r="K8" s="6">
+        <v>0</v>
+      </c>
+      <c r="L8" s="6">
+        <v>0</v>
+      </c>
+      <c r="M8" s="6">
+        <v>0</v>
+      </c>
+      <c r="N8" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="32" t="s">
         <v>100</v>
       </c>
@@ -7251,8 +7862,26 @@
       <c r="H9" s="32">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I9" s="6">
+        <v>0</v>
+      </c>
+      <c r="J9" s="6">
+        <v>0</v>
+      </c>
+      <c r="K9" s="6">
+        <v>0</v>
+      </c>
+      <c r="L9" s="6">
+        <v>0</v>
+      </c>
+      <c r="M9" s="6">
+        <v>0</v>
+      </c>
+      <c r="N9" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="32" t="s">
         <v>101</v>
       </c>
@@ -7277,8 +7906,26 @@
       <c r="H10" s="32">
         <v>0.90526300000000004</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I10" s="6">
+        <v>0</v>
+      </c>
+      <c r="J10" s="6">
+        <v>0</v>
+      </c>
+      <c r="K10" s="6">
+        <v>0</v>
+      </c>
+      <c r="L10" s="6">
+        <v>0</v>
+      </c>
+      <c r="M10" s="6">
+        <v>0</v>
+      </c>
+      <c r="N10" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="32" t="s">
         <v>102</v>
       </c>
@@ -7303,8 +7950,26 @@
       <c r="H11" s="32">
         <v>0.90526300000000004</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I11" s="6">
+        <v>0</v>
+      </c>
+      <c r="J11" s="6">
+        <v>0</v>
+      </c>
+      <c r="K11" s="6">
+        <v>0</v>
+      </c>
+      <c r="L11" s="6">
+        <v>0</v>
+      </c>
+      <c r="M11" s="6">
+        <v>0</v>
+      </c>
+      <c r="N11" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="32" t="s">
         <v>103</v>
       </c>
@@ -7328,20 +7993,39 @@
       </c>
       <c r="H12" s="32">
         <v>9.4737000000000016E-2</v>
+      </c>
+      <c r="I12" s="6">
+        <v>0</v>
+      </c>
+      <c r="J12" s="6">
+        <v>0</v>
+      </c>
+      <c r="K12" s="6">
+        <v>0</v>
+      </c>
+      <c r="L12" s="6">
+        <v>0</v>
+      </c>
+      <c r="M12" s="6">
+        <v>0</v>
+      </c>
+      <c r="N12" s="6">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7350,7 +8034,7 @@
     <col min="2" max="2" width="27.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="6" t="s">
         <v>68</v>
       </c>
@@ -7375,8 +8059,26 @@
       <c r="H1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I1" t="s">
+        <v>111</v>
+      </c>
+      <c r="J1" t="s">
+        <v>112</v>
+      </c>
+      <c r="K1" t="s">
+        <v>113</v>
+      </c>
+      <c r="L1" t="s">
+        <v>114</v>
+      </c>
+      <c r="M1" t="s">
+        <v>115</v>
+      </c>
+      <c r="N1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
         <v>64</v>
       </c>
@@ -7401,8 +8103,26 @@
       <c r="H2" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I2" s="6">
+        <v>0</v>
+      </c>
+      <c r="J2" s="6">
+        <v>0</v>
+      </c>
+      <c r="K2" s="6">
+        <v>0</v>
+      </c>
+      <c r="L2" s="6">
+        <v>0</v>
+      </c>
+      <c r="M2" s="6">
+        <v>0</v>
+      </c>
+      <c r="N2" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="6" t="s">
         <v>36</v>
       </c>
@@ -7424,8 +8144,26 @@
       <c r="H3" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I3" s="6">
+        <v>0</v>
+      </c>
+      <c r="J3" s="6">
+        <v>0</v>
+      </c>
+      <c r="K3" s="6">
+        <v>0</v>
+      </c>
+      <c r="L3" s="6">
+        <v>0</v>
+      </c>
+      <c r="M3" s="6">
+        <v>0</v>
+      </c>
+      <c r="N3" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="32" t="s">
         <v>95</v>
       </c>
@@ -7450,8 +8188,26 @@
       <c r="H4" s="32">
         <v>0.98</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I4" s="6">
+        <v>0</v>
+      </c>
+      <c r="J4" s="6">
+        <v>0</v>
+      </c>
+      <c r="K4" s="6">
+        <v>0</v>
+      </c>
+      <c r="L4" s="6">
+        <v>0</v>
+      </c>
+      <c r="M4" s="6">
+        <v>0</v>
+      </c>
+      <c r="N4" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="32" t="s">
         <v>96</v>
       </c>
@@ -7476,8 +8232,26 @@
       <c r="H5" s="32">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I5" s="6">
+        <v>0</v>
+      </c>
+      <c r="J5" s="6">
+        <v>0</v>
+      </c>
+      <c r="K5" s="6">
+        <v>0</v>
+      </c>
+      <c r="L5" s="6">
+        <v>0</v>
+      </c>
+      <c r="M5" s="6">
+        <v>0</v>
+      </c>
+      <c r="N5" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="32" t="s">
         <v>97</v>
       </c>
@@ -7502,8 +8276,26 @@
       <c r="H6" s="32">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I6" s="6">
+        <v>0</v>
+      </c>
+      <c r="J6" s="6">
+        <v>0</v>
+      </c>
+      <c r="K6" s="6">
+        <v>0</v>
+      </c>
+      <c r="L6" s="6">
+        <v>0</v>
+      </c>
+      <c r="M6" s="6">
+        <v>0</v>
+      </c>
+      <c r="N6" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="32" t="s">
         <v>98</v>
       </c>
@@ -7528,8 +8320,26 @@
       <c r="H7" s="32">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I7" s="6">
+        <v>0</v>
+      </c>
+      <c r="J7" s="6">
+        <v>0</v>
+      </c>
+      <c r="K7" s="6">
+        <v>0</v>
+      </c>
+      <c r="L7" s="6">
+        <v>0</v>
+      </c>
+      <c r="M7" s="6">
+        <v>0</v>
+      </c>
+      <c r="N7" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="32" t="s">
         <v>99</v>
       </c>
@@ -7554,8 +8364,26 @@
       <c r="H8" s="32">
         <v>0.59</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I8" s="6">
+        <v>0</v>
+      </c>
+      <c r="J8" s="6">
+        <v>0</v>
+      </c>
+      <c r="K8" s="6">
+        <v>0</v>
+      </c>
+      <c r="L8" s="6">
+        <v>0</v>
+      </c>
+      <c r="M8" s="6">
+        <v>0</v>
+      </c>
+      <c r="N8" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="32" t="s">
         <v>100</v>
       </c>
@@ -7580,8 +8408,26 @@
       <c r="H9" s="32">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I9" s="6">
+        <v>0</v>
+      </c>
+      <c r="J9" s="6">
+        <v>0</v>
+      </c>
+      <c r="K9" s="6">
+        <v>0</v>
+      </c>
+      <c r="L9" s="6">
+        <v>0</v>
+      </c>
+      <c r="M9" s="6">
+        <v>0</v>
+      </c>
+      <c r="N9" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="32" t="s">
         <v>101</v>
       </c>
@@ -7606,8 +8452,26 @@
       <c r="H10" s="32">
         <v>0.95</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I10" s="6">
+        <v>0</v>
+      </c>
+      <c r="J10" s="6">
+        <v>0</v>
+      </c>
+      <c r="K10" s="6">
+        <v>0</v>
+      </c>
+      <c r="L10" s="6">
+        <v>0</v>
+      </c>
+      <c r="M10" s="6">
+        <v>0</v>
+      </c>
+      <c r="N10" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="32" t="s">
         <v>102</v>
       </c>
@@ -7632,8 +8496,26 @@
       <c r="H11" s="32">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I11" s="6">
+        <v>0</v>
+      </c>
+      <c r="J11" s="6">
+        <v>0</v>
+      </c>
+      <c r="K11" s="6">
+        <v>0</v>
+      </c>
+      <c r="L11" s="6">
+        <v>0</v>
+      </c>
+      <c r="M11" s="6">
+        <v>0</v>
+      </c>
+      <c r="N11" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="32" t="s">
         <v>103</v>
       </c>
@@ -7657,11 +8539,30 @@
       </c>
       <c r="H12" s="32">
         <v>0.9</v>
+      </c>
+      <c r="I12" s="6">
+        <v>0</v>
+      </c>
+      <c r="J12" s="6">
+        <v>0</v>
+      </c>
+      <c r="K12" s="6">
+        <v>0</v>
+      </c>
+      <c r="L12" s="6">
+        <v>0</v>
+      </c>
+      <c r="M12" s="6">
+        <v>0</v>
+      </c>
+      <c r="N12" s="6">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added anemia interventions to workbook
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Jan/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Jan/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-43980" yWindow="-19580" windowWidth="32620" windowHeight="18080" tabRatio="500" firstSheet="19" activeTab="26"/>
+    <workbookView xWindow="-6680" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" firstSheet="11" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="demographics" sheetId="1" r:id="rId1"/>
@@ -30,18 +30,20 @@
     <sheet name="RR diarrhoea" sheetId="13" r:id="rId16"/>
     <sheet name="OR stunting by condition" sheetId="14" r:id="rId17"/>
     <sheet name="OR stunting by birth outcome" sheetId="15" r:id="rId18"/>
-    <sheet name="OR stunting by intervention" sheetId="16" r:id="rId19"/>
-    <sheet name="OR stunting by compfeeding" sheetId="17" r:id="rId20"/>
-    <sheet name="OR correctBF by interventn" sheetId="18" r:id="rId21"/>
-    <sheet name="Appropriate breastfeeding" sheetId="19" r:id="rId22"/>
-    <sheet name="Interventions cost and coverage" sheetId="20" r:id="rId23"/>
-    <sheet name="Interventions target population" sheetId="21" r:id="rId24"/>
-    <sheet name="Interventions birth outcome" sheetId="22" r:id="rId25"/>
-    <sheet name="Interventions affected fraction" sheetId="23" r:id="rId26"/>
-    <sheet name="Interventions mortality eff" sheetId="24" r:id="rId27"/>
-    <sheet name="Interventions incidence eff" sheetId="25" r:id="rId28"/>
-    <sheet name="Interventions maternal aff frac" sheetId="26" r:id="rId29"/>
-    <sheet name="Interventions maternal eff" sheetId="27" r:id="rId30"/>
+    <sheet name="RR anemic by intervention" sheetId="31" r:id="rId19"/>
+    <sheet name="OR anemic by intervention" sheetId="32" r:id="rId20"/>
+    <sheet name="OR stunting by intervention" sheetId="16" r:id="rId21"/>
+    <sheet name="OR stunting by compfeeding" sheetId="17" r:id="rId22"/>
+    <sheet name="OR correctBF by interventn" sheetId="18" r:id="rId23"/>
+    <sheet name="Appropriate breastfeeding" sheetId="19" r:id="rId24"/>
+    <sheet name="Interventions cost and coverage" sheetId="20" r:id="rId25"/>
+    <sheet name="Interventions target population" sheetId="21" r:id="rId26"/>
+    <sheet name="Interventions birth outcome" sheetId="22" r:id="rId27"/>
+    <sheet name="Interventions affected fraction" sheetId="23" r:id="rId28"/>
+    <sheet name="Interventions mortality eff" sheetId="24" r:id="rId29"/>
+    <sheet name="Interventions incidence eff" sheetId="25" r:id="rId30"/>
+    <sheet name="Interventions maternal aff frac" sheetId="26" r:id="rId31"/>
+    <sheet name="Interventions maternal eff" sheetId="27" r:id="rId32"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -156,9 +158,11 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Sam</author>
+    <author>Janka Petravic</author>
+    <author>Ruth</author>
   </authors>
   <commentList>
-    <comment ref="I2" authorId="0">
+    <comment ref="H2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -176,7 +180,95 @@
             <rFont val="Calibri"/>
           </rPr>
           <t xml:space="preserve">
-WRA all fictional</t>
+WRA values (possibly?) fictional </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D4" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+2 lowest wealth quintiles</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E4" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+2 lowest wealth quintiles</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G6" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+2 lowest wealth quintiles</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A18" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Active management of the third stage of labor</t>
         </r>
       </text>
     </comment>
@@ -217,6 +309,38 @@
 </file>
 
 <file path=xl/comments12.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Sam</author>
+  </authors>
+  <commentList>
+    <comment ref="I2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Sam:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+WRA all fictional</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments13.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Ruth</author>
@@ -292,7 +416,7 @@
 </comments>
 </file>
 
-<file path=xl/comments13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments14.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Ruth</author>
@@ -635,6 +759,38 @@
 <file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
+    <author>Sam</author>
+  </authors>
+  <commentList>
+    <comment ref="G2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Sam:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+What is this RR?</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
     <author>Janka Petravic</author>
   </authors>
   <commentList>
@@ -664,7 +820,7 @@
 </comments>
 </file>
 
-<file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Ruth</author>
@@ -696,130 +852,8 @@
 </comments>
 </file>
 
-<file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Sam</author>
-    <author>Janka Petravic</author>
-    <author>Ruth</author>
-  </authors>
-  <commentList>
-    <comment ref="H2" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>Sam:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">
-WRA values fictional</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D4" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-2 lowest wealth quintiles</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E4" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-2 lowest wealth quintiles</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G6" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-2 lowest wealth quintiles</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A18" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>Ruth:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Active management of the third stage of labor</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="129">
   <si>
     <t>indicators</t>
   </si>
@@ -1187,21 +1221,6 @@
     <t>Anemia Status</t>
   </si>
   <si>
-    <t>Cause1</t>
-  </si>
-  <si>
-    <t>Cause2</t>
-  </si>
-  <si>
-    <t>Cause3</t>
-  </si>
-  <si>
-    <t>Anemic</t>
-  </si>
-  <si>
-    <t>Not Anemic</t>
-  </si>
-  <si>
     <t>WRA: cause1</t>
   </si>
   <si>
@@ -1209,6 +1228,18 @@
   </si>
   <si>
     <t>WRA: cause3</t>
+  </si>
+  <si>
+    <t>Iron and folic acid for non-pregnant women</t>
+  </si>
+  <si>
+    <t>Food fortification</t>
+  </si>
+  <si>
+    <t>IPTp</t>
+  </si>
+  <si>
+    <t>Anenatal micronutrient supplementation</t>
   </si>
 </sst>
 </file>
@@ -3101,11 +3132,12 @@
   <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:N1"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
+    <col min="1" max="1" width="10.83203125" customWidth="1"/>
     <col min="2" max="2" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3158,16 +3190,16 @@
         <v>122</v>
       </c>
       <c r="B2" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -3199,7 +3231,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.15">
       <c r="B3" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -3243,7 +3275,7 @@
         <v>123</v>
       </c>
       <c r="B4" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -3284,7 +3316,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.15">
       <c r="B5" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -3328,7 +3360,7 @@
         <v>124</v>
       </c>
       <c r="B6" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -3369,7 +3401,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.15">
       <c r="B7" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -5595,19 +5627,19 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="37.6640625" customWidth="1"/>
+    <col min="1" max="1" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
         <v>56</v>
       </c>
       <c r="B1" t="s">
@@ -5625,53 +5657,153 @@
       <c r="F1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="B2" s="6">
-        <v>1</v>
-      </c>
-      <c r="C2" s="6">
-        <v>1</v>
-      </c>
-      <c r="D2" s="6">
-        <v>1</v>
-      </c>
-      <c r="E2" s="6">
-        <v>0.9</v>
-      </c>
-      <c r="F2" s="6">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
+      <c r="G1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I1" t="s">
+        <v>112</v>
+      </c>
+      <c r="J1" t="s">
+        <v>113</v>
+      </c>
+      <c r="K1" t="s">
+        <v>114</v>
+      </c>
+      <c r="L1" t="s">
+        <v>115</v>
+      </c>
+      <c r="M1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>0.83</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>0.73</v>
+      </c>
+      <c r="I4">
+        <v>0.73</v>
+      </c>
+      <c r="J4">
+        <v>0.73</v>
+      </c>
+      <c r="K4">
+        <v>0.73</v>
+      </c>
+      <c r="L4">
+        <v>0.73</v>
+      </c>
+      <c r="M4">
+        <v>0.73</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -5817,6 +5949,186 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I1" t="s">
+        <v>112</v>
+      </c>
+      <c r="J1" t="s">
+        <v>113</v>
+      </c>
+      <c r="K1" t="s">
+        <v>114</v>
+      </c>
+      <c r="L1" t="s">
+        <v>115</v>
+      </c>
+      <c r="M1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="37.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="6">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6">
+        <v>1</v>
+      </c>
+      <c r="D2" s="6">
+        <v>1</v>
+      </c>
+      <c r="E2" s="6">
+        <v>0.9</v>
+      </c>
+      <c r="F2" s="6">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5933,7 +6245,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
@@ -6020,7 +6332,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -6086,12 +6398,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6433,20 +6745,46 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
+      <c r="A22" t="s">
+        <v>127</v>
+      </c>
+      <c r="B22" s="6">
+        <v>0</v>
+      </c>
+      <c r="C22" s="6">
+        <v>0.85</v>
+      </c>
+      <c r="D22" s="39">
+        <v>1</v>
+      </c>
     </row>
     <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
+      <c r="A23" t="s">
+        <v>125</v>
+      </c>
+      <c r="B23" s="6">
+        <v>0</v>
+      </c>
+      <c r="C23" s="6">
+        <v>0.85</v>
+      </c>
+      <c r="D23" s="39">
+        <v>1</v>
+      </c>
     </row>
     <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-    </row>
-    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
+      <c r="A24" t="s">
+        <v>126</v>
+      </c>
+      <c r="B24" s="6">
+        <v>0</v>
+      </c>
+      <c r="C24" s="6">
+        <v>0.85</v>
+      </c>
+      <c r="D24" s="39">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -6455,12 +6793,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M25"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7338,20 +7676,127 @@
       </c>
     </row>
     <row r="22" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
+      <c r="A22" t="s">
+        <v>127</v>
+      </c>
+      <c r="B22" s="6">
+        <v>0</v>
+      </c>
+      <c r="C22" s="6">
+        <v>0</v>
+      </c>
+      <c r="D22" s="6">
+        <v>0</v>
+      </c>
+      <c r="E22" s="6">
+        <v>0</v>
+      </c>
+      <c r="F22" s="6">
+        <v>0</v>
+      </c>
+      <c r="G22" s="39">
+        <v>1</v>
+      </c>
+      <c r="H22" s="4">
+        <v>0</v>
+      </c>
+      <c r="I22" s="4">
+        <v>0</v>
+      </c>
+      <c r="J22" s="4">
+        <v>0</v>
+      </c>
+      <c r="K22" s="4">
+        <v>0</v>
+      </c>
+      <c r="L22" s="4">
+        <v>0</v>
+      </c>
+      <c r="M22" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
+      <c r="A23" t="s">
+        <v>125</v>
+      </c>
+      <c r="B23" s="6">
+        <v>0</v>
+      </c>
+      <c r="C23" s="6">
+        <v>0</v>
+      </c>
+      <c r="D23" s="6">
+        <v>0</v>
+      </c>
+      <c r="E23" s="6">
+        <v>0</v>
+      </c>
+      <c r="F23" s="6">
+        <v>0</v>
+      </c>
+      <c r="G23" s="6">
+        <v>0</v>
+      </c>
+      <c r="H23" s="4">
+        <v>1</v>
+      </c>
+      <c r="I23" s="4">
+        <v>1</v>
+      </c>
+      <c r="J23" s="4">
+        <v>1</v>
+      </c>
+      <c r="K23" s="4">
+        <v>1</v>
+      </c>
+      <c r="L23" s="4">
+        <v>1</v>
+      </c>
+      <c r="M23" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="24" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-    </row>
-    <row r="25" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
+      <c r="A24" t="s">
+        <v>126</v>
+      </c>
+      <c r="B24" s="6">
+        <v>1</v>
+      </c>
+      <c r="C24" s="6">
+        <v>1</v>
+      </c>
+      <c r="D24" s="6">
+        <v>1</v>
+      </c>
+      <c r="E24" s="6">
+        <v>1</v>
+      </c>
+      <c r="F24" s="6">
+        <v>1</v>
+      </c>
+      <c r="G24" s="6">
+        <v>1</v>
+      </c>
+      <c r="H24" s="6">
+        <v>1</v>
+      </c>
+      <c r="I24" s="6">
+        <v>1</v>
+      </c>
+      <c r="J24" s="6">
+        <v>1</v>
+      </c>
+      <c r="K24" s="6">
+        <v>1</v>
+      </c>
+      <c r="L24" s="6">
+        <v>1</v>
+      </c>
+      <c r="M24" s="6">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -7360,7 +7805,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
@@ -7474,12 +7919,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -8020,11 +8465,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
@@ -8560,433 +9005,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="28.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="6">
-        <v>0</v>
-      </c>
-      <c r="D2" s="6">
-        <v>0</v>
-      </c>
-      <c r="E2" s="6">
-        <v>0.62</v>
-      </c>
-      <c r="F2" s="6">
-        <v>0.62</v>
-      </c>
-      <c r="G2" s="6">
-        <v>0.62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B3" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" s="6">
-        <v>0</v>
-      </c>
-      <c r="D3" s="6">
-        <v>0</v>
-      </c>
-      <c r="E3" s="6">
-        <v>0</v>
-      </c>
-      <c r="F3" s="6">
-        <v>0</v>
-      </c>
-      <c r="G3" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H35"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="42.5" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" customWidth="1"/>
-    <col min="4" max="4" width="17.33203125" customWidth="1"/>
-    <col min="5" max="5" width="15.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="35" t="s">
-        <v>68</v>
-      </c>
-      <c r="B1" s="35" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="40" t="s">
-        <v>92</v>
-      </c>
-      <c r="D1" s="40" t="s">
-        <v>93</v>
-      </c>
-      <c r="E1" s="40" t="s">
-        <v>94</v>
-      </c>
-      <c r="F1" s="40" t="s">
-        <v>89</v>
-      </c>
-      <c r="G1" s="40" t="s">
-        <v>90</v>
-      </c>
-      <c r="H1" s="41"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A2" s="23" t="s">
-        <v>105</v>
-      </c>
-      <c r="B2" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="C2" s="35">
-        <v>1</v>
-      </c>
-      <c r="D2" s="35">
-        <v>1</v>
-      </c>
-      <c r="E2" s="35">
-        <v>1</v>
-      </c>
-      <c r="F2" s="35">
-        <v>1</v>
-      </c>
-      <c r="G2" s="41">
-        <v>1</v>
-      </c>
-      <c r="H2" s="41"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A3" s="41"/>
-      <c r="B3" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="C3" s="35">
-        <v>1</v>
-      </c>
-      <c r="D3" s="35">
-        <v>1</v>
-      </c>
-      <c r="E3" s="35">
-        <v>1</v>
-      </c>
-      <c r="F3" s="35">
-        <v>1</v>
-      </c>
-      <c r="G3" s="41">
-        <v>1</v>
-      </c>
-      <c r="H3" s="41"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A4" s="37"/>
-      <c r="B4" s="23" t="s">
-        <v>82</v>
-      </c>
-      <c r="C4" s="35">
-        <v>1</v>
-      </c>
-      <c r="D4" s="35">
-        <v>1</v>
-      </c>
-      <c r="E4" s="35">
-        <v>1</v>
-      </c>
-      <c r="F4" s="35">
-        <v>1</v>
-      </c>
-      <c r="G4" s="41">
-        <v>1</v>
-      </c>
-      <c r="H4" s="41"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A5" s="37"/>
-      <c r="B5" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="C5" s="35">
-        <v>1</v>
-      </c>
-      <c r="D5" s="35">
-        <v>1</v>
-      </c>
-      <c r="E5" s="35">
-        <v>1</v>
-      </c>
-      <c r="F5" s="35">
-        <v>1</v>
-      </c>
-      <c r="G5" s="41">
-        <v>1</v>
-      </c>
-      <c r="H5" s="41"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A6" s="37"/>
-      <c r="B6" s="36" t="s">
-        <v>87</v>
-      </c>
-      <c r="C6" s="35">
-        <v>7.8159999999999993E-2</v>
-      </c>
-      <c r="D6" s="35">
-        <v>7.8159999999999993E-2</v>
-      </c>
-      <c r="E6" s="35">
-        <v>7.8159999999999993E-2</v>
-      </c>
-      <c r="F6" s="35">
-        <v>7.8159999999999993E-2</v>
-      </c>
-      <c r="G6" s="35">
-        <v>7.8159999999999993E-2</v>
-      </c>
-      <c r="H6" s="41"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A7" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="B7" s="23" t="s">
-        <v>82</v>
-      </c>
-      <c r="C7" s="35">
-        <v>1</v>
-      </c>
-      <c r="D7" s="35">
-        <v>1</v>
-      </c>
-      <c r="E7" s="35">
-        <v>1</v>
-      </c>
-      <c r="F7" s="35">
-        <v>1</v>
-      </c>
-      <c r="G7" s="41">
-        <v>1</v>
-      </c>
-      <c r="H7" s="41"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A8" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="B8" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="C8" s="35">
-        <v>1</v>
-      </c>
-      <c r="D8" s="35">
-        <v>1</v>
-      </c>
-      <c r="E8" s="35">
-        <v>1</v>
-      </c>
-      <c r="F8" s="35">
-        <v>1</v>
-      </c>
-      <c r="G8" s="41">
-        <v>1</v>
-      </c>
-      <c r="H8" s="41"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A9" s="23" t="s">
-        <v>106</v>
-      </c>
-      <c r="B9" s="37" t="s">
-        <v>84</v>
-      </c>
-      <c r="C9" s="35">
-        <v>1</v>
-      </c>
-      <c r="D9" s="35">
-        <v>1</v>
-      </c>
-      <c r="E9" s="35">
-        <v>1</v>
-      </c>
-      <c r="F9" s="35">
-        <v>1</v>
-      </c>
-      <c r="G9" s="41">
-        <v>1</v>
-      </c>
-      <c r="H9" s="41"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A10" s="23" t="s">
-        <v>107</v>
-      </c>
-      <c r="B10" s="37" t="s">
-        <v>84</v>
-      </c>
-      <c r="C10" s="35">
-        <v>0.33</v>
-      </c>
-      <c r="D10" s="35">
-        <v>0.33</v>
-      </c>
-      <c r="E10" s="35">
-        <v>0.33</v>
-      </c>
-      <c r="F10" s="35">
-        <v>0.33</v>
-      </c>
-      <c r="G10" s="35">
-        <v>0.33</v>
-      </c>
-      <c r="H10" s="41"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A11" s="37"/>
-      <c r="B11" s="37"/>
-      <c r="C11" s="35"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="41"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A12" s="37"/>
-      <c r="C12" s="35"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="41"/>
-      <c r="H12" s="41"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A13" s="41"/>
-      <c r="B13" s="41"/>
-      <c r="C13" s="41"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="41"/>
-      <c r="G13" s="41"/>
-      <c r="H13" s="41"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A14" s="41"/>
-      <c r="B14" s="41"/>
-      <c r="C14" s="41"/>
-      <c r="D14" s="41"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="41"/>
-      <c r="H14" s="41"/>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A27" s="36"/>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A28" s="37"/>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A29" s="37"/>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A30" s="37"/>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A31" s="37"/>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A32" s="37"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A33" s="37"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A34" s="37"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A35" s="37"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="14" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
@@ -9148,6 +9166,433 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="28.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="6">
+        <v>0</v>
+      </c>
+      <c r="D2" s="6">
+        <v>0</v>
+      </c>
+      <c r="E2" s="6">
+        <v>0.62</v>
+      </c>
+      <c r="F2" s="6">
+        <v>0.62</v>
+      </c>
+      <c r="G2" s="6">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B3" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0</v>
+      </c>
+      <c r="D3" s="6">
+        <v>0</v>
+      </c>
+      <c r="E3" s="6">
+        <v>0</v>
+      </c>
+      <c r="F3" s="6">
+        <v>0</v>
+      </c>
+      <c r="G3" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="42.5" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" customWidth="1"/>
+    <col min="5" max="5" width="15.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A1" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="40" t="s">
+        <v>92</v>
+      </c>
+      <c r="D1" s="40" t="s">
+        <v>93</v>
+      </c>
+      <c r="E1" s="40" t="s">
+        <v>94</v>
+      </c>
+      <c r="F1" s="40" t="s">
+        <v>89</v>
+      </c>
+      <c r="G1" s="40" t="s">
+        <v>90</v>
+      </c>
+      <c r="H1" s="41"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A2" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="35">
+        <v>1</v>
+      </c>
+      <c r="D2" s="35">
+        <v>1</v>
+      </c>
+      <c r="E2" s="35">
+        <v>1</v>
+      </c>
+      <c r="F2" s="35">
+        <v>1</v>
+      </c>
+      <c r="G2" s="41">
+        <v>1</v>
+      </c>
+      <c r="H2" s="41"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A3" s="41"/>
+      <c r="B3" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" s="35">
+        <v>1</v>
+      </c>
+      <c r="D3" s="35">
+        <v>1</v>
+      </c>
+      <c r="E3" s="35">
+        <v>1</v>
+      </c>
+      <c r="F3" s="35">
+        <v>1</v>
+      </c>
+      <c r="G3" s="41">
+        <v>1</v>
+      </c>
+      <c r="H3" s="41"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A4" s="37"/>
+      <c r="B4" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" s="35">
+        <v>1</v>
+      </c>
+      <c r="D4" s="35">
+        <v>1</v>
+      </c>
+      <c r="E4" s="35">
+        <v>1</v>
+      </c>
+      <c r="F4" s="35">
+        <v>1</v>
+      </c>
+      <c r="G4" s="41">
+        <v>1</v>
+      </c>
+      <c r="H4" s="41"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A5" s="37"/>
+      <c r="B5" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="C5" s="35">
+        <v>1</v>
+      </c>
+      <c r="D5" s="35">
+        <v>1</v>
+      </c>
+      <c r="E5" s="35">
+        <v>1</v>
+      </c>
+      <c r="F5" s="35">
+        <v>1</v>
+      </c>
+      <c r="G5" s="41">
+        <v>1</v>
+      </c>
+      <c r="H5" s="41"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A6" s="37"/>
+      <c r="B6" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" s="35">
+        <v>7.8159999999999993E-2</v>
+      </c>
+      <c r="D6" s="35">
+        <v>7.8159999999999993E-2</v>
+      </c>
+      <c r="E6" s="35">
+        <v>7.8159999999999993E-2</v>
+      </c>
+      <c r="F6" s="35">
+        <v>7.8159999999999993E-2</v>
+      </c>
+      <c r="G6" s="35">
+        <v>7.8159999999999993E-2</v>
+      </c>
+      <c r="H6" s="41"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A7" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" s="35">
+        <v>1</v>
+      </c>
+      <c r="D7" s="35">
+        <v>1</v>
+      </c>
+      <c r="E7" s="35">
+        <v>1</v>
+      </c>
+      <c r="F7" s="35">
+        <v>1</v>
+      </c>
+      <c r="G7" s="41">
+        <v>1</v>
+      </c>
+      <c r="H7" s="41"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A8" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" s="35">
+        <v>1</v>
+      </c>
+      <c r="D8" s="35">
+        <v>1</v>
+      </c>
+      <c r="E8" s="35">
+        <v>1</v>
+      </c>
+      <c r="F8" s="35">
+        <v>1</v>
+      </c>
+      <c r="G8" s="41">
+        <v>1</v>
+      </c>
+      <c r="H8" s="41"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A9" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="B9" s="37" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9" s="35">
+        <v>1</v>
+      </c>
+      <c r="D9" s="35">
+        <v>1</v>
+      </c>
+      <c r="E9" s="35">
+        <v>1</v>
+      </c>
+      <c r="F9" s="35">
+        <v>1</v>
+      </c>
+      <c r="G9" s="41">
+        <v>1</v>
+      </c>
+      <c r="H9" s="41"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A10" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="B10" s="37" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" s="35">
+        <v>0.33</v>
+      </c>
+      <c r="D10" s="35">
+        <v>0.33</v>
+      </c>
+      <c r="E10" s="35">
+        <v>0.33</v>
+      </c>
+      <c r="F10" s="35">
+        <v>0.33</v>
+      </c>
+      <c r="G10" s="35">
+        <v>0.33</v>
+      </c>
+      <c r="H10" s="41"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A11" s="37"/>
+      <c r="B11" s="37"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="41"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A12" s="37"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="41"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A13" s="41"/>
+      <c r="B13" s="41"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="41"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A14" s="41"/>
+      <c r="B14" s="41"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="41"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A27" s="36"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A28" s="37"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A29" s="37"/>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A30" s="37"/>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A31" s="37"/>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A32" s="37"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A33" s="37"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A34" s="37"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A35" s="37"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="14" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
@@ -9476,7 +9921,7 @@
   <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -10593,7 +11038,7 @@
     </row>
     <row r="28" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B28" s="6">
         <v>0</v>
@@ -10634,7 +11079,7 @@
     </row>
     <row r="29" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B29" s="6">
         <v>0</v>
@@ -10675,7 +11120,7 @@
     </row>
     <row r="30" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B30" s="6">
         <v>0</v>
@@ -11128,7 +11573,7 @@
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="M54" sqref="M54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Added proportion exposed to malaria tab
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Jan/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Jan/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-6680" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" firstSheet="11" activeTab="19"/>
+    <workbookView xWindow="-6680" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" firstSheet="21" activeTab="28"/>
   </bookViews>
   <sheets>
     <sheet name="demographics" sheetId="1" r:id="rId1"/>
@@ -40,10 +40,11 @@
     <sheet name="Interventions target population" sheetId="21" r:id="rId26"/>
     <sheet name="Interventions birth outcome" sheetId="22" r:id="rId27"/>
     <sheet name="Interventions affected fraction" sheetId="23" r:id="rId28"/>
-    <sheet name="Interventions mortality eff" sheetId="24" r:id="rId29"/>
-    <sheet name="Interventions incidence eff" sheetId="25" r:id="rId30"/>
-    <sheet name="Interventions maternal aff frac" sheetId="26" r:id="rId31"/>
-    <sheet name="Interventions maternal eff" sheetId="27" r:id="rId32"/>
+    <sheet name="Proportion exposed to malaria" sheetId="33" r:id="rId29"/>
+    <sheet name="Interventions mortality eff" sheetId="24" r:id="rId30"/>
+    <sheet name="Interventions incidence eff" sheetId="25" r:id="rId31"/>
+    <sheet name="Interventions maternal aff frac" sheetId="26" r:id="rId32"/>
+    <sheet name="Interventions maternal eff" sheetId="27" r:id="rId33"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -314,6 +315,38 @@
     <author>Sam</author>
   </authors>
   <commentList>
+    <comment ref="A2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Sam:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Fictional values</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments13.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Sam</author>
+  </authors>
+  <commentList>
     <comment ref="I2" authorId="0">
       <text>
         <r>
@@ -340,7 +373,7 @@
 </comments>
 </file>
 
-<file path=xl/comments13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments14.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Ruth</author>
@@ -416,7 +449,7 @@
 </comments>
 </file>
 
-<file path=xl/comments14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments15.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Ruth</author>
@@ -853,7 +886,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="129">
   <si>
     <t>indicators</t>
   </si>
@@ -5630,7 +5663,7 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B1" sqref="B1:M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5951,7 +5984,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
@@ -8467,546 +8500,92 @@
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="28.83203125" customWidth="1"/>
-    <col min="2" max="2" width="27.83203125" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>10</v>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F1" t="s">
-        <v>14</v>
+        <v>67</v>
       </c>
       <c r="G1" t="s">
-        <v>15</v>
+        <v>111</v>
       </c>
       <c r="H1" t="s">
-        <v>67</v>
+        <v>112</v>
       </c>
       <c r="I1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="J1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="K1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="L1" t="s">
-        <v>114</v>
-      </c>
-      <c r="M1" t="s">
-        <v>115</v>
-      </c>
-      <c r="N1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="6">
-        <v>0</v>
-      </c>
-      <c r="D2" s="6">
-        <v>0</v>
-      </c>
-      <c r="E2" s="6">
-        <v>0.3</v>
-      </c>
-      <c r="F2" s="6">
-        <v>0.3</v>
-      </c>
-      <c r="G2" s="6">
-        <v>0.3</v>
-      </c>
-      <c r="H2" s="6">
-        <v>0</v>
-      </c>
-      <c r="I2" s="6">
-        <v>0</v>
-      </c>
-      <c r="J2" s="6">
-        <v>0</v>
-      </c>
-      <c r="K2" s="6">
-        <v>0</v>
-      </c>
-      <c r="L2" s="6">
-        <v>0</v>
-      </c>
-      <c r="M2" s="6">
-        <v>0</v>
-      </c>
-      <c r="N2" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B3" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" s="6">
-        <v>0</v>
-      </c>
-      <c r="D3" s="6">
-        <v>0</v>
-      </c>
-      <c r="E3" s="6">
-        <v>0</v>
-      </c>
-      <c r="F3" s="6">
-        <v>0</v>
-      </c>
-      <c r="G3" s="6">
-        <v>0</v>
-      </c>
-      <c r="H3" s="6">
-        <v>0</v>
-      </c>
-      <c r="I3" s="6">
-        <v>0</v>
-      </c>
-      <c r="J3" s="6">
-        <v>0</v>
-      </c>
-      <c r="K3" s="6">
-        <v>0</v>
-      </c>
-      <c r="L3" s="6">
-        <v>0</v>
-      </c>
-      <c r="M3" s="6">
-        <v>0</v>
-      </c>
-      <c r="N3" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="32" t="s">
-        <v>95</v>
-      </c>
-      <c r="B4" s="33" t="s">
-        <v>88</v>
-      </c>
-      <c r="C4" s="6">
-        <v>0</v>
-      </c>
-      <c r="D4" s="6">
-        <v>0</v>
-      </c>
-      <c r="E4" s="6">
-        <v>0</v>
-      </c>
-      <c r="F4" s="6">
-        <v>0</v>
-      </c>
-      <c r="G4" s="6">
-        <v>0</v>
-      </c>
-      <c r="H4" s="32">
-        <v>0.98</v>
-      </c>
-      <c r="I4" s="6">
-        <v>0</v>
-      </c>
-      <c r="J4" s="6">
-        <v>0</v>
-      </c>
-      <c r="K4" s="6">
-        <v>0</v>
-      </c>
-      <c r="L4" s="6">
-        <v>0</v>
-      </c>
-      <c r="M4" s="6">
-        <v>0</v>
-      </c>
-      <c r="N4" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="32" t="s">
-        <v>96</v>
-      </c>
-      <c r="B5" s="32" t="s">
-        <v>88</v>
-      </c>
-      <c r="C5" s="6">
-        <v>0</v>
-      </c>
-      <c r="D5" s="6">
-        <v>0</v>
-      </c>
-      <c r="E5" s="6">
-        <v>0</v>
-      </c>
-      <c r="F5" s="6">
-        <v>0</v>
-      </c>
-      <c r="G5" s="6">
-        <v>0</v>
-      </c>
-      <c r="H5" s="32">
-        <v>0.8</v>
-      </c>
-      <c r="I5" s="6">
-        <v>0</v>
-      </c>
-      <c r="J5" s="6">
-        <v>0</v>
-      </c>
-      <c r="K5" s="6">
-        <v>0</v>
-      </c>
-      <c r="L5" s="6">
-        <v>0</v>
-      </c>
-      <c r="M5" s="6">
-        <v>0</v>
-      </c>
-      <c r="N5" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="32" t="s">
-        <v>97</v>
-      </c>
-      <c r="B6" s="32" t="s">
-        <v>83</v>
-      </c>
-      <c r="C6" s="6">
-        <v>0</v>
-      </c>
-      <c r="D6" s="6">
-        <v>0</v>
-      </c>
-      <c r="E6" s="6">
-        <v>0</v>
-      </c>
-      <c r="F6" s="6">
-        <v>0</v>
-      </c>
-      <c r="G6" s="6">
-        <v>0</v>
-      </c>
-      <c r="H6" s="32">
-        <v>0.2</v>
-      </c>
-      <c r="I6" s="6">
-        <v>0</v>
-      </c>
-      <c r="J6" s="6">
-        <v>0</v>
-      </c>
-      <c r="K6" s="6">
-        <v>0</v>
-      </c>
-      <c r="L6" s="6">
-        <v>0</v>
-      </c>
-      <c r="M6" s="6">
-        <v>0</v>
-      </c>
-      <c r="N6" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="32" t="s">
-        <v>98</v>
-      </c>
-      <c r="B7" s="32" t="s">
-        <v>83</v>
-      </c>
-      <c r="C7" s="6">
-        <v>0</v>
-      </c>
-      <c r="D7" s="6">
-        <v>0</v>
-      </c>
-      <c r="E7" s="6">
-        <v>0</v>
-      </c>
-      <c r="F7" s="6">
-        <v>0</v>
-      </c>
-      <c r="G7" s="6">
-        <v>0</v>
-      </c>
-      <c r="H7" s="32">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A2">
         <v>0.5</v>
       </c>
-      <c r="I7" s="6">
-        <v>0</v>
-      </c>
-      <c r="J7" s="6">
-        <v>0</v>
-      </c>
-      <c r="K7" s="6">
-        <v>0</v>
-      </c>
-      <c r="L7" s="6">
-        <v>0</v>
-      </c>
-      <c r="M7" s="6">
-        <v>0</v>
-      </c>
-      <c r="N7" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="32" t="s">
-        <v>99</v>
-      </c>
-      <c r="B8" s="32" t="s">
-        <v>83</v>
-      </c>
-      <c r="C8" s="6">
-        <v>0</v>
-      </c>
-      <c r="D8" s="6">
-        <v>0</v>
-      </c>
-      <c r="E8" s="6">
-        <v>0</v>
-      </c>
-      <c r="F8" s="6">
-        <v>0</v>
-      </c>
-      <c r="G8" s="6">
-        <v>0</v>
-      </c>
-      <c r="H8" s="32">
-        <v>0.59</v>
-      </c>
-      <c r="I8" s="6">
-        <v>0</v>
-      </c>
-      <c r="J8" s="6">
-        <v>0</v>
-      </c>
-      <c r="K8" s="6">
-        <v>0</v>
-      </c>
-      <c r="L8" s="6">
-        <v>0</v>
-      </c>
-      <c r="M8" s="6">
-        <v>0</v>
-      </c>
-      <c r="N8" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="32" t="s">
-        <v>100</v>
-      </c>
-      <c r="B9" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="C9" s="6">
-        <v>0</v>
-      </c>
-      <c r="D9" s="6">
-        <v>0</v>
-      </c>
-      <c r="E9" s="6">
-        <v>0</v>
-      </c>
-      <c r="F9" s="6">
-        <v>0</v>
-      </c>
-      <c r="G9" s="6">
-        <v>0</v>
-      </c>
-      <c r="H9" s="32">
-        <v>0.8</v>
-      </c>
-      <c r="I9" s="6">
-        <v>0</v>
-      </c>
-      <c r="J9" s="6">
-        <v>0</v>
-      </c>
-      <c r="K9" s="6">
-        <v>0</v>
-      </c>
-      <c r="L9" s="6">
-        <v>0</v>
-      </c>
-      <c r="M9" s="6">
-        <v>0</v>
-      </c>
-      <c r="N9" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="32" t="s">
-        <v>101</v>
-      </c>
-      <c r="B10" s="32" t="s">
-        <v>85</v>
-      </c>
-      <c r="C10" s="6">
-        <v>0</v>
-      </c>
-      <c r="D10" s="6">
-        <v>0</v>
-      </c>
-      <c r="E10" s="6">
-        <v>0</v>
-      </c>
-      <c r="F10" s="6">
-        <v>0</v>
-      </c>
-      <c r="G10" s="6">
-        <v>0</v>
-      </c>
-      <c r="H10" s="32">
-        <v>0.95</v>
-      </c>
-      <c r="I10" s="6">
-        <v>0</v>
-      </c>
-      <c r="J10" s="6">
-        <v>0</v>
-      </c>
-      <c r="K10" s="6">
-        <v>0</v>
-      </c>
-      <c r="L10" s="6">
-        <v>0</v>
-      </c>
-      <c r="M10" s="6">
-        <v>0</v>
-      </c>
-      <c r="N10" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="32" t="s">
-        <v>102</v>
-      </c>
-      <c r="B11" s="32" t="s">
-        <v>85</v>
-      </c>
-      <c r="C11" s="6">
-        <v>0</v>
-      </c>
-      <c r="D11" s="6">
-        <v>0</v>
-      </c>
-      <c r="E11" s="6">
-        <v>0</v>
-      </c>
-      <c r="F11" s="6">
-        <v>0</v>
-      </c>
-      <c r="G11" s="6">
-        <v>0</v>
-      </c>
-      <c r="H11" s="32">
-        <v>0.8</v>
-      </c>
-      <c r="I11" s="6">
-        <v>0</v>
-      </c>
-      <c r="J11" s="6">
-        <v>0</v>
-      </c>
-      <c r="K11" s="6">
-        <v>0</v>
-      </c>
-      <c r="L11" s="6">
-        <v>0</v>
-      </c>
-      <c r="M11" s="6">
-        <v>0</v>
-      </c>
-      <c r="N11" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="32" t="s">
-        <v>103</v>
-      </c>
-      <c r="B12" s="32" t="s">
-        <v>85</v>
-      </c>
-      <c r="C12" s="6">
-        <v>0</v>
-      </c>
-      <c r="D12" s="6">
-        <v>0</v>
-      </c>
-      <c r="E12" s="6">
-        <v>0</v>
-      </c>
-      <c r="F12" s="6">
-        <v>0</v>
-      </c>
-      <c r="G12" s="6">
-        <v>0</v>
-      </c>
-      <c r="H12" s="32">
-        <v>0.9</v>
-      </c>
-      <c r="I12" s="6">
-        <v>0</v>
-      </c>
-      <c r="J12" s="6">
-        <v>0</v>
-      </c>
-      <c r="K12" s="6">
-        <v>0</v>
-      </c>
-      <c r="L12" s="6">
-        <v>0</v>
-      </c>
-      <c r="M12" s="6">
-        <v>0</v>
-      </c>
-      <c r="N12" s="6">
-        <v>0</v>
+      <c r="B2">
+        <v>0.5</v>
+      </c>
+      <c r="C2">
+        <v>0.5</v>
+      </c>
+      <c r="D2">
+        <v>0.5</v>
+      </c>
+      <c r="E2">
+        <v>0.5</v>
+      </c>
+      <c r="F2">
+        <v>0.5</v>
+      </c>
+      <c r="G2">
+        <v>0.5</v>
+      </c>
+      <c r="H2">
+        <v>0.5</v>
+      </c>
+      <c r="I2">
+        <v>0.5</v>
+      </c>
+      <c r="J2">
+        <v>0.5</v>
+      </c>
+      <c r="K2">
+        <v>0.5</v>
+      </c>
+      <c r="L2">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -9166,6 +8745,552 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="28.83203125" customWidth="1"/>
+    <col min="2" max="2" width="27.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I1" t="s">
+        <v>111</v>
+      </c>
+      <c r="J1" t="s">
+        <v>112</v>
+      </c>
+      <c r="K1" t="s">
+        <v>113</v>
+      </c>
+      <c r="L1" t="s">
+        <v>114</v>
+      </c>
+      <c r="M1" t="s">
+        <v>115</v>
+      </c>
+      <c r="N1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="6">
+        <v>0</v>
+      </c>
+      <c r="D2" s="6">
+        <v>0</v>
+      </c>
+      <c r="E2" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="F2" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="G2" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="H2" s="6">
+        <v>0</v>
+      </c>
+      <c r="I2" s="6">
+        <v>0</v>
+      </c>
+      <c r="J2" s="6">
+        <v>0</v>
+      </c>
+      <c r="K2" s="6">
+        <v>0</v>
+      </c>
+      <c r="L2" s="6">
+        <v>0</v>
+      </c>
+      <c r="M2" s="6">
+        <v>0</v>
+      </c>
+      <c r="N2" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B3" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0</v>
+      </c>
+      <c r="D3" s="6">
+        <v>0</v>
+      </c>
+      <c r="E3" s="6">
+        <v>0</v>
+      </c>
+      <c r="F3" s="6">
+        <v>0</v>
+      </c>
+      <c r="G3" s="6">
+        <v>0</v>
+      </c>
+      <c r="H3" s="6">
+        <v>0</v>
+      </c>
+      <c r="I3" s="6">
+        <v>0</v>
+      </c>
+      <c r="J3" s="6">
+        <v>0</v>
+      </c>
+      <c r="K3" s="6">
+        <v>0</v>
+      </c>
+      <c r="L3" s="6">
+        <v>0</v>
+      </c>
+      <c r="M3" s="6">
+        <v>0</v>
+      </c>
+      <c r="N3" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" s="6">
+        <v>0</v>
+      </c>
+      <c r="D4" s="6">
+        <v>0</v>
+      </c>
+      <c r="E4" s="6">
+        <v>0</v>
+      </c>
+      <c r="F4" s="6">
+        <v>0</v>
+      </c>
+      <c r="G4" s="6">
+        <v>0</v>
+      </c>
+      <c r="H4" s="32">
+        <v>0.98</v>
+      </c>
+      <c r="I4" s="6">
+        <v>0</v>
+      </c>
+      <c r="J4" s="6">
+        <v>0</v>
+      </c>
+      <c r="K4" s="6">
+        <v>0</v>
+      </c>
+      <c r="L4" s="6">
+        <v>0</v>
+      </c>
+      <c r="M4" s="6">
+        <v>0</v>
+      </c>
+      <c r="N4" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5" s="6">
+        <v>0</v>
+      </c>
+      <c r="D5" s="6">
+        <v>0</v>
+      </c>
+      <c r="E5" s="6">
+        <v>0</v>
+      </c>
+      <c r="F5" s="6">
+        <v>0</v>
+      </c>
+      <c r="G5" s="6">
+        <v>0</v>
+      </c>
+      <c r="H5" s="32">
+        <v>0.8</v>
+      </c>
+      <c r="I5" s="6">
+        <v>0</v>
+      </c>
+      <c r="J5" s="6">
+        <v>0</v>
+      </c>
+      <c r="K5" s="6">
+        <v>0</v>
+      </c>
+      <c r="L5" s="6">
+        <v>0</v>
+      </c>
+      <c r="M5" s="6">
+        <v>0</v>
+      </c>
+      <c r="N5" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" s="6">
+        <v>0</v>
+      </c>
+      <c r="D6" s="6">
+        <v>0</v>
+      </c>
+      <c r="E6" s="6">
+        <v>0</v>
+      </c>
+      <c r="F6" s="6">
+        <v>0</v>
+      </c>
+      <c r="G6" s="6">
+        <v>0</v>
+      </c>
+      <c r="H6" s="32">
+        <v>0.2</v>
+      </c>
+      <c r="I6" s="6">
+        <v>0</v>
+      </c>
+      <c r="J6" s="6">
+        <v>0</v>
+      </c>
+      <c r="K6" s="6">
+        <v>0</v>
+      </c>
+      <c r="L6" s="6">
+        <v>0</v>
+      </c>
+      <c r="M6" s="6">
+        <v>0</v>
+      </c>
+      <c r="N6" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="32" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" s="6">
+        <v>0</v>
+      </c>
+      <c r="D7" s="6">
+        <v>0</v>
+      </c>
+      <c r="E7" s="6">
+        <v>0</v>
+      </c>
+      <c r="F7" s="6">
+        <v>0</v>
+      </c>
+      <c r="G7" s="6">
+        <v>0</v>
+      </c>
+      <c r="H7" s="32">
+        <v>0.5</v>
+      </c>
+      <c r="I7" s="6">
+        <v>0</v>
+      </c>
+      <c r="J7" s="6">
+        <v>0</v>
+      </c>
+      <c r="K7" s="6">
+        <v>0</v>
+      </c>
+      <c r="L7" s="6">
+        <v>0</v>
+      </c>
+      <c r="M7" s="6">
+        <v>0</v>
+      </c>
+      <c r="N7" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="32" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" s="6">
+        <v>0</v>
+      </c>
+      <c r="D8" s="6">
+        <v>0</v>
+      </c>
+      <c r="E8" s="6">
+        <v>0</v>
+      </c>
+      <c r="F8" s="6">
+        <v>0</v>
+      </c>
+      <c r="G8" s="6">
+        <v>0</v>
+      </c>
+      <c r="H8" s="32">
+        <v>0.59</v>
+      </c>
+      <c r="I8" s="6">
+        <v>0</v>
+      </c>
+      <c r="J8" s="6">
+        <v>0</v>
+      </c>
+      <c r="K8" s="6">
+        <v>0</v>
+      </c>
+      <c r="L8" s="6">
+        <v>0</v>
+      </c>
+      <c r="M8" s="6">
+        <v>0</v>
+      </c>
+      <c r="N8" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="B9" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9" s="6">
+        <v>0</v>
+      </c>
+      <c r="D9" s="6">
+        <v>0</v>
+      </c>
+      <c r="E9" s="6">
+        <v>0</v>
+      </c>
+      <c r="F9" s="6">
+        <v>0</v>
+      </c>
+      <c r="G9" s="6">
+        <v>0</v>
+      </c>
+      <c r="H9" s="32">
+        <v>0.8</v>
+      </c>
+      <c r="I9" s="6">
+        <v>0</v>
+      </c>
+      <c r="J9" s="6">
+        <v>0</v>
+      </c>
+      <c r="K9" s="6">
+        <v>0</v>
+      </c>
+      <c r="L9" s="6">
+        <v>0</v>
+      </c>
+      <c r="M9" s="6">
+        <v>0</v>
+      </c>
+      <c r="N9" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="C10" s="6">
+        <v>0</v>
+      </c>
+      <c r="D10" s="6">
+        <v>0</v>
+      </c>
+      <c r="E10" s="6">
+        <v>0</v>
+      </c>
+      <c r="F10" s="6">
+        <v>0</v>
+      </c>
+      <c r="G10" s="6">
+        <v>0</v>
+      </c>
+      <c r="H10" s="32">
+        <v>0.95</v>
+      </c>
+      <c r="I10" s="6">
+        <v>0</v>
+      </c>
+      <c r="J10" s="6">
+        <v>0</v>
+      </c>
+      <c r="K10" s="6">
+        <v>0</v>
+      </c>
+      <c r="L10" s="6">
+        <v>0</v>
+      </c>
+      <c r="M10" s="6">
+        <v>0</v>
+      </c>
+      <c r="N10" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="B11" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="C11" s="6">
+        <v>0</v>
+      </c>
+      <c r="D11" s="6">
+        <v>0</v>
+      </c>
+      <c r="E11" s="6">
+        <v>0</v>
+      </c>
+      <c r="F11" s="6">
+        <v>0</v>
+      </c>
+      <c r="G11" s="6">
+        <v>0</v>
+      </c>
+      <c r="H11" s="32">
+        <v>0.8</v>
+      </c>
+      <c r="I11" s="6">
+        <v>0</v>
+      </c>
+      <c r="J11" s="6">
+        <v>0</v>
+      </c>
+      <c r="K11" s="6">
+        <v>0</v>
+      </c>
+      <c r="L11" s="6">
+        <v>0</v>
+      </c>
+      <c r="M11" s="6">
+        <v>0</v>
+      </c>
+      <c r="N11" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="32" t="s">
+        <v>103</v>
+      </c>
+      <c r="B12" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="C12" s="6">
+        <v>0</v>
+      </c>
+      <c r="D12" s="6">
+        <v>0</v>
+      </c>
+      <c r="E12" s="6">
+        <v>0</v>
+      </c>
+      <c r="F12" s="6">
+        <v>0</v>
+      </c>
+      <c r="G12" s="6">
+        <v>0</v>
+      </c>
+      <c r="H12" s="32">
+        <v>0.9</v>
+      </c>
+      <c r="I12" s="6">
+        <v>0</v>
+      </c>
+      <c r="J12" s="6">
+        <v>0</v>
+      </c>
+      <c r="K12" s="6">
+        <v>0</v>
+      </c>
+      <c r="L12" s="6">
+        <v>0</v>
+      </c>
+      <c r="M12" s="6">
+        <v>0</v>
+      </c>
+      <c r="N12" s="6">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
@@ -9270,7 +9395,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H35"/>
   <sheetViews>
@@ -9592,7 +9717,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>

</xml_diff>

<commit_message>
Changed name of sheets to match 'pregnant women' & altered test mortality rates for pregnant women
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Jan/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Jan/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-6680" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" firstSheet="21" activeTab="28"/>
+    <workbookView xWindow="-6680" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="demographics" sheetId="1" r:id="rId1"/>
@@ -43,8 +43,8 @@
     <sheet name="Proportion exposed to malaria" sheetId="33" r:id="rId29"/>
     <sheet name="Interventions mortality eff" sheetId="24" r:id="rId30"/>
     <sheet name="Interventions incidence eff" sheetId="25" r:id="rId31"/>
-    <sheet name="Interventions maternal aff frac" sheetId="26" r:id="rId32"/>
-    <sheet name="Interventions maternal eff" sheetId="27" r:id="rId33"/>
+    <sheet name="Inter. pregnant women aff frac" sheetId="26" r:id="rId32"/>
+    <sheet name="Inter. pregnant women eff" sheetId="27" r:id="rId33"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -8502,7 +8502,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -9964,8 +9964,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -10016,22 +10016,22 @@
         <v>1.819</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="J2">
-        <v>1</v>
+        <v>0.01</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates to anemia interventions update
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Jan/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Jan/InputForCode_Bangladesh.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28209"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/Github Projects/Nutrition/input_spreadsheets/Bangladesh/2017Jan/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-6680" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="-36920" yWindow="-2800" windowWidth="30560" windowHeight="15640" tabRatio="500" firstSheet="27" activeTab="29"/>
   </bookViews>
   <sheets>
     <sheet name="demographics" sheetId="1" r:id="rId1"/>
@@ -40,19 +35,20 @@
     <sheet name="Interventions target population" sheetId="21" r:id="rId26"/>
     <sheet name="Interventions birth outcome" sheetId="22" r:id="rId27"/>
     <sheet name="Interventions affected fraction" sheetId="23" r:id="rId28"/>
-    <sheet name="Proportion exposed to malaria" sheetId="33" r:id="rId29"/>
-    <sheet name="Interventions mortality eff" sheetId="24" r:id="rId30"/>
-    <sheet name="Interventions incidence eff" sheetId="25" r:id="rId31"/>
-    <sheet name="Inter. pregnant women aff frac" sheetId="26" r:id="rId32"/>
-    <sheet name="Inter. pregnant women eff" sheetId="27" r:id="rId33"/>
+    <sheet name="Frac anemic exposed malaria" sheetId="33" r:id="rId29"/>
+    <sheet name="Frac exposed malaria" sheetId="34" r:id="rId30"/>
+    <sheet name="Interventions mortality eff" sheetId="24" r:id="rId31"/>
+    <sheet name="Interventions incidence eff" sheetId="25" r:id="rId32"/>
+    <sheet name="Inter. pregnant women aff frac" sheetId="26" r:id="rId33"/>
+    <sheet name="Inter. pregnant women eff" sheetId="27" r:id="rId34"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
@@ -347,6 +343,38 @@
     <author>Sam</author>
   </authors>
   <commentList>
+    <comment ref="A2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Sam:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Fictional values</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments14.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Sam</author>
+  </authors>
+  <commentList>
     <comment ref="I2" authorId="0">
       <text>
         <r>
@@ -373,7 +401,7 @@
 </comments>
 </file>
 
-<file path=xl/comments14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments15.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Ruth</author>
@@ -449,7 +477,7 @@
 </comments>
 </file>
 
-<file path=xl/comments15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments16.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Ruth</author>
@@ -886,7 +914,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="129">
   <si>
     <t>indicators</t>
   </si>
@@ -3081,15 +3109,15 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="32.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3097,7 +3125,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1">
       <c r="A2" s="6" t="s">
         <v>4</v>
       </c>
@@ -3105,7 +3133,7 @@
         <v>15204000</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1">
       <c r="A3" s="6" t="s">
         <v>8</v>
       </c>
@@ -3113,7 +3141,7 @@
         <v>3118117</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1">
       <c r="A4" s="6" t="s">
         <v>9</v>
       </c>
@@ -3121,7 +3149,7 @@
         <v>3689944</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1">
       <c r="A5" s="6" t="s">
         <v>110</v>
       </c>
@@ -3130,7 +3158,7 @@
         <v>36899440</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1">
       <c r="A6" s="6" t="s">
         <v>71</v>
       </c>
@@ -3138,7 +3166,7 @@
         <v>0.56799999999999995</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1">
       <c r="A7" s="6" t="s">
         <v>70</v>
       </c>
@@ -3146,7 +3174,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1">
       <c r="A8" s="6" t="s">
         <v>72</v>
       </c>
@@ -3157,6 +3185,11 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3168,13 +3201,13 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="10.83203125" customWidth="1"/>
     <col min="2" max="2" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -3218,7 +3251,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>122</v>
       </c>
@@ -3262,7 +3295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:14">
       <c r="B3" t="s">
         <v>119</v>
       </c>
@@ -3303,7 +3336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
         <v>123</v>
       </c>
@@ -3347,7 +3380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:14">
       <c r="B5" t="s">
         <v>119</v>
       </c>
@@ -3388,7 +3421,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:14">
       <c r="A6" t="s">
         <v>124</v>
       </c>
@@ -3432,7 +3465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:14">
       <c r="B7" t="s">
         <v>119</v>
       </c>
@@ -3476,6 +3509,11 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3487,9 +3525,9 @@
       <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>10</v>
       </c>
@@ -3512,7 +3550,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -3535,7 +3573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="B3" s="6" t="s">
         <v>29</v>
       </c>
@@ -3555,7 +3593,7 @@
         <v>1.67</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="B4" s="6" t="s">
         <v>32</v>
       </c>
@@ -3575,7 +3613,7 @@
         <v>2.38</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="B5" s="6" t="s">
         <v>33</v>
       </c>
@@ -3595,7 +3633,7 @@
         <v>6.33</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -3618,7 +3656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="B7" s="6" t="s">
         <v>29</v>
       </c>
@@ -3638,7 +3676,7 @@
         <v>1.55</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="B8" s="6" t="s">
         <v>32</v>
       </c>
@@ -3658,7 +3696,7 @@
         <v>2.1800000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="B9" s="6" t="s">
         <v>33</v>
       </c>
@@ -3678,7 +3716,7 @@
         <v>6.39</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -3701,7 +3739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="B11" s="6" t="s">
         <v>29</v>
       </c>
@@ -3721,7 +3759,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="B12" s="6" t="s">
         <v>32</v>
       </c>
@@ -3741,7 +3779,7 @@
         <v>2.79</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="B13" s="6" t="s">
         <v>33</v>
       </c>
@@ -3761,7 +3799,7 @@
         <v>6.01</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -3784,7 +3822,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="B15" s="6" t="s">
         <v>29</v>
       </c>
@@ -3804,7 +3842,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="B16" s="6" t="s">
         <v>32</v>
       </c>
@@ -3824,7 +3862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1">
       <c r="B17" s="6" t="s">
         <v>33</v>
       </c>
@@ -3844,7 +3882,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1">
       <c r="A18" t="s">
         <v>43</v>
       </c>
@@ -3867,7 +3905,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1">
       <c r="B19" s="6" t="s">
         <v>29</v>
       </c>
@@ -3887,7 +3925,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1">
       <c r="B20" s="6" t="s">
         <v>32</v>
       </c>
@@ -3907,7 +3945,7 @@
         <v>1.86</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1">
       <c r="B21" s="6" t="s">
         <v>33</v>
       </c>
@@ -3929,6 +3967,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3940,9 +3983,9 @@
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>10</v>
       </c>
@@ -3965,7 +4008,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -3988,7 +4031,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="B3" s="6" t="s">
         <v>20</v>
       </c>
@@ -4008,7 +4051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="B4" s="6" t="s">
         <v>29</v>
       </c>
@@ -4028,7 +4071,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="B5" s="6" t="s">
         <v>32</v>
       </c>
@@ -4048,7 +4091,7 @@
         <v>3.41</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="B6" s="6" t="s">
         <v>33</v>
       </c>
@@ -4068,7 +4111,7 @@
         <v>12.33</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -4091,7 +4134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="B8" s="6" t="s">
         <v>20</v>
       </c>
@@ -4111,7 +4154,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="B9" s="6" t="s">
         <v>29</v>
       </c>
@@ -4131,7 +4174,7 @@
         <v>1.92</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="B10" s="6" t="s">
         <v>32</v>
       </c>
@@ -4151,7 +4194,7 @@
         <v>4.66</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="B11" s="6" t="s">
         <v>33</v>
       </c>
@@ -4171,7 +4214,7 @@
         <v>9.68</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -4194,7 +4237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="B13" s="6" t="s">
         <v>20</v>
       </c>
@@ -4214,7 +4257,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="B14" s="6" t="s">
         <v>29</v>
       </c>
@@ -4234,7 +4277,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="B15" s="6" t="s">
         <v>32</v>
       </c>
@@ -4254,7 +4297,7 @@
         <v>2.58</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="B16" s="6" t="s">
         <v>33</v>
       </c>
@@ -4274,7 +4317,7 @@
         <v>9.6300000000000008</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -4297,7 +4340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1">
       <c r="B18" s="6" t="s">
         <v>20</v>
       </c>
@@ -4317,7 +4360,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1">
       <c r="B19" s="6" t="s">
         <v>29</v>
       </c>
@@ -4337,7 +4380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1">
       <c r="B20" s="6" t="s">
         <v>32</v>
       </c>
@@ -4357,7 +4400,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1">
       <c r="B21" s="6" t="s">
         <v>33</v>
       </c>
@@ -4377,7 +4420,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:7" ht="15.75" customHeight="1">
       <c r="A22" t="s">
         <v>43</v>
       </c>
@@ -4400,7 +4443,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:7" ht="15.75" customHeight="1">
       <c r="B23" s="6" t="s">
         <v>20</v>
       </c>
@@ -4420,7 +4463,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:7" ht="15.75" customHeight="1">
       <c r="B24" s="6" t="s">
         <v>29</v>
       </c>
@@ -4440,7 +4483,7 @@
         <v>1.65</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:7" ht="15.75" customHeight="1">
       <c r="B25" s="6" t="s">
         <v>32</v>
       </c>
@@ -4460,7 +4503,7 @@
         <v>2.73</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:7" ht="15.75" customHeight="1">
       <c r="B26" s="6" t="s">
         <v>33</v>
       </c>
@@ -4483,6 +4526,11 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4494,12 +4542,12 @@
       <selection activeCell="C2" sqref="C2:D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="2" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>10</v>
       </c>
@@ -4522,7 +4570,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -4545,7 +4593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="B3" s="6" t="s">
         <v>46</v>
       </c>
@@ -4565,7 +4613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="B4" s="6" t="s">
         <v>47</v>
       </c>
@@ -4585,7 +4633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="B5" s="6" t="s">
         <v>48</v>
       </c>
@@ -4605,7 +4653,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -4628,7 +4676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="B7" s="6" t="s">
         <v>46</v>
       </c>
@@ -4648,7 +4696,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="B8" s="6" t="s">
         <v>47</v>
       </c>
@@ -4668,7 +4716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="B9" s="6" t="s">
         <v>48</v>
       </c>
@@ -4688,7 +4736,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -4711,7 +4759,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="B11" s="6" t="s">
         <v>46</v>
       </c>
@@ -4731,7 +4779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="B12" s="6" t="s">
         <v>47</v>
       </c>
@@ -4751,7 +4799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="B13" s="6" t="s">
         <v>48</v>
       </c>
@@ -4771,7 +4819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -4794,7 +4842,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="B15" s="6" t="s">
         <v>46</v>
       </c>
@@ -4814,7 +4862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="B16" s="6" t="s">
         <v>47</v>
       </c>
@@ -4834,7 +4882,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1">
       <c r="B17" s="6" t="s">
         <v>48</v>
       </c>
@@ -4854,7 +4902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -4877,7 +4925,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1">
       <c r="B19" s="6" t="s">
         <v>46</v>
       </c>
@@ -4897,7 +4945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1">
       <c r="B20" s="6" t="s">
         <v>47</v>
       </c>
@@ -4917,7 +4965,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1">
       <c r="B21" s="6" t="s">
         <v>48</v>
       </c>
@@ -4937,7 +4985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:7" ht="15.75" customHeight="1">
       <c r="A22" t="s">
         <v>36</v>
       </c>
@@ -4960,7 +5008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:7" ht="15.75" customHeight="1">
       <c r="B23" s="6" t="s">
         <v>46</v>
       </c>
@@ -4980,7 +5028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:7" ht="15.75" customHeight="1">
       <c r="B24" s="6" t="s">
         <v>47</v>
       </c>
@@ -5000,7 +5048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:7" ht="15.75" customHeight="1">
       <c r="B25" s="6" t="s">
         <v>48</v>
       </c>
@@ -5020,7 +5068,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:7" ht="15.75" customHeight="1">
       <c r="A26" t="s">
         <v>37</v>
       </c>
@@ -5043,7 +5091,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:7" ht="15.75" customHeight="1">
       <c r="B27" s="6" t="s">
         <v>46</v>
       </c>
@@ -5063,7 +5111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:7" ht="15.75" customHeight="1">
       <c r="B28" s="6" t="s">
         <v>47</v>
       </c>
@@ -5083,7 +5131,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:7" ht="15.75" customHeight="1">
       <c r="B29" s="6" t="s">
         <v>48</v>
       </c>
@@ -5105,6 +5153,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5116,13 +5169,13 @@
       <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="33.83203125" customWidth="1"/>
     <col min="2" max="2" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>10</v>
       </c>
@@ -5139,7 +5192,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" s="13" t="s">
         <v>16</v>
       </c>
@@ -5158,7 +5211,7 @@
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="A3" s="13" t="s">
         <v>21</v>
       </c>
@@ -5177,7 +5230,7 @@
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="A4" s="13" t="s">
         <v>22</v>
       </c>
@@ -5196,7 +5249,7 @@
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="A5" s="13" t="s">
         <v>24</v>
       </c>
@@ -5215,7 +5268,7 @@
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" s="13" t="s">
         <v>27</v>
       </c>
@@ -5234,7 +5287,7 @@
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="A7" s="13" t="s">
         <v>28</v>
       </c>
@@ -5253,7 +5306,7 @@
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="A8" s="13" t="s">
         <v>54</v>
       </c>
@@ -5272,7 +5325,7 @@
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="A9" s="13" t="s">
         <v>31</v>
       </c>
@@ -5291,113 +5344,118 @@
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="B10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="B11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="B12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="B13" s="6"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="B14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="B15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="B16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
     </row>
-    <row r="17" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:7" ht="15.75" customHeight="1">
       <c r="B17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
     </row>
-    <row r="18" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:7" ht="15.75" customHeight="1">
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
     </row>
-    <row r="19" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:7" ht="15.75" customHeight="1">
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
     </row>
-    <row r="20" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:7" ht="15.75" customHeight="1">
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
     </row>
-    <row r="21" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:7" ht="15.75" customHeight="1">
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
     </row>
-    <row r="22" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:7" ht="15.75" customHeight="1">
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
     </row>
-    <row r="23" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:7" ht="15.75" customHeight="1">
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
     </row>
-    <row r="24" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="2:7" ht="15.75" customHeight="1">
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
     </row>
-    <row r="25" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="2:7" ht="15.75" customHeight="1">
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
     </row>
-    <row r="26" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="2:7" ht="15.75" customHeight="1">
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
     </row>
-    <row r="27" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="2:7" ht="15.75" customHeight="1">
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
     </row>
-    <row r="28" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="2:7" ht="15.75" customHeight="1">
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
     </row>
-    <row r="29" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="2:7" ht="15.75" customHeight="1">
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5409,9 +5467,9 @@
       <selection activeCell="A2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -5425,7 +5483,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" ht="15.75" customHeight="1">
       <c r="A2" s="6">
         <v>45</v>
       </c>
@@ -5441,6 +5499,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5450,12 +5513,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="25.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>55</v>
       </c>
@@ -5475,7 +5538,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" s="6" t="s">
         <v>45</v>
       </c>
@@ -5495,7 +5558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1">
       <c r="A3" s="6" t="s">
         <v>46</v>
       </c>
@@ -5515,7 +5578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1">
       <c r="A4" s="6" t="s">
         <v>47</v>
       </c>
@@ -5535,7 +5598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1">
       <c r="A5" s="6" t="s">
         <v>48</v>
       </c>
@@ -5557,6 +5620,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5568,9 +5636,9 @@
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>49</v>
       </c>
@@ -5590,7 +5658,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" s="6" t="s">
         <v>34</v>
       </c>
@@ -5612,6 +5680,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5623,9 +5696,9 @@
       <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1">
       <c r="A1" s="14" t="s">
         <v>53</v>
       </c>
@@ -5639,7 +5712,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="15.75" customHeight="1">
       <c r="A2" s="15">
         <v>1</v>
       </c>
@@ -5655,6 +5728,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5666,12 +5744,12 @@
       <selection activeCell="B1" sqref="B1:M1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>56</v>
       </c>
@@ -5712,7 +5790,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>128</v>
       </c>
@@ -5753,7 +5831,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
         <v>127</v>
       </c>
@@ -5794,7 +5872,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
         <v>125</v>
       </c>
@@ -5838,6 +5916,11 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5849,13 +5932,13 @@
       <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="12.5" customWidth="1"/>
     <col min="2" max="2" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -5863,7 +5946,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1">
       <c r="A2" s="4">
         <v>2017</v>
       </c>
@@ -5871,7 +5954,7 @@
         <v>3095470</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1">
       <c r="A3" s="4">
         <v>2018</v>
       </c>
@@ -5879,7 +5962,7 @@
         <v>3071259</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1">
       <c r="A4" s="4">
         <v>2019</v>
       </c>
@@ -5887,7 +5970,7 @@
         <v>3045241</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1">
       <c r="A5" s="4">
         <v>2020</v>
       </c>
@@ -5895,7 +5978,7 @@
         <v>3017266</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1">
       <c r="A6" s="4">
         <v>2021</v>
       </c>
@@ -5903,7 +5986,7 @@
         <v>2990677</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1">
       <c r="A7" s="4">
         <v>2022</v>
       </c>
@@ -5911,7 +5994,7 @@
         <v>2962144</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1">
       <c r="A8" s="4">
         <v>2023</v>
       </c>
@@ -5919,7 +6002,7 @@
         <v>2931643</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1">
       <c r="A9" s="4">
         <v>2024</v>
       </c>
@@ -5927,7 +6010,7 @@
         <v>2899255</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1">
       <c r="A10" s="4">
         <v>2025</v>
       </c>
@@ -5935,7 +6018,7 @@
         <v>2865008</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1">
       <c r="A11" s="4">
         <v>2026</v>
       </c>
@@ -5943,7 +6026,7 @@
         <v>2836142</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:2" ht="15.75" customHeight="1">
       <c r="A12" s="4">
         <v>2027</v>
       </c>
@@ -5951,7 +6034,7 @@
         <v>2805541</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:2" ht="15.75" customHeight="1">
       <c r="A13" s="4">
         <v>2028</v>
       </c>
@@ -5959,7 +6042,7 @@
         <v>2773236</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:2" ht="15.75" customHeight="1">
       <c r="A14" s="4">
         <v>2029</v>
       </c>
@@ -5967,7 +6050,7 @@
         <v>2739273</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:2" ht="15.75" customHeight="1">
       <c r="A15" s="4">
         <v>2030</v>
       </c>
@@ -5977,6 +6060,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5988,9 +6076,9 @@
       <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>56</v>
       </c>
@@ -6031,7 +6119,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>126</v>
       </c>
@@ -6074,6 +6162,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -6085,12 +6178,12 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="37.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>56</v>
       </c>
@@ -6110,7 +6203,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" s="6" t="s">
         <v>73</v>
       </c>
@@ -6130,7 +6223,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -6138,7 +6231,7 @@
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -6146,7 +6239,7 @@
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -6157,6 +6250,11 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -6168,12 +6266,12 @@
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="70.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>78</v>
       </c>
@@ -6193,7 +6291,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" s="6" t="s">
         <v>57</v>
       </c>
@@ -6213,7 +6311,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1">
       <c r="A3" s="6" t="s">
         <v>58</v>
       </c>
@@ -6233,7 +6331,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1">
       <c r="A4" s="6" t="s">
         <v>59</v>
       </c>
@@ -6253,7 +6351,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1">
       <c r="A5" s="6" t="s">
         <v>60</v>
       </c>
@@ -6275,6 +6373,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -6286,13 +6389,13 @@
       <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="43.1640625" customWidth="1"/>
     <col min="2" max="6" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>56</v>
       </c>
@@ -6312,7 +6415,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="14">
       <c r="A2" s="6" t="s">
         <v>74</v>
       </c>
@@ -6332,7 +6435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="14">
       <c r="A3" s="6" t="s">
         <v>75</v>
       </c>
@@ -6352,7 +6455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -6362,6 +6465,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -6373,12 +6481,12 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="5" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -6395,7 +6503,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="14">
       <c r="A2" s="16" t="s">
         <v>45</v>
       </c>
@@ -6412,14 +6520,14 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
     </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -6428,6 +6536,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -6436,10 +6549,10 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="43.6640625" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
@@ -6447,7 +6560,7 @@
     <col min="4" max="4" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>56</v>
       </c>
@@ -6461,7 +6574,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" s="6" t="s">
         <v>64</v>
       </c>
@@ -6478,7 +6591,7 @@
       <c r="F2" s="19"/>
       <c r="G2" s="6"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="A3" s="6" t="s">
         <v>75</v>
       </c>
@@ -6495,7 +6608,7 @@
       <c r="F3" s="19"/>
       <c r="G3" s="6"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="A4" s="6" t="s">
         <v>76</v>
       </c>
@@ -6512,7 +6625,7 @@
       <c r="F4" s="19"/>
       <c r="G4" s="6"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="A5" s="6" t="s">
         <v>74</v>
       </c>
@@ -6529,7 +6642,7 @@
       <c r="F5" s="19"/>
       <c r="G5" s="6"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" t="s">
         <v>77</v>
       </c>
@@ -6546,7 +6659,7 @@
       <c r="F6" s="19"/>
       <c r="G6" s="6"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="A7" t="s">
         <v>79</v>
       </c>
@@ -6563,7 +6676,7 @@
       <c r="F7" s="19"/>
       <c r="G7" s="6"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="A8" s="32" t="s">
         <v>95</v>
       </c>
@@ -6580,7 +6693,7 @@
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="A9" s="32" t="s">
         <v>96</v>
       </c>
@@ -6597,7 +6710,7 @@
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="A10" s="32" t="s">
         <v>97</v>
       </c>
@@ -6614,7 +6727,7 @@
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="A11" s="32" t="s">
         <v>98</v>
       </c>
@@ -6631,7 +6744,7 @@
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="A12" s="32" t="s">
         <v>99</v>
       </c>
@@ -6648,7 +6761,7 @@
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="A13" s="32" t="s">
         <v>100</v>
       </c>
@@ -6665,7 +6778,7 @@
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="A14" s="32" t="s">
         <v>101</v>
       </c>
@@ -6679,7 +6792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="A15" s="32" t="s">
         <v>102</v>
       </c>
@@ -6693,7 +6806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="A16" s="32" t="s">
         <v>103</v>
       </c>
@@ -6707,7 +6820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4" ht="15.75" customHeight="1">
       <c r="A17" s="23" t="s">
         <v>105</v>
       </c>
@@ -6721,7 +6834,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:4" ht="15.75" customHeight="1">
       <c r="A18" s="23" t="s">
         <v>109</v>
       </c>
@@ -6735,7 +6848,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:4" ht="15.75" customHeight="1">
       <c r="A19" s="23" t="s">
         <v>106</v>
       </c>
@@ -6749,7 +6862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:4" ht="15.75" customHeight="1">
       <c r="A20" s="23" t="s">
         <v>107</v>
       </c>
@@ -6763,7 +6876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:4" ht="15.75" customHeight="1">
       <c r="A21" s="23" t="s">
         <v>108</v>
       </c>
@@ -6777,7 +6890,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:4" ht="15.75" customHeight="1">
       <c r="A22" t="s">
         <v>127</v>
       </c>
@@ -6791,7 +6904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4" ht="15.75" customHeight="1">
       <c r="A23" t="s">
         <v>125</v>
       </c>
@@ -6805,7 +6918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:4" ht="15.75" customHeight="1">
       <c r="A24" t="s">
         <v>126</v>
       </c>
@@ -6823,6 +6936,11 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -6831,10 +6949,10 @@
   <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="48" customWidth="1"/>
     <col min="2" max="6" width="13.5" customWidth="1"/>
@@ -6844,7 +6962,7 @@
     <col min="10" max="10" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:13" ht="15.75" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>56</v>
       </c>
@@ -6885,7 +7003,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:13" ht="15.75" customHeight="1">
       <c r="A2" s="6" t="s">
         <v>64</v>
       </c>
@@ -6926,7 +7044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:13" ht="15.75" customHeight="1">
       <c r="A3" s="6" t="s">
         <v>75</v>
       </c>
@@ -6967,7 +7085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:13" ht="15.75" customHeight="1">
       <c r="A4" s="6" t="s">
         <v>76</v>
       </c>
@@ -7010,7 +7128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:13" ht="15.75" customHeight="1">
       <c r="A5" s="6" t="s">
         <v>74</v>
       </c>
@@ -7051,7 +7169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:13" ht="15.75" customHeight="1">
       <c r="A6" t="s">
         <v>77</v>
       </c>
@@ -7093,7 +7211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:13" ht="15.75" customHeight="1">
       <c r="A7" t="s">
         <v>79</v>
       </c>
@@ -7134,7 +7252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:13" ht="15.75" customHeight="1">
       <c r="A8" s="32" t="s">
         <v>95</v>
       </c>
@@ -7175,7 +7293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:13" ht="15.75" customHeight="1">
       <c r="A9" s="32" t="s">
         <v>96</v>
       </c>
@@ -7216,7 +7334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:13" ht="15.75" customHeight="1">
       <c r="A10" s="32" t="s">
         <v>97</v>
       </c>
@@ -7257,7 +7375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:13" ht="15.75" customHeight="1">
       <c r="A11" s="32" t="s">
         <v>98</v>
       </c>
@@ -7298,7 +7416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:13" ht="15.75" customHeight="1">
       <c r="A12" s="32" t="s">
         <v>99</v>
       </c>
@@ -7339,7 +7457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:13" ht="15.75" customHeight="1">
       <c r="A13" s="32" t="s">
         <v>100</v>
       </c>
@@ -7380,7 +7498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:13" ht="15.75" customHeight="1">
       <c r="A14" s="32" t="s">
         <v>101</v>
       </c>
@@ -7421,7 +7539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:13" ht="15.75" customHeight="1">
       <c r="A15" s="32" t="s">
         <v>102</v>
       </c>
@@ -7462,7 +7580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:13" ht="15.75" customHeight="1">
       <c r="A16" s="32" t="s">
         <v>103</v>
       </c>
@@ -7503,7 +7621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:13" ht="15.75" customHeight="1">
       <c r="A17" s="23" t="s">
         <v>105</v>
       </c>
@@ -7544,7 +7662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:13" ht="15.75" customHeight="1">
       <c r="A18" s="23" t="s">
         <v>109</v>
       </c>
@@ -7585,7 +7703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:13" ht="15.75" customHeight="1">
       <c r="A19" s="23" t="s">
         <v>106</v>
       </c>
@@ -7626,7 +7744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:13" ht="15.75" customHeight="1">
       <c r="A20" s="23" t="s">
         <v>107</v>
       </c>
@@ -7667,7 +7785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" ht="15.75" customHeight="1">
       <c r="A21" s="14" t="s">
         <v>108</v>
       </c>
@@ -7708,7 +7826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:13" ht="15.75" customHeight="1">
       <c r="A22" t="s">
         <v>127</v>
       </c>
@@ -7749,7 +7867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:13" ht="15.75" customHeight="1">
       <c r="A23" t="s">
         <v>125</v>
       </c>
@@ -7790,7 +7908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:13" ht="15.75" customHeight="1">
       <c r="A24" t="s">
         <v>126</v>
       </c>
@@ -7835,6 +7953,11 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -7846,12 +7969,12 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="33.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>56</v>
       </c>
@@ -7871,7 +7994,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" t="s">
         <v>77</v>
       </c>
@@ -7891,7 +8014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1">
       <c r="B3" t="s">
         <v>69</v>
       </c>
@@ -7910,7 +8033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1">
       <c r="A4" t="s">
         <v>79</v>
       </c>
@@ -7930,7 +8053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1">
       <c r="B5" t="s">
         <v>69</v>
       </c>
@@ -7949,6 +8072,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -7960,13 +8088,13 @@
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
     <col min="2" max="2" width="28.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:14" ht="15.75" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>68</v>
       </c>
@@ -8010,7 +8138,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:14" ht="15.75" customHeight="1">
       <c r="A2" s="6" t="s">
         <v>64</v>
       </c>
@@ -8054,7 +8182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:14" ht="15.75" customHeight="1">
       <c r="B3" s="35" t="s">
         <v>36</v>
       </c>
@@ -8095,7 +8223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:14" ht="15.75" customHeight="1">
       <c r="A4" s="32" t="s">
         <v>95</v>
       </c>
@@ -8139,7 +8267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:14" ht="15.75" customHeight="1">
       <c r="A5" s="32" t="s">
         <v>96</v>
       </c>
@@ -8183,7 +8311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:14" ht="15.75" customHeight="1">
       <c r="A6" s="32" t="s">
         <v>97</v>
       </c>
@@ -8227,7 +8355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:14" ht="15.75" customHeight="1">
       <c r="A7" s="32" t="s">
         <v>98</v>
       </c>
@@ -8271,7 +8399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:14" ht="15.75" customHeight="1">
       <c r="A8" s="32" t="s">
         <v>99</v>
       </c>
@@ -8315,7 +8443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:14" ht="15.75" customHeight="1">
       <c r="A9" s="32" t="s">
         <v>100</v>
       </c>
@@ -8359,7 +8487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:14" ht="15.75" customHeight="1">
       <c r="A10" s="32" t="s">
         <v>101</v>
       </c>
@@ -8403,7 +8531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:14" ht="15.75" customHeight="1">
       <c r="A11" s="32" t="s">
         <v>102</v>
       </c>
@@ -8447,7 +8575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:14" ht="15.75" customHeight="1">
       <c r="A12" s="32" t="s">
         <v>103</v>
       </c>
@@ -8495,6 +8623,11 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -8506,9 +8639,9 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -8546,7 +8679,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:12">
       <c r="A2">
         <v>0.5</v>
       </c>
@@ -8587,6 +8720,11 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -8598,13 +8736,13 @@
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="12.5" customWidth="1"/>
     <col min="2" max="2" width="32.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -8612,7 +8750,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1">
       <c r="A2" s="4">
         <v>2017</v>
       </c>
@@ -8620,7 +8758,7 @@
         <v>5000000</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1">
       <c r="A3" s="4">
         <v>2018</v>
       </c>
@@ -8629,7 +8767,7 @@
         <v>5050000</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1">
       <c r="A4" s="4">
         <v>2019</v>
       </c>
@@ -8638,7 +8776,7 @@
         <v>5100500</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1">
       <c r="A5" s="4">
         <v>2020</v>
       </c>
@@ -8647,7 +8785,7 @@
         <v>5151505</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1">
       <c r="A6" s="4">
         <v>2021</v>
       </c>
@@ -8656,7 +8794,7 @@
         <v>5203020.05</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1">
       <c r="A7" s="4">
         <v>2022</v>
       </c>
@@ -8665,7 +8803,7 @@
         <v>5255050.2505000001</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1">
       <c r="A8" s="4">
         <v>2023</v>
       </c>
@@ -8674,7 +8812,7 @@
         <v>5307600.7530049998</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1">
       <c r="A9" s="4">
         <v>2024</v>
       </c>
@@ -8683,7 +8821,7 @@
         <v>5360676.7605350502</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1">
       <c r="A10" s="4">
         <v>2025</v>
       </c>
@@ -8692,7 +8830,7 @@
         <v>5414283.5281404005</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1">
       <c r="A11" s="4">
         <v>2026</v>
       </c>
@@ -8701,7 +8839,7 @@
         <v>5468426.3634218043</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:2" ht="15.75" customHeight="1">
       <c r="A12" s="4">
         <v>2027</v>
       </c>
@@ -8710,7 +8848,7 @@
         <v>5523110.6270560222</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:2" ht="15.75" customHeight="1">
       <c r="A13" s="4">
         <v>2028</v>
       </c>
@@ -8719,7 +8857,7 @@
         <v>5578341.7333265822</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:2" ht="15.75" customHeight="1">
       <c r="A14" s="4">
         <v>2029</v>
       </c>
@@ -8728,7 +8866,7 @@
         <v>5634125.150659848</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:2" ht="15.75" customHeight="1">
       <c r="A15" s="4">
         <v>2030</v>
       </c>
@@ -8741,10 +8879,112 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H1" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1" t="s">
+        <v>113</v>
+      </c>
+      <c r="J1" t="s">
+        <v>114</v>
+      </c>
+      <c r="K1" t="s">
+        <v>115</v>
+      </c>
+      <c r="L1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2">
+        <v>0.5</v>
+      </c>
+      <c r="B2">
+        <v>0.5</v>
+      </c>
+      <c r="C2">
+        <v>0.5</v>
+      </c>
+      <c r="D2">
+        <v>0.5</v>
+      </c>
+      <c r="E2">
+        <v>0.5</v>
+      </c>
+      <c r="F2">
+        <v>0.5</v>
+      </c>
+      <c r="G2">
+        <v>0.5</v>
+      </c>
+      <c r="H2">
+        <v>0.5</v>
+      </c>
+      <c r="I2">
+        <v>0.5</v>
+      </c>
+      <c r="J2">
+        <v>0.5</v>
+      </c>
+      <c r="K2">
+        <v>0.5</v>
+      </c>
+      <c r="L2">
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N12"/>
   <sheetViews>
@@ -8752,13 +8992,13 @@
       <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="28.83203125" customWidth="1"/>
     <col min="2" max="2" width="27.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:14" ht="15.75" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>68</v>
       </c>
@@ -8802,7 +9042,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:14" ht="15.75" customHeight="1">
       <c r="A2" s="6" t="s">
         <v>64</v>
       </c>
@@ -8846,7 +9086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:14" ht="15.75" customHeight="1">
       <c r="B3" s="6" t="s">
         <v>36</v>
       </c>
@@ -8887,7 +9127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:14" ht="15.75" customHeight="1">
       <c r="A4" s="32" t="s">
         <v>95</v>
       </c>
@@ -8931,7 +9171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:14" ht="15.75" customHeight="1">
       <c r="A5" s="32" t="s">
         <v>96</v>
       </c>
@@ -8975,7 +9215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:14" ht="15.75" customHeight="1">
       <c r="A6" s="32" t="s">
         <v>97</v>
       </c>
@@ -9019,7 +9259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:14" ht="15.75" customHeight="1">
       <c r="A7" s="32" t="s">
         <v>98</v>
       </c>
@@ -9063,7 +9303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:14" ht="15.75" customHeight="1">
       <c r="A8" s="32" t="s">
         <v>99</v>
       </c>
@@ -9107,7 +9347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:14" ht="15.75" customHeight="1">
       <c r="A9" s="32" t="s">
         <v>100</v>
       </c>
@@ -9151,7 +9391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:14" ht="15.75" customHeight="1">
       <c r="A10" s="32" t="s">
         <v>101</v>
       </c>
@@ -9195,7 +9435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:14" ht="15.75" customHeight="1">
       <c r="A11" s="32" t="s">
         <v>102</v>
       </c>
@@ -9239,7 +9479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:14" ht="15.75" customHeight="1">
       <c r="A12" s="32" t="s">
         <v>103</v>
       </c>
@@ -9287,10 +9527,15 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
@@ -9298,12 +9543,12 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="28.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>68</v>
       </c>
@@ -9326,7 +9571,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" s="6" t="s">
         <v>64</v>
       </c>
@@ -9349,7 +9594,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="B3" s="6" t="s">
         <v>36</v>
       </c>
@@ -9369,33 +9614,38 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H35"/>
   <sheetViews>
@@ -9403,7 +9653,7 @@
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="42.5" customWidth="1"/>
     <col min="2" max="2" width="30.6640625" customWidth="1"/>
@@ -9411,7 +9661,7 @@
     <col min="5" max="5" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8">
       <c r="A1" s="35" t="s">
         <v>68</v>
       </c>
@@ -9435,7 +9685,7 @@
       </c>
       <c r="H1" s="41"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8">
       <c r="A2" s="23" t="s">
         <v>105</v>
       </c>
@@ -9459,7 +9709,7 @@
       </c>
       <c r="H2" s="41"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8">
       <c r="A3" s="41"/>
       <c r="B3" s="23" t="s">
         <v>81</v>
@@ -9481,7 +9731,7 @@
       </c>
       <c r="H3" s="41"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8">
       <c r="A4" s="37"/>
       <c r="B4" s="23" t="s">
         <v>82</v>
@@ -9503,7 +9753,7 @@
       </c>
       <c r="H4" s="41"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:8">
       <c r="A5" s="37"/>
       <c r="B5" s="23" t="s">
         <v>83</v>
@@ -9525,7 +9775,7 @@
       </c>
       <c r="H5" s="41"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:8">
       <c r="A6" s="37"/>
       <c r="B6" s="36" t="s">
         <v>87</v>
@@ -9547,7 +9797,7 @@
       </c>
       <c r="H6" s="41"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:8">
       <c r="A7" s="23" t="s">
         <v>109</v>
       </c>
@@ -9571,7 +9821,7 @@
       </c>
       <c r="H7" s="41"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:8">
       <c r="A8" s="23" t="s">
         <v>108</v>
       </c>
@@ -9595,7 +9845,7 @@
       </c>
       <c r="H8" s="41"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:8">
       <c r="A9" s="23" t="s">
         <v>106</v>
       </c>
@@ -9619,7 +9869,7 @@
       </c>
       <c r="H9" s="41"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:8">
       <c r="A10" s="23" t="s">
         <v>107</v>
       </c>
@@ -9643,7 +9893,7 @@
       </c>
       <c r="H10" s="41"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:8">
       <c r="A11" s="37"/>
       <c r="B11" s="37"/>
       <c r="C11" s="35"/>
@@ -9653,7 +9903,7 @@
       <c r="G11" s="41"/>
       <c r="H11" s="41"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:8">
       <c r="A12" s="37"/>
       <c r="C12" s="35"/>
       <c r="D12" s="35"/>
@@ -9662,7 +9912,7 @@
       <c r="G12" s="41"/>
       <c r="H12" s="41"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:8">
       <c r="A13" s="41"/>
       <c r="B13" s="41"/>
       <c r="C13" s="41"/>
@@ -9672,7 +9922,7 @@
       <c r="G13" s="41"/>
       <c r="H13" s="41"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:8">
       <c r="A14" s="41"/>
       <c r="B14" s="41"/>
       <c r="C14" s="41"/>
@@ -9682,31 +9932,31 @@
       <c r="G14" s="41"/>
       <c r="H14" s="41"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:1">
       <c r="A27" s="36"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:1">
       <c r="A28" s="37"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:1">
       <c r="A29" s="37"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:1">
       <c r="A30" s="37"/>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:1">
       <c r="A31" s="37"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:1">
       <c r="A32" s="37"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:1">
       <c r="A33" s="37"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:1">
       <c r="A34" s="37"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:1">
       <c r="A35" s="37"/>
     </row>
   </sheetData>
@@ -9714,10 +9964,15 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
@@ -9725,7 +9980,7 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="31.6640625" customWidth="1"/>
     <col min="2" max="2" width="28" customWidth="1"/>
@@ -9733,7 +9988,7 @@
     <col min="5" max="5" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7">
       <c r="A1" s="6" t="s">
         <v>68</v>
       </c>
@@ -9756,7 +10011,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7">
       <c r="A2" s="42" t="s">
         <v>105</v>
       </c>
@@ -9779,7 +10034,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7">
       <c r="B3" s="42" t="s">
         <v>81</v>
       </c>
@@ -9799,7 +10054,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7">
       <c r="A4" s="43"/>
       <c r="B4" s="42" t="s">
         <v>82</v>
@@ -9820,7 +10075,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7">
       <c r="A5" s="43"/>
       <c r="B5" s="42" t="s">
         <v>83</v>
@@ -9841,7 +10096,7 @@
         <v>0.68</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7">
       <c r="A6" s="43"/>
       <c r="B6" s="33" t="s">
         <v>87</v>
@@ -9862,7 +10117,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7">
       <c r="A7" s="42" t="s">
         <v>109</v>
       </c>
@@ -9885,7 +10140,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7">
       <c r="A8" s="42" t="s">
         <v>108</v>
       </c>
@@ -9908,7 +10163,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7">
       <c r="A9" s="42" t="s">
         <v>106</v>
       </c>
@@ -9931,7 +10186,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7">
       <c r="A10" s="42" t="s">
         <v>107</v>
       </c>
@@ -9957,6 +10212,11 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -9964,13 +10224,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2:J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" ht="15.75" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -10002,7 +10262,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:10" ht="15.75" customHeight="1">
       <c r="A2" s="7">
         <v>25.4</v>
       </c>
@@ -10038,6 +10298,11 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -10049,12 +10314,12 @@
       <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="28.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:13" ht="15.75" customHeight="1">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -10095,7 +10360,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:13" ht="15.75" customHeight="1">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -10136,7 +10401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:13" ht="15.75" customHeight="1">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -10177,7 +10442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:13" ht="15.75" customHeight="1">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -10218,7 +10483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:13" ht="15.75" customHeight="1">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -10259,7 +10524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:13" ht="15.75" customHeight="1">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -10300,7 +10565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:13" ht="15.75" customHeight="1">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -10341,7 +10606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:13" ht="15.75" customHeight="1">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -10382,7 +10647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:13" ht="15.75" customHeight="1">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -10423,7 +10688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:13" ht="15.75" customHeight="1">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -10464,7 +10729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:13" ht="15.75" customHeight="1">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -10505,7 +10770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:13" ht="15.75" customHeight="1">
       <c r="A12" t="s">
         <v>37</v>
       </c>
@@ -10546,7 +10811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:13" ht="15.75" customHeight="1">
       <c r="A13" t="s">
         <v>38</v>
       </c>
@@ -10587,7 +10852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:13" ht="15.75" customHeight="1">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -10628,7 +10893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:13" ht="15.75" customHeight="1">
       <c r="A15" t="s">
         <v>40</v>
       </c>
@@ -10669,7 +10934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:13" ht="15.75" customHeight="1">
       <c r="A16" t="s">
         <v>41</v>
       </c>
@@ -10710,7 +10975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:13" ht="15.75" customHeight="1">
       <c r="A17" t="s">
         <v>42</v>
       </c>
@@ -10751,7 +11016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:13" ht="15.75" customHeight="1">
       <c r="A18" t="s">
         <v>43</v>
       </c>
@@ -10792,7 +11057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:13" ht="15.75" customHeight="1">
       <c r="A19" s="23" t="s">
         <v>80</v>
       </c>
@@ -10833,7 +11098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:13" ht="15.75" customHeight="1">
       <c r="A20" s="23" t="s">
         <v>81</v>
       </c>
@@ -10874,7 +11139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:13" ht="15.75" customHeight="1">
       <c r="A21" s="23" t="s">
         <v>82</v>
       </c>
@@ -10915,7 +11180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:13" ht="15.75" customHeight="1">
       <c r="A22" s="23" t="s">
         <v>83</v>
       </c>
@@ -10956,7 +11221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:13" ht="15.75" customHeight="1">
       <c r="A23" s="23" t="s">
         <v>84</v>
       </c>
@@ -10997,7 +11262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:13" ht="15.75" customHeight="1">
       <c r="A24" s="23" t="s">
         <v>85</v>
       </c>
@@ -11038,7 +11303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:13" ht="15.75" customHeight="1">
       <c r="A25" s="23" t="s">
         <v>86</v>
       </c>
@@ -11079,7 +11344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:13" ht="15.75" customHeight="1">
       <c r="A26" s="23" t="s">
         <v>87</v>
       </c>
@@ -11120,7 +11385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:13" ht="15.75" customHeight="1">
       <c r="A27" s="23" t="s">
         <v>88</v>
       </c>
@@ -11161,7 +11426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:13" ht="15.75" customHeight="1">
       <c r="A28" t="s">
         <v>122</v>
       </c>
@@ -11202,7 +11467,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:13" ht="15.75" customHeight="1">
       <c r="A29" t="s">
         <v>123</v>
       </c>
@@ -11243,7 +11508,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:13" ht="15.75" customHeight="1">
       <c r="A30" t="s">
         <v>124</v>
       </c>
@@ -11292,6 +11557,11 @@
     <brk id="8" max="1048575" man="1"/>
   </colBreaks>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -11303,12 +11573,12 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>17</v>
       </c>
@@ -11334,7 +11604,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8" ht="15.75" customHeight="1">
       <c r="A2" s="6" t="s">
         <v>19</v>
       </c>
@@ -11358,7 +11628,7 @@
       </c>
       <c r="H2" s="25"/>
     </row>
-    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8" ht="15.75" customHeight="1">
       <c r="B3" s="6" t="s">
         <v>29</v>
       </c>
@@ -11379,7 +11649,7 @@
       </c>
       <c r="H3" s="25"/>
     </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8" ht="15.75" customHeight="1">
       <c r="B4" s="6" t="s">
         <v>32</v>
       </c>
@@ -11400,7 +11670,7 @@
       </c>
       <c r="H4" s="25"/>
     </row>
-    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:8" ht="15.75" customHeight="1">
       <c r="B5" s="6" t="s">
         <v>33</v>
       </c>
@@ -11421,7 +11691,7 @@
       </c>
       <c r="H5" s="25"/>
     </row>
-    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:8" ht="15.75" customHeight="1">
       <c r="A6" s="6" t="s">
         <v>35</v>
       </c>
@@ -11445,7 +11715,7 @@
       </c>
       <c r="H6" s="26"/>
     </row>
-    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:8" ht="15.75" customHeight="1">
       <c r="A7" s="6"/>
       <c r="B7" s="6" t="s">
         <v>20</v>
@@ -11467,7 +11737,7 @@
       </c>
       <c r="H7" s="26"/>
     </row>
-    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:8" ht="15.75" customHeight="1">
       <c r="B8" s="6" t="s">
         <v>29</v>
       </c>
@@ -11488,7 +11758,7 @@
       </c>
       <c r="H8" s="26"/>
     </row>
-    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:8" ht="15.75" customHeight="1">
       <c r="B9" s="6" t="s">
         <v>32</v>
       </c>
@@ -11509,7 +11779,7 @@
       </c>
       <c r="H9" s="26"/>
     </row>
-    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:8" ht="15.75" customHeight="1">
       <c r="B10" s="6" t="s">
         <v>33</v>
       </c>
@@ -11530,7 +11800,7 @@
       </c>
       <c r="H10" s="26"/>
     </row>
-    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:8" ht="15.75" customHeight="1">
       <c r="A11" s="6" t="s">
         <v>44</v>
       </c>
@@ -11554,7 +11824,7 @@
       </c>
       <c r="H11" s="27"/>
     </row>
-    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:8" ht="15.75" customHeight="1">
       <c r="B12" s="6" t="s">
         <v>46</v>
       </c>
@@ -11575,7 +11845,7 @@
       </c>
       <c r="H12" s="27"/>
     </row>
-    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:8" ht="15.75" customHeight="1">
       <c r="B13" s="6" t="s">
         <v>47</v>
       </c>
@@ -11596,7 +11866,7 @@
       </c>
       <c r="H13" s="27"/>
     </row>
-    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:8" ht="15.75" customHeight="1">
       <c r="B14" s="6" t="s">
         <v>48</v>
       </c>
@@ -11617,7 +11887,7 @@
       </c>
       <c r="H14" s="27"/>
     </row>
-    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:8" ht="15.75" customHeight="1">
       <c r="A15" t="s">
         <v>91</v>
       </c>
@@ -11633,7 +11903,7 @@
         <v>57.9</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:8" ht="15.75" customHeight="1">
       <c r="B16" s="23" t="s">
         <v>93</v>
       </c>
@@ -11646,7 +11916,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="17" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:8" ht="15.75" customHeight="1">
       <c r="B17" s="23" t="s">
         <v>94</v>
       </c>
@@ -11659,7 +11929,7 @@
         <v>18.7</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:8" ht="15.75" customHeight="1">
       <c r="B18" s="23" t="s">
         <v>89</v>
       </c>
@@ -11672,7 +11942,7 @@
         <v>11.22</v>
       </c>
     </row>
-    <row r="19" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:8" ht="15.75" customHeight="1">
       <c r="B19" s="23" t="s">
         <v>90</v>
       </c>
@@ -11690,6 +11960,11 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -11701,12 +11976,12 @@
       <selection activeCell="M54" sqref="M54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="8" max="8" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -11750,7 +12025,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>117</v>
       </c>
@@ -11794,7 +12069,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:14">
       <c r="B3" t="s">
         <v>119</v>
       </c>
@@ -11850,6 +12125,11 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -11861,9 +12141,9 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>23</v>
       </c>
@@ -11874,7 +12154,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" ht="15.75" customHeight="1">
       <c r="A2" s="6">
         <v>3.1128200000000002E-2</v>
       </c>
@@ -11887,6 +12167,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -11898,9 +12183,9 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>49</v>
       </c>
@@ -11920,7 +12205,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" s="6" t="s">
         <v>34</v>
       </c>
@@ -11940,7 +12225,7 @@
         <v>1.92</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1">
       <c r="A3" s="6" t="s">
         <v>36</v>
       </c>
@@ -11963,5 +12248,10 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added all remaining interventions for anemia, fixed some bugs, added data, changed calculation of probabilities
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Jan/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Jan/InputForCode_Bangladesh.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-36920" yWindow="-2800" windowWidth="30560" windowHeight="15640" tabRatio="500" firstSheet="27" activeTab="29"/>
+    <workbookView xWindow="-73340" yWindow="-3240" windowWidth="30680" windowHeight="16920" tabRatio="500" firstSheet="18" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="demographics" sheetId="1" r:id="rId1"/>
@@ -35,14 +35,16 @@
     <sheet name="Interventions target population" sheetId="21" r:id="rId26"/>
     <sheet name="Interventions birth outcome" sheetId="22" r:id="rId27"/>
     <sheet name="Interventions affected fraction" sheetId="23" r:id="rId28"/>
-    <sheet name="Frac anemic exposed malaria" sheetId="33" r:id="rId29"/>
-    <sheet name="Frac exposed malaria" sheetId="34" r:id="rId30"/>
-    <sheet name="Interventions mortality eff" sheetId="24" r:id="rId31"/>
-    <sheet name="Interventions incidence eff" sheetId="25" r:id="rId32"/>
-    <sheet name="Inter. pregnant women aff frac" sheetId="26" r:id="rId33"/>
-    <sheet name="Inter. pregnant women eff" sheetId="27" r:id="rId34"/>
+    <sheet name="Frac anemic not poor" sheetId="36" r:id="rId29"/>
+    <sheet name="Frac anemic poor" sheetId="35" r:id="rId30"/>
+    <sheet name="Frac anemic exposed malaria" sheetId="33" r:id="rId31"/>
+    <sheet name="Frac exposed malaria" sheetId="34" r:id="rId32"/>
+    <sheet name="Interventions mortality eff" sheetId="24" r:id="rId33"/>
+    <sheet name="Interventions incidence eff" sheetId="25" r:id="rId34"/>
+    <sheet name="Inter. pregnant women aff frac" sheetId="26" r:id="rId35"/>
+    <sheet name="Inter. pregnant women eff" sheetId="27" r:id="rId36"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -144,6 +146,28 @@
           </rPr>
           <t xml:space="preserve">
 </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+number from google</t>
         </r>
       </text>
     </comment>
@@ -269,6 +293,50 @@
         </r>
       </text>
     </comment>
+    <comment ref="G22" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+fraction exposed to malaria - take from spreadsheet value</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H23" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+taget only faction poor</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -375,6 +443,70 @@
     <author>Sam</author>
   </authors>
   <commentList>
+    <comment ref="A2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Sam:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Fictional values</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments15.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Sam</author>
+  </authors>
+  <commentList>
+    <comment ref="A2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Sam:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Fictional values</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments16.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Sam</author>
+  </authors>
+  <commentList>
     <comment ref="I2" authorId="0">
       <text>
         <r>
@@ -401,7 +533,7 @@
 </comments>
 </file>
 
-<file path=xl/comments15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments17.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Ruth</author>
@@ -477,7 +609,7 @@
 </comments>
 </file>
 
-<file path=xl/comments16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments18.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Ruth</author>
@@ -909,12 +1041,103 @@
         </r>
       </text>
     </comment>
+    <comment ref="B22" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+this should be coverage amongst those exposed to malaria
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B23" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+this is baseline coverage of only those who are poor
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B27" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+this is baseline coverage of only those who are not poor</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B30" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+amongst general population
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="139">
   <si>
     <t>indicators</t>
   </si>
@@ -1291,24 +1514,56 @@
     <t>WRA: cause3</t>
   </si>
   <si>
-    <t>Iron and folic acid for non-pregnant women</t>
-  </si>
-  <si>
-    <t>Food fortification</t>
-  </si>
-  <si>
     <t>IPTp</t>
   </si>
   <si>
     <t>Anenatal micronutrient supplementation</t>
+  </si>
+  <si>
+    <t>general population</t>
+  </si>
+  <si>
+    <t>Food fortification maize</t>
+  </si>
+  <si>
+    <t>Food fortification rice</t>
+  </si>
+  <si>
+    <t>Food fortification wheat</t>
+  </si>
+  <si>
+    <t>IFA poor: school</t>
+  </si>
+  <si>
+    <t>IFA poor: community</t>
+  </si>
+  <si>
+    <t>IFA poor: hospital</t>
+  </si>
+  <si>
+    <t>IFA not poor: school</t>
+  </si>
+  <si>
+    <t>IFA not poor: community</t>
+  </si>
+  <si>
+    <t>IFA not poor: hospital</t>
+  </si>
+  <si>
+    <t>IFA not poor: retailer</t>
+  </si>
+  <si>
+    <t>general population size</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.00000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="17" x14ac:knownFonts="1">
     <font>
@@ -1458,7 +1713,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="96">
+  <cellStyleXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1555,8 +1810,28 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1643,10 +1918,34 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="15" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="15" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="15" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="15" fillId="0" borderId="0" xfId="15" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="15" fillId="0" borderId="0" xfId="15" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="96">
+  <cellStyles count="116">
     <cellStyle name="Excel Built-in Normal" xfId="15"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -1695,6 +1994,16 @@
     <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1742,6 +2051,16 @@
     <cellStyle name="Hyperlink" xfId="90" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="92" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="94" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="96" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="98" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="100" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="102" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="104" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="106" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="108" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="110" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="112" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="114" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3106,10 +3425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -3180,6 +3499,14 @@
       </c>
       <c r="B8" s="22">
         <v>0.20599999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A9" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="B9" s="22">
+        <v>161000000</v>
       </c>
     </row>
   </sheetData>
@@ -5738,10 +6065,10 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:M1"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -5749,7 +6076,7 @@
     <col min="1" max="1" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>56</v>
       </c>
@@ -5789,10 +6116,13 @@
       <c r="M1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="2" spans="1:13">
+      <c r="N1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -5830,10 +6160,13 @@
       <c r="M2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:13">
+      <c r="N2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -5871,10 +6204,13 @@
       <c r="M3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:13">
+      <c r="N3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -5912,9 +6248,277 @@
       <c r="M4">
         <v>0.73</v>
       </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>0.73</v>
+      </c>
+      <c r="I5">
+        <v>0.73</v>
+      </c>
+      <c r="J5">
+        <v>0.73</v>
+      </c>
+      <c r="K5">
+        <v>0.73</v>
+      </c>
+      <c r="L5">
+        <v>0.73</v>
+      </c>
+      <c r="M5">
+        <v>0.73</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>0.73</v>
+      </c>
+      <c r="I6">
+        <v>0.73</v>
+      </c>
+      <c r="J6">
+        <v>0.73</v>
+      </c>
+      <c r="K6">
+        <v>0.73</v>
+      </c>
+      <c r="L6">
+        <v>0.73</v>
+      </c>
+      <c r="M6">
+        <v>0.73</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" t="s">
+        <v>134</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>0.73</v>
+      </c>
+      <c r="I7">
+        <v>0.73</v>
+      </c>
+      <c r="J7">
+        <v>0.73</v>
+      </c>
+      <c r="K7">
+        <v>0.73</v>
+      </c>
+      <c r="L7">
+        <v>0.73</v>
+      </c>
+      <c r="M7">
+        <v>0.73</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" t="s">
+        <v>135</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>0.73</v>
+      </c>
+      <c r="I8">
+        <v>0.73</v>
+      </c>
+      <c r="J8">
+        <v>0.73</v>
+      </c>
+      <c r="K8">
+        <v>0.73</v>
+      </c>
+      <c r="L8">
+        <v>0.73</v>
+      </c>
+      <c r="M8">
+        <v>0.73</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" t="s">
+        <v>136</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>0.73</v>
+      </c>
+      <c r="I9">
+        <v>0.73</v>
+      </c>
+      <c r="J9">
+        <v>0.73</v>
+      </c>
+      <c r="K9">
+        <v>0.73</v>
+      </c>
+      <c r="L9">
+        <v>0.73</v>
+      </c>
+      <c r="M9">
+        <v>0.73</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" t="s">
+        <v>137</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>0.73</v>
+      </c>
+      <c r="I10">
+        <v>0.73</v>
+      </c>
+      <c r="J10">
+        <v>0.73</v>
+      </c>
+      <c r="K10">
+        <v>0.73</v>
+      </c>
+      <c r="L10">
+        <v>0.73</v>
+      </c>
+      <c r="M10">
+        <v>0.73</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -6070,15 +6674,18 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="19.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>56</v>
       </c>
@@ -6118,10 +6725,13 @@
       <c r="M1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="2" spans="1:13">
+      <c r="N1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -6158,10 +6768,102 @@
       </c>
       <c r="M2">
         <v>1</v>
+      </c>
+      <c r="N2" s="45">
+        <v>0.97599999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3" s="45">
+        <v>0.97599999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4" s="45">
+        <v>0.97599999999999998</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -6546,10 +7248,10 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -6892,7 +7594,7 @@
     </row>
     <row r="22" spans="1:4" ht="15.75" customHeight="1">
       <c r="A22" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B22" s="6">
         <v>0</v>
@@ -6906,30 +7608,142 @@
     </row>
     <row r="23" spans="1:4" ht="15.75" customHeight="1">
       <c r="A23" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="B23" s="6">
         <v>0</v>
       </c>
       <c r="C23" s="6">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="D23" s="39">
-        <v>1</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15.75" customHeight="1">
       <c r="A24" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="B24" s="6">
         <v>0</v>
       </c>
       <c r="C24" s="6">
+        <v>0.7</v>
+      </c>
+      <c r="D24" s="39">
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A25" t="s">
+        <v>133</v>
+      </c>
+      <c r="B25" s="6">
+        <v>0</v>
+      </c>
+      <c r="C25" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="D25" s="39">
+        <v>1.78</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A26" t="s">
+        <v>134</v>
+      </c>
+      <c r="B26" s="6">
+        <v>0</v>
+      </c>
+      <c r="C26" s="6">
+        <v>1</v>
+      </c>
+      <c r="D26" s="39">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A27" t="s">
+        <v>135</v>
+      </c>
+      <c r="B27" s="6">
+        <v>0</v>
+      </c>
+      <c r="C27" s="6">
+        <v>0.49</v>
+      </c>
+      <c r="D27" s="39">
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A28" t="s">
+        <v>136</v>
+      </c>
+      <c r="B28" s="6">
+        <v>0</v>
+      </c>
+      <c r="C28" s="6">
+        <v>0.21</v>
+      </c>
+      <c r="D28" s="39">
+        <v>1.78</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A29" t="s">
+        <v>137</v>
+      </c>
+      <c r="B29" s="6">
+        <v>0</v>
+      </c>
+      <c r="C29" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="D29" s="39">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A30" t="s">
+        <v>128</v>
+      </c>
+      <c r="B30" s="6">
+        <v>0</v>
+      </c>
+      <c r="C30" s="6">
         <v>0.85</v>
       </c>
-      <c r="D24" s="39">
-        <v>1</v>
+      <c r="D30" s="39">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A31" t="s">
+        <v>129</v>
+      </c>
+      <c r="B31" s="6">
+        <v>0</v>
+      </c>
+      <c r="C31" s="6">
+        <v>0.85</v>
+      </c>
+      <c r="D31" s="39">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A32" t="s">
+        <v>130</v>
+      </c>
+      <c r="B32" s="6">
+        <v>0</v>
+      </c>
+      <c r="C32" s="6">
+        <v>0.85</v>
+      </c>
+      <c r="D32" s="39">
+        <v>0.18</v>
       </c>
     </row>
   </sheetData>
@@ -6946,10 +7760,10 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -6962,7 +7776,7 @@
     <col min="10" max="10" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" customHeight="1">
+    <row r="1" spans="1:14" ht="15.75" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>56</v>
       </c>
@@ -7002,950 +7816,1417 @@
       <c r="M1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" ht="15.75" customHeight="1">
+      <c r="N1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="15.75" customHeight="1">
       <c r="A2" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="4">
-        <v>0</v>
-      </c>
-      <c r="C2" s="4">
-        <v>0</v>
-      </c>
-      <c r="D2" s="4">
-        <v>1</v>
-      </c>
-      <c r="E2" s="4">
-        <v>1</v>
-      </c>
-      <c r="F2" s="4">
-        <v>1</v>
-      </c>
-      <c r="G2" s="4">
-        <v>0</v>
-      </c>
-      <c r="H2" s="4">
-        <v>0</v>
-      </c>
-      <c r="I2" s="4">
-        <v>0</v>
-      </c>
-      <c r="J2" s="4">
-        <v>0</v>
-      </c>
-      <c r="K2" s="4">
-        <v>0</v>
-      </c>
-      <c r="L2" s="4">
-        <v>0</v>
-      </c>
-      <c r="M2" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="15.75" customHeight="1">
+      <c r="B2" s="47">
+        <v>0</v>
+      </c>
+      <c r="C2" s="47">
+        <v>0</v>
+      </c>
+      <c r="D2" s="47">
+        <v>1</v>
+      </c>
+      <c r="E2" s="47">
+        <v>1</v>
+      </c>
+      <c r="F2" s="47">
+        <v>1</v>
+      </c>
+      <c r="G2" s="47">
+        <v>0</v>
+      </c>
+      <c r="H2" s="47">
+        <v>0</v>
+      </c>
+      <c r="I2" s="47">
+        <v>0</v>
+      </c>
+      <c r="J2" s="47">
+        <v>0</v>
+      </c>
+      <c r="K2" s="47">
+        <v>0</v>
+      </c>
+      <c r="L2" s="47">
+        <v>0</v>
+      </c>
+      <c r="M2" s="47">
+        <v>0</v>
+      </c>
+      <c r="N2" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="15.75" customHeight="1">
       <c r="A3" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="B3" s="4">
-        <v>0</v>
-      </c>
-      <c r="C3" s="4">
-        <v>0</v>
-      </c>
-      <c r="D3" s="4">
-        <v>1</v>
-      </c>
-      <c r="E3" s="4">
-        <v>1</v>
-      </c>
-      <c r="F3" s="4">
-        <v>0</v>
-      </c>
-      <c r="G3" s="4">
-        <v>0</v>
-      </c>
-      <c r="H3" s="4">
-        <v>0</v>
-      </c>
-      <c r="I3" s="4">
-        <v>0</v>
-      </c>
-      <c r="J3" s="4">
-        <v>0</v>
-      </c>
-      <c r="K3" s="4">
-        <v>0</v>
-      </c>
-      <c r="L3" s="4">
-        <v>0</v>
-      </c>
-      <c r="M3" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="15.75" customHeight="1">
+      <c r="B3" s="47">
+        <v>0</v>
+      </c>
+      <c r="C3" s="47">
+        <v>0</v>
+      </c>
+      <c r="D3" s="47">
+        <v>1</v>
+      </c>
+      <c r="E3" s="47">
+        <v>1</v>
+      </c>
+      <c r="F3" s="47">
+        <v>0</v>
+      </c>
+      <c r="G3" s="47">
+        <v>0</v>
+      </c>
+      <c r="H3" s="47">
+        <v>0</v>
+      </c>
+      <c r="I3" s="47">
+        <v>0</v>
+      </c>
+      <c r="J3" s="47">
+        <v>0</v>
+      </c>
+      <c r="K3" s="47">
+        <v>0</v>
+      </c>
+      <c r="L3" s="47">
+        <v>0</v>
+      </c>
+      <c r="M3" s="47">
+        <v>0</v>
+      </c>
+      <c r="N3" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="15.75" customHeight="1">
       <c r="A4" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="B4" s="4">
-        <v>0</v>
-      </c>
-      <c r="C4" s="4">
-        <v>0</v>
-      </c>
-      <c r="D4" s="4">
+      <c r="B4" s="47">
+        <v>0</v>
+      </c>
+      <c r="C4" s="47">
+        <v>0</v>
+      </c>
+      <c r="D4" s="46">
         <f>demographics!$B$7</f>
         <v>0.4</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="46">
         <f>demographics!$B$7</f>
         <v>0.4</v>
       </c>
-      <c r="F4" s="4">
-        <v>0</v>
-      </c>
-      <c r="G4" s="4">
-        <v>0</v>
-      </c>
-      <c r="H4" s="4">
-        <v>0</v>
-      </c>
-      <c r="I4" s="4">
-        <v>0</v>
-      </c>
-      <c r="J4" s="4">
-        <v>0</v>
-      </c>
-      <c r="K4" s="4">
-        <v>0</v>
-      </c>
-      <c r="L4" s="4">
-        <v>0</v>
-      </c>
-      <c r="M4" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="15.75" customHeight="1">
+      <c r="F4" s="47">
+        <v>0</v>
+      </c>
+      <c r="G4" s="47">
+        <v>0</v>
+      </c>
+      <c r="H4" s="47">
+        <v>0</v>
+      </c>
+      <c r="I4" s="47">
+        <v>0</v>
+      </c>
+      <c r="J4" s="47">
+        <v>0</v>
+      </c>
+      <c r="K4" s="47">
+        <v>0</v>
+      </c>
+      <c r="L4" s="47">
+        <v>0</v>
+      </c>
+      <c r="M4" s="47">
+        <v>0</v>
+      </c>
+      <c r="N4" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="15.75" customHeight="1">
       <c r="A5" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="B5" s="4">
-        <v>1</v>
-      </c>
-      <c r="C5" s="4">
-        <v>1</v>
-      </c>
-      <c r="D5" s="4">
-        <v>0</v>
-      </c>
-      <c r="E5" s="4">
-        <v>0</v>
-      </c>
-      <c r="F5" s="4">
-        <v>0</v>
-      </c>
-      <c r="G5" s="4">
-        <v>1</v>
-      </c>
-      <c r="H5" s="4">
-        <v>0</v>
-      </c>
-      <c r="I5" s="4">
-        <v>0</v>
-      </c>
-      <c r="J5" s="4">
-        <v>0</v>
-      </c>
-      <c r="K5" s="4">
-        <v>0</v>
-      </c>
-      <c r="L5" s="4">
-        <v>0</v>
-      </c>
-      <c r="M5" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="15.75" customHeight="1">
+      <c r="B5" s="47">
+        <v>1</v>
+      </c>
+      <c r="C5" s="47">
+        <v>1</v>
+      </c>
+      <c r="D5" s="47">
+        <v>0</v>
+      </c>
+      <c r="E5" s="47">
+        <v>0</v>
+      </c>
+      <c r="F5" s="47">
+        <v>0</v>
+      </c>
+      <c r="G5" s="47">
+        <v>1</v>
+      </c>
+      <c r="H5" s="47">
+        <v>0</v>
+      </c>
+      <c r="I5" s="47">
+        <v>0</v>
+      </c>
+      <c r="J5" s="47">
+        <v>0</v>
+      </c>
+      <c r="K5" s="47">
+        <v>0</v>
+      </c>
+      <c r="L5" s="47">
+        <v>0</v>
+      </c>
+      <c r="M5" s="47">
+        <v>0</v>
+      </c>
+      <c r="N5" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="15.75" customHeight="1">
       <c r="A6" t="s">
         <v>77</v>
       </c>
-      <c r="B6" s="4">
-        <v>0</v>
-      </c>
-      <c r="C6" s="4">
-        <v>0</v>
-      </c>
-      <c r="D6" s="4">
-        <v>0</v>
-      </c>
-      <c r="E6" s="4">
-        <v>0</v>
-      </c>
-      <c r="F6" s="4">
-        <v>0</v>
-      </c>
-      <c r="G6" s="4">
+      <c r="B6" s="47">
+        <v>0</v>
+      </c>
+      <c r="C6" s="47">
+        <v>0</v>
+      </c>
+      <c r="D6" s="47">
+        <v>0</v>
+      </c>
+      <c r="E6" s="47">
+        <v>0</v>
+      </c>
+      <c r="F6" s="47">
+        <v>0</v>
+      </c>
+      <c r="G6" s="46">
         <f>demographics!$B$7</f>
         <v>0.4</v>
       </c>
-      <c r="H6" s="4">
-        <v>0</v>
-      </c>
-      <c r="I6" s="4">
-        <v>0</v>
-      </c>
-      <c r="J6" s="4">
-        <v>0</v>
-      </c>
-      <c r="K6" s="4">
-        <v>0</v>
-      </c>
-      <c r="L6" s="4">
-        <v>0</v>
-      </c>
-      <c r="M6" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="15.75" customHeight="1">
+      <c r="H6" s="47">
+        <v>0</v>
+      </c>
+      <c r="I6" s="47">
+        <v>0</v>
+      </c>
+      <c r="J6" s="47">
+        <v>0</v>
+      </c>
+      <c r="K6" s="47">
+        <v>0</v>
+      </c>
+      <c r="L6" s="47">
+        <v>0</v>
+      </c>
+      <c r="M6" s="47">
+        <v>0</v>
+      </c>
+      <c r="N6" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="15.75" customHeight="1">
       <c r="A7" t="s">
         <v>79</v>
       </c>
-      <c r="B7" s="4">
-        <v>0</v>
-      </c>
-      <c r="C7" s="4">
-        <v>0</v>
-      </c>
-      <c r="D7" s="4">
-        <v>0</v>
-      </c>
-      <c r="E7" s="4">
-        <v>0</v>
-      </c>
-      <c r="F7" s="4">
-        <v>0</v>
-      </c>
-      <c r="G7" s="4">
-        <v>1</v>
-      </c>
-      <c r="H7" s="4">
-        <v>0</v>
-      </c>
-      <c r="I7" s="4">
-        <v>0</v>
-      </c>
-      <c r="J7" s="4">
-        <v>0</v>
-      </c>
-      <c r="K7" s="4">
-        <v>0</v>
-      </c>
-      <c r="L7" s="4">
-        <v>0</v>
-      </c>
-      <c r="M7" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="15.75" customHeight="1">
+      <c r="B7" s="47">
+        <v>0</v>
+      </c>
+      <c r="C7" s="47">
+        <v>0</v>
+      </c>
+      <c r="D7" s="47">
+        <v>0</v>
+      </c>
+      <c r="E7" s="47">
+        <v>0</v>
+      </c>
+      <c r="F7" s="47">
+        <v>0</v>
+      </c>
+      <c r="G7" s="47">
+        <v>1</v>
+      </c>
+      <c r="H7" s="47">
+        <v>0</v>
+      </c>
+      <c r="I7" s="47">
+        <v>0</v>
+      </c>
+      <c r="J7" s="47">
+        <v>0</v>
+      </c>
+      <c r="K7" s="47">
+        <v>0</v>
+      </c>
+      <c r="L7" s="47">
+        <v>0</v>
+      </c>
+      <c r="M7" s="47">
+        <v>0</v>
+      </c>
+      <c r="N7" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="15.75" customHeight="1">
       <c r="A8" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="B8" s="33">
-        <v>0</v>
-      </c>
-      <c r="C8" s="33">
-        <v>0</v>
-      </c>
-      <c r="D8" s="33">
-        <v>0</v>
-      </c>
-      <c r="E8" s="33">
-        <v>0</v>
-      </c>
-      <c r="F8" s="33">
-        <v>0</v>
-      </c>
-      <c r="G8" s="33">
-        <v>1</v>
-      </c>
-      <c r="H8" s="4">
-        <v>0</v>
-      </c>
-      <c r="I8" s="4">
-        <v>0</v>
-      </c>
-      <c r="J8" s="4">
-        <v>0</v>
-      </c>
-      <c r="K8" s="4">
-        <v>0</v>
-      </c>
-      <c r="L8" s="4">
-        <v>0</v>
-      </c>
-      <c r="M8" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="15.75" customHeight="1">
+      <c r="B8" s="49">
+        <v>0</v>
+      </c>
+      <c r="C8" s="49">
+        <v>0</v>
+      </c>
+      <c r="D8" s="49">
+        <v>0</v>
+      </c>
+      <c r="E8" s="49">
+        <v>0</v>
+      </c>
+      <c r="F8" s="49">
+        <v>0</v>
+      </c>
+      <c r="G8" s="49">
+        <v>1</v>
+      </c>
+      <c r="H8" s="47">
+        <v>0</v>
+      </c>
+      <c r="I8" s="47">
+        <v>0</v>
+      </c>
+      <c r="J8" s="47">
+        <v>0</v>
+      </c>
+      <c r="K8" s="47">
+        <v>0</v>
+      </c>
+      <c r="L8" s="47">
+        <v>0</v>
+      </c>
+      <c r="M8" s="47">
+        <v>0</v>
+      </c>
+      <c r="N8" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="15.75" customHeight="1">
       <c r="A9" s="32" t="s">
         <v>96</v>
       </c>
-      <c r="B9" s="33">
-        <v>0</v>
-      </c>
-      <c r="C9" s="33">
-        <v>0</v>
-      </c>
-      <c r="D9" s="33">
-        <v>0</v>
-      </c>
-      <c r="E9" s="33">
-        <v>0</v>
-      </c>
-      <c r="F9" s="33">
-        <v>0</v>
-      </c>
-      <c r="G9" s="33">
-        <v>1</v>
-      </c>
-      <c r="H9" s="4">
-        <v>0</v>
-      </c>
-      <c r="I9" s="4">
-        <v>0</v>
-      </c>
-      <c r="J9" s="4">
-        <v>0</v>
-      </c>
-      <c r="K9" s="4">
-        <v>0</v>
-      </c>
-      <c r="L9" s="4">
-        <v>0</v>
-      </c>
-      <c r="M9" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="15.75" customHeight="1">
+      <c r="B9" s="49">
+        <v>0</v>
+      </c>
+      <c r="C9" s="49">
+        <v>0</v>
+      </c>
+      <c r="D9" s="49">
+        <v>0</v>
+      </c>
+      <c r="E9" s="49">
+        <v>0</v>
+      </c>
+      <c r="F9" s="49">
+        <v>0</v>
+      </c>
+      <c r="G9" s="49">
+        <v>1</v>
+      </c>
+      <c r="H9" s="47">
+        <v>0</v>
+      </c>
+      <c r="I9" s="47">
+        <v>0</v>
+      </c>
+      <c r="J9" s="47">
+        <v>0</v>
+      </c>
+      <c r="K9" s="47">
+        <v>0</v>
+      </c>
+      <c r="L9" s="47">
+        <v>0</v>
+      </c>
+      <c r="M9" s="47">
+        <v>0</v>
+      </c>
+      <c r="N9" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="15.75" customHeight="1">
       <c r="A10" s="32" t="s">
         <v>97</v>
       </c>
-      <c r="B10" s="33">
-        <v>0</v>
-      </c>
-      <c r="C10" s="33">
-        <v>0</v>
-      </c>
-      <c r="D10" s="33">
-        <v>0</v>
-      </c>
-      <c r="E10" s="33">
-        <v>0</v>
-      </c>
-      <c r="F10" s="33">
-        <v>0</v>
-      </c>
-      <c r="G10" s="33">
-        <v>1</v>
-      </c>
-      <c r="H10" s="4">
-        <v>0</v>
-      </c>
-      <c r="I10" s="4">
-        <v>0</v>
-      </c>
-      <c r="J10" s="4">
-        <v>0</v>
-      </c>
-      <c r="K10" s="4">
-        <v>0</v>
-      </c>
-      <c r="L10" s="4">
-        <v>0</v>
-      </c>
-      <c r="M10" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="15.75" customHeight="1">
+      <c r="B10" s="49">
+        <v>0</v>
+      </c>
+      <c r="C10" s="49">
+        <v>0</v>
+      </c>
+      <c r="D10" s="49">
+        <v>0</v>
+      </c>
+      <c r="E10" s="49">
+        <v>0</v>
+      </c>
+      <c r="F10" s="49">
+        <v>0</v>
+      </c>
+      <c r="G10" s="49">
+        <v>1</v>
+      </c>
+      <c r="H10" s="47">
+        <v>0</v>
+      </c>
+      <c r="I10" s="47">
+        <v>0</v>
+      </c>
+      <c r="J10" s="47">
+        <v>0</v>
+      </c>
+      <c r="K10" s="47">
+        <v>0</v>
+      </c>
+      <c r="L10" s="47">
+        <v>0</v>
+      </c>
+      <c r="M10" s="47">
+        <v>0</v>
+      </c>
+      <c r="N10" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="15.75" customHeight="1">
       <c r="A11" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="B11" s="33">
-        <v>0</v>
-      </c>
-      <c r="C11" s="33">
-        <v>0</v>
-      </c>
-      <c r="D11" s="33">
-        <v>0</v>
-      </c>
-      <c r="E11" s="33">
-        <v>0</v>
-      </c>
-      <c r="F11" s="33">
-        <v>0</v>
-      </c>
-      <c r="G11" s="33">
-        <v>1</v>
-      </c>
-      <c r="H11" s="4">
-        <v>0</v>
-      </c>
-      <c r="I11" s="4">
-        <v>0</v>
-      </c>
-      <c r="J11" s="4">
-        <v>0</v>
-      </c>
-      <c r="K11" s="4">
-        <v>0</v>
-      </c>
-      <c r="L11" s="4">
-        <v>0</v>
-      </c>
-      <c r="M11" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="15.75" customHeight="1">
+      <c r="B11" s="49">
+        <v>0</v>
+      </c>
+      <c r="C11" s="49">
+        <v>0</v>
+      </c>
+      <c r="D11" s="49">
+        <v>0</v>
+      </c>
+      <c r="E11" s="49">
+        <v>0</v>
+      </c>
+      <c r="F11" s="49">
+        <v>0</v>
+      </c>
+      <c r="G11" s="49">
+        <v>1</v>
+      </c>
+      <c r="H11" s="47">
+        <v>0</v>
+      </c>
+      <c r="I11" s="47">
+        <v>0</v>
+      </c>
+      <c r="J11" s="47">
+        <v>0</v>
+      </c>
+      <c r="K11" s="47">
+        <v>0</v>
+      </c>
+      <c r="L11" s="47">
+        <v>0</v>
+      </c>
+      <c r="M11" s="47">
+        <v>0</v>
+      </c>
+      <c r="N11" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="15.75" customHeight="1">
       <c r="A12" s="32" t="s">
         <v>99</v>
       </c>
-      <c r="B12" s="33">
-        <v>0</v>
-      </c>
-      <c r="C12" s="33">
-        <v>0</v>
-      </c>
-      <c r="D12" s="33">
-        <v>0</v>
-      </c>
-      <c r="E12" s="33">
-        <v>0</v>
-      </c>
-      <c r="F12" s="33">
-        <v>0</v>
-      </c>
-      <c r="G12" s="33">
-        <v>1</v>
-      </c>
-      <c r="H12" s="4">
-        <v>0</v>
-      </c>
-      <c r="I12" s="4">
-        <v>0</v>
-      </c>
-      <c r="J12" s="4">
-        <v>0</v>
-      </c>
-      <c r="K12" s="4">
-        <v>0</v>
-      </c>
-      <c r="L12" s="4">
-        <v>0</v>
-      </c>
-      <c r="M12" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="15.75" customHeight="1">
+      <c r="B12" s="49">
+        <v>0</v>
+      </c>
+      <c r="C12" s="49">
+        <v>0</v>
+      </c>
+      <c r="D12" s="49">
+        <v>0</v>
+      </c>
+      <c r="E12" s="49">
+        <v>0</v>
+      </c>
+      <c r="F12" s="49">
+        <v>0</v>
+      </c>
+      <c r="G12" s="49">
+        <v>1</v>
+      </c>
+      <c r="H12" s="47">
+        <v>0</v>
+      </c>
+      <c r="I12" s="47">
+        <v>0</v>
+      </c>
+      <c r="J12" s="47">
+        <v>0</v>
+      </c>
+      <c r="K12" s="47">
+        <v>0</v>
+      </c>
+      <c r="L12" s="47">
+        <v>0</v>
+      </c>
+      <c r="M12" s="47">
+        <v>0</v>
+      </c>
+      <c r="N12" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="15.75" customHeight="1">
       <c r="A13" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="B13" s="33">
-        <v>0</v>
-      </c>
-      <c r="C13" s="33">
-        <v>0</v>
-      </c>
-      <c r="D13" s="33">
-        <v>0</v>
-      </c>
-      <c r="E13" s="33">
-        <v>0</v>
-      </c>
-      <c r="F13" s="33">
-        <v>0</v>
-      </c>
-      <c r="G13" s="33">
-        <v>1</v>
-      </c>
-      <c r="H13" s="4">
-        <v>0</v>
-      </c>
-      <c r="I13" s="4">
-        <v>0</v>
-      </c>
-      <c r="J13" s="4">
-        <v>0</v>
-      </c>
-      <c r="K13" s="4">
-        <v>0</v>
-      </c>
-      <c r="L13" s="4">
-        <v>0</v>
-      </c>
-      <c r="M13" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="15.75" customHeight="1">
+      <c r="B13" s="49">
+        <v>0</v>
+      </c>
+      <c r="C13" s="49">
+        <v>0</v>
+      </c>
+      <c r="D13" s="49">
+        <v>0</v>
+      </c>
+      <c r="E13" s="49">
+        <v>0</v>
+      </c>
+      <c r="F13" s="49">
+        <v>0</v>
+      </c>
+      <c r="G13" s="49">
+        <v>1</v>
+      </c>
+      <c r="H13" s="47">
+        <v>0</v>
+      </c>
+      <c r="I13" s="47">
+        <v>0</v>
+      </c>
+      <c r="J13" s="47">
+        <v>0</v>
+      </c>
+      <c r="K13" s="47">
+        <v>0</v>
+      </c>
+      <c r="L13" s="47">
+        <v>0</v>
+      </c>
+      <c r="M13" s="47">
+        <v>0</v>
+      </c>
+      <c r="N13" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="15.75" customHeight="1">
       <c r="A14" s="32" t="s">
         <v>101</v>
       </c>
-      <c r="B14" s="33">
-        <v>0</v>
-      </c>
-      <c r="C14" s="33">
-        <v>0</v>
-      </c>
-      <c r="D14" s="33">
-        <v>0</v>
-      </c>
-      <c r="E14" s="33">
-        <v>0</v>
-      </c>
-      <c r="F14" s="33">
-        <v>0</v>
-      </c>
-      <c r="G14" s="32">
-        <v>1</v>
-      </c>
-      <c r="H14" s="4">
-        <v>0</v>
-      </c>
-      <c r="I14" s="4">
-        <v>0</v>
-      </c>
-      <c r="J14" s="4">
-        <v>0</v>
-      </c>
-      <c r="K14" s="4">
-        <v>0</v>
-      </c>
-      <c r="L14" s="4">
-        <v>0</v>
-      </c>
-      <c r="M14" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="15.75" customHeight="1">
+      <c r="B14" s="49">
+        <v>0</v>
+      </c>
+      <c r="C14" s="49">
+        <v>0</v>
+      </c>
+      <c r="D14" s="49">
+        <v>0</v>
+      </c>
+      <c r="E14" s="49">
+        <v>0</v>
+      </c>
+      <c r="F14" s="49">
+        <v>0</v>
+      </c>
+      <c r="G14" s="50">
+        <v>1</v>
+      </c>
+      <c r="H14" s="47">
+        <v>0</v>
+      </c>
+      <c r="I14" s="47">
+        <v>0</v>
+      </c>
+      <c r="J14" s="47">
+        <v>0</v>
+      </c>
+      <c r="K14" s="47">
+        <v>0</v>
+      </c>
+      <c r="L14" s="47">
+        <v>0</v>
+      </c>
+      <c r="M14" s="47">
+        <v>0</v>
+      </c>
+      <c r="N14" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="15.75" customHeight="1">
       <c r="A15" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="B15" s="33">
-        <v>0</v>
-      </c>
-      <c r="C15" s="33">
-        <v>0</v>
-      </c>
-      <c r="D15" s="33">
-        <v>0</v>
-      </c>
-      <c r="E15" s="33">
-        <v>0</v>
-      </c>
-      <c r="F15" s="33">
-        <v>0</v>
-      </c>
-      <c r="G15" s="32">
-        <v>1</v>
-      </c>
-      <c r="H15" s="4">
-        <v>0</v>
-      </c>
-      <c r="I15" s="4">
-        <v>0</v>
-      </c>
-      <c r="J15" s="4">
-        <v>0</v>
-      </c>
-      <c r="K15" s="4">
-        <v>0</v>
-      </c>
-      <c r="L15" s="4">
-        <v>0</v>
-      </c>
-      <c r="M15" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="15.75" customHeight="1">
+      <c r="B15" s="49">
+        <v>0</v>
+      </c>
+      <c r="C15" s="49">
+        <v>0</v>
+      </c>
+      <c r="D15" s="49">
+        <v>0</v>
+      </c>
+      <c r="E15" s="49">
+        <v>0</v>
+      </c>
+      <c r="F15" s="49">
+        <v>0</v>
+      </c>
+      <c r="G15" s="50">
+        <v>1</v>
+      </c>
+      <c r="H15" s="47">
+        <v>0</v>
+      </c>
+      <c r="I15" s="47">
+        <v>0</v>
+      </c>
+      <c r="J15" s="47">
+        <v>0</v>
+      </c>
+      <c r="K15" s="47">
+        <v>0</v>
+      </c>
+      <c r="L15" s="47">
+        <v>0</v>
+      </c>
+      <c r="M15" s="47">
+        <v>0</v>
+      </c>
+      <c r="N15" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="15.75" customHeight="1">
       <c r="A16" s="32" t="s">
         <v>103</v>
       </c>
-      <c r="B16" s="33">
-        <v>0</v>
-      </c>
-      <c r="C16" s="33">
-        <v>0</v>
-      </c>
-      <c r="D16" s="33">
-        <v>0</v>
-      </c>
-      <c r="E16" s="33">
-        <v>0</v>
-      </c>
-      <c r="F16" s="33">
-        <v>0</v>
-      </c>
-      <c r="G16" s="32">
-        <v>1</v>
-      </c>
-      <c r="H16" s="4">
-        <v>0</v>
-      </c>
-      <c r="I16" s="4">
-        <v>0</v>
-      </c>
-      <c r="J16" s="4">
-        <v>0</v>
-      </c>
-      <c r="K16" s="4">
-        <v>0</v>
-      </c>
-      <c r="L16" s="4">
-        <v>0</v>
-      </c>
-      <c r="M16" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="15.75" customHeight="1">
+      <c r="B16" s="49">
+        <v>0</v>
+      </c>
+      <c r="C16" s="49">
+        <v>0</v>
+      </c>
+      <c r="D16" s="49">
+        <v>0</v>
+      </c>
+      <c r="E16" s="49">
+        <v>0</v>
+      </c>
+      <c r="F16" s="49">
+        <v>0</v>
+      </c>
+      <c r="G16" s="50">
+        <v>1</v>
+      </c>
+      <c r="H16" s="47">
+        <v>0</v>
+      </c>
+      <c r="I16" s="47">
+        <v>0</v>
+      </c>
+      <c r="J16" s="47">
+        <v>0</v>
+      </c>
+      <c r="K16" s="47">
+        <v>0</v>
+      </c>
+      <c r="L16" s="47">
+        <v>0</v>
+      </c>
+      <c r="M16" s="47">
+        <v>0</v>
+      </c>
+      <c r="N16" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="15.75" customHeight="1">
       <c r="A17" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="B17" s="33">
-        <v>0</v>
-      </c>
-      <c r="C17" s="33">
-        <v>0</v>
-      </c>
-      <c r="D17" s="33">
-        <v>0</v>
-      </c>
-      <c r="E17" s="33">
-        <v>0</v>
-      </c>
-      <c r="F17" s="33">
-        <v>0</v>
-      </c>
-      <c r="G17" s="33">
-        <v>1</v>
-      </c>
-      <c r="H17" s="4">
-        <v>0</v>
-      </c>
-      <c r="I17" s="4">
-        <v>0</v>
-      </c>
-      <c r="J17" s="4">
-        <v>0</v>
-      </c>
-      <c r="K17" s="4">
-        <v>0</v>
-      </c>
-      <c r="L17" s="4">
-        <v>0</v>
-      </c>
-      <c r="M17" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="15.75" customHeight="1">
+      <c r="B17" s="49">
+        <v>0</v>
+      </c>
+      <c r="C17" s="49">
+        <v>0</v>
+      </c>
+      <c r="D17" s="49">
+        <v>0</v>
+      </c>
+      <c r="E17" s="49">
+        <v>0</v>
+      </c>
+      <c r="F17" s="49">
+        <v>0</v>
+      </c>
+      <c r="G17" s="49">
+        <v>1</v>
+      </c>
+      <c r="H17" s="47">
+        <v>0</v>
+      </c>
+      <c r="I17" s="47">
+        <v>0</v>
+      </c>
+      <c r="J17" s="47">
+        <v>0</v>
+      </c>
+      <c r="K17" s="47">
+        <v>0</v>
+      </c>
+      <c r="L17" s="47">
+        <v>0</v>
+      </c>
+      <c r="M17" s="47">
+        <v>0</v>
+      </c>
+      <c r="N17" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="15.75" customHeight="1">
       <c r="A18" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="B18" s="33">
-        <v>0</v>
-      </c>
-      <c r="C18" s="33">
-        <v>0</v>
-      </c>
-      <c r="D18" s="33">
-        <v>0</v>
-      </c>
-      <c r="E18" s="33">
-        <v>0</v>
-      </c>
-      <c r="F18" s="33">
-        <v>0</v>
-      </c>
-      <c r="G18" s="32">
-        <v>1</v>
-      </c>
-      <c r="H18" s="4">
-        <v>0</v>
-      </c>
-      <c r="I18" s="4">
-        <v>0</v>
-      </c>
-      <c r="J18" s="4">
-        <v>0</v>
-      </c>
-      <c r="K18" s="4">
-        <v>0</v>
-      </c>
-      <c r="L18" s="4">
-        <v>0</v>
-      </c>
-      <c r="M18" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" ht="15.75" customHeight="1">
+      <c r="B18" s="49">
+        <v>0</v>
+      </c>
+      <c r="C18" s="49">
+        <v>0</v>
+      </c>
+      <c r="D18" s="49">
+        <v>0</v>
+      </c>
+      <c r="E18" s="49">
+        <v>0</v>
+      </c>
+      <c r="F18" s="49">
+        <v>0</v>
+      </c>
+      <c r="G18" s="50">
+        <v>1</v>
+      </c>
+      <c r="H18" s="47">
+        <v>0</v>
+      </c>
+      <c r="I18" s="47">
+        <v>0</v>
+      </c>
+      <c r="J18" s="47">
+        <v>0</v>
+      </c>
+      <c r="K18" s="47">
+        <v>0</v>
+      </c>
+      <c r="L18" s="47">
+        <v>0</v>
+      </c>
+      <c r="M18" s="47">
+        <v>0</v>
+      </c>
+      <c r="N18" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="15.75" customHeight="1">
       <c r="A19" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="B19" s="33">
-        <v>0</v>
-      </c>
-      <c r="C19" s="33">
-        <v>0</v>
-      </c>
-      <c r="D19" s="33">
-        <v>0</v>
-      </c>
-      <c r="E19" s="33">
-        <v>0</v>
-      </c>
-      <c r="F19" s="33">
-        <v>0</v>
-      </c>
-      <c r="G19" s="32">
-        <v>1</v>
-      </c>
-      <c r="H19" s="4">
-        <v>0</v>
-      </c>
-      <c r="I19" s="4">
-        <v>0</v>
-      </c>
-      <c r="J19" s="4">
-        <v>0</v>
-      </c>
-      <c r="K19" s="4">
-        <v>0</v>
-      </c>
-      <c r="L19" s="4">
-        <v>0</v>
-      </c>
-      <c r="M19" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" ht="15.75" customHeight="1">
+      <c r="B19" s="49">
+        <v>0</v>
+      </c>
+      <c r="C19" s="49">
+        <v>0</v>
+      </c>
+      <c r="D19" s="49">
+        <v>0</v>
+      </c>
+      <c r="E19" s="49">
+        <v>0</v>
+      </c>
+      <c r="F19" s="49">
+        <v>0</v>
+      </c>
+      <c r="G19" s="50">
+        <v>1</v>
+      </c>
+      <c r="H19" s="47">
+        <v>0</v>
+      </c>
+      <c r="I19" s="47">
+        <v>0</v>
+      </c>
+      <c r="J19" s="47">
+        <v>0</v>
+      </c>
+      <c r="K19" s="47">
+        <v>0</v>
+      </c>
+      <c r="L19" s="47">
+        <v>0</v>
+      </c>
+      <c r="M19" s="47">
+        <v>0</v>
+      </c>
+      <c r="N19" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="15.75" customHeight="1">
       <c r="A20" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="B20" s="33">
-        <v>0</v>
-      </c>
-      <c r="C20" s="33">
-        <v>0</v>
-      </c>
-      <c r="D20" s="33">
-        <v>0</v>
-      </c>
-      <c r="E20" s="33">
-        <v>0</v>
-      </c>
-      <c r="F20" s="33">
-        <v>0</v>
-      </c>
-      <c r="G20" s="32">
-        <v>1</v>
-      </c>
-      <c r="H20" s="4">
-        <v>0</v>
-      </c>
-      <c r="I20" s="4">
-        <v>0</v>
-      </c>
-      <c r="J20" s="4">
-        <v>0</v>
-      </c>
-      <c r="K20" s="4">
-        <v>0</v>
-      </c>
-      <c r="L20" s="4">
-        <v>0</v>
-      </c>
-      <c r="M20" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" ht="15.75" customHeight="1">
+      <c r="B20" s="49">
+        <v>0</v>
+      </c>
+      <c r="C20" s="49">
+        <v>0</v>
+      </c>
+      <c r="D20" s="49">
+        <v>0</v>
+      </c>
+      <c r="E20" s="49">
+        <v>0</v>
+      </c>
+      <c r="F20" s="49">
+        <v>0</v>
+      </c>
+      <c r="G20" s="50">
+        <v>1</v>
+      </c>
+      <c r="H20" s="47">
+        <v>0</v>
+      </c>
+      <c r="I20" s="47">
+        <v>0</v>
+      </c>
+      <c r="J20" s="47">
+        <v>0</v>
+      </c>
+      <c r="K20" s="47">
+        <v>0</v>
+      </c>
+      <c r="L20" s="47">
+        <v>0</v>
+      </c>
+      <c r="M20" s="47">
+        <v>0</v>
+      </c>
+      <c r="N20" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="15.75" customHeight="1">
       <c r="A21" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="B21" s="6">
-        <v>0</v>
-      </c>
-      <c r="C21" s="6">
-        <v>0</v>
-      </c>
-      <c r="D21" s="44">
-        <v>0</v>
-      </c>
-      <c r="E21" s="44">
-        <v>0</v>
-      </c>
-      <c r="F21" s="44">
-        <v>0</v>
-      </c>
-      <c r="G21" s="39">
-        <v>1</v>
-      </c>
-      <c r="H21" s="4">
-        <v>0</v>
-      </c>
-      <c r="I21" s="4">
-        <v>0</v>
-      </c>
-      <c r="J21" s="4">
-        <v>0</v>
-      </c>
-      <c r="K21" s="4">
-        <v>0</v>
-      </c>
-      <c r="L21" s="4">
-        <v>0</v>
-      </c>
-      <c r="M21" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" ht="15.75" customHeight="1">
+      <c r="B21" s="47">
+        <v>0</v>
+      </c>
+      <c r="C21" s="47">
+        <v>0</v>
+      </c>
+      <c r="D21" s="51">
+        <v>0</v>
+      </c>
+      <c r="E21" s="51">
+        <v>0</v>
+      </c>
+      <c r="F21" s="51">
+        <v>0</v>
+      </c>
+      <c r="G21" s="52">
+        <v>1</v>
+      </c>
+      <c r="H21" s="47">
+        <v>0</v>
+      </c>
+      <c r="I21" s="47">
+        <v>0</v>
+      </c>
+      <c r="J21" s="47">
+        <v>0</v>
+      </c>
+      <c r="K21" s="47">
+        <v>0</v>
+      </c>
+      <c r="L21" s="47">
+        <v>0</v>
+      </c>
+      <c r="M21" s="47">
+        <v>0</v>
+      </c>
+      <c r="N21" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="15.75" customHeight="1">
       <c r="A22" t="s">
-        <v>127</v>
-      </c>
-      <c r="B22" s="6">
-        <v>0</v>
-      </c>
-      <c r="C22" s="6">
-        <v>0</v>
-      </c>
-      <c r="D22" s="6">
-        <v>0</v>
-      </c>
-      <c r="E22" s="6">
-        <v>0</v>
-      </c>
-      <c r="F22" s="6">
-        <v>0</v>
-      </c>
-      <c r="G22" s="39">
-        <v>1</v>
-      </c>
-      <c r="H22" s="4">
-        <v>0</v>
-      </c>
-      <c r="I22" s="4">
-        <v>0</v>
-      </c>
-      <c r="J22" s="4">
-        <v>0</v>
-      </c>
-      <c r="K22" s="4">
-        <v>0</v>
-      </c>
-      <c r="L22" s="4">
-        <v>0</v>
-      </c>
-      <c r="M22" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" ht="15.75" customHeight="1">
+        <v>125</v>
+      </c>
+      <c r="B22" s="53">
+        <v>0</v>
+      </c>
+      <c r="C22" s="53">
+        <v>0</v>
+      </c>
+      <c r="D22" s="53">
+        <v>0</v>
+      </c>
+      <c r="E22" s="53">
+        <v>0</v>
+      </c>
+      <c r="F22" s="53">
+        <v>0</v>
+      </c>
+      <c r="G22" s="48">
+        <f>'Frac exposed malaria'!F2</f>
+        <v>0.5</v>
+      </c>
+      <c r="H22" s="53">
+        <v>0</v>
+      </c>
+      <c r="I22" s="53">
+        <v>0</v>
+      </c>
+      <c r="J22" s="53">
+        <v>0</v>
+      </c>
+      <c r="K22" s="53">
+        <v>0</v>
+      </c>
+      <c r="L22" s="53">
+        <v>0</v>
+      </c>
+      <c r="M22" s="53">
+        <v>0</v>
+      </c>
+      <c r="N22" s="53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="15.75" customHeight="1">
       <c r="A23" t="s">
-        <v>125</v>
-      </c>
-      <c r="B23" s="6">
-        <v>0</v>
-      </c>
-      <c r="C23" s="6">
-        <v>0</v>
-      </c>
-      <c r="D23" s="6">
-        <v>0</v>
-      </c>
-      <c r="E23" s="6">
-        <v>0</v>
-      </c>
-      <c r="F23" s="6">
-        <v>0</v>
-      </c>
-      <c r="G23" s="6">
-        <v>0</v>
-      </c>
-      <c r="H23" s="4">
-        <v>1</v>
-      </c>
-      <c r="I23" s="4">
-        <v>1</v>
-      </c>
-      <c r="J23" s="4">
-        <v>1</v>
-      </c>
-      <c r="K23" s="4">
-        <v>1</v>
-      </c>
-      <c r="L23" s="4">
-        <v>1</v>
-      </c>
-      <c r="M23" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" ht="15.75" customHeight="1">
+        <v>131</v>
+      </c>
+      <c r="B23" s="47">
+        <v>0</v>
+      </c>
+      <c r="C23" s="47">
+        <v>0</v>
+      </c>
+      <c r="D23" s="47">
+        <v>0</v>
+      </c>
+      <c r="E23" s="47">
+        <v>0</v>
+      </c>
+      <c r="F23" s="47">
+        <v>0</v>
+      </c>
+      <c r="G23" s="47">
+        <v>0</v>
+      </c>
+      <c r="H23" s="46">
+        <f>1*demographics!B7</f>
+        <v>0.4</v>
+      </c>
+      <c r="I23" s="46">
+        <f>1*demographics!B7</f>
+        <v>0.4</v>
+      </c>
+      <c r="J23" s="46">
+        <f>1*demographics!B7</f>
+        <v>0.4</v>
+      </c>
+      <c r="K23" s="46">
+        <f>1*demographics!B7</f>
+        <v>0.4</v>
+      </c>
+      <c r="L23" s="46">
+        <f>1*demographics!B7</f>
+        <v>0.4</v>
+      </c>
+      <c r="M23" s="46">
+        <f>1*demographics!B7</f>
+        <v>0.4</v>
+      </c>
+      <c r="N23" s="53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="15.75" customHeight="1">
       <c r="A24" t="s">
-        <v>126</v>
-      </c>
-      <c r="B24" s="6">
-        <v>1</v>
-      </c>
-      <c r="C24" s="6">
-        <v>1</v>
-      </c>
-      <c r="D24" s="6">
-        <v>1</v>
-      </c>
-      <c r="E24" s="6">
-        <v>1</v>
-      </c>
-      <c r="F24" s="6">
-        <v>1</v>
-      </c>
-      <c r="G24" s="6">
-        <v>1</v>
-      </c>
-      <c r="H24" s="6">
-        <v>1</v>
-      </c>
-      <c r="I24" s="6">
-        <v>1</v>
-      </c>
-      <c r="J24" s="6">
-        <v>1</v>
-      </c>
-      <c r="K24" s="6">
-        <v>1</v>
-      </c>
-      <c r="L24" s="6">
-        <v>1</v>
-      </c>
-      <c r="M24" s="6">
+        <v>132</v>
+      </c>
+      <c r="B24" s="47">
+        <v>0</v>
+      </c>
+      <c r="C24" s="47">
+        <v>0</v>
+      </c>
+      <c r="D24" s="47">
+        <v>0</v>
+      </c>
+      <c r="E24" s="47">
+        <v>0</v>
+      </c>
+      <c r="F24" s="47">
+        <v>0</v>
+      </c>
+      <c r="G24" s="47">
+        <v>0</v>
+      </c>
+      <c r="H24" s="46">
+        <f>1*demographics!B7</f>
+        <v>0.4</v>
+      </c>
+      <c r="I24" s="46">
+        <f>1*demographics!B7</f>
+        <v>0.4</v>
+      </c>
+      <c r="J24" s="46">
+        <f>1*demographics!B7</f>
+        <v>0.4</v>
+      </c>
+      <c r="K24" s="46">
+        <f>1*demographics!B7</f>
+        <v>0.4</v>
+      </c>
+      <c r="L24" s="46">
+        <f>1*demographics!B7</f>
+        <v>0.4</v>
+      </c>
+      <c r="M24" s="46">
+        <f>1*demographics!B7</f>
+        <v>0.4</v>
+      </c>
+      <c r="N24" s="53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A25" t="s">
+        <v>133</v>
+      </c>
+      <c r="B25" s="47">
+        <v>0</v>
+      </c>
+      <c r="C25" s="47">
+        <v>0</v>
+      </c>
+      <c r="D25" s="47">
+        <v>0</v>
+      </c>
+      <c r="E25" s="47">
+        <v>0</v>
+      </c>
+      <c r="F25" s="47">
+        <v>0</v>
+      </c>
+      <c r="G25" s="47">
+        <v>0</v>
+      </c>
+      <c r="H25" s="46">
+        <f>1*demographics!B7</f>
+        <v>0.4</v>
+      </c>
+      <c r="I25" s="46">
+        <f>1*demographics!B7</f>
+        <v>0.4</v>
+      </c>
+      <c r="J25" s="46">
+        <f>1*demographics!B7</f>
+        <v>0.4</v>
+      </c>
+      <c r="K25" s="46">
+        <f>1*demographics!B7</f>
+        <v>0.4</v>
+      </c>
+      <c r="L25" s="46">
+        <f>1*demographics!B7</f>
+        <v>0.4</v>
+      </c>
+      <c r="M25" s="46">
+        <f>1*demographics!B7</f>
+        <v>0.4</v>
+      </c>
+      <c r="N25" s="53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A26" t="s">
+        <v>134</v>
+      </c>
+      <c r="B26" s="47">
+        <v>0</v>
+      </c>
+      <c r="C26" s="47">
+        <v>0</v>
+      </c>
+      <c r="D26" s="47">
+        <v>0</v>
+      </c>
+      <c r="E26" s="47">
+        <v>0</v>
+      </c>
+      <c r="F26" s="47">
+        <v>0</v>
+      </c>
+      <c r="G26" s="47">
+        <v>0</v>
+      </c>
+      <c r="H26" s="46">
+        <f>1*(1-demographics!B7)</f>
+        <v>0.6</v>
+      </c>
+      <c r="I26" s="46">
+        <f>1*(1-demographics!B7)</f>
+        <v>0.6</v>
+      </c>
+      <c r="J26" s="46">
+        <f>1*(1-demographics!B7)</f>
+        <v>0.6</v>
+      </c>
+      <c r="K26" s="46">
+        <f>1*(1-demographics!B7)</f>
+        <v>0.6</v>
+      </c>
+      <c r="L26" s="46">
+        <f>1*(1-demographics!B7)</f>
+        <v>0.6</v>
+      </c>
+      <c r="M26" s="46">
+        <f>1*(1-demographics!B7)</f>
+        <v>0.6</v>
+      </c>
+      <c r="N26" s="53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A27" t="s">
+        <v>135</v>
+      </c>
+      <c r="B27" s="47">
+        <v>0</v>
+      </c>
+      <c r="C27" s="47">
+        <v>0</v>
+      </c>
+      <c r="D27" s="47">
+        <v>0</v>
+      </c>
+      <c r="E27" s="47">
+        <v>0</v>
+      </c>
+      <c r="F27" s="47">
+        <v>0</v>
+      </c>
+      <c r="G27" s="47">
+        <v>0</v>
+      </c>
+      <c r="H27" s="46">
+        <f>1*(1-demographics!B7)</f>
+        <v>0.6</v>
+      </c>
+      <c r="I27" s="46">
+        <f>1*(1-demographics!B7)</f>
+        <v>0.6</v>
+      </c>
+      <c r="J27" s="46">
+        <f>1*(1-demographics!B7)</f>
+        <v>0.6</v>
+      </c>
+      <c r="K27" s="46">
+        <f>1*(1-demographics!B7)</f>
+        <v>0.6</v>
+      </c>
+      <c r="L27" s="46">
+        <f>1*(1-demographics!B7)</f>
+        <v>0.6</v>
+      </c>
+      <c r="M27" s="46">
+        <f>1*(1-demographics!B7)</f>
+        <v>0.6</v>
+      </c>
+      <c r="N27" s="53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A28" t="s">
+        <v>136</v>
+      </c>
+      <c r="B28" s="47">
+        <v>0</v>
+      </c>
+      <c r="C28" s="47">
+        <v>0</v>
+      </c>
+      <c r="D28" s="47">
+        <v>0</v>
+      </c>
+      <c r="E28" s="47">
+        <v>0</v>
+      </c>
+      <c r="F28" s="47">
+        <v>0</v>
+      </c>
+      <c r="G28" s="47">
+        <v>0</v>
+      </c>
+      <c r="H28" s="46">
+        <f>1*(1-demographics!B7)</f>
+        <v>0.6</v>
+      </c>
+      <c r="I28" s="46">
+        <f>1*(1-demographics!B7)</f>
+        <v>0.6</v>
+      </c>
+      <c r="J28" s="46">
+        <f>1*(1-demographics!B7)</f>
+        <v>0.6</v>
+      </c>
+      <c r="K28" s="46">
+        <f>1*(1-demographics!B7)</f>
+        <v>0.6</v>
+      </c>
+      <c r="L28" s="46">
+        <f>1*(1-demographics!B7)</f>
+        <v>0.6</v>
+      </c>
+      <c r="M28" s="46">
+        <f>1*(1-demographics!B7)</f>
+        <v>0.6</v>
+      </c>
+      <c r="N28" s="53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A29" t="s">
+        <v>137</v>
+      </c>
+      <c r="B29" s="47">
+        <v>0</v>
+      </c>
+      <c r="C29" s="47">
+        <v>0</v>
+      </c>
+      <c r="D29" s="47">
+        <v>0</v>
+      </c>
+      <c r="E29" s="47">
+        <v>0</v>
+      </c>
+      <c r="F29" s="47">
+        <v>0</v>
+      </c>
+      <c r="G29" s="47">
+        <v>0</v>
+      </c>
+      <c r="H29" s="46">
+        <f>1*(1-demographics!B7)</f>
+        <v>0.6</v>
+      </c>
+      <c r="I29" s="46">
+        <f>1*(1-demographics!B7)</f>
+        <v>0.6</v>
+      </c>
+      <c r="J29" s="46">
+        <f>1*(1-demographics!B7)</f>
+        <v>0.6</v>
+      </c>
+      <c r="K29" s="46">
+        <f>1*(1-demographics!B7)</f>
+        <v>0.6</v>
+      </c>
+      <c r="L29" s="46">
+        <f>1*(1-demographics!B7)</f>
+        <v>0.6</v>
+      </c>
+      <c r="M29" s="46">
+        <f>1*(1-demographics!B7)</f>
+        <v>0.6</v>
+      </c>
+      <c r="N29" s="53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A30" t="s">
+        <v>128</v>
+      </c>
+      <c r="B30" s="53">
+        <v>0</v>
+      </c>
+      <c r="C30" s="53">
+        <v>0</v>
+      </c>
+      <c r="D30" s="53">
+        <v>0</v>
+      </c>
+      <c r="E30" s="53">
+        <v>0</v>
+      </c>
+      <c r="F30" s="53">
+        <v>0</v>
+      </c>
+      <c r="G30" s="53">
+        <v>0</v>
+      </c>
+      <c r="H30" s="53">
+        <v>0</v>
+      </c>
+      <c r="I30" s="53">
+        <v>0</v>
+      </c>
+      <c r="J30" s="53">
+        <v>0</v>
+      </c>
+      <c r="K30" s="53">
+        <v>0</v>
+      </c>
+      <c r="L30" s="53">
+        <v>0</v>
+      </c>
+      <c r="M30" s="53">
+        <v>0</v>
+      </c>
+      <c r="N30" s="53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A31" t="s">
+        <v>129</v>
+      </c>
+      <c r="B31" s="53">
+        <v>0</v>
+      </c>
+      <c r="C31" s="53">
+        <v>0</v>
+      </c>
+      <c r="D31" s="53">
+        <v>0</v>
+      </c>
+      <c r="E31" s="53">
+        <v>0</v>
+      </c>
+      <c r="F31" s="53">
+        <v>0</v>
+      </c>
+      <c r="G31" s="53">
+        <v>0</v>
+      </c>
+      <c r="H31" s="53">
+        <v>0</v>
+      </c>
+      <c r="I31" s="53">
+        <v>0</v>
+      </c>
+      <c r="J31" s="53">
+        <v>0</v>
+      </c>
+      <c r="K31" s="53">
+        <v>0</v>
+      </c>
+      <c r="L31" s="53">
+        <v>0</v>
+      </c>
+      <c r="M31" s="53">
+        <v>0</v>
+      </c>
+      <c r="N31" s="53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A32" t="s">
+        <v>130</v>
+      </c>
+      <c r="B32" s="53">
+        <v>0</v>
+      </c>
+      <c r="C32" s="53">
+        <v>0</v>
+      </c>
+      <c r="D32" s="53">
+        <v>0</v>
+      </c>
+      <c r="E32" s="53">
+        <v>0</v>
+      </c>
+      <c r="F32" s="53">
+        <v>0</v>
+      </c>
+      <c r="G32" s="53">
+        <v>0</v>
+      </c>
+      <c r="H32" s="53">
+        <v>0</v>
+      </c>
+      <c r="I32" s="53">
+        <v>0</v>
+      </c>
+      <c r="J32" s="53">
+        <v>0</v>
+      </c>
+      <c r="K32" s="53">
+        <v>0</v>
+      </c>
+      <c r="L32" s="53">
+        <v>0</v>
+      </c>
+      <c r="M32" s="53">
+        <v>0</v>
+      </c>
+      <c r="N32" s="53">
         <v>1</v>
       </c>
     </row>
@@ -8633,15 +9914,15 @@
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -8678,8 +9959,11 @@
       <c r="L1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="M1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2">
         <v>0.5</v>
       </c>
@@ -8714,6 +9998,9 @@
         <v>0.5</v>
       </c>
       <c r="L2">
+        <v>0.5</v>
+      </c>
+      <c r="M2">
         <v>0.5</v>
       </c>
     </row>
@@ -8889,15 +10176,15 @@
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -8934,8 +10221,11 @@
       <c r="L1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="M1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2">
         <v>0.5</v>
       </c>
@@ -8970,6 +10260,9 @@
         <v>0.5</v>
       </c>
       <c r="L2">
+        <v>0.5</v>
+      </c>
+      <c r="M2">
         <v>0.5</v>
       </c>
     </row>
@@ -8986,10 +10279,210 @@
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H1" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1" t="s">
+        <v>113</v>
+      </c>
+      <c r="J1" t="s">
+        <v>114</v>
+      </c>
+      <c r="K1" t="s">
+        <v>115</v>
+      </c>
+      <c r="L1" t="s">
+        <v>116</v>
+      </c>
+      <c r="M1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2">
+        <v>0.5</v>
+      </c>
+      <c r="B2">
+        <v>0.5</v>
+      </c>
+      <c r="C2">
+        <v>0.5</v>
+      </c>
+      <c r="D2">
+        <v>0.5</v>
+      </c>
+      <c r="E2">
+        <v>0.5</v>
+      </c>
+      <c r="F2">
+        <v>0.5</v>
+      </c>
+      <c r="G2">
+        <v>0.5</v>
+      </c>
+      <c r="H2">
+        <v>0.5</v>
+      </c>
+      <c r="I2">
+        <v>0.5</v>
+      </c>
+      <c r="J2">
+        <v>0.5</v>
+      </c>
+      <c r="K2">
+        <v>0.5</v>
+      </c>
+      <c r="L2">
+        <v>0.5</v>
+      </c>
+      <c r="M2">
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H1" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1" t="s">
+        <v>113</v>
+      </c>
+      <c r="J1" t="s">
+        <v>114</v>
+      </c>
+      <c r="K1" t="s">
+        <v>115</v>
+      </c>
+      <c r="L1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2">
+        <v>0.5</v>
+      </c>
+      <c r="B2">
+        <v>0.5</v>
+      </c>
+      <c r="C2">
+        <v>0.5</v>
+      </c>
+      <c r="D2">
+        <v>0.5</v>
+      </c>
+      <c r="E2">
+        <v>0.5</v>
+      </c>
+      <c r="F2">
+        <v>0.5</v>
+      </c>
+      <c r="G2">
+        <v>0.5</v>
+      </c>
+      <c r="H2">
+        <v>0.5</v>
+      </c>
+      <c r="I2">
+        <v>0.5</v>
+      </c>
+      <c r="J2">
+        <v>0.5</v>
+      </c>
+      <c r="K2">
+        <v>0.5</v>
+      </c>
+      <c r="L2">
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -9535,7 +11028,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
@@ -9645,7 +11138,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H35"/>
   <sheetViews>
@@ -9972,7 +11465,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
@@ -10243,22 +11736,22 @@
       <c r="D1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E1" s="45" t="s">
+      <c r="E1" s="44" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="45" t="s">
+      <c r="F1" s="44" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="45" t="s">
+      <c r="G1" s="44" t="s">
         <v>113</v>
       </c>
-      <c r="H1" s="45" t="s">
+      <c r="H1" s="44" t="s">
         <v>114</v>
       </c>
-      <c r="I1" s="45" t="s">
+      <c r="I1" s="44" t="s">
         <v>115</v>
       </c>
-      <c r="J1" s="45" t="s">
+      <c r="J1" s="44" t="s">
         <v>116</v>
       </c>
     </row>
@@ -11970,10 +13463,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M54" sqref="M54"/>
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -11981,51 +13474,54 @@
     <col min="8" max="8" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>17</v>
       </c>
       <c r="B1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="45" t="s">
+      <c r="D1" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="45" t="s">
+      <c r="E1" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="45" t="s">
+      <c r="F1" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="45" t="s">
+      <c r="G1" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="45" t="s">
+      <c r="H1" s="44" t="s">
         <v>67</v>
       </c>
-      <c r="I1" s="45" t="s">
+      <c r="I1" s="44" t="s">
         <v>111</v>
       </c>
-      <c r="J1" s="45" t="s">
+      <c r="J1" s="44" t="s">
         <v>112</v>
       </c>
-      <c r="K1" s="45" t="s">
+      <c r="K1" s="44" t="s">
         <v>113</v>
       </c>
-      <c r="L1" s="45" t="s">
+      <c r="L1" s="44" t="s">
         <v>114</v>
       </c>
-      <c r="M1" s="45" t="s">
+      <c r="M1" s="44" t="s">
         <v>115</v>
       </c>
-      <c r="N1" s="45" t="s">
+      <c r="N1" s="44" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="2" spans="1:14">
+      <c r="O1" s="44" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>117</v>
       </c>
@@ -12068,8 +13564,11 @@
       <c r="N2">
         <v>50</v>
       </c>
-    </row>
-    <row r="3" spans="1:14">
+      <c r="O2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="B3" t="s">
         <v>119</v>
       </c>
@@ -12119,6 +13618,9 @@
       </c>
       <c r="N3">
         <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="O3">
         <v>50</v>
       </c>
     </row>

</xml_diff>

<commit_message>
started demo script, updated RR in spreadsheet
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Jan/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Jan/InputForCode_Bangladesh.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-73340" yWindow="-3240" windowWidth="30680" windowHeight="16920" tabRatio="500" firstSheet="18" activeTab="19"/>
+    <workbookView xWindow="-73120" yWindow="-3640" windowWidth="30680" windowHeight="16920" tabRatio="500" firstSheet="17" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="demographics" sheetId="1" r:id="rId1"/>
@@ -179,172 +179,6 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Sam</author>
-    <author>Janka Petravic</author>
-    <author>Ruth</author>
-  </authors>
-  <commentList>
-    <comment ref="H2" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>Sam:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">
-WRA values (possibly?) fictional </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D4" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-2 lowest wealth quintiles</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E4" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-2 lowest wealth quintiles</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G6" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-2 lowest wealth quintiles</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A18" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>Ruth:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Active management of the third stage of labor</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G22" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>Ruth:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-fraction exposed to malaria - take from spreadsheet value</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H23" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>Ruth:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-taget only faction poor</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments11.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Sam</author>
   </authors>
   <commentList>
     <comment ref="I2" authorId="0">
@@ -366,6 +200,38 @@
           </rPr>
           <t xml:space="preserve">
 WRA all fictional</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments11.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Sam</author>
+  </authors>
+  <commentList>
+    <comment ref="A2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Sam:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Fictional values</t>
         </r>
       </text>
     </comment>
@@ -475,38 +341,6 @@
     <author>Sam</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>Sam:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">
-Fictional values</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments16.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Sam</author>
-  </authors>
-  <commentList>
     <comment ref="I2" authorId="0">
       <text>
         <r>
@@ -533,7 +367,7 @@
 </comments>
 </file>
 
-<file path=xl/comments17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments16.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Ruth</author>
@@ -609,7 +443,7 @@
 </comments>
 </file>
 
-<file path=xl/comments18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments17.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Ruth</author>
@@ -952,38 +786,6 @@
 <file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Sam</author>
-  </authors>
-  <commentList>
-    <comment ref="G2" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>Sam:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">
-What is this RR?</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
     <author>Janka Petravic</author>
   </authors>
   <commentList>
@@ -1013,7 +815,7 @@
 </comments>
 </file>
 
-<file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Ruth</author>
@@ -1129,6 +931,172 @@
           <t xml:space="preserve">
 amongst general population
 </t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Sam</author>
+    <author>Janka Petravic</author>
+    <author>Ruth</author>
+  </authors>
+  <commentList>
+    <comment ref="H2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Sam:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+WRA values (possibly?) fictional </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D4" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+2 lowest wealth quintiles</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E4" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+2 lowest wealth quintiles</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G6" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+2 lowest wealth quintiles</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A18" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Active management of the third stage of labor</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G22" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+fraction exposed to malaria - take from spreadsheet value</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H23" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+taget only faction poor</t>
         </r>
       </text>
     </comment>
@@ -1713,7 +1681,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="116">
+  <cellStyleXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1730,6 +1698,8 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1945,7 +1915,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="116">
+  <cellStyles count="118">
     <cellStyle name="Excel Built-in Normal" xfId="15"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -2004,6 +1974,7 @@
     <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2061,6 +2032,7 @@
     <cellStyle name="Hyperlink" xfId="110" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="112" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="114" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="116" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6064,11 +6036,11 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -6140,7 +6112,7 @@
         <v>1</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -6519,7 +6491,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -6676,7 +6647,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -7251,7 +7222,7 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
fixed typo, added a RR anemia
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Jan/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Jan/InputForCode_Bangladesh.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-73120" yWindow="-3640" windowWidth="30680" windowHeight="16920" tabRatio="500" firstSheet="17" activeTab="18"/>
+    <workbookView xWindow="-37300" yWindow="-3800" windowWidth="27880" windowHeight="16560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="demographics" sheetId="1" r:id="rId1"/>
@@ -1105,7 +1105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="138">
   <si>
     <t>indicators</t>
   </si>
@@ -1485,9 +1485,6 @@
     <t>IPTp</t>
   </si>
   <si>
-    <t>Anenatal micronutrient supplementation</t>
-  </si>
-  <si>
     <t>general population</t>
   </si>
   <si>
@@ -1681,7 +1678,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="118">
+  <cellStyleXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1698,6 +1695,8 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1915,7 +1914,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="118">
+  <cellStyles count="120">
     <cellStyle name="Excel Built-in Normal" xfId="15"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -1975,6 +1974,7 @@
     <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="119" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2033,6 +2033,7 @@
     <cellStyle name="Hyperlink" xfId="112" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="114" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="116" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="118" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3399,8 +3400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -3475,7 +3476,7 @@
     </row>
     <row r="9" spans="1:2" ht="15.75" customHeight="1">
       <c r="A9" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B9" s="22">
         <v>161000000</v>
@@ -6039,8 +6040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -6089,12 +6090,12 @@
         <v>116</v>
       </c>
       <c r="N1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>126</v>
+        <v>79</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -6182,7 +6183,7 @@
     </row>
     <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -6226,7 +6227,7 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -6270,7 +6271,7 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -6314,7 +6315,7 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -6358,7 +6359,7 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -6402,7 +6403,7 @@
     </row>
     <row r="9" spans="1:14">
       <c r="A9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -6446,7 +6447,7 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -6697,12 +6698,12 @@
         <v>116</v>
       </c>
       <c r="N1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -6746,7 +6747,7 @@
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -6790,7 +6791,7 @@
     </row>
     <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -7222,7 +7223,7 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -7579,7 +7580,7 @@
     </row>
     <row r="23" spans="1:4" ht="15.75" customHeight="1">
       <c r="A23" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B23" s="6">
         <v>0</v>
@@ -7593,7 +7594,7 @@
     </row>
     <row r="24" spans="1:4" ht="15.75" customHeight="1">
       <c r="A24" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B24" s="6">
         <v>0</v>
@@ -7607,7 +7608,7 @@
     </row>
     <row r="25" spans="1:4" ht="15.75" customHeight="1">
       <c r="A25" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B25" s="6">
         <v>0</v>
@@ -7621,7 +7622,7 @@
     </row>
     <row r="26" spans="1:4" ht="15.75" customHeight="1">
       <c r="A26" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B26" s="6">
         <v>0</v>
@@ -7635,7 +7636,7 @@
     </row>
     <row r="27" spans="1:4" ht="15.75" customHeight="1">
       <c r="A27" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B27" s="6">
         <v>0</v>
@@ -7649,7 +7650,7 @@
     </row>
     <row r="28" spans="1:4" ht="15.75" customHeight="1">
       <c r="A28" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B28" s="6">
         <v>0</v>
@@ -7663,7 +7664,7 @@
     </row>
     <row r="29" spans="1:4" ht="15.75" customHeight="1">
       <c r="A29" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B29" s="6">
         <v>0</v>
@@ -7677,7 +7678,7 @@
     </row>
     <row r="30" spans="1:4" ht="15.75" customHeight="1">
       <c r="A30" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B30" s="6">
         <v>0</v>
@@ -7691,7 +7692,7 @@
     </row>
     <row r="31" spans="1:4" ht="15.75" customHeight="1">
       <c r="A31" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B31" s="6">
         <v>0</v>
@@ -7705,7 +7706,7 @@
     </row>
     <row r="32" spans="1:4" ht="15.75" customHeight="1">
       <c r="A32" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B32" s="6">
         <v>0</v>
@@ -7788,7 +7789,7 @@
         <v>116</v>
       </c>
       <c r="N1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="15.75" customHeight="1">
@@ -8721,7 +8722,7 @@
     </row>
     <row r="23" spans="1:14" ht="15.75" customHeight="1">
       <c r="A23" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B23" s="47">
         <v>0</v>
@@ -8771,7 +8772,7 @@
     </row>
     <row r="24" spans="1:14" ht="15.75" customHeight="1">
       <c r="A24" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B24" s="47">
         <v>0</v>
@@ -8821,7 +8822,7 @@
     </row>
     <row r="25" spans="1:14" ht="15.75" customHeight="1">
       <c r="A25" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B25" s="47">
         <v>0</v>
@@ -8871,7 +8872,7 @@
     </row>
     <row r="26" spans="1:14" ht="15.75" customHeight="1">
       <c r="A26" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B26" s="47">
         <v>0</v>
@@ -8921,7 +8922,7 @@
     </row>
     <row r="27" spans="1:14" ht="15.75" customHeight="1">
       <c r="A27" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B27" s="47">
         <v>0</v>
@@ -8971,7 +8972,7 @@
     </row>
     <row r="28" spans="1:14" ht="15.75" customHeight="1">
       <c r="A28" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B28" s="47">
         <v>0</v>
@@ -9021,7 +9022,7 @@
     </row>
     <row r="29" spans="1:14" ht="15.75" customHeight="1">
       <c r="A29" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B29" s="47">
         <v>0</v>
@@ -9071,7 +9072,7 @@
     </row>
     <row r="30" spans="1:14" ht="15.75" customHeight="1">
       <c r="A30" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B30" s="53">
         <v>0</v>
@@ -9115,7 +9116,7 @@
     </row>
     <row r="31" spans="1:14" ht="15.75" customHeight="1">
       <c r="A31" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B31" s="53">
         <v>0</v>
@@ -9159,7 +9160,7 @@
     </row>
     <row r="32" spans="1:14" ht="15.75" customHeight="1">
       <c r="A32" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B32" s="53">
         <v>0</v>
@@ -9931,7 +9932,7 @@
         <v>116</v>
       </c>
       <c r="M1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -10193,7 +10194,7 @@
         <v>116</v>
       </c>
       <c r="M1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -10296,7 +10297,7 @@
         <v>116</v>
       </c>
       <c r="M1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -13489,7 +13490,7 @@
         <v>116</v>
       </c>
       <c r="O1" s="44" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:15">

</xml_diff>

<commit_message>
Updated WRA age groups to the same same as PW
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Jan/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Jan/InputForCode_Bangladesh.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/Github Projects/Nutrition/input_spreadsheets/Bangladesh/2017Jan/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-45080" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" firstSheet="10" activeTab="19"/>
+    <workbookView xWindow="-45080" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" firstSheet="26" activeTab="33"/>
   </bookViews>
   <sheets>
     <sheet name="demographics" sheetId="1" r:id="rId1"/>
@@ -607,7 +607,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J2" authorId="0">
+    <comment ref="H2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1017,7 +1017,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M6" authorId="1">
+    <comment ref="K6" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1061,7 +1061,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M22" authorId="2">
+    <comment ref="K22" authorId="2">
       <text>
         <r>
           <rPr>
@@ -1110,7 +1110,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="143">
   <si>
     <t>indicators</t>
   </si>
@@ -1493,21 +1493,6 @@
     <t>WRA: 15-19 years</t>
   </si>
   <si>
-    <t>WRA: 20-24 years</t>
-  </si>
-  <si>
-    <t>WRA: 25-29 years</t>
-  </si>
-  <si>
-    <t>WRA: 30-34 years</t>
-  </si>
-  <si>
-    <t>WRA: 35-39 years</t>
-  </si>
-  <si>
-    <t>WRA: 40-44 years</t>
-  </si>
-  <si>
     <t>PW: 15-19 years</t>
   </si>
   <si>
@@ -1545,6 +1530,15 @@
   </si>
   <si>
     <t>PW: Indirect causes</t>
+  </si>
+  <si>
+    <t>WRA: 20-29 years</t>
+  </si>
+  <si>
+    <t>WRA: 30-39 years</t>
+  </si>
+  <si>
+    <t>WRA: 40-49 years</t>
   </si>
 </sst>
 </file>
@@ -1698,7 +1692,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="130">
+  <cellStyleXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1715,6 +1709,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1942,7 +1940,7 @@
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="130">
+  <cellStyles count="134">
     <cellStyle name="Excel Built-in Normal" xfId="15"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -2008,6 +2006,8 @@
     <cellStyle name="Followed Hyperlink" xfId="125" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="127" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="129" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="131" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="133" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2072,6 +2072,8 @@
     <cellStyle name="Hyperlink" xfId="124" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="126" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="128" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="130" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="132" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2094,7 +2096,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>546100</xdr:colOff>
       <xdr:row>66</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
@@ -2145,7 +2147,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>546100</xdr:colOff>
       <xdr:row>66</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
@@ -3528,10 +3530,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q7"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3540,7 +3542,7 @@
     <col min="2" max="2" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -3562,38 +3564,32 @@
       <c r="G1" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="41" t="s">
+      <c r="H1" t="s">
         <v>126</v>
       </c>
-      <c r="I1" s="41" t="s">
+      <c r="I1" t="s">
+        <v>140</v>
+      </c>
+      <c r="J1" t="s">
+        <v>141</v>
+      </c>
+      <c r="K1" t="s">
+        <v>142</v>
+      </c>
+      <c r="L1" t="s">
         <v>127</v>
       </c>
-      <c r="J1" s="41" t="s">
+      <c r="M1" t="s">
         <v>128</v>
       </c>
-      <c r="K1" s="41" t="s">
+      <c r="N1" t="s">
         <v>129</v>
       </c>
-      <c r="L1" s="41" t="s">
+      <c r="O1" t="s">
         <v>130</v>
       </c>
-      <c r="M1" s="41" t="s">
-        <v>131</v>
-      </c>
-      <c r="N1" s="41" t="s">
-        <v>132</v>
-      </c>
-      <c r="O1" s="41" t="s">
-        <v>133</v>
-      </c>
-      <c r="P1" s="41" t="s">
-        <v>134</v>
-      </c>
-      <c r="Q1" s="41" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.15">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>110</v>
       </c>
@@ -3639,14 +3635,8 @@
       <c r="O2">
         <v>1</v>
       </c>
-      <c r="P2">
-        <v>1</v>
-      </c>
-      <c r="Q2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.15">
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B3" t="s">
         <v>107</v>
       </c>
@@ -3689,14 +3679,8 @@
       <c r="O3">
         <v>1</v>
       </c>
-      <c r="P3">
-        <v>1</v>
-      </c>
-      <c r="Q3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.15">
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>111</v>
       </c>
@@ -3742,14 +3726,8 @@
       <c r="O4">
         <v>1</v>
       </c>
-      <c r="P4">
-        <v>1</v>
-      </c>
-      <c r="Q4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.15">
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B5" t="s">
         <v>107</v>
       </c>
@@ -3792,14 +3770,8 @@
       <c r="O5">
         <v>1</v>
       </c>
-      <c r="P5">
-        <v>1</v>
-      </c>
-      <c r="Q5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.15">
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>112</v>
       </c>
@@ -3845,14 +3817,8 @@
       <c r="O6">
         <v>1</v>
       </c>
-      <c r="P6">
-        <v>1</v>
-      </c>
-      <c r="Q6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.15">
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B7" t="s">
         <v>107</v>
       </c>
@@ -3893,12 +3859,6 @@
         <v>1</v>
       </c>
       <c r="O7">
-        <v>1</v>
-      </c>
-      <c r="P7">
-        <v>1</v>
-      </c>
-      <c r="Q7">
         <v>1</v>
       </c>
     </row>
@@ -6089,10 +6049,10 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q10"/>
+  <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:Q1"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6100,7 +6060,7 @@
     <col min="1" max="1" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>56</v>
       </c>
@@ -6119,41 +6079,35 @@
       <c r="F1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="41" t="s">
+      <c r="G1" t="s">
         <v>126</v>
       </c>
-      <c r="H1" s="41" t="s">
+      <c r="H1" t="s">
+        <v>140</v>
+      </c>
+      <c r="I1" t="s">
+        <v>141</v>
+      </c>
+      <c r="J1" t="s">
+        <v>142</v>
+      </c>
+      <c r="K1" t="s">
         <v>127</v>
       </c>
-      <c r="I1" s="41" t="s">
+      <c r="L1" t="s">
         <v>128</v>
       </c>
-      <c r="J1" s="41" t="s">
+      <c r="M1" t="s">
         <v>129</v>
       </c>
-      <c r="K1" s="41" t="s">
+      <c r="N1" t="s">
         <v>130</v>
       </c>
-      <c r="L1" s="41" t="s">
-        <v>131</v>
-      </c>
-      <c r="M1" s="41" t="s">
-        <v>132</v>
-      </c>
-      <c r="N1" s="41" t="s">
-        <v>133</v>
-      </c>
-      <c r="O1" s="41" t="s">
-        <v>134</v>
-      </c>
-      <c r="P1" s="41" t="s">
-        <v>135</v>
-      </c>
-      <c r="Q1" s="41" t="s">
+      <c r="O1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>78</v>
       </c>
@@ -6185,10 +6139,10 @@
         <v>1</v>
       </c>
       <c r="K2">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="L2">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="M2">
         <v>0.3</v>
@@ -6197,16 +6151,10 @@
         <v>0.3</v>
       </c>
       <c r="O2">
-        <v>0.3</v>
-      </c>
-      <c r="P2">
-        <v>0.3</v>
-      </c>
-      <c r="Q2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>113</v>
       </c>
@@ -6238,10 +6186,10 @@
         <v>1</v>
       </c>
       <c r="K3">
-        <v>1</v>
+        <v>0.83</v>
       </c>
       <c r="L3">
-        <v>1</v>
+        <v>0.83</v>
       </c>
       <c r="M3">
         <v>0.83</v>
@@ -6250,16 +6198,10 @@
         <v>0.83</v>
       </c>
       <c r="O3">
-        <v>0.83</v>
-      </c>
-      <c r="P3">
-        <v>0.83</v>
-      </c>
-      <c r="Q3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>118</v>
       </c>
@@ -6291,10 +6233,10 @@
         <v>0.73</v>
       </c>
       <c r="K4">
-        <v>0.73</v>
+        <v>1</v>
       </c>
       <c r="L4">
-        <v>0.73</v>
+        <v>1</v>
       </c>
       <c r="M4">
         <v>1</v>
@@ -6305,14 +6247,8 @@
       <c r="O4">
         <v>1</v>
       </c>
-      <c r="P4">
-        <v>1</v>
-      </c>
-      <c r="Q4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.15">
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>119</v>
       </c>
@@ -6344,10 +6280,10 @@
         <v>0.73</v>
       </c>
       <c r="K5">
-        <v>0.73</v>
+        <v>1</v>
       </c>
       <c r="L5">
-        <v>0.73</v>
+        <v>1</v>
       </c>
       <c r="M5">
         <v>1</v>
@@ -6358,14 +6294,8 @@
       <c r="O5">
         <v>1</v>
       </c>
-      <c r="P5">
-        <v>1</v>
-      </c>
-      <c r="Q5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.15">
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>120</v>
       </c>
@@ -6397,10 +6327,10 @@
         <v>0.73</v>
       </c>
       <c r="K6">
-        <v>0.73</v>
+        <v>1</v>
       </c>
       <c r="L6">
-        <v>0.73</v>
+        <v>1</v>
       </c>
       <c r="M6">
         <v>1</v>
@@ -6411,14 +6341,8 @@
       <c r="O6">
         <v>1</v>
       </c>
-      <c r="P6">
-        <v>1</v>
-      </c>
-      <c r="Q6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.15">
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>121</v>
       </c>
@@ -6450,10 +6374,10 @@
         <v>0.73</v>
       </c>
       <c r="K7">
-        <v>0.73</v>
+        <v>1</v>
       </c>
       <c r="L7">
-        <v>0.73</v>
+        <v>1</v>
       </c>
       <c r="M7">
         <v>1</v>
@@ -6464,14 +6388,8 @@
       <c r="O7">
         <v>1</v>
       </c>
-      <c r="P7">
-        <v>1</v>
-      </c>
-      <c r="Q7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.15">
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>122</v>
       </c>
@@ -6503,10 +6421,10 @@
         <v>0.73</v>
       </c>
       <c r="K8">
-        <v>0.73</v>
+        <v>1</v>
       </c>
       <c r="L8">
-        <v>0.73</v>
+        <v>1</v>
       </c>
       <c r="M8">
         <v>1</v>
@@ -6517,14 +6435,8 @@
       <c r="O8">
         <v>1</v>
       </c>
-      <c r="P8">
-        <v>1</v>
-      </c>
-      <c r="Q8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.15">
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>123</v>
       </c>
@@ -6556,10 +6468,10 @@
         <v>0.73</v>
       </c>
       <c r="K9">
-        <v>0.73</v>
+        <v>1</v>
       </c>
       <c r="L9">
-        <v>0.73</v>
+        <v>1</v>
       </c>
       <c r="M9">
         <v>1</v>
@@ -6570,14 +6482,8 @@
       <c r="O9">
         <v>1</v>
       </c>
-      <c r="P9">
-        <v>1</v>
-      </c>
-      <c r="Q9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.15">
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>124</v>
       </c>
@@ -6609,10 +6515,10 @@
         <v>0.73</v>
       </c>
       <c r="K10">
-        <v>0.73</v>
+        <v>1</v>
       </c>
       <c r="L10">
-        <v>0.73</v>
+        <v>1</v>
       </c>
       <c r="M10">
         <v>1</v>
@@ -6621,12 +6527,6 @@
         <v>1</v>
       </c>
       <c r="O10">
-        <v>1</v>
-      </c>
-      <c r="P10">
-        <v>1</v>
-      </c>
-      <c r="Q10">
         <v>1</v>
       </c>
     </row>
@@ -6777,10 +6677,10 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q45" sqref="Q45"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6788,7 +6688,7 @@
     <col min="1" max="1" width="19.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>56</v>
       </c>
@@ -6807,41 +6707,35 @@
       <c r="F1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="41" t="s">
+      <c r="G1" t="s">
         <v>126</v>
       </c>
-      <c r="H1" s="41" t="s">
+      <c r="H1" t="s">
+        <v>140</v>
+      </c>
+      <c r="I1" t="s">
+        <v>141</v>
+      </c>
+      <c r="J1" t="s">
+        <v>142</v>
+      </c>
+      <c r="K1" t="s">
         <v>127</v>
       </c>
-      <c r="I1" s="41" t="s">
+      <c r="L1" t="s">
         <v>128</v>
       </c>
-      <c r="J1" s="41" t="s">
+      <c r="M1" t="s">
         <v>129</v>
       </c>
-      <c r="K1" s="41" t="s">
+      <c r="N1" t="s">
         <v>130</v>
       </c>
-      <c r="L1" s="41" t="s">
-        <v>131</v>
-      </c>
-      <c r="M1" s="41" t="s">
-        <v>132</v>
-      </c>
-      <c r="N1" s="41" t="s">
-        <v>133</v>
-      </c>
-      <c r="O1" s="41" t="s">
-        <v>134</v>
-      </c>
-      <c r="P1" s="41" t="s">
-        <v>135</v>
-      </c>
-      <c r="Q1" s="41" t="s">
+      <c r="O1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>115</v>
       </c>
@@ -6884,17 +6778,11 @@
       <c r="N2">
         <v>1</v>
       </c>
-      <c r="O2">
-        <v>1</v>
-      </c>
-      <c r="P2">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="42">
+      <c r="O2" s="42">
         <v>0.97599999999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>116</v>
       </c>
@@ -6937,17 +6825,11 @@
       <c r="N3">
         <v>1</v>
       </c>
-      <c r="O3">
-        <v>1</v>
-      </c>
-      <c r="P3">
-        <v>1</v>
-      </c>
-      <c r="Q3" s="42">
+      <c r="O3" s="42">
         <v>0.97599999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>117</v>
       </c>
@@ -6990,13 +6872,7 @@
       <c r="N4">
         <v>1</v>
       </c>
-      <c r="O4">
-        <v>1</v>
-      </c>
-      <c r="P4">
-        <v>1</v>
-      </c>
-      <c r="Q4" s="42">
+      <c r="O4" s="42">
         <v>0.97599999999999998</v>
       </c>
     </row>
@@ -7869,10 +7745,10 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q32"/>
+  <dimension ref="A1:O32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K34" sqref="K34"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7884,7 +7760,7 @@
     <col min="9" max="9" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="6" t="s">
         <v>56</v>
       </c>
@@ -7903,41 +7779,35 @@
       <c r="F1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="41" t="s">
+      <c r="G1" t="s">
         <v>126</v>
       </c>
-      <c r="H1" s="41" t="s">
+      <c r="H1" t="s">
+        <v>140</v>
+      </c>
+      <c r="I1" t="s">
+        <v>141</v>
+      </c>
+      <c r="J1" t="s">
+        <v>142</v>
+      </c>
+      <c r="K1" t="s">
         <v>127</v>
       </c>
-      <c r="I1" s="41" t="s">
+      <c r="L1" t="s">
         <v>128</v>
       </c>
-      <c r="J1" s="41" t="s">
+      <c r="M1" t="s">
         <v>129</v>
       </c>
-      <c r="K1" s="41" t="s">
+      <c r="N1" t="s">
         <v>130</v>
       </c>
-      <c r="L1" s="41" t="s">
-        <v>131</v>
-      </c>
-      <c r="M1" s="41" t="s">
-        <v>132</v>
-      </c>
-      <c r="N1" s="41" t="s">
-        <v>133</v>
-      </c>
-      <c r="O1" s="41" t="s">
-        <v>134</v>
-      </c>
-      <c r="P1" s="41" t="s">
-        <v>135</v>
-      </c>
-      <c r="Q1" s="41" t="s">
+      <c r="O1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
         <v>64</v>
       </c>
@@ -7983,14 +7853,8 @@
       <c r="O2" s="44">
         <v>0</v>
       </c>
-      <c r="P2" s="44">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
         <v>74</v>
       </c>
@@ -8036,14 +7900,8 @@
       <c r="O3" s="44">
         <v>0</v>
       </c>
-      <c r="P3" s="44">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
         <v>75</v>
       </c>
@@ -8091,14 +7949,8 @@
       <c r="O4" s="44">
         <v>0</v>
       </c>
-      <c r="P4" s="44">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
         <v>73</v>
       </c>
@@ -8130,10 +7982,10 @@
         <v>0</v>
       </c>
       <c r="K5" s="44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L5" s="44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M5" s="44">
         <v>1</v>
@@ -8142,16 +7994,10 @@
         <v>1</v>
       </c>
       <c r="O5" s="44">
-        <v>1</v>
-      </c>
-      <c r="P5" s="44">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>76</v>
       </c>
@@ -8182,11 +8028,13 @@
       <c r="J6" s="44">
         <v>0</v>
       </c>
-      <c r="K6" s="44">
-        <v>0</v>
-      </c>
-      <c r="L6" s="44">
-        <v>0</v>
+      <c r="K6" s="43">
+        <f>demographics!$B$7</f>
+        <v>0.4</v>
+      </c>
+      <c r="L6" s="43">
+        <f>demographics!$B$7</f>
+        <v>0.4</v>
       </c>
       <c r="M6" s="43">
         <f>demographics!$B$7</f>
@@ -8196,19 +8044,11 @@
         <f>demographics!$B$7</f>
         <v>0.4</v>
       </c>
-      <c r="O6" s="43">
-        <f>demographics!$B$7</f>
-        <v>0.4</v>
-      </c>
-      <c r="P6" s="43">
-        <f>demographics!$B$7</f>
-        <v>0.4</v>
-      </c>
-      <c r="Q6" s="44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="O6" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>78</v>
       </c>
@@ -8240,10 +8080,10 @@
         <v>0</v>
       </c>
       <c r="K7" s="44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L7" s="44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M7" s="44">
         <v>1</v>
@@ -8252,16 +8092,10 @@
         <v>1</v>
       </c>
       <c r="O7" s="44">
-        <v>1</v>
-      </c>
-      <c r="P7" s="44">
-        <v>1</v>
-      </c>
-      <c r="Q7" s="44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="29" t="s">
         <v>89</v>
       </c>
@@ -8292,11 +8126,11 @@
       <c r="J8" s="44">
         <v>0</v>
       </c>
-      <c r="K8" s="44">
-        <v>0</v>
-      </c>
-      <c r="L8" s="44">
-        <v>0</v>
+      <c r="K8" s="46">
+        <v>1</v>
+      </c>
+      <c r="L8" s="46">
+        <v>1</v>
       </c>
       <c r="M8" s="46">
         <v>1</v>
@@ -8304,17 +8138,11 @@
       <c r="N8" s="46">
         <v>1</v>
       </c>
-      <c r="O8" s="46">
-        <v>1</v>
-      </c>
-      <c r="P8" s="46">
-        <v>1</v>
-      </c>
-      <c r="Q8" s="44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="O8" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="29" t="s">
         <v>90</v>
       </c>
@@ -8345,11 +8173,11 @@
       <c r="J9" s="44">
         <v>0</v>
       </c>
-      <c r="K9" s="44">
-        <v>0</v>
-      </c>
-      <c r="L9" s="44">
-        <v>0</v>
+      <c r="K9" s="46">
+        <v>1</v>
+      </c>
+      <c r="L9" s="46">
+        <v>1</v>
       </c>
       <c r="M9" s="46">
         <v>1</v>
@@ -8357,17 +8185,11 @@
       <c r="N9" s="46">
         <v>1</v>
       </c>
-      <c r="O9" s="46">
-        <v>1</v>
-      </c>
-      <c r="P9" s="46">
-        <v>1</v>
-      </c>
-      <c r="Q9" s="44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="O9" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="29" t="s">
         <v>91</v>
       </c>
@@ -8398,11 +8220,11 @@
       <c r="J10" s="44">
         <v>0</v>
       </c>
-      <c r="K10" s="44">
-        <v>0</v>
-      </c>
-      <c r="L10" s="44">
-        <v>0</v>
+      <c r="K10" s="46">
+        <v>1</v>
+      </c>
+      <c r="L10" s="46">
+        <v>1</v>
       </c>
       <c r="M10" s="46">
         <v>1</v>
@@ -8410,17 +8232,11 @@
       <c r="N10" s="46">
         <v>1</v>
       </c>
-      <c r="O10" s="46">
-        <v>1</v>
-      </c>
-      <c r="P10" s="46">
-        <v>1</v>
-      </c>
-      <c r="Q10" s="44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="O10" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="29" t="s">
         <v>92</v>
       </c>
@@ -8451,11 +8267,11 @@
       <c r="J11" s="44">
         <v>0</v>
       </c>
-      <c r="K11" s="44">
-        <v>0</v>
-      </c>
-      <c r="L11" s="44">
-        <v>0</v>
+      <c r="K11" s="46">
+        <v>1</v>
+      </c>
+      <c r="L11" s="46">
+        <v>1</v>
       </c>
       <c r="M11" s="46">
         <v>1</v>
@@ -8463,17 +8279,11 @@
       <c r="N11" s="46">
         <v>1</v>
       </c>
-      <c r="O11" s="46">
-        <v>1</v>
-      </c>
-      <c r="P11" s="46">
-        <v>1</v>
-      </c>
-      <c r="Q11" s="44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="O11" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="29" t="s">
         <v>93</v>
       </c>
@@ -8504,11 +8314,11 @@
       <c r="J12" s="44">
         <v>0</v>
       </c>
-      <c r="K12" s="44">
-        <v>0</v>
-      </c>
-      <c r="L12" s="44">
-        <v>0</v>
+      <c r="K12" s="46">
+        <v>1</v>
+      </c>
+      <c r="L12" s="46">
+        <v>1</v>
       </c>
       <c r="M12" s="46">
         <v>1</v>
@@ -8516,17 +8326,11 @@
       <c r="N12" s="46">
         <v>1</v>
       </c>
-      <c r="O12" s="46">
-        <v>1</v>
-      </c>
-      <c r="P12" s="46">
-        <v>1</v>
-      </c>
-      <c r="Q12" s="44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="O12" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="29" t="s">
         <v>94</v>
       </c>
@@ -8557,11 +8361,11 @@
       <c r="J13" s="44">
         <v>0</v>
       </c>
-      <c r="K13" s="44">
-        <v>0</v>
-      </c>
-      <c r="L13" s="44">
-        <v>0</v>
+      <c r="K13" s="46">
+        <v>1</v>
+      </c>
+      <c r="L13" s="46">
+        <v>1</v>
       </c>
       <c r="M13" s="46">
         <v>1</v>
@@ -8569,17 +8373,11 @@
       <c r="N13" s="46">
         <v>1</v>
       </c>
-      <c r="O13" s="46">
-        <v>1</v>
-      </c>
-      <c r="P13" s="46">
-        <v>1</v>
-      </c>
-      <c r="Q13" s="44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="O13" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="29" t="s">
         <v>95</v>
       </c>
@@ -8610,11 +8408,11 @@
       <c r="J14" s="44">
         <v>0</v>
       </c>
-      <c r="K14" s="44">
-        <v>0</v>
-      </c>
-      <c r="L14" s="44">
-        <v>0</v>
+      <c r="K14" s="47">
+        <v>1</v>
+      </c>
+      <c r="L14" s="47">
+        <v>1</v>
       </c>
       <c r="M14" s="47">
         <v>1</v>
@@ -8622,17 +8420,11 @@
       <c r="N14" s="47">
         <v>1</v>
       </c>
-      <c r="O14" s="47">
-        <v>1</v>
-      </c>
-      <c r="P14" s="47">
-        <v>1</v>
-      </c>
-      <c r="Q14" s="44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="O14" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="29" t="s">
         <v>96</v>
       </c>
@@ -8663,11 +8455,11 @@
       <c r="J15" s="44">
         <v>0</v>
       </c>
-      <c r="K15" s="44">
-        <v>0</v>
-      </c>
-      <c r="L15" s="44">
-        <v>0</v>
+      <c r="K15" s="47">
+        <v>1</v>
+      </c>
+      <c r="L15" s="47">
+        <v>1</v>
       </c>
       <c r="M15" s="47">
         <v>1</v>
@@ -8675,17 +8467,11 @@
       <c r="N15" s="47">
         <v>1</v>
       </c>
-      <c r="O15" s="47">
-        <v>1</v>
-      </c>
-      <c r="P15" s="47">
-        <v>1</v>
-      </c>
-      <c r="Q15" s="44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="O15" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="29" t="s">
         <v>97</v>
       </c>
@@ -8716,11 +8502,11 @@
       <c r="J16" s="44">
         <v>0</v>
       </c>
-      <c r="K16" s="44">
-        <v>0</v>
-      </c>
-      <c r="L16" s="44">
-        <v>0</v>
+      <c r="K16" s="47">
+        <v>1</v>
+      </c>
+      <c r="L16" s="47">
+        <v>1</v>
       </c>
       <c r="M16" s="47">
         <v>1</v>
@@ -8728,17 +8514,11 @@
       <c r="N16" s="47">
         <v>1</v>
       </c>
-      <c r="O16" s="47">
-        <v>1</v>
-      </c>
-      <c r="P16" s="47">
-        <v>1</v>
-      </c>
-      <c r="Q16" s="44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="O16" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="23" t="s">
         <v>99</v>
       </c>
@@ -8769,11 +8549,11 @@
       <c r="J17" s="44">
         <v>0</v>
       </c>
-      <c r="K17" s="44">
-        <v>0</v>
-      </c>
-      <c r="L17" s="44">
-        <v>0</v>
+      <c r="K17" s="46">
+        <v>1</v>
+      </c>
+      <c r="L17" s="46">
+        <v>1</v>
       </c>
       <c r="M17" s="46">
         <v>1</v>
@@ -8781,17 +8561,11 @@
       <c r="N17" s="46">
         <v>1</v>
       </c>
-      <c r="O17" s="46">
-        <v>1</v>
-      </c>
-      <c r="P17" s="46">
-        <v>1</v>
-      </c>
-      <c r="Q17" s="44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="O17" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="23" t="s">
         <v>103</v>
       </c>
@@ -8822,11 +8596,11 @@
       <c r="J18" s="44">
         <v>0</v>
       </c>
-      <c r="K18" s="44">
-        <v>0</v>
-      </c>
-      <c r="L18" s="44">
-        <v>0</v>
+      <c r="K18" s="47">
+        <v>1</v>
+      </c>
+      <c r="L18" s="47">
+        <v>1</v>
       </c>
       <c r="M18" s="47">
         <v>1</v>
@@ -8834,17 +8608,11 @@
       <c r="N18" s="47">
         <v>1</v>
       </c>
-      <c r="O18" s="47">
-        <v>1</v>
-      </c>
-      <c r="P18" s="47">
-        <v>1</v>
-      </c>
-      <c r="Q18" s="44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="O18" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="23" t="s">
         <v>100</v>
       </c>
@@ -8875,11 +8643,11 @@
       <c r="J19" s="44">
         <v>0</v>
       </c>
-      <c r="K19" s="44">
-        <v>0</v>
-      </c>
-      <c r="L19" s="44">
-        <v>0</v>
+      <c r="K19" s="47">
+        <v>1</v>
+      </c>
+      <c r="L19" s="47">
+        <v>1</v>
       </c>
       <c r="M19" s="47">
         <v>1</v>
@@ -8887,17 +8655,11 @@
       <c r="N19" s="47">
         <v>1</v>
       </c>
-      <c r="O19" s="47">
-        <v>1</v>
-      </c>
-      <c r="P19" s="47">
-        <v>1</v>
-      </c>
-      <c r="Q19" s="44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="O19" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="23" t="s">
         <v>101</v>
       </c>
@@ -8928,11 +8690,11 @@
       <c r="J20" s="44">
         <v>0</v>
       </c>
-      <c r="K20" s="44">
-        <v>0</v>
-      </c>
-      <c r="L20" s="44">
-        <v>0</v>
+      <c r="K20" s="47">
+        <v>1</v>
+      </c>
+      <c r="L20" s="47">
+        <v>1</v>
       </c>
       <c r="M20" s="47">
         <v>1</v>
@@ -8940,17 +8702,11 @@
       <c r="N20" s="47">
         <v>1</v>
       </c>
-      <c r="O20" s="47">
-        <v>1</v>
-      </c>
-      <c r="P20" s="47">
-        <v>1</v>
-      </c>
-      <c r="Q20" s="44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O20" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="14" t="s">
         <v>102</v>
       </c>
@@ -8981,11 +8737,11 @@
       <c r="J21" s="44">
         <v>0</v>
       </c>
-      <c r="K21" s="44">
-        <v>0</v>
-      </c>
-      <c r="L21" s="44">
-        <v>0</v>
+      <c r="K21" s="49">
+        <v>1</v>
+      </c>
+      <c r="L21" s="49">
+        <v>1</v>
       </c>
       <c r="M21" s="49">
         <v>1</v>
@@ -8993,17 +8749,11 @@
       <c r="N21" s="49">
         <v>1</v>
       </c>
-      <c r="O21" s="49">
-        <v>1</v>
-      </c>
-      <c r="P21" s="49">
-        <v>1</v>
-      </c>
-      <c r="Q21" s="44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="O21" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>113</v>
       </c>
@@ -9034,11 +8784,13 @@
       <c r="J22" s="50">
         <v>0</v>
       </c>
-      <c r="K22" s="50">
-        <v>0</v>
-      </c>
-      <c r="L22" s="50">
-        <v>0</v>
+      <c r="K22" s="45">
+        <f>'Frac exposed malaria'!J2</f>
+        <v>0.5</v>
+      </c>
+      <c r="L22" s="45">
+        <f>'Frac exposed malaria'!K2</f>
+        <v>0.5</v>
       </c>
       <c r="M22" s="45">
         <f>'Frac exposed malaria'!L2</f>
@@ -9048,19 +8800,11 @@
         <f>'Frac exposed malaria'!M2</f>
         <v>0.5</v>
       </c>
-      <c r="O22" s="45">
-        <f>'Frac exposed malaria'!N2</f>
-        <v>0.5</v>
-      </c>
-      <c r="P22" s="45">
-        <f>'Frac exposed malaria'!O2</f>
-        <v>0.5</v>
-      </c>
-      <c r="Q22" s="50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="O22" s="50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>118</v>
       </c>
@@ -9095,13 +8839,11 @@
         <f>1*demographics!B7</f>
         <v>0.4</v>
       </c>
-      <c r="K23" s="43">
-        <f>1*demographics!B7</f>
-        <v>0.4</v>
-      </c>
-      <c r="L23" s="43">
-        <f>1*demographics!B7</f>
-        <v>0.4</v>
+      <c r="K23" s="44">
+        <v>0</v>
+      </c>
+      <c r="L23" s="44">
+        <v>0</v>
       </c>
       <c r="M23" s="44">
         <v>0</v>
@@ -9109,17 +8851,11 @@
       <c r="N23" s="44">
         <v>0</v>
       </c>
-      <c r="O23" s="44">
-        <v>0</v>
-      </c>
-      <c r="P23" s="44">
-        <v>0</v>
-      </c>
-      <c r="Q23" s="50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="O23" s="50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>119</v>
       </c>
@@ -9154,13 +8890,11 @@
         <f>1*demographics!B7</f>
         <v>0.4</v>
       </c>
-      <c r="K24" s="43">
-        <f>1*demographics!B7</f>
-        <v>0.4</v>
-      </c>
-      <c r="L24" s="43">
-        <f>1*demographics!B7</f>
-        <v>0.4</v>
+      <c r="K24" s="44">
+        <v>0</v>
+      </c>
+      <c r="L24" s="44">
+        <v>0</v>
       </c>
       <c r="M24" s="44">
         <v>0</v>
@@ -9168,17 +8902,11 @@
       <c r="N24" s="44">
         <v>0</v>
       </c>
-      <c r="O24" s="44">
-        <v>0</v>
-      </c>
-      <c r="P24" s="44">
-        <v>0</v>
-      </c>
-      <c r="Q24" s="50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="O24" s="50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>120</v>
       </c>
@@ -9213,13 +8941,11 @@
         <f>1*demographics!B7</f>
         <v>0.4</v>
       </c>
-      <c r="K25" s="43">
-        <f>1*demographics!B7</f>
-        <v>0.4</v>
-      </c>
-      <c r="L25" s="43">
-        <f>1*demographics!B7</f>
-        <v>0.4</v>
+      <c r="K25" s="44">
+        <v>0</v>
+      </c>
+      <c r="L25" s="44">
+        <v>0</v>
       </c>
       <c r="M25" s="44">
         <v>0</v>
@@ -9227,17 +8953,11 @@
       <c r="N25" s="44">
         <v>0</v>
       </c>
-      <c r="O25" s="44">
-        <v>0</v>
-      </c>
-      <c r="P25" s="44">
-        <v>0</v>
-      </c>
-      <c r="Q25" s="50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="O25" s="50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>121</v>
       </c>
@@ -9272,13 +8992,11 @@
         <f>1*(1-demographics!B7)</f>
         <v>0.6</v>
       </c>
-      <c r="K26" s="43">
-        <f>1*(1-demographics!B7)</f>
-        <v>0.6</v>
-      </c>
-      <c r="L26" s="43">
-        <f>1*(1-demographics!B7)</f>
-        <v>0.6</v>
+      <c r="K26" s="44">
+        <v>0</v>
+      </c>
+      <c r="L26" s="44">
+        <v>0</v>
       </c>
       <c r="M26" s="44">
         <v>0</v>
@@ -9286,17 +9004,11 @@
       <c r="N26" s="44">
         <v>0</v>
       </c>
-      <c r="O26" s="44">
-        <v>0</v>
-      </c>
-      <c r="P26" s="44">
-        <v>0</v>
-      </c>
-      <c r="Q26" s="50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="O26" s="50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>122</v>
       </c>
@@ -9331,13 +9043,11 @@
         <f>1*(1-demographics!B7)</f>
         <v>0.6</v>
       </c>
-      <c r="K27" s="43">
-        <f>1*(1-demographics!B7)</f>
-        <v>0.6</v>
-      </c>
-      <c r="L27" s="43">
-        <f>1*(1-demographics!B7)</f>
-        <v>0.6</v>
+      <c r="K27" s="44">
+        <v>0</v>
+      </c>
+      <c r="L27" s="44">
+        <v>0</v>
       </c>
       <c r="M27" s="44">
         <v>0</v>
@@ -9345,17 +9055,11 @@
       <c r="N27" s="44">
         <v>0</v>
       </c>
-      <c r="O27" s="44">
-        <v>0</v>
-      </c>
-      <c r="P27" s="44">
-        <v>0</v>
-      </c>
-      <c r="Q27" s="50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="O27" s="50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>123</v>
       </c>
@@ -9390,13 +9094,11 @@
         <f>1*(1-demographics!B7)</f>
         <v>0.6</v>
       </c>
-      <c r="K28" s="43">
-        <f>1*(1-demographics!B7)</f>
-        <v>0.6</v>
-      </c>
-      <c r="L28" s="43">
-        <f>1*(1-demographics!B7)</f>
-        <v>0.6</v>
+      <c r="K28" s="44">
+        <v>0</v>
+      </c>
+      <c r="L28" s="44">
+        <v>0</v>
       </c>
       <c r="M28" s="44">
         <v>0</v>
@@ -9404,17 +9106,11 @@
       <c r="N28" s="44">
         <v>0</v>
       </c>
-      <c r="O28" s="44">
-        <v>0</v>
-      </c>
-      <c r="P28" s="44">
-        <v>0</v>
-      </c>
-      <c r="Q28" s="50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="O28" s="50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>124</v>
       </c>
@@ -9449,13 +9145,11 @@
         <f>1*(1-demographics!B7)</f>
         <v>0.6</v>
       </c>
-      <c r="K29" s="43">
-        <f>1*(1-demographics!B7)</f>
-        <v>0.6</v>
-      </c>
-      <c r="L29" s="43">
-        <f>1*(1-demographics!B7)</f>
-        <v>0.6</v>
+      <c r="K29" s="44">
+        <v>0</v>
+      </c>
+      <c r="L29" s="44">
+        <v>0</v>
       </c>
       <c r="M29" s="44">
         <v>0</v>
@@ -9463,17 +9157,11 @@
       <c r="N29" s="44">
         <v>0</v>
       </c>
-      <c r="O29" s="44">
-        <v>0</v>
-      </c>
-      <c r="P29" s="44">
-        <v>0</v>
-      </c>
-      <c r="Q29" s="50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="O29" s="50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>115</v>
       </c>
@@ -9517,16 +9205,10 @@
         <v>0</v>
       </c>
       <c r="O30" s="50">
-        <v>0</v>
-      </c>
-      <c r="P30" s="50">
-        <v>0</v>
-      </c>
-      <c r="Q30" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>116</v>
       </c>
@@ -9570,16 +9252,10 @@
         <v>0</v>
       </c>
       <c r="O31" s="50">
-        <v>0</v>
-      </c>
-      <c r="P31" s="50">
-        <v>0</v>
-      </c>
-      <c r="Q31" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>117</v>
       </c>
@@ -9623,12 +9299,6 @@
         <v>0</v>
       </c>
       <c r="O32" s="50">
-        <v>0</v>
-      </c>
-      <c r="P32" s="50">
-        <v>0</v>
-      </c>
-      <c r="Q32" s="50">
         <v>1</v>
       </c>
     </row>
@@ -9755,10 +9425,10 @@
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q12"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="H1:Q1"/>
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -9767,7 +9437,7 @@
     <col min="2" max="2" width="28.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="6" t="s">
         <v>67</v>
       </c>
@@ -9789,38 +9459,32 @@
       <c r="G1" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="41" t="s">
+      <c r="H1" t="s">
         <v>126</v>
       </c>
-      <c r="I1" s="41" t="s">
+      <c r="I1" t="s">
+        <v>140</v>
+      </c>
+      <c r="J1" t="s">
+        <v>141</v>
+      </c>
+      <c r="K1" t="s">
+        <v>142</v>
+      </c>
+      <c r="L1" t="s">
         <v>127</v>
       </c>
-      <c r="J1" s="41" t="s">
+      <c r="M1" t="s">
         <v>128</v>
       </c>
-      <c r="K1" s="41" t="s">
+      <c r="N1" t="s">
         <v>129</v>
       </c>
-      <c r="L1" s="41" t="s">
+      <c r="O1" t="s">
         <v>130</v>
       </c>
-      <c r="M1" s="41" t="s">
-        <v>131</v>
-      </c>
-      <c r="N1" s="41" t="s">
-        <v>132</v>
-      </c>
-      <c r="O1" s="41" t="s">
-        <v>133</v>
-      </c>
-      <c r="P1" s="41" t="s">
-        <v>134</v>
-      </c>
-      <c r="Q1" s="41" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
         <v>64</v>
       </c>
@@ -9866,14 +9530,8 @@
       <c r="O2" s="6">
         <v>0</v>
       </c>
-      <c r="P2" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="32" t="s">
         <v>36</v>
       </c>
@@ -9916,14 +9574,8 @@
       <c r="O3" s="6">
         <v>0</v>
       </c>
-      <c r="P3" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="29" t="s">
         <v>89</v>
       </c>
@@ -9957,11 +9609,11 @@
       <c r="K4" s="6">
         <v>0</v>
       </c>
-      <c r="L4" s="6">
-        <v>0</v>
-      </c>
-      <c r="M4" s="6">
-        <v>0</v>
+      <c r="L4" s="29">
+        <v>4.895E-3</v>
+      </c>
+      <c r="M4" s="29">
+        <v>4.895E-3</v>
       </c>
       <c r="N4" s="29">
         <v>4.895E-3</v>
@@ -9969,14 +9621,8 @@
       <c r="O4" s="29">
         <v>4.895E-3</v>
       </c>
-      <c r="P4" s="29">
-        <v>4.895E-3</v>
-      </c>
-      <c r="Q4" s="29">
-        <v>4.895E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="29" t="s">
         <v>90</v>
       </c>
@@ -10010,11 +9656,11 @@
       <c r="K5" s="6">
         <v>0</v>
       </c>
-      <c r="L5" s="6">
-        <v>0</v>
-      </c>
-      <c r="M5" s="6">
-        <v>0</v>
+      <c r="L5" s="29">
+        <v>2.0998000000000003E-2</v>
+      </c>
+      <c r="M5" s="29">
+        <v>2.0998000000000003E-2</v>
       </c>
       <c r="N5" s="29">
         <v>2.0998000000000003E-2</v>
@@ -10022,14 +9668,8 @@
       <c r="O5" s="29">
         <v>2.0998000000000003E-2</v>
       </c>
-      <c r="P5" s="29">
-        <v>2.0998000000000003E-2</v>
-      </c>
-      <c r="Q5" s="29">
-        <v>2.0998000000000003E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="29" t="s">
         <v>91</v>
       </c>
@@ -10063,11 +9703,11 @@
       <c r="K6" s="6">
         <v>0</v>
       </c>
-      <c r="L6" s="6">
-        <v>0</v>
-      </c>
-      <c r="M6" s="6">
-        <v>0</v>
+      <c r="L6" s="29">
+        <v>1</v>
+      </c>
+      <c r="M6" s="29">
+        <v>1</v>
       </c>
       <c r="N6" s="29">
         <v>1</v>
@@ -10075,14 +9715,8 @@
       <c r="O6" s="29">
         <v>1</v>
       </c>
-      <c r="P6" s="29">
-        <v>1</v>
-      </c>
-      <c r="Q6" s="29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="29" t="s">
         <v>92</v>
       </c>
@@ -10116,11 +9750,11 @@
       <c r="K7" s="6">
         <v>0</v>
       </c>
-      <c r="L7" s="6">
-        <v>0</v>
-      </c>
-      <c r="M7" s="6">
-        <v>0</v>
+      <c r="L7" s="29">
+        <v>1</v>
+      </c>
+      <c r="M7" s="29">
+        <v>1</v>
       </c>
       <c r="N7" s="29">
         <v>1</v>
@@ -10128,14 +9762,8 @@
       <c r="O7" s="29">
         <v>1</v>
       </c>
-      <c r="P7" s="29">
-        <v>1</v>
-      </c>
-      <c r="Q7" s="29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="29" t="s">
         <v>93</v>
       </c>
@@ -10169,11 +9797,11 @@
       <c r="K8" s="6">
         <v>0</v>
       </c>
-      <c r="L8" s="6">
-        <v>0</v>
-      </c>
-      <c r="M8" s="6">
-        <v>0</v>
+      <c r="L8" s="29">
+        <v>1</v>
+      </c>
+      <c r="M8" s="29">
+        <v>1</v>
       </c>
       <c r="N8" s="29">
         <v>1</v>
@@ -10181,14 +9809,8 @@
       <c r="O8" s="29">
         <v>1</v>
       </c>
-      <c r="P8" s="29">
-        <v>1</v>
-      </c>
-      <c r="Q8" s="29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="29" t="s">
         <v>94</v>
       </c>
@@ -10222,11 +9844,11 @@
       <c r="K9" s="6">
         <v>0</v>
       </c>
-      <c r="L9" s="6">
-        <v>0</v>
-      </c>
-      <c r="M9" s="6">
-        <v>0</v>
+      <c r="L9" s="29">
+        <v>1</v>
+      </c>
+      <c r="M9" s="29">
+        <v>1</v>
       </c>
       <c r="N9" s="29">
         <v>1</v>
@@ -10234,14 +9856,8 @@
       <c r="O9" s="29">
         <v>1</v>
       </c>
-      <c r="P9" s="29">
-        <v>1</v>
-      </c>
-      <c r="Q9" s="29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="29" t="s">
         <v>95</v>
       </c>
@@ -10275,11 +9891,11 @@
       <c r="K10" s="6">
         <v>0</v>
       </c>
-      <c r="L10" s="6">
-        <v>0</v>
-      </c>
-      <c r="M10" s="6">
-        <v>0</v>
+      <c r="L10" s="29">
+        <v>0.90526300000000004</v>
+      </c>
+      <c r="M10" s="29">
+        <v>0.90526300000000004</v>
       </c>
       <c r="N10" s="29">
         <v>0.90526300000000004</v>
@@ -10287,14 +9903,8 @@
       <c r="O10" s="29">
         <v>0.90526300000000004</v>
       </c>
-      <c r="P10" s="29">
-        <v>0.90526300000000004</v>
-      </c>
-      <c r="Q10" s="29">
-        <v>0.90526300000000004</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="29" t="s">
         <v>96</v>
       </c>
@@ -10328,11 +9938,11 @@
       <c r="K11" s="6">
         <v>0</v>
       </c>
-      <c r="L11" s="6">
-        <v>0</v>
-      </c>
-      <c r="M11" s="6">
-        <v>0</v>
+      <c r="L11" s="29">
+        <v>0.90526300000000004</v>
+      </c>
+      <c r="M11" s="29">
+        <v>0.90526300000000004</v>
       </c>
       <c r="N11" s="29">
         <v>0.90526300000000004</v>
@@ -10340,14 +9950,8 @@
       <c r="O11" s="29">
         <v>0.90526300000000004</v>
       </c>
-      <c r="P11" s="29">
-        <v>0.90526300000000004</v>
-      </c>
-      <c r="Q11" s="29">
-        <v>0.90526300000000004</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="29" t="s">
         <v>97</v>
       </c>
@@ -10381,22 +9985,16 @@
       <c r="K12" s="6">
         <v>0</v>
       </c>
-      <c r="L12" s="6">
-        <v>0</v>
-      </c>
-      <c r="M12" s="6">
-        <v>0</v>
+      <c r="L12" s="29">
+        <v>9.4737000000000016E-2</v>
+      </c>
+      <c r="M12" s="29">
+        <v>9.4737000000000016E-2</v>
       </c>
       <c r="N12" s="29">
         <v>9.4737000000000016E-2</v>
       </c>
       <c r="O12" s="29">
-        <v>9.4737000000000016E-2</v>
-      </c>
-      <c r="P12" s="29">
-        <v>9.4737000000000016E-2</v>
-      </c>
-      <c r="Q12" s="29">
         <v>9.4737000000000016E-2</v>
       </c>
     </row>
@@ -10409,15 +10007,15 @@
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -10433,41 +10031,35 @@
       <c r="E1" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="F1" t="s">
         <v>126</v>
       </c>
-      <c r="G1" s="41" t="s">
+      <c r="G1" t="s">
+        <v>140</v>
+      </c>
+      <c r="H1" t="s">
+        <v>141</v>
+      </c>
+      <c r="I1" t="s">
+        <v>142</v>
+      </c>
+      <c r="J1" t="s">
         <v>127</v>
       </c>
-      <c r="H1" s="41" t="s">
+      <c r="K1" t="s">
         <v>128</v>
       </c>
-      <c r="I1" s="41" t="s">
+      <c r="L1" t="s">
         <v>129</v>
       </c>
-      <c r="J1" s="41" t="s">
+      <c r="M1" t="s">
         <v>130</v>
       </c>
-      <c r="K1" s="41" t="s">
-        <v>131</v>
-      </c>
-      <c r="L1" s="41" t="s">
-        <v>132</v>
-      </c>
-      <c r="M1" s="41" t="s">
-        <v>133</v>
-      </c>
-      <c r="N1" s="41" t="s">
-        <v>134</v>
-      </c>
-      <c r="O1" s="41" t="s">
-        <v>135</v>
-      </c>
-      <c r="P1" s="41" t="s">
+      <c r="N1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>0.5</v>
       </c>
@@ -10508,12 +10100,6 @@
         <v>0.5</v>
       </c>
       <c r="N2">
-        <v>0.5</v>
-      </c>
-      <c r="O2">
-        <v>0.5</v>
-      </c>
-      <c r="P2">
         <v>0.5</v>
       </c>
     </row>
@@ -10679,15 +10265,15 @@
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -10703,41 +10289,35 @@
       <c r="E1" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="F1" t="s">
         <v>126</v>
       </c>
-      <c r="G1" s="41" t="s">
+      <c r="G1" t="s">
+        <v>140</v>
+      </c>
+      <c r="H1" t="s">
+        <v>141</v>
+      </c>
+      <c r="I1" t="s">
+        <v>142</v>
+      </c>
+      <c r="J1" t="s">
         <v>127</v>
       </c>
-      <c r="H1" s="41" t="s">
+      <c r="K1" t="s">
         <v>128</v>
       </c>
-      <c r="I1" s="41" t="s">
+      <c r="L1" t="s">
         <v>129</v>
       </c>
-      <c r="J1" s="41" t="s">
+      <c r="M1" t="s">
         <v>130</v>
       </c>
-      <c r="K1" s="41" t="s">
-        <v>131</v>
-      </c>
-      <c r="L1" s="41" t="s">
-        <v>132</v>
-      </c>
-      <c r="M1" s="41" t="s">
-        <v>133</v>
-      </c>
-      <c r="N1" s="41" t="s">
-        <v>134</v>
-      </c>
-      <c r="O1" s="41" t="s">
-        <v>135</v>
-      </c>
-      <c r="P1" s="41" t="s">
+      <c r="N1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>0.5</v>
       </c>
@@ -10778,12 +10358,6 @@
         <v>0.5</v>
       </c>
       <c r="N2">
-        <v>0.5</v>
-      </c>
-      <c r="O2">
-        <v>0.5</v>
-      </c>
-      <c r="P2">
         <v>0.5</v>
       </c>
     </row>
@@ -10795,15 +10369,15 @@
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -10819,41 +10393,35 @@
       <c r="E1" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="F1" t="s">
         <v>126</v>
       </c>
-      <c r="G1" s="41" t="s">
+      <c r="G1" t="s">
+        <v>140</v>
+      </c>
+      <c r="H1" t="s">
+        <v>141</v>
+      </c>
+      <c r="I1" t="s">
+        <v>142</v>
+      </c>
+      <c r="J1" t="s">
         <v>127</v>
       </c>
-      <c r="H1" s="41" t="s">
+      <c r="K1" t="s">
         <v>128</v>
       </c>
-      <c r="I1" s="41" t="s">
+      <c r="L1" t="s">
         <v>129</v>
       </c>
-      <c r="J1" s="41" t="s">
+      <c r="M1" t="s">
         <v>130</v>
       </c>
-      <c r="K1" s="41" t="s">
-        <v>131</v>
-      </c>
-      <c r="L1" s="41" t="s">
-        <v>132</v>
-      </c>
-      <c r="M1" s="41" t="s">
-        <v>133</v>
-      </c>
-      <c r="N1" s="41" t="s">
-        <v>134</v>
-      </c>
-      <c r="O1" s="41" t="s">
-        <v>135</v>
-      </c>
-      <c r="P1" s="41" t="s">
+      <c r="N1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>0.5</v>
       </c>
@@ -10894,12 +10462,6 @@
         <v>0.5</v>
       </c>
       <c r="N2">
-        <v>0.5</v>
-      </c>
-      <c r="O2">
-        <v>0.5</v>
-      </c>
-      <c r="P2">
         <v>0.5</v>
       </c>
     </row>
@@ -10911,15 +10473,15 @@
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S43" sqref="S43"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -10935,38 +10497,32 @@
       <c r="E1" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="F1" t="s">
         <v>126</v>
       </c>
-      <c r="G1" s="41" t="s">
+      <c r="G1" t="s">
+        <v>140</v>
+      </c>
+      <c r="H1" t="s">
+        <v>141</v>
+      </c>
+      <c r="I1" t="s">
+        <v>142</v>
+      </c>
+      <c r="J1" t="s">
         <v>127</v>
       </c>
-      <c r="H1" s="41" t="s">
+      <c r="K1" t="s">
         <v>128</v>
       </c>
-      <c r="I1" s="41" t="s">
+      <c r="L1" t="s">
         <v>129</v>
       </c>
-      <c r="J1" s="41" t="s">
+      <c r="M1" t="s">
         <v>130</v>
       </c>
-      <c r="K1" s="41" t="s">
-        <v>131</v>
-      </c>
-      <c r="L1" s="41" t="s">
-        <v>132</v>
-      </c>
-      <c r="M1" s="41" t="s">
-        <v>133</v>
-      </c>
-      <c r="N1" s="41" t="s">
-        <v>134</v>
-      </c>
-      <c r="O1" s="41" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.15">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>0.5</v>
       </c>
@@ -11004,12 +10560,6 @@
         <v>0.5</v>
       </c>
       <c r="M2">
-        <v>0.5</v>
-      </c>
-      <c r="N2">
-        <v>0.5</v>
-      </c>
-      <c r="O2">
         <v>0.5</v>
       </c>
     </row>
@@ -11021,10 +10571,10 @@
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q12"/>
+  <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -11033,7 +10583,7 @@
     <col min="2" max="2" width="27.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="6" t="s">
         <v>67</v>
       </c>
@@ -11055,38 +10605,32 @@
       <c r="G1" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="41" t="s">
+      <c r="H1" t="s">
         <v>126</v>
       </c>
-      <c r="I1" s="41" t="s">
+      <c r="I1" t="s">
+        <v>140</v>
+      </c>
+      <c r="J1" t="s">
+        <v>141</v>
+      </c>
+      <c r="K1" t="s">
+        <v>142</v>
+      </c>
+      <c r="L1" t="s">
         <v>127</v>
       </c>
-      <c r="J1" s="41" t="s">
+      <c r="M1" t="s">
         <v>128</v>
       </c>
-      <c r="K1" s="41" t="s">
+      <c r="N1" t="s">
         <v>129</v>
       </c>
-      <c r="L1" s="41" t="s">
+      <c r="O1" t="s">
         <v>130</v>
       </c>
-      <c r="M1" s="41" t="s">
-        <v>131</v>
-      </c>
-      <c r="N1" s="41" t="s">
-        <v>132</v>
-      </c>
-      <c r="O1" s="41" t="s">
-        <v>133</v>
-      </c>
-      <c r="P1" s="41" t="s">
-        <v>134</v>
-      </c>
-      <c r="Q1" s="41" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
         <v>64</v>
       </c>
@@ -11132,14 +10676,8 @@
       <c r="O2" s="6">
         <v>0</v>
       </c>
-      <c r="P2" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="6" t="s">
         <v>36</v>
       </c>
@@ -11182,19 +10720,13 @@
       <c r="O3" s="6">
         <v>0</v>
       </c>
-      <c r="P3" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="29" t="s">
         <v>89</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="C4" s="6">
         <v>0</v>
@@ -11223,11 +10755,11 @@
       <c r="K4" s="6">
         <v>0</v>
       </c>
-      <c r="L4" s="6">
-        <v>0</v>
-      </c>
-      <c r="M4" s="6">
-        <v>0</v>
+      <c r="L4" s="29">
+        <v>0.98</v>
+      </c>
+      <c r="M4" s="29">
+        <v>0.98</v>
       </c>
       <c r="N4" s="29">
         <v>0.98</v>
@@ -11235,19 +10767,13 @@
       <c r="O4" s="29">
         <v>0.98</v>
       </c>
-      <c r="P4" s="29">
-        <v>0.98</v>
-      </c>
-      <c r="Q4" s="29">
-        <v>0.98</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="29" t="s">
         <v>90</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="C5" s="6">
         <v>0</v>
@@ -11276,11 +10802,11 @@
       <c r="K5" s="6">
         <v>0</v>
       </c>
-      <c r="L5" s="6">
-        <v>0</v>
-      </c>
-      <c r="M5" s="6">
-        <v>0</v>
+      <c r="L5" s="29">
+        <v>0.8</v>
+      </c>
+      <c r="M5" s="29">
+        <v>0.8</v>
       </c>
       <c r="N5" s="29">
         <v>0.8</v>
@@ -11288,19 +10814,13 @@
       <c r="O5" s="29">
         <v>0.8</v>
       </c>
-      <c r="P5" s="29">
-        <v>0.8</v>
-      </c>
-      <c r="Q5" s="29">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="29" t="s">
         <v>91</v>
       </c>
       <c r="B6" s="29" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="C6" s="6">
         <v>0</v>
@@ -11329,11 +10849,11 @@
       <c r="K6" s="6">
         <v>0</v>
       </c>
-      <c r="L6" s="6">
-        <v>0</v>
-      </c>
-      <c r="M6" s="6">
-        <v>0</v>
+      <c r="L6" s="29">
+        <v>0.2</v>
+      </c>
+      <c r="M6" s="29">
+        <v>0.2</v>
       </c>
       <c r="N6" s="29">
         <v>0.2</v>
@@ -11341,19 +10861,13 @@
       <c r="O6" s="29">
         <v>0.2</v>
       </c>
-      <c r="P6" s="29">
-        <v>0.2</v>
-      </c>
-      <c r="Q6" s="29">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="29" t="s">
         <v>92</v>
       </c>
       <c r="B7" s="29" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="C7" s="6">
         <v>0</v>
@@ -11382,11 +10896,11 @@
       <c r="K7" s="6">
         <v>0</v>
       </c>
-      <c r="L7" s="6">
-        <v>0</v>
-      </c>
-      <c r="M7" s="6">
-        <v>0</v>
+      <c r="L7" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="M7" s="29">
+        <v>0.5</v>
       </c>
       <c r="N7" s="29">
         <v>0.5</v>
@@ -11394,19 +10908,13 @@
       <c r="O7" s="29">
         <v>0.5</v>
       </c>
-      <c r="P7" s="29">
-        <v>0.5</v>
-      </c>
-      <c r="Q7" s="29">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="29" t="s">
         <v>93</v>
       </c>
       <c r="B8" s="29" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="C8" s="6">
         <v>0</v>
@@ -11435,11 +10943,11 @@
       <c r="K8" s="6">
         <v>0</v>
       </c>
-      <c r="L8" s="6">
-        <v>0</v>
-      </c>
-      <c r="M8" s="6">
-        <v>0</v>
+      <c r="L8" s="29">
+        <v>0.59</v>
+      </c>
+      <c r="M8" s="29">
+        <v>0.59</v>
       </c>
       <c r="N8" s="29">
         <v>0.59</v>
@@ -11447,19 +10955,13 @@
       <c r="O8" s="29">
         <v>0.59</v>
       </c>
-      <c r="P8" s="29">
-        <v>0.59</v>
-      </c>
-      <c r="Q8" s="29">
-        <v>0.59</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="29" t="s">
         <v>94</v>
       </c>
       <c r="B9" s="29" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C9" s="6">
         <v>0</v>
@@ -11488,11 +10990,11 @@
       <c r="K9" s="6">
         <v>0</v>
       </c>
-      <c r="L9" s="6">
-        <v>0</v>
-      </c>
-      <c r="M9" s="6">
-        <v>0</v>
+      <c r="L9" s="29">
+        <v>0.8</v>
+      </c>
+      <c r="M9" s="29">
+        <v>0.8</v>
       </c>
       <c r="N9" s="29">
         <v>0.8</v>
@@ -11500,19 +11002,13 @@
       <c r="O9" s="29">
         <v>0.8</v>
       </c>
-      <c r="P9" s="29">
-        <v>0.8</v>
-      </c>
-      <c r="Q9" s="29">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="29" t="s">
         <v>95</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="C10" s="6">
         <v>0</v>
@@ -11541,11 +11037,11 @@
       <c r="K10" s="6">
         <v>0</v>
       </c>
-      <c r="L10" s="6">
-        <v>0</v>
-      </c>
-      <c r="M10" s="6">
-        <v>0</v>
+      <c r="L10" s="29">
+        <v>0.95</v>
+      </c>
+      <c r="M10" s="29">
+        <v>0.95</v>
       </c>
       <c r="N10" s="29">
         <v>0.95</v>
@@ -11553,19 +11049,13 @@
       <c r="O10" s="29">
         <v>0.95</v>
       </c>
-      <c r="P10" s="29">
-        <v>0.95</v>
-      </c>
-      <c r="Q10" s="29">
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="29" t="s">
         <v>96</v>
       </c>
       <c r="B11" s="29" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="C11" s="6">
         <v>0</v>
@@ -11594,11 +11084,11 @@
       <c r="K11" s="6">
         <v>0</v>
       </c>
-      <c r="L11" s="6">
-        <v>0</v>
-      </c>
-      <c r="M11" s="6">
-        <v>0</v>
+      <c r="L11" s="29">
+        <v>0.8</v>
+      </c>
+      <c r="M11" s="29">
+        <v>0.8</v>
       </c>
       <c r="N11" s="29">
         <v>0.8</v>
@@ -11606,19 +11096,13 @@
       <c r="O11" s="29">
         <v>0.8</v>
       </c>
-      <c r="P11" s="29">
-        <v>0.8</v>
-      </c>
-      <c r="Q11" s="29">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="29" t="s">
         <v>97</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="C12" s="6">
         <v>0</v>
@@ -11647,11 +11131,11 @@
       <c r="K12" s="6">
         <v>0</v>
       </c>
-      <c r="L12" s="6">
-        <v>0</v>
-      </c>
-      <c r="M12" s="6">
-        <v>0</v>
+      <c r="L12" s="29">
+        <v>0.9</v>
+      </c>
+      <c r="M12" s="29">
+        <v>0.9</v>
       </c>
       <c r="N12" s="29">
         <v>0.9</v>
@@ -11659,12 +11143,12 @@
       <c r="O12" s="29">
         <v>0.9</v>
       </c>
-      <c r="P12" s="29">
-        <v>0.9</v>
-      </c>
-      <c r="Q12" s="29">
-        <v>0.9</v>
-      </c>
+    </row>
+    <row r="19" spans="8:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H19" s="41"/>
+      <c r="I19" s="41"/>
+      <c r="J19" s="41"/>
+      <c r="K19" s="41"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -11677,8 +11161,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -11823,7 +11307,7 @@
         <v>99</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C2" s="32">
         <v>1</v>
@@ -11845,7 +11329,7 @@
     <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A3" s="38"/>
       <c r="B3" s="23" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C3" s="32">
         <v>1</v>
@@ -11867,7 +11351,7 @@
     <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4" s="34"/>
       <c r="B4" s="23" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C4" s="32">
         <v>1</v>
@@ -11889,7 +11373,7 @@
     <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5" s="34"/>
       <c r="B5" s="23" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="C5" s="32">
         <v>1</v>
@@ -11911,7 +11395,7 @@
     <row r="6" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A6" s="34"/>
       <c r="B6" s="33" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C6" s="32">
         <v>7.8159999999999993E-2</v>
@@ -11935,7 +11419,7 @@
         <v>103</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C7" s="32">
         <v>1</v>
@@ -11959,7 +11443,7 @@
         <v>102</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="C8" s="32">
         <v>1</v>
@@ -11983,7 +11467,7 @@
         <v>100</v>
       </c>
       <c r="B9" s="34" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C9" s="32">
         <v>1</v>
@@ -12007,7 +11491,7 @@
         <v>101</v>
       </c>
       <c r="B10" s="34" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C10" s="32">
         <v>0.33</v>
@@ -12144,7 +11628,7 @@
         <v>99</v>
       </c>
       <c r="B2" s="39" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C2" s="23">
         <v>0</v>
@@ -12164,7 +11648,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B3" s="39" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C3" s="23">
         <v>0</v>
@@ -12185,7 +11669,7 @@
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="40"/>
       <c r="B4" s="39" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C4" s="23">
         <v>0</v>
@@ -12206,7 +11690,7 @@
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="40"/>
       <c r="B5" s="39" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="C5" s="23">
         <v>0</v>
@@ -12227,7 +11711,7 @@
     <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="40"/>
       <c r="B6" s="30" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C6" s="23">
         <v>0</v>
@@ -12250,7 +11734,7 @@
         <v>103</v>
       </c>
       <c r="B7" s="39" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C7" s="23">
         <v>0</v>
@@ -12273,7 +11757,7 @@
         <v>102</v>
       </c>
       <c r="B8" s="39" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="C8" s="23">
         <v>0</v>
@@ -12296,7 +11780,7 @@
         <v>100</v>
       </c>
       <c r="B9" s="40" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C9" s="23">
         <v>0</v>
@@ -12319,7 +11803,7 @@
         <v>101</v>
       </c>
       <c r="B10" s="40" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C10" s="23">
         <v>0</v>
@@ -12345,15 +11829,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:M1"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -12363,38 +11847,32 @@
       <c r="C1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="D1" t="s">
         <v>126</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="E1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G1" t="s">
+        <v>142</v>
+      </c>
+      <c r="H1" t="s">
         <v>127</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="I1" t="s">
         <v>128</v>
       </c>
-      <c r="G1" s="41" t="s">
+      <c r="J1" t="s">
         <v>129</v>
       </c>
-      <c r="H1" s="41" t="s">
+      <c r="K1" t="s">
         <v>130</v>
       </c>
-      <c r="I1" s="41" t="s">
-        <v>131</v>
-      </c>
-      <c r="J1" s="41" t="s">
-        <v>132</v>
-      </c>
-      <c r="K1" s="41" t="s">
-        <v>133</v>
-      </c>
-      <c r="L1" s="41" t="s">
-        <v>134</v>
-      </c>
-      <c r="M1" s="41" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="7">
         <v>25.4</v>
       </c>
@@ -12417,21 +11895,15 @@
         <v>0.01</v>
       </c>
       <c r="H2">
-        <v>0.01</v>
+        <v>1.819</v>
       </c>
       <c r="I2">
-        <v>0.01</v>
+        <v>1.819</v>
       </c>
       <c r="J2">
         <v>1.819</v>
       </c>
       <c r="K2">
-        <v>1.819</v>
-      </c>
-      <c r="L2">
-        <v>1.819</v>
-      </c>
-      <c r="M2">
         <v>1.819</v>
       </c>
     </row>
@@ -12444,10 +11916,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P31"/>
+  <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -12455,7 +11927,7 @@
     <col min="1" max="1" width="28.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -12474,38 +11946,32 @@
       <c r="F1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="41" t="s">
+      <c r="G1" t="s">
         <v>126</v>
       </c>
-      <c r="H1" s="41" t="s">
+      <c r="H1" t="s">
+        <v>140</v>
+      </c>
+      <c r="I1" t="s">
+        <v>141</v>
+      </c>
+      <c r="J1" t="s">
+        <v>142</v>
+      </c>
+      <c r="K1" t="s">
         <v>127</v>
       </c>
-      <c r="I1" s="41" t="s">
+      <c r="L1" t="s">
         <v>128</v>
       </c>
-      <c r="J1" s="41" t="s">
+      <c r="M1" t="s">
         <v>129</v>
       </c>
-      <c r="K1" s="41" t="s">
+      <c r="N1" t="s">
         <v>130</v>
       </c>
-      <c r="L1" s="41" t="s">
-        <v>131</v>
-      </c>
-      <c r="M1" s="41" t="s">
-        <v>132</v>
-      </c>
-      <c r="N1" s="41" t="s">
-        <v>133</v>
-      </c>
-      <c r="O1" s="41" t="s">
-        <v>134</v>
-      </c>
-      <c r="P1" s="41" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="2" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -12548,14 +12014,8 @@
       <c r="N2" s="6">
         <v>0</v>
       </c>
-      <c r="O2" s="6">
-        <v>0</v>
-      </c>
-      <c r="P2" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -12598,14 +12058,8 @@
       <c r="N3" s="6">
         <v>0</v>
       </c>
-      <c r="O3" s="6">
-        <v>0</v>
-      </c>
-      <c r="P3" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -12648,14 +12102,8 @@
       <c r="N4" s="6">
         <v>0</v>
       </c>
-      <c r="O4" s="6">
-        <v>0</v>
-      </c>
-      <c r="P4" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -12698,14 +12146,8 @@
       <c r="N5" s="6">
         <v>0</v>
       </c>
-      <c r="O5" s="6">
-        <v>0</v>
-      </c>
-      <c r="P5" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -12748,14 +12190,8 @@
       <c r="N6" s="6">
         <v>0</v>
       </c>
-      <c r="O6" s="6">
-        <v>0</v>
-      </c>
-      <c r="P6" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -12798,14 +12234,8 @@
       <c r="N7" s="6">
         <v>0</v>
       </c>
-      <c r="O7" s="6">
-        <v>0</v>
-      </c>
-      <c r="P7" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -12848,14 +12278,8 @@
       <c r="N8" s="6">
         <v>0</v>
       </c>
-      <c r="O8" s="6">
-        <v>0</v>
-      </c>
-      <c r="P8" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -12898,14 +12322,8 @@
       <c r="N9" s="6">
         <v>0</v>
       </c>
-      <c r="O9" s="6">
-        <v>0</v>
-      </c>
-      <c r="P9" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -12948,14 +12366,8 @@
       <c r="N10" s="6">
         <v>0</v>
       </c>
-      <c r="O10" s="6">
-        <v>0</v>
-      </c>
-      <c r="P10" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -12998,14 +12410,8 @@
       <c r="N11" s="6">
         <v>0</v>
       </c>
-      <c r="O11" s="6">
-        <v>0</v>
-      </c>
-      <c r="P11" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>37</v>
       </c>
@@ -13048,14 +12454,8 @@
       <c r="N12" s="6">
         <v>0</v>
       </c>
-      <c r="O12" s="6">
-        <v>0</v>
-      </c>
-      <c r="P12" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>38</v>
       </c>
@@ -13098,14 +12498,8 @@
       <c r="N13" s="6">
         <v>0</v>
       </c>
-      <c r="O13" s="6">
-        <v>0</v>
-      </c>
-      <c r="P13" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="14" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -13148,14 +12542,8 @@
       <c r="N14" s="6">
         <v>0</v>
       </c>
-      <c r="O14" s="6">
-        <v>0</v>
-      </c>
-      <c r="P14" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="15" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>40</v>
       </c>
@@ -13198,14 +12586,8 @@
       <c r="N15" s="6">
         <v>0</v>
       </c>
-      <c r="O15" s="6">
-        <v>0</v>
-      </c>
-      <c r="P15" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="16" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>41</v>
       </c>
@@ -13248,14 +12630,8 @@
       <c r="N16" s="6">
         <v>0</v>
       </c>
-      <c r="O16" s="6">
-        <v>0</v>
-      </c>
-      <c r="P16" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="17" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>42</v>
       </c>
@@ -13298,14 +12674,8 @@
       <c r="N17" s="6">
         <v>0</v>
       </c>
-      <c r="O17" s="6">
-        <v>0</v>
-      </c>
-      <c r="P17" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>43</v>
       </c>
@@ -13348,16 +12718,10 @@
       <c r="N18" s="6">
         <v>0</v>
       </c>
-      <c r="O18" s="6">
-        <v>0</v>
-      </c>
-      <c r="P18" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="19" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="23" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="B19" s="6">
         <v>0</v>
@@ -13386,11 +12750,11 @@
       <c r="J19" s="6">
         <v>0</v>
       </c>
-      <c r="K19" s="6">
-        <v>0</v>
-      </c>
-      <c r="L19" s="6">
-        <v>0</v>
+      <c r="K19" s="24">
+        <v>2.5897E-2</v>
+      </c>
+      <c r="L19" s="24">
+        <v>2.5897E-2</v>
       </c>
       <c r="M19" s="24">
         <v>2.5897E-2</v>
@@ -13398,16 +12762,10 @@
       <c r="N19" s="24">
         <v>2.5897E-2</v>
       </c>
-      <c r="O19" s="24">
-        <v>2.5897E-2</v>
-      </c>
-      <c r="P19" s="24">
-        <v>2.5897E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="20" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="23" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B20" s="6">
         <v>0</v>
@@ -13436,11 +12794,11 @@
       <c r="J20" s="6">
         <v>0</v>
       </c>
-      <c r="K20" s="6">
-        <v>0</v>
-      </c>
-      <c r="L20" s="6">
-        <v>0</v>
+      <c r="K20" s="24">
+        <v>7.1409999999999998E-3</v>
+      </c>
+      <c r="L20" s="24">
+        <v>7.1409999999999998E-3</v>
       </c>
       <c r="M20" s="24">
         <v>7.1409999999999998E-3</v>
@@ -13448,16 +12806,10 @@
       <c r="N20" s="24">
         <v>7.1409999999999998E-3</v>
       </c>
-      <c r="O20" s="24">
-        <v>7.1409999999999998E-3</v>
-      </c>
-      <c r="P20" s="24">
-        <v>7.1409999999999998E-3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="23" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B21" s="6">
         <v>0</v>
@@ -13486,11 +12838,11 @@
       <c r="J21" s="6">
         <v>0</v>
       </c>
-      <c r="K21" s="6">
-        <v>0</v>
-      </c>
-      <c r="L21" s="6">
-        <v>0</v>
+      <c r="K21" s="24">
+        <v>0.255942</v>
+      </c>
+      <c r="L21" s="24">
+        <v>0.255942</v>
       </c>
       <c r="M21" s="24">
         <v>0.255942</v>
@@ -13498,16 +12850,10 @@
       <c r="N21" s="24">
         <v>0.255942</v>
       </c>
-      <c r="O21" s="24">
-        <v>0.255942</v>
-      </c>
-      <c r="P21" s="24">
-        <v>0.255942</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="23" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B22" s="6">
         <v>0</v>
@@ -13536,11 +12882,11 @@
       <c r="J22" s="6">
         <v>0</v>
       </c>
-      <c r="K22" s="6">
-        <v>0</v>
-      </c>
-      <c r="L22" s="6">
-        <v>0</v>
+      <c r="K22" s="24">
+        <v>0.146367</v>
+      </c>
+      <c r="L22" s="24">
+        <v>0.146367</v>
       </c>
       <c r="M22" s="24">
         <v>0.146367</v>
@@ -13548,16 +12894,10 @@
       <c r="N22" s="24">
         <v>0.146367</v>
       </c>
-      <c r="O22" s="24">
-        <v>0.146367</v>
-      </c>
-      <c r="P22" s="24">
-        <v>0.146367</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="23" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B23" s="6">
         <v>0</v>
@@ -13586,11 +12926,11 @@
       <c r="J23" s="6">
         <v>0</v>
       </c>
-      <c r="K23" s="6">
-        <v>0</v>
-      </c>
-      <c r="L23" s="6">
-        <v>0</v>
+      <c r="K23" s="24">
+        <v>1.7554E-2</v>
+      </c>
+      <c r="L23" s="24">
+        <v>1.7554E-2</v>
       </c>
       <c r="M23" s="24">
         <v>1.7554E-2</v>
@@ -13598,16 +12938,10 @@
       <c r="N23" s="24">
         <v>1.7554E-2</v>
       </c>
-      <c r="O23" s="24">
-        <v>1.7554E-2</v>
-      </c>
-      <c r="P23" s="24">
-        <v>1.7554E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="23" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B24" s="6">
         <v>0</v>
@@ -13636,11 +12970,11 @@
       <c r="J24" s="6">
         <v>0</v>
       </c>
-      <c r="K24" s="6">
-        <v>0</v>
-      </c>
-      <c r="L24" s="6">
-        <v>0</v>
+      <c r="K24" s="24">
+        <v>1.8078E-2</v>
+      </c>
+      <c r="L24" s="24">
+        <v>1.8078E-2</v>
       </c>
       <c r="M24" s="24">
         <v>1.8078E-2</v>
@@ -13648,16 +12982,10 @@
       <c r="N24" s="24">
         <v>1.8078E-2</v>
       </c>
-      <c r="O24" s="24">
-        <v>1.8078E-2</v>
-      </c>
-      <c r="P24" s="24">
-        <v>1.8078E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="23" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="B25" s="6">
         <v>0</v>
@@ -13686,11 +13014,11 @@
       <c r="J25" s="6">
         <v>0</v>
       </c>
-      <c r="K25" s="6">
-        <v>0</v>
-      </c>
-      <c r="L25" s="6">
-        <v>0</v>
+      <c r="K25" s="24">
+        <v>1.1440000000000001E-2</v>
+      </c>
+      <c r="L25" s="24">
+        <v>1.1440000000000001E-2</v>
       </c>
       <c r="M25" s="24">
         <v>1.1440000000000001E-2</v>
@@ -13698,16 +13026,10 @@
       <c r="N25" s="24">
         <v>1.1440000000000001E-2</v>
       </c>
-      <c r="O25" s="24">
-        <v>1.1440000000000001E-2</v>
-      </c>
-      <c r="P25" s="24">
-        <v>1.1440000000000001E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="23" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="B26" s="6">
         <v>0</v>
@@ -13736,11 +13058,11 @@
       <c r="J26" s="6">
         <v>0</v>
       </c>
-      <c r="K26" s="6">
-        <v>0</v>
-      </c>
-      <c r="L26" s="6">
-        <v>0</v>
+      <c r="K26" s="24">
+        <v>0.15128800000000001</v>
+      </c>
+      <c r="L26" s="24">
+        <v>0.15128800000000001</v>
       </c>
       <c r="M26" s="24">
         <v>0.15128800000000001</v>
@@ -13748,16 +13070,10 @@
       <c r="N26" s="24">
         <v>0.15128800000000001</v>
       </c>
-      <c r="O26" s="24">
-        <v>0.15128800000000001</v>
-      </c>
-      <c r="P26" s="24">
-        <v>0.15128800000000001</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="23" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="B27" s="6">
         <v>0</v>
@@ -13786,11 +13102,11 @@
       <c r="J27" s="6">
         <v>0</v>
       </c>
-      <c r="K27" s="6">
-        <v>0</v>
-      </c>
-      <c r="L27" s="6">
-        <v>0</v>
+      <c r="K27" s="24">
+        <v>0.36629299999999998</v>
+      </c>
+      <c r="L27" s="24">
+        <v>0.36629299999999998</v>
       </c>
       <c r="M27" s="24">
         <v>0.36629299999999998</v>
@@ -13798,14 +13114,8 @@
       <c r="N27" s="24">
         <v>0.36629299999999998</v>
       </c>
-      <c r="O27" s="24">
-        <v>0.36629299999999998</v>
-      </c>
-      <c r="P27" s="24">
-        <v>0.36629299999999998</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>110</v>
       </c>
@@ -13836,11 +13146,11 @@
       <c r="J28" s="9">
         <v>0.25</v>
       </c>
-      <c r="K28" s="9">
-        <v>0.25</v>
-      </c>
-      <c r="L28" s="9">
-        <v>0.25</v>
+      <c r="K28" s="51">
+        <v>0</v>
+      </c>
+      <c r="L28" s="51">
+        <v>0</v>
       </c>
       <c r="M28" s="51">
         <v>0</v>
@@ -13848,14 +13158,8 @@
       <c r="N28" s="51">
         <v>0</v>
       </c>
-      <c r="O28" s="51">
-        <v>0</v>
-      </c>
-      <c r="P28" s="51">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="29" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>111</v>
       </c>
@@ -13886,11 +13190,11 @@
       <c r="J29" s="9">
         <v>0.25</v>
       </c>
-      <c r="K29" s="9">
-        <v>0.25</v>
-      </c>
-      <c r="L29" s="9">
-        <v>0.25</v>
+      <c r="K29" s="51">
+        <v>0</v>
+      </c>
+      <c r="L29" s="51">
+        <v>0</v>
       </c>
       <c r="M29" s="51">
         <v>0</v>
@@ -13898,14 +13202,8 @@
       <c r="N29" s="51">
         <v>0</v>
       </c>
-      <c r="O29" s="51">
-        <v>0</v>
-      </c>
-      <c r="P29" s="51">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="30" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>112</v>
       </c>
@@ -13936,11 +13234,11 @@
       <c r="J30" s="9">
         <v>0.5</v>
       </c>
-      <c r="K30" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="L30" s="9">
-        <v>0.5</v>
+      <c r="K30" s="51">
+        <v>0</v>
+      </c>
+      <c r="L30" s="51">
+        <v>0</v>
       </c>
       <c r="M30" s="51">
         <v>0</v>
@@ -13948,15 +13246,9 @@
       <c r="N30" s="51">
         <v>0</v>
       </c>
-      <c r="O30" s="51">
-        <v>0</v>
-      </c>
-      <c r="P30" s="51">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="M31" s="51"/>
+    </row>
+    <row r="31" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="K31" s="51"/>
     </row>
   </sheetData>
   <phoneticPr fontId="14" type="noConversion"/>
@@ -14338,71 +13630,65 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>17</v>
       </c>
       <c r="B1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="D1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="E1" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="F1" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="41" t="s">
+      <c r="G1" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="41" t="s">
+      <c r="H1" t="s">
         <v>126</v>
       </c>
-      <c r="I1" s="41" t="s">
+      <c r="I1" t="s">
+        <v>140</v>
+      </c>
+      <c r="J1" t="s">
+        <v>141</v>
+      </c>
+      <c r="K1" t="s">
+        <v>142</v>
+      </c>
+      <c r="L1" t="s">
         <v>127</v>
       </c>
-      <c r="J1" s="41" t="s">
+      <c r="M1" t="s">
         <v>128</v>
       </c>
-      <c r="K1" s="41" t="s">
+      <c r="N1" t="s">
         <v>129</v>
       </c>
-      <c r="L1" s="41" t="s">
+      <c r="O1" t="s">
         <v>130</v>
       </c>
-      <c r="M1" s="41" t="s">
-        <v>131</v>
-      </c>
-      <c r="N1" s="41" t="s">
-        <v>132</v>
-      </c>
-      <c r="O1" s="41" t="s">
-        <v>133</v>
-      </c>
-      <c r="P1" s="41" t="s">
-        <v>134</v>
-      </c>
-      <c r="Q1" s="41" t="s">
-        <v>135</v>
-      </c>
-      <c r="R1" s="41" t="s">
+      <c r="P1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>105</v>
       </c>
@@ -14451,14 +13737,8 @@
       <c r="P2">
         <v>50</v>
       </c>
-      <c r="Q2">
-        <v>50</v>
-      </c>
-      <c r="R2">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.15">
       <c r="B3" t="s">
         <v>107</v>
       </c>
@@ -14467,7 +13747,7 @@
         <v>50</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:M3" si="0">100-D2</f>
+        <f t="shared" ref="D3:K3" si="0">100-D2</f>
         <v>50</v>
       </c>
       <c r="E3">
@@ -14499,11 +13779,9 @@
         <v>50</v>
       </c>
       <c r="L3">
-        <f t="shared" si="0"/>
         <v>50</v>
       </c>
       <c r="M3">
-        <f t="shared" si="0"/>
         <v>50</v>
       </c>
       <c r="N3">
@@ -14513,12 +13791,6 @@
         <v>50</v>
       </c>
       <c r="P3">
-        <v>50</v>
-      </c>
-      <c r="Q3">
-        <v>50</v>
-      </c>
-      <c r="R3">
         <v>50</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed linked cells in interventions birth outcomes tab
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Jan/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Jan/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-45080" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" firstSheet="26" activeTab="33"/>
+    <workbookView xWindow="-45080" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" firstSheet="24" activeTab="26"/>
   </bookViews>
   <sheets>
     <sheet name="demographics" sheetId="1" r:id="rId1"/>
@@ -186,6 +186,38 @@
     <author>Sam</author>
   </authors>
   <commentList>
+    <comment ref="C3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Sam:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Assuming all PW age groups have same target pop value</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments11.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Sam</author>
+  </authors>
+  <commentList>
     <comment ref="H2" authorId="0">
       <text>
         <r>
@@ -205,38 +237,6 @@
           </rPr>
           <t xml:space="preserve">
 WRA all fictional</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments11.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Sam</author>
-  </authors>
-  <commentList>
-    <comment ref="A2" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>Sam:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">
-Fictional values</t>
         </r>
       </text>
     </comment>
@@ -346,6 +346,38 @@
     <author>Sam</author>
   </authors>
   <commentList>
+    <comment ref="A2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Sam:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Fictional values</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments16.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Sam</author>
+  </authors>
+  <commentList>
     <comment ref="H2" authorId="0">
       <text>
         <r>
@@ -372,7 +404,7 @@
 </comments>
 </file>
 
-<file path=xl/comments16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments17.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Ruth</author>
@@ -448,7 +480,7 @@
 </comments>
 </file>
 
-<file path=xl/comments17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments18.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Ruth</author>
@@ -7748,7 +7780,7 @@
   <dimension ref="A1:O32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -9310,11 +9342,11 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -9366,13 +9398,13 @@
       <c r="B3" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="20" t="e">
-        <f>demographics!$B$6 * 'Interventions target population'!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D3" s="20" t="e">
-        <f>demographics!$B$6 * 'Interventions target population'!#REF!</f>
-        <v>#REF!</v>
+      <c r="C3" s="20">
+        <f>demographics!$B$6 * 'Interventions target population'!$K$6</f>
+        <v>0.22719999999999999</v>
+      </c>
+      <c r="D3" s="20">
+        <f>demographics!$B$6 * 'Interventions target population'!$K$6</f>
+        <v>0.22719999999999999</v>
       </c>
       <c r="E3" s="20">
         <v>0</v>
@@ -9420,6 +9452,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -11161,7 +11194,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
removed general population for fortification anemai interventions. Added fortification RR/OR in sub-populations instead.
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Jan/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Jan/InputForCode_Bangladesh.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-33220" yWindow="-2320" windowWidth="25600" windowHeight="14680" tabRatio="500" firstSheet="15" activeTab="17"/>
+    <workbookView xWindow="-64100" yWindow="-4440" windowWidth="25720" windowHeight="16900" tabRatio="500" firstSheet="18" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="demographics" sheetId="1" r:id="rId1"/>
@@ -1171,7 +1171,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="143">
   <si>
     <t>indicators</t>
   </si>
@@ -1753,7 +1753,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="134">
+  <cellStyleXfs count="136">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1770,6 +1770,8 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2001,7 +2003,7 @@
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="134">
+  <cellStyles count="136">
     <cellStyle name="Excel Built-in Normal" xfId="15"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -2069,6 +2071,7 @@
     <cellStyle name="Followed Hyperlink" xfId="129" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="131" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="133" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="135" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2135,6 +2138,7 @@
     <cellStyle name="Hyperlink" xfId="128" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="130" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="132" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="134" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6114,7 +6118,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -6365,10 +6369,10 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O10"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="O1" sqref="O1:O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -6376,7 +6380,7 @@
     <col min="1" max="1" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>56</v>
       </c>
@@ -6419,11 +6423,8 @@
       <c r="N1" t="s">
         <v>130</v>
       </c>
-      <c r="O1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15">
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>78</v>
       </c>
@@ -6466,11 +6467,8 @@
       <c r="N2">
         <v>0.3</v>
       </c>
-      <c r="O2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15">
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
         <v>113</v>
       </c>
@@ -6513,11 +6511,8 @@
       <c r="N3">
         <v>0.83</v>
       </c>
-      <c r="O3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15">
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
         <v>118</v>
       </c>
@@ -6560,11 +6555,8 @@
       <c r="N4">
         <v>1</v>
       </c>
-      <c r="O4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15">
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" t="s">
         <v>119</v>
       </c>
@@ -6607,11 +6599,8 @@
       <c r="N5">
         <v>1</v>
       </c>
-      <c r="O5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15">
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" t="s">
         <v>120</v>
       </c>
@@ -6654,11 +6643,8 @@
       <c r="N6">
         <v>1</v>
       </c>
-      <c r="O6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15">
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" t="s">
         <v>121</v>
       </c>
@@ -6701,11 +6687,8 @@
       <c r="N7">
         <v>1</v>
       </c>
-      <c r="O7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15">
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" t="s">
         <v>122</v>
       </c>
@@ -6748,11 +6731,8 @@
       <c r="N8">
         <v>1</v>
       </c>
-      <c r="O8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15">
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" t="s">
         <v>123</v>
       </c>
@@ -6795,11 +6775,8 @@
       <c r="N9">
         <v>1</v>
       </c>
-      <c r="O9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15">
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" t="s">
         <v>124</v>
       </c>
@@ -6840,9 +6817,6 @@
         <v>1</v>
       </c>
       <c r="N10">
-        <v>1</v>
-      </c>
-      <c r="O10">
         <v>1</v>
       </c>
     </row>
@@ -6861,8 +6835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -6913,9 +6887,6 @@
       <c r="N1" t="s">
         <v>130</v>
       </c>
-      <c r="O1" t="s">
-        <v>114</v>
-      </c>
     </row>
     <row r="2" spans="1:15">
       <c r="A2" t="s">
@@ -6927,42 +6898,40 @@
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
-      <c r="M2">
-        <v>1</v>
-      </c>
-      <c r="N2">
-        <v>1</v>
-      </c>
-      <c r="O2" s="42">
+      <c r="D2" s="42">
         <v>0.97599999999999998</v>
       </c>
+      <c r="E2" s="42">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="F2" s="42">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="G2" s="42">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="H2" s="42">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="I2" s="42">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="J2" s="42">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="K2" s="42">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="L2" s="42">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="M2" s="42">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="N2" s="42">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="O2" s="42"/>
     </row>
     <row r="3" spans="1:15">
       <c r="A3" t="s">
@@ -6974,42 +6943,40 @@
       <c r="C3">
         <v>1</v>
       </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-      <c r="K3">
-        <v>1</v>
-      </c>
-      <c r="L3">
-        <v>1</v>
-      </c>
-      <c r="M3">
-        <v>1</v>
-      </c>
-      <c r="N3">
-        <v>1</v>
-      </c>
-      <c r="O3" s="42">
+      <c r="D3" s="42">
         <v>0.97599999999999998</v>
       </c>
+      <c r="E3" s="42">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="F3" s="42">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="G3" s="42">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="H3" s="42">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="I3" s="42">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="J3" s="42">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="K3" s="42">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="L3" s="42">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="M3" s="42">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="N3" s="42">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="O3" s="42"/>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" t="s">
@@ -7021,42 +6988,40 @@
       <c r="C4">
         <v>1</v>
       </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-      <c r="J4">
-        <v>1</v>
-      </c>
-      <c r="K4">
-        <v>1</v>
-      </c>
-      <c r="L4">
-        <v>1</v>
-      </c>
-      <c r="M4">
-        <v>1</v>
-      </c>
-      <c r="N4">
-        <v>1</v>
-      </c>
-      <c r="O4" s="42">
+      <c r="D4" s="42">
         <v>0.97599999999999998</v>
       </c>
+      <c r="E4" s="42">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="F4" s="42">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="G4" s="42">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="H4" s="42">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="I4" s="42">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="J4" s="42">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="K4" s="42">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="L4" s="42">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="M4" s="42">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="N4" s="42">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="O4" s="42"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>